<commit_message>
Update on 20181116.1325 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RCommands" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="162">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -547,12 +547,152 @@
     <t>add all modified files to local repo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>strsplit()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>strsplit("a_b_c","_")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>split out "_"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sub()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sub("_",'",c("a_b","b_c","c_d"))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>replace "_" with ""</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gsub()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gsub("_","","Take_this_lesson")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>replace all "_" with "", note sub() only replace the first "_"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grep()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grep("Course",c("Coursera","None","ChineseCourse"))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>find the location where the element contains "Course"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grepl()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grepl("Course",c("Coursera","None","ChineseCourse"))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return logical values for each element indicating whether the element contains "Course"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grep("Course",c("Coursera","None","ChineseCourse"), value=TRUE)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the elements which contains "Course"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: stringr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nchar()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nchar("Jeffrey Leek")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the number of the characters contained</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>substr()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>substr("Jeffrey Leek",1,7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subset the string from the 1st character to the 7th one</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paste()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paste("Jeffrey","Leek")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>put the two strings togerther, separated by SPACE in default</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>put the two strings togerther, separated by "-"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paste("Jeffrey","Leek",sep="-")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paste0()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>put the two strings togerther, separated by nothing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paste0("Jeffrey","Leek")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>str_trim()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>str_trim("Jeffrey Leek       ")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>remove all the SPACE at the end of the string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -582,6 +722,12 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -604,8 +750,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -619,13 +768,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -905,470 +1057,689 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="99.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="E3" s="4"/>
       <c r="F3"/>
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
         <v>55</v>
       </c>
+      <c r="E4" s="4"/>
       <c r="F4"/>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="E5" s="4"/>
       <c r="F5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="4"/>
+      <c r="D7" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="1" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="1" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="1" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="1" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="2" t="s">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="1" t="s">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="2" t="s">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="4" t="s">
         <v>43</v>
       </c>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="2" t="s">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="4" t="s">
         <v>49</v>
       </c>
+      <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="4" t="s">
         <v>53</v>
       </c>
+      <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>61</v>
       </c>
+      <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="5"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="5"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="5"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="5"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="C28" s="4"/>
+      <c r="D28" s="4" t="s">
         <v>69</v>
       </c>
+      <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="4" t="s">
         <v>73</v>
       </c>
+      <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="4" t="s">
         <v>91</v>
       </c>
+      <c r="E30" s="4"/>
       <c r="F30"/>
     </row>
     <row r="31" spans="1:6" ht="54" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="5" t="s">
         <v>79</v>
       </c>
+      <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="6" t="s">
         <v>82</v>
       </c>
+      <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="4"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="C34" s="4"/>
+      <c r="D34" s="4" t="s">
         <v>84</v>
       </c>
+      <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="4" t="s">
         <v>88</v>
       </c>
+      <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="4" t="s">
         <v>94</v>
       </c>
+      <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="C37" s="4"/>
+      <c r="D37" s="4" t="s">
         <v>96</v>
       </c>
+      <c r="E37" s="4"/>
       <c r="F37"/>
     </row>
     <row r="38" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="C38" s="4"/>
+      <c r="D38" s="4" t="s">
         <v>98</v>
       </c>
+      <c r="E38" s="4"/>
       <c r="F38"/>
     </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E40" s="9"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F43"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="23">
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A11:A13"/>
     <mergeCell ref="D32:D33"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="B32:B33"/>
@@ -1383,11 +1754,6 @@
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="B23:B27"/>
     <mergeCell ref="A23:A27"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A11:A13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -1444,7 +1810,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="7" t="s">
         <v>107</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1455,7 +1821,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="3" t="s">
         <v>125</v>
       </c>
@@ -1491,7 +1857,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="7" t="s">
         <v>117</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1502,7 +1868,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="2" t="s">
         <v>120</v>
       </c>

</xml_diff>

<commit_message>
Update on 20181116.1521 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="172">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -685,6 +685,46 @@
   </si>
   <si>
     <t>remove all the SPACE at the end of the string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: lubridate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sys.getlocale()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sys.getlocale("LC_TIME")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view your locale, returns something like "zh_CN.UTF-8", "en_US.UTF-8"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>help()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>General</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>help(package = lubridate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bring up the help document of package lubridate, including a list of functions in the package</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>today()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return today's date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -750,7 +790,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -768,7 +808,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -776,8 +819,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1057,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1174,10 +1217,10 @@
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1186,20 +1229,20 @@
       <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
@@ -1217,10 +1260,10 @@
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1232,8 +1275,8 @@
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="4" t="s">
         <v>26</v>
       </c>
@@ -1243,8 +1286,8 @@
       <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
@@ -1254,10 +1297,10 @@
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1269,8 +1312,8 @@
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="4" t="s">
         <v>34</v>
       </c>
@@ -1280,10 +1323,10 @@
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -1295,8 +1338,8 @@
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="4" t="s">
         <v>39</v>
       </c>
@@ -1306,8 +1349,8 @@
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="4" t="s">
         <v>41</v>
       </c>
@@ -1317,8 +1360,8 @@
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="4" t="s">
         <v>44</v>
       </c>
@@ -1328,10 +1371,10 @@
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -1343,8 +1386,8 @@
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="4" t="s">
         <v>47</v>
       </c>
@@ -1369,46 +1412,46 @@
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="10" t="s">
         <v>61</v>
       </c>
       <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="7"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="8"/>
       <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="7"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="8"/>
       <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="7"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="8"/>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="7"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="8"/>
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1471,25 +1514,25 @@
       <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="10" t="s">
         <v>82</v>
       </c>
       <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
       <c r="E33" s="4"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1591,7 +1634,7 @@
       <c r="D40" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="E40" s="9"/>
+      <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
@@ -1609,10 +1652,10 @@
       <c r="E41" s="4"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="8" t="s">
         <v>136</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -1624,8 +1667,8 @@
       <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
       <c r="C43" s="4" t="s">
         <v>142</v>
       </c>
@@ -1678,10 +1721,10 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="8" t="s">
         <v>151</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -1692,8 +1735,8 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
       <c r="C48" s="4" t="s">
         <v>155</v>
       </c>
@@ -1701,7 +1744,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>144</v>
       </c>
@@ -1715,7 +1758,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>144</v>
       </c>
@@ -1729,13 +1772,48 @@
         <v>161</v>
       </c>
     </row>
+    <row r="51" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F51"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B8:B9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B11:B13"/>
@@ -1752,6 +1830,11 @@
     <mergeCell ref="D23:D27"/>
     <mergeCell ref="A16:A19"/>
     <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B8:B9"/>
     <mergeCell ref="B23:B27"/>
     <mergeCell ref="A23:A27"/>
   </mergeCells>
@@ -1810,7 +1893,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>107</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1821,7 +1904,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>125</v>
       </c>
@@ -1857,7 +1940,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>117</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1868,7 +1951,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="2" t="s">
         <v>120</v>
       </c>

</xml_diff>

<commit_message>
Update on 20181117.1730 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -17,6 +17,9 @@
     <sheet name="ShellCommands" sheetId="3" r:id="rId3"/>
     <sheet name="PythonCommands" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RCommands!$A$1:$A$71</definedName>
+  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="216">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -725,6 +728,185 @@
   </si>
   <si>
     <t>return today's date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Regular Expressions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>represent the start of a line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>represent the end of a line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>list a set of characters we will accept at a given point</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grepl("[Bb][Uu][Ss][Hh]",c("Bush", "BUSH", "bush")) will return T T T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pick one character in a range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grepl("^[^5]",c("56","36","5t")) returns F T F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>represent NOT, note that use[] to view ^ as NOT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grepl("^you think", c("you think", "Hi, you think)) returns T F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grepl("morning$",c("this morning","this morning!")) returns T F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grepl("[0-9][a-zA-Z]",c("7t","0H","H0")) will return T T F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>represent any character</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>|</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grepl("flood|fire|quake",c("flood!","fire!","earthquake!")) returns T T T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grepl("^good|bad",c("good day", "not bad")) returns T T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>represent the indicated expression is optional</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grepl("9.11",c("9-11","9 11","911")) returns T T F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Note that use [] or \\ to view . as character dot
+grepl("[^?.]$",c("haha.","haha?","haha")) returns F F T
+grepl("9\\.11",c("9-11","9 11","911")) returns F F F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>represent OR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grepl("^good|^bad",c("good day", "not bad", "ghost")) returns T T F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grepl("^(good|bad)",c("good day", "bad day", "gho")) returns T T F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Note that use \\ view ( as a character</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grepl("good( old)? day", c("good old day","good day") returns T T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>represent at least one time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grepl("[a-z]*",c("erv","234","","d23")) returns T T T T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grepl("[a-z]+",c("erv","234","","d23")) returns T F F T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grepl("go( +[^ ]+){1,2} d", c("go k d", "go d", "go k b d")) returns T F T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{min,max} specify the min and max number of matches of an expression</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{m} matches an expression exactly m times</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{m,} matches an expression at least m times</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grepl("go( +[^ ]+){2} d", c("go k d", "go d", "go k b d")) returns F F T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grepl("go( +[^ ]+){3,} d", c("go k d", "go d", "go k b q d")) returns F F T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>()\\1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grepl("2(35)\\1",c("235","23535","235 35","2353535")) returns F T F T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>()\\1 match the repetition expressed in the parenthesis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>represent any number of times, including 0.
+Match as many as possible, use ?, like *?, to turn off its greediness</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -790,7 +972,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -816,7 +998,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1100,17 +1288,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="72.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="99.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
@@ -1217,10 +1405,10 @@
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1229,20 +1417,20 @@
       <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="9"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
@@ -1260,10 +1448,10 @@
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1275,8 +1463,8 @@
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="4" t="s">
         <v>26</v>
       </c>
@@ -1286,8 +1474,8 @@
       <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
@@ -1297,10 +1485,10 @@
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1312,8 +1500,8 @@
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="4" t="s">
         <v>34</v>
       </c>
@@ -1323,10 +1511,10 @@
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="11" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -1338,8 +1526,8 @@
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="4" t="s">
         <v>39</v>
       </c>
@@ -1349,8 +1537,8 @@
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="4" t="s">
         <v>41</v>
       </c>
@@ -1360,8 +1548,8 @@
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="4" t="s">
         <v>44</v>
       </c>
@@ -1371,10 +1559,10 @@
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -1386,8 +1574,8 @@
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="4" t="s">
         <v>47</v>
       </c>
@@ -1412,46 +1600,46 @@
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="12" t="s">
         <v>61</v>
       </c>
       <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="8"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="11"/>
       <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="8"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="11"/>
       <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="8"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="11"/>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="8"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="11"/>
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1514,25 +1702,25 @@
       <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="12" t="s">
         <v>82</v>
       </c>
       <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
       <c r="E33" s="4"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1652,10 +1840,10 @@
       <c r="E41" s="4"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="11" t="s">
         <v>136</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -1667,8 +1855,8 @@
       <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
       <c r="C43" s="4" t="s">
         <v>142</v>
       </c>
@@ -1692,128 +1880,379 @@
       </c>
       <c r="E44" s="4"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="F45"/>
+    </row>
+    <row r="46" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F46"/>
+    </row>
+    <row r="47" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="F47"/>
+    </row>
+    <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="F48"/>
+    </row>
+    <row r="49" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="11"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="F49"/>
+    </row>
+    <row r="50" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="1:6" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="F51"/>
+    </row>
+    <row r="52" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F52"/>
+    </row>
+    <row r="53" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="11"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D53" s="11"/>
+      <c r="F53"/>
+    </row>
+    <row r="54" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="11"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D54" s="11"/>
+      <c r="F54"/>
+    </row>
+    <row r="55" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="11"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F55"/>
+    </row>
+    <row r="56" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F56"/>
+    </row>
+    <row r="57" spans="1:6" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A57" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="F57"/>
+    </row>
+    <row r="58" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="F58"/>
+    </row>
+    <row r="59" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F59"/>
+    </row>
+    <row r="60" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="11"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="F60"/>
+    </row>
+    <row r="61" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="11"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="F61"/>
+    </row>
+    <row r="62" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="F62"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="8" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B65" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="4" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="11"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D66" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C67" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D67" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D68" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="6" t="s">
+    <row r="69" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B69" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C69" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="D69" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="F51"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+      <c r="F69"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D70" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D71" s="1" t="s">
         <v>169</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="35">
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="A59:A61"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B11:B13"/>
@@ -1830,13 +2269,6 @@
     <mergeCell ref="D23:D27"/>
     <mergeCell ref="A16:A19"/>
     <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="A23:A27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -1893,7 +2325,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="11" t="s">
         <v>107</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1904,7 +2336,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="3" t="s">
         <v>125</v>
       </c>
@@ -1940,7 +2372,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="11" t="s">
         <v>117</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1951,7 +2383,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="2" t="s">
         <v>120</v>
       </c>

</xml_diff>

<commit_message>
Update on 20181117.2335 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -16,9 +16,10 @@
     <sheet name="GitCommands" sheetId="2" r:id="rId2"/>
     <sheet name="ShellCommands" sheetId="3" r:id="rId3"/>
     <sheet name="PythonCommands" sheetId="4" r:id="rId4"/>
+    <sheet name="Date Source Link" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RCommands!$A$1:$A$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RCommands!$A$1:$A$72</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="302">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -699,10 +700,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sys.getlocale("LC_TIME")</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>view your locale, returns something like "zh_CN.UTF-8", "en_US.UTF-8"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -907,6 +904,353 @@
   <si>
     <t>represent any number of times, including 0.
 Match as many as possible, use ?, like *?, to turn off its greediness</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time Operation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>date()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sys.Date()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the current date, Date class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sys.time()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the current date and time, POSIXct class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the current date and time as characters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>format()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>format the time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%d = day as number (0-31)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%a = abbreviated weekday</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%A = unabbreviated weekday</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%m = month (00-12)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%b = abbreviated month</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%B = unabbreviated month</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%y = 2 digit year</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%Y = 4 digit year</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>format(Sys.Date(), "%a %b %d")</t>
+  </si>
+  <si>
+    <t>as.Date()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sys.getlocale("LC_TIME")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>system("defaults write org.R-project.R force.LANG en_US.UTF-8")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>run this code, close, don't save, reopen, time format becomes en_US.UTF-8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>as.Date(c("1jan1960","2jan1960"), "%d%b%y")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>turn date in character format to Date class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>General</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>as.numeric()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transfer to numeric data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>weekdays()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>weekdays(Sys.Date())</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the weekday</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>months()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>months(Sys.Date())</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the month</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>julian()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>julian(Sys.Date())</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the number of days passed since the origin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ymd()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ymd("20140108")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transfer date time in character format to Date class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mdy()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mdy("08042013"); mdy("08/04/2013"); mdy("08-04-2013")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dmy()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dmy("03042013")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ymd_hms()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transfer time in character format to POSIXct class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ymd_hms("2011-08-03 10:15:03")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ymd_hms("2011-08-03 10:15:03", tz="Pacific/Auckland")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>using tz to set the time zone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wday()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wday(Sys.Date())</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the nth date in a week, count from Sunday</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wday(Sys.Date(),label=TRUE)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return weekday as order (factor) data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://cran.r-project.org/web/packages/lubridate/vignettes/lubridate.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Government</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Site</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>United Nations</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://data.un.org/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U.S.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.data.gov/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://data.gov.uk/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>France</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.data.gouv.fr/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ghana</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://data.gov.gh/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Australia</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://data.gov.au/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Germany</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.govdata.de/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://data.gov.hk/en-datasets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Japan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.data.go.jp/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.data.gov/opendatasites</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Many more</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.gapminder.org/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.asdfree.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>survey data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>infochimps marketplace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.infochimps.com/marketplace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kaggle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.kaggle.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jeff Hammerbacher</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.quora.com/Jeff-Hammerbacher/Introduction-to-Data-Science-Data-Sets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gregory Piatetsky-Shapiro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.kdnuggets.com/gps.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -972,7 +1316,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1001,14 +1345,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1288,10 +1638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1378,281 +1728,280 @@
       <c r="E5" s="4"/>
       <c r="F5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="4"/>
+    <row r="6" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="F6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E9" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="4" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B12" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="4" t="s">
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="4" t="s">
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B15" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="4" t="s">
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B17" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="4" t="s">
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="4" t="s">
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="4" t="s">
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B21" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="4" t="s">
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B24" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C24" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D24" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="11"/>
       <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="11"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="12"/>
       <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="11"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="12"/>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="11"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="12"/>
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="12"/>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1660,619 +2009,907 @@
         <v>62</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>72</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="C29" s="4"/>
       <c r="D29" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E30" s="4"/>
-      <c r="F30"/>
-    </row>
-    <row r="31" spans="1:6" ht="54" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+      <c r="E31" s="4"/>
+      <c r="F31"/>
+    </row>
+    <row r="32" spans="1:6" ht="54" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D32" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="11" t="s">
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B33" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C33" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D33" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
       <c r="E33" s="4"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
       <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>87</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D37" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="E37" s="4"/>
-      <c r="F37"/>
     </row>
     <row r="38" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>128</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="E39" s="4"/>
+      <c r="F39"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E40" s="7"/>
+        <v>129</v>
+      </c>
+      <c r="E40" s="4"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E41" s="7"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E41" s="4"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="11" t="s">
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B43" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E42" s="4"/>
-    </row>
-    <row r="43" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="4" t="s">
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="F43"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
+      <c r="F44"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E44" s="4"/>
-    </row>
-    <row r="45" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="11" t="s">
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B46" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="C46" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D46" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="F46"/>
+    </row>
+    <row r="47" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="F47"/>
+    </row>
+    <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C48" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="D45" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="F45"/>
-    </row>
-    <row r="46" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="11"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="F46"/>
-    </row>
-    <row r="47" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="B47" s="8" t="s">
+      <c r="D48" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="F48"/>
+    </row>
+    <row r="49" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="F49"/>
+    </row>
+    <row r="50" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="D47" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="F47"/>
-    </row>
-    <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="C48" s="8" t="s">
+      <c r="D50" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="D48" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="F48"/>
-    </row>
-    <row r="49" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="11"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="9" t="s">
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B51" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="D49" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="F49"/>
-    </row>
-    <row r="50" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="B50" s="11" t="s">
+      <c r="C51" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="D51" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="F51"/>
+    </row>
+    <row r="52" spans="1:6" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="F52"/>
+    </row>
+    <row r="53" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B53" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="F50"/>
-    </row>
-    <row r="51" spans="1:6" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A51" s="11"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="9" t="s">
+      <c r="C53" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D53" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="F51"/>
-    </row>
-    <row r="52" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="C52" s="8" t="s">
+      <c r="F53"/>
+    </row>
+    <row r="54" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="D54" s="12"/>
+      <c r="F54"/>
+    </row>
+    <row r="55" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="F52"/>
-    </row>
-    <row r="53" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="11"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="8" t="s">
+      <c r="D55" s="12"/>
+      <c r="F55"/>
+    </row>
+    <row r="56" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="12"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="F56"/>
+    </row>
+    <row r="57" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="D53" s="11"/>
-      <c r="F53"/>
-    </row>
-    <row r="54" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="11"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="D54" s="11"/>
-      <c r="F54"/>
-    </row>
-    <row r="55" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="11"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="D55" s="8" t="s">
+      <c r="C57" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="F55"/>
-    </row>
-    <row r="56" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="B56" s="8" t="s">
+      <c r="D57" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="F57"/>
+    </row>
+    <row r="58" spans="1:6" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A58" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B58" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="D56" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="F56"/>
-    </row>
-    <row r="57" spans="1:6" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A57" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="B57" s="8" t="s">
+      <c r="C58" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="F58"/>
+    </row>
+    <row r="59" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D59" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="C57" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="D57" s="9" t="s">
+      <c r="F59"/>
+    </row>
+    <row r="60" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="F60"/>
+    </row>
+    <row r="61" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="12"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F61"/>
+    </row>
+    <row r="62" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="12"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="F62"/>
+    </row>
+    <row r="63" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="F63"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B66" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="12"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="F70"/>
+    </row>
+    <row r="71" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="12"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="F71"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="F57"/>
-    </row>
-    <row r="58" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="F58"/>
-    </row>
-    <row r="59" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="F59"/>
-    </row>
-    <row r="60" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="11"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="F60"/>
-    </row>
-    <row r="61" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="11"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="F61"/>
-    </row>
-    <row r="62" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="F62"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="B65" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="11"/>
-      <c r="B66" s="11"/>
-      <c r="C66" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="F69"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
+      <c r="B73" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B76" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="12"/>
+      <c r="B77" s="12"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="12"/>
+      <c r="B78" s="12"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="12"/>
+      <c r="B79" s="12"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="12"/>
+      <c r="B80" s="12"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="12"/>
+      <c r="B81" s="12"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="12"/>
+      <c r="B82" s="12"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="12"/>
+      <c r="B83" s="12"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="12"/>
+      <c r="B84" s="12"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B89" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>169</v>
+      <c r="E89" s="14" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D90" s="12" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" s="12"/>
+      <c r="B91" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D91" s="12"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="12"/>
+      <c r="B92" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D92" s="12"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B93" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" s="12"/>
+      <c r="B94" s="12"/>
+      <c r="C94" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B95" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" s="12"/>
+      <c r="B96" s="12"/>
+      <c r="C96" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A21"/>
+  <mergeCells count="46">
+    <mergeCell ref="A90:A92"/>
+    <mergeCell ref="D90:D92"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="C76:C84"/>
+    <mergeCell ref="B76:B84"/>
+    <mergeCell ref="A76:A84"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="D24:D28"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="B53:B56"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1"/>
+    <hyperlink ref="E9" r:id="rId1"/>
+    <hyperlink ref="E89" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2325,7 +2962,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>107</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -2336,7 +2973,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="3" t="s">
         <v>125</v>
       </c>
@@ -2372,7 +3009,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="12" t="s">
         <v>117</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -2383,7 +3020,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="2" t="s">
         <v>120</v>
       </c>
@@ -2471,4 +3108,182 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" s="14"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" s="14" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="14"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="B12" r:id="rId10"/>
+    <hyperlink ref="B13" r:id="rId11"/>
+    <hyperlink ref="B14" r:id="rId12"/>
+    <hyperlink ref="B15" r:id="rId13"/>
+    <hyperlink ref="B16" r:id="rId14"/>
+    <hyperlink ref="B20" r:id="rId15"/>
+    <hyperlink ref="B19" r:id="rId16"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update on 20181118.1157 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -19,7 +19,7 @@
     <sheet name="Date Source Link" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RCommands!$A$1:$A$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RCommands!$A$1:$A$73</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="347">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -724,10 +724,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>return today's date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Regular Expressions</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1054,10 +1050,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ymd("20140108")</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>transfer date time in character format to Date class</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1074,10 +1066,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>dmy("03042013")</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ymd_hms()</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1252,6 +1240,195 @@
   <si>
     <t>http://www.kdnuggets.com/gps.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>year()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>month()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>day()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>year(today())</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>extract the year</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>month(today())</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>day(today())</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>extract the month</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>extract the day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>now()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return today's date as Date class (no hour, minute, second)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the current date and time (hour, minute, second) as POSIXct class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>minute()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>second()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hour()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hour(now())</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>minute(now())</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>second(now())</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>extract the hour</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>extract the minute</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>extract the second</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dmy("03042013"); dmy(03042013); dmy(3042013)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hms()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hms("03:03:03")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create time, period class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update(this_moment,hours = 8,mintes=8,seconds=8)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>modify the time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/List_of_tz_database_time_zones</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>now(tzone="America/New_York")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>days()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hours()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>minutes()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>now()+days(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>now()+hours(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>now()+minutes(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>time calculation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ymd("20140108",tz="Singapore")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interval()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>as.period()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create a time interval</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interval(ymd(20090201), ymd(20090101))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>as.period(interval(ymd(20090201), ymd(20090101)))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calculate the time diff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>find.package()</t>
+  </si>
+  <si>
+    <t>check all packages loaded</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.quantmod.com/</t>
+  </si>
+  <si>
+    <t>Quantitative Financial Modelling &amp; Trading Framework for R</t>
   </si>
 </sst>
 </file>
@@ -1316,7 +1493,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1349,7 +1526,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1357,8 +1537,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1638,10 +1818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F96"/>
+  <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1730,13 +1910,13 @@
     </row>
     <row r="6" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="D6" s="10" t="s">
         <v>240</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>241</v>
       </c>
       <c r="F6"/>
     </row>
@@ -1766,255 +1946,254 @@
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="F9"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E10" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="4" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="13"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="4" t="s">
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="4" t="s">
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B16" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="4" t="s">
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B18" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="4" t="s">
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="4" t="s">
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="4" t="s">
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B22" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="4" t="s">
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="12" t="s">
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B25" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C25" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D25" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="12"/>
       <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="12"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="13"/>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="12"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="13"/>
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="12"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="13"/>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="13"/>
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -2022,894 +2201,1108 @@
         <v>62</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>72</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="C30" s="4"/>
       <c r="D30" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E31" s="4"/>
-      <c r="F31"/>
-    </row>
-    <row r="32" spans="1:6" ht="54" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+      <c r="E32" s="4"/>
+      <c r="F32"/>
+    </row>
+    <row r="33" spans="1:6" ht="54" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D33" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B34" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C34" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D34" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="E33" s="4"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
       <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
       <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>87</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="C36" s="4"/>
       <c r="D36" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E37" s="4"/>
-    </row>
-    <row r="38" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="E38" s="4"/>
-      <c r="F38"/>
     </row>
     <row r="39" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>128</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="E40" s="4"/>
+      <c r="F40"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E41" s="7"/>
+        <v>129</v>
+      </c>
+      <c r="E41" s="4"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B42" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E42" s="7"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E42" s="4"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="12" t="s">
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B44" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E43" s="4"/>
-    </row>
-    <row r="44" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="4" t="s">
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="F44"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+      <c r="F45"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C46" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D46" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E45" s="4"/>
-    </row>
-    <row r="46" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="12" t="s">
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B47" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="C47" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="F47"/>
+    </row>
+    <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="F48"/>
+    </row>
+    <row r="49" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="D46" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="F46"/>
-    </row>
-    <row r="47" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="F47"/>
-    </row>
-    <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="B48" s="8" t="s">
+      <c r="D49" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="F49"/>
+    </row>
+    <row r="50" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="13"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="D48" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="F48"/>
-    </row>
-    <row r="49" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="C49" s="8" t="s">
+      <c r="D51" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="D49" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="F49"/>
-    </row>
-    <row r="50" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="9" t="s">
+      <c r="F51"/>
+    </row>
+    <row r="52" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B52" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D50" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="F50"/>
-    </row>
-    <row r="51" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="B51" s="12" t="s">
+      <c r="C52" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="D52" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="F52"/>
+    </row>
+    <row r="53" spans="1:6" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+      <c r="A53" s="13"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="F53"/>
+    </row>
+    <row r="54" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B54" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="F51"/>
-    </row>
-    <row r="52" spans="1:6" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="9" t="s">
+      <c r="C54" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D54" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="F52"/>
-    </row>
-    <row r="53" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="C53" s="8" t="s">
+      <c r="F54"/>
+    </row>
+    <row r="55" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="13"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D55" s="13"/>
+      <c r="F55"/>
+    </row>
+    <row r="56" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="13"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="F53"/>
-    </row>
-    <row r="54" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="8" t="s">
+      <c r="D56" s="13"/>
+      <c r="F56"/>
+    </row>
+    <row r="57" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="13"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="F57"/>
+    </row>
+    <row r="58" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B58" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="D54" s="12"/>
-      <c r="F54"/>
-    </row>
-    <row r="55" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="D55" s="12"/>
-      <c r="F55"/>
-    </row>
-    <row r="56" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="12"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="D56" s="8" t="s">
+      <c r="C58" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="F56"/>
-    </row>
-    <row r="57" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="B57" s="8" t="s">
+      <c r="D58" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="F58"/>
+    </row>
+    <row r="59" spans="1:6" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A59" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B59" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="D57" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="F57"/>
-    </row>
-    <row r="58" spans="1:6" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A58" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="B58" s="8" t="s">
+      <c r="C59" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="F59"/>
+    </row>
+    <row r="60" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="D60" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="C58" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="F58"/>
-    </row>
-    <row r="59" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="C59" s="8" t="s">
+      <c r="F60"/>
+    </row>
+    <row r="61" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B61" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="D59" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="F59"/>
-    </row>
-    <row r="60" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="B60" s="12" t="s">
+      <c r="C61" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="D61" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="D60" s="8" t="s">
+      <c r="F61"/>
+    </row>
+    <row r="62" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="13"/>
+      <c r="B62" s="13"/>
+      <c r="C62" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D62" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="F60"/>
-    </row>
-    <row r="61" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="12"/>
-      <c r="B61" s="12"/>
-      <c r="C61" s="8" t="s">
+      <c r="F62"/>
+    </row>
+    <row r="63" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="13"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="D63" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="F61"/>
-    </row>
-    <row r="62" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="12"/>
-      <c r="B62" s="12"/>
-      <c r="C62" s="8" t="s">
+      <c r="F63"/>
+    </row>
+    <row r="64" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B64" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="D62" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="F62"/>
-    </row>
-    <row r="63" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="B63" s="8" t="s">
+      <c r="C64" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="C63" s="8" t="s">
+      <c r="D64" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="D63" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="F63"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+      <c r="F64"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="12" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="B66" s="12" t="s">
+      <c r="B67" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="12"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="4" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="13"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D68" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C69" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D69" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D70" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="12" t="s">
+    <row r="71" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B70" s="12" t="s">
+      <c r="B71" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C71" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="F71"/>
+    </row>
+    <row r="72" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="13"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="D70" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="F70"/>
-    </row>
-    <row r="71" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="12"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="10" t="s">
+      <c r="D72" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="D71" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="F71"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>168</v>
-      </c>
+      <c r="F72"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="D74" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="D75" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="B76" s="12" t="s">
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="C77" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C76" s="12" t="s">
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="13"/>
+      <c r="B78" s="13"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="13"/>
+      <c r="B79" s="13"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="13"/>
+      <c r="B80" s="13"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="13"/>
+      <c r="B81" s="13"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="13"/>
+      <c r="B82" s="13"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="13"/>
+      <c r="B83" s="13"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="13"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="13"/>
+      <c r="B85" s="13"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D76" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="12"/>
-      <c r="B77" s="12"/>
-      <c r="C77" s="12"/>
-      <c r="D77" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="12"/>
-      <c r="B78" s="12"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="12"/>
-      <c r="B79" s="12"/>
-      <c r="C79" s="12"/>
-      <c r="D79" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="12"/>
-      <c r="B80" s="12"/>
-      <c r="C80" s="12"/>
-      <c r="D80" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" s="12"/>
-      <c r="B81" s="12"/>
-      <c r="C81" s="12"/>
-      <c r="D81" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82" s="12"/>
-      <c r="B82" s="12"/>
-      <c r="C82" s="12"/>
-      <c r="D82" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" s="12"/>
-      <c r="B83" s="12"/>
-      <c r="C83" s="12"/>
-      <c r="D83" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" s="12"/>
-      <c r="B84" s="12"/>
-      <c r="C84" s="12"/>
-      <c r="D84" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C85" s="1" t="s">
+      <c r="C86" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="D85" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="B86" s="1" t="s">
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="D87" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D86" s="1" t="s">
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="B87" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="D88" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D87" s="1" t="s">
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="B88" s="1" t="s">
+      <c r="C89" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="D89" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D88" s="1" t="s">
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E90" s="12" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B91" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="C91" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="D91" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="E91" s="12"/>
+      <c r="F91"/>
+    </row>
+    <row r="92" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B92" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="C92" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="D92" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="E92" s="12"/>
+      <c r="F92"/>
+    </row>
+    <row r="93" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B93" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="C93" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="D93" s="11" t="s">
+        <v>307</v>
+      </c>
+      <c r="E93" s="12"/>
+      <c r="F93"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
+      <c r="C94" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D94" s="13" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="13"/>
+      <c r="B95" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D95" s="13"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="13"/>
+      <c r="B96" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D96" s="13"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E89" s="14" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90" s="12" t="s">
+      <c r="B97" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="13"/>
+      <c r="B98" s="13"/>
+      <c r="C98" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="D90" s="12" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" s="12"/>
-      <c r="B91" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="D91" s="12"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" s="12"/>
-      <c r="B92" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D92" s="12"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" s="12" t="s">
+      <c r="B99" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="C99" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="D99" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="F99"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="B93" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="C93" s="1" t="s">
+      <c r="B100" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="D93" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" s="12"/>
-      <c r="B94" s="12"/>
-      <c r="C94" s="10" t="s">
+      <c r="C100" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="D100" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95" s="12" t="s">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="13"/>
+      <c r="B101" s="13"/>
+      <c r="C101" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="B95" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96" s="12"/>
-      <c r="B96" s="12"/>
-      <c r="C96" s="10" t="s">
-        <v>266</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>267</v>
+      <c r="B102" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="E102" s="12" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B104" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B105" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D107" s="13" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" s="13"/>
+      <c r="B108" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C108" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="D108" s="13"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" s="13"/>
+      <c r="B109" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C109" s="11" t="s">
+        <v>334</v>
+      </c>
+      <c r="D109" s="13"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C110" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="A90:A92"/>
-    <mergeCell ref="D90:D92"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="C76:C84"/>
-    <mergeCell ref="B76:B84"/>
-    <mergeCell ref="A76:A84"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="A70:A71"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C24:C28"/>
-    <mergeCell ref="D24:D28"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="B53:B56"/>
+  <mergeCells count="48">
+    <mergeCell ref="A107:A109"/>
+    <mergeCell ref="D107:D109"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="D54:D56"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="D25:D29"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="C77:C85"/>
+    <mergeCell ref="B77:B85"/>
+    <mergeCell ref="A77:A85"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="A94:A96"/>
+    <mergeCell ref="D94:D96"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="B100:B101"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1"/>
-    <hyperlink ref="E89" r:id="rId2"/>
+    <hyperlink ref="E10" r:id="rId1"/>
+    <hyperlink ref="E90" r:id="rId2"/>
+    <hyperlink ref="E102" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2962,7 +3355,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>107</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -2973,7 +3366,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="3" t="s">
         <v>125</v>
       </c>
@@ -3009,7 +3402,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="13" t="s">
         <v>117</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -3020,7 +3413,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="2" t="s">
         <v>120</v>
       </c>
@@ -3114,155 +3507,160 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.83203125" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>272</v>
+        <v>268</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>274</v>
+        <v>270</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>276</v>
+        <v>272</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>278</v>
+        <v>274</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>280</v>
+        <v>276</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>282</v>
+        <v>278</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>283</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>284</v>
+        <v>280</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>285</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>286</v>
+        <v>282</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>288</v>
+        <v>284</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B11" s="14"/>
+      <c r="B11" s="12"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>290</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B13" s="14" t="s">
-        <v>291</v>
+      <c r="B13" s="12" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>292</v>
+        <v>290</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>295</v>
+        <v>291</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>297</v>
+        <v>293</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>301</v>
+        <v>297</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>299</v>
+        <v>295</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="14"/>
+      <c r="A22" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>345</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Update on 20181121.1633 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -19,7 +19,7 @@
     <sheet name="Date Source Link" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RCommands!$A$1:$A$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RCommands!$A$1:$A$74</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="393">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1429,6 +1429,189 @@
   </si>
   <si>
     <t>Quantitative Financial Modelling &amp; Trading Framework for R</t>
+  </si>
+  <si>
+    <t>:set number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:set nonumber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ls -a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>list all files, including hidden files under the directory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>move to the end of a line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>display line number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>un-display line number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>move to the top of a file</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>move to the bottom of a file</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>w</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>move backward to the begin letter of a word</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>move forward to the begin letter of a word</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>move to the begin of a line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>move (not remove) all displays away, so as to leave a tidy screen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>General</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>object.size()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>print(object.size(Var1),units="Mb")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>display how many memories in Mb have been taken up by the variable Var1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storage.mode()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>display Var1's storage mode; change its storage mode to be "integer"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storage.mode(Var1); storage.mode(Var1) &lt;- "integer"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ctrl+shift+C</t>
+  </si>
+  <si>
+    <t>highlight multiple lines and comment or un-comment in one shot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RStudio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>file.edit()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>file.edit("filename.R")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>open filename.R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gc()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>release the space taken up by the removed variables and display the usage of memory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>source()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>source("filename.R")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>excute filename.R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>View()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>View(Var1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>open Var1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1493,7 +1676,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1534,11 +1717,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1818,10 +2004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F111"/>
+  <dimension ref="A1:F118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1864,948 +2050,949 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="4"/>
+      <c r="B3" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>386</v>
+      </c>
       <c r="F3"/>
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4"/>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>66</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5"/>
     </row>
-    <row r="6" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6"/>
+    </row>
+    <row r="7" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B7" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="F6"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="4"/>
+      <c r="F7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B10" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D10" s="11" t="s">
         <v>344</v>
       </c>
-      <c r="F9"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+      <c r="F10"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E11" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="4" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="14"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B14" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="4" t="s">
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="4" t="s">
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B17" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="4" t="s">
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B19" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="4" t="s">
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="4" t="s">
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="4" t="s">
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="13" t="s">
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B23" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="4" t="s">
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="13" t="s">
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B26" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C26" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D26" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="13"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
       <c r="C27" s="15"/>
-      <c r="D27" s="13"/>
+      <c r="D27" s="14"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
       <c r="C28" s="15"/>
-      <c r="D28" s="13"/>
+      <c r="D28" s="14"/>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="15"/>
-      <c r="D29" s="13"/>
+      <c r="D29" s="14"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4" t="s">
-        <v>69</v>
-      </c>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="14"/>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>72</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="C31" s="4"/>
       <c r="D31" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E32" s="4"/>
-      <c r="F32"/>
-    </row>
-    <row r="33" spans="1:6" ht="54" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+      <c r="E33" s="4"/>
+      <c r="F33"/>
+    </row>
+    <row r="34" spans="1:6" ht="54" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E33" s="4"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="13" t="s">
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B35" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C35" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D35" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
       <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
       <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>87</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E37" s="4"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="E39" s="4"/>
-      <c r="F39"/>
     </row>
     <row r="40" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>128</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="E41" s="4"/>
+      <c r="F41"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E42" s="7"/>
+        <v>129</v>
+      </c>
+      <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B43" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E43" s="4"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="13" t="s">
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B45" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E44" s="4"/>
-    </row>
-    <row r="45" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="4" t="s">
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="14"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D46" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="F45"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+      <c r="F46"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C47" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D47" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E46" s="4"/>
-    </row>
-    <row r="47" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="13" t="s">
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B48" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C48" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D48" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="F47"/>
-    </row>
-    <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="9" t="s">
+      <c r="F48"/>
+    </row>
+    <row r="49" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="14"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D49" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="F48"/>
-    </row>
-    <row r="49" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
+      <c r="F49"/>
+    </row>
+    <row r="50" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B50" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C50" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D50" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="F49"/>
-    </row>
-    <row r="50" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="13" t="s">
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B51" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C51" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D51" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="F50"/>
-    </row>
-    <row r="51" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="13"/>
-      <c r="B51" s="13"/>
-      <c r="C51" s="9" t="s">
+      <c r="F51"/>
+    </row>
+    <row r="52" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="14"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D52" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="F51"/>
-    </row>
-    <row r="52" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="13" t="s">
+      <c r="F52"/>
+    </row>
+    <row r="53" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B52" s="13" t="s">
+      <c r="B53" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C53" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D53" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="F52"/>
-    </row>
-    <row r="53" spans="1:6" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A53" s="13"/>
-      <c r="B53" s="13"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="9" t="s">
+      <c r="F53"/>
+    </row>
+    <row r="54" spans="1:6" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+      <c r="A54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="F53"/>
-    </row>
-    <row r="54" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="13" t="s">
+      <c r="F54"/>
+    </row>
+    <row r="55" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B55" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C55" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="D54" s="13" t="s">
+      <c r="D55" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="F54"/>
-    </row>
-    <row r="55" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="13"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="8" t="s">
+      <c r="F55"/>
+    </row>
+    <row r="56" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="14"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="D55" s="13"/>
-      <c r="F55"/>
-    </row>
-    <row r="56" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="13"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="8" t="s">
+      <c r="D56" s="14"/>
+      <c r="F56"/>
+    </row>
+    <row r="57" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="14"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="D56" s="13"/>
-      <c r="F56"/>
-    </row>
-    <row r="57" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="13"/>
-      <c r="B57" s="13"/>
-      <c r="C57" s="8" t="s">
+      <c r="D57" s="14"/>
+      <c r="F57"/>
+    </row>
+    <row r="58" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="14"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="D57" s="8" t="s">
+      <c r="D58" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="F57"/>
-    </row>
-    <row r="58" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>190</v>
-      </c>
       <c r="F58"/>
     </row>
-    <row r="59" spans="1:6" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
         <v>170</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>213</v>
+        <v>197</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>190</v>
       </c>
       <c r="F59"/>
     </row>
-    <row r="60" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
         <v>170</v>
       </c>
       <c r="B60" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="F60"/>
+    </row>
+    <row r="61" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B61" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="C61" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="D60" s="8" t="s">
+      <c r="D61" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="F60"/>
-    </row>
-    <row r="61" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="13" t="s">
+      <c r="F61"/>
+    </row>
+    <row r="62" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B62" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C62" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="D62" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="F61"/>
-    </row>
-    <row r="62" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="13"/>
-      <c r="B62" s="13"/>
-      <c r="C62" s="8" t="s">
+      <c r="F62"/>
+    </row>
+    <row r="63" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="14"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="D63" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="F62"/>
-    </row>
-    <row r="63" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="13"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="8" t="s">
+      <c r="F63"/>
+    </row>
+    <row r="64" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="14"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="D63" s="8" t="s">
+      <c r="D64" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="F63"/>
-    </row>
-    <row r="64" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="8" t="s">
+      <c r="F64"/>
+    </row>
+    <row r="65" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B65" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="C65" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="D65" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="F64"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
+      <c r="F65"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="13" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="B67" s="13" t="s">
+      <c r="B68" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D68" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="13"/>
-      <c r="B68" s="13"/>
-      <c r="C68" s="4" t="s">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="14"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D69" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C70" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D70" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D71" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="13" t="s">
+    <row r="72" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B71" s="13" t="s">
+      <c r="B72" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C72" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="D71" s="6" t="s">
+      <c r="D72" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="F71"/>
-    </row>
-    <row r="72" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="13"/>
-      <c r="B72" s="13"/>
-      <c r="C72" s="10" t="s">
+      <c r="F72"/>
+    </row>
+    <row r="73" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="14"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="D72" s="10" t="s">
+      <c r="D73" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="F72"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>168</v>
-      </c>
+      <c r="F73"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D75" s="1" t="s">
         <v>220</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -2813,116 +3000,113 @@
         <v>214</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D77" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="13" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="B77" s="13" t="s">
+      <c r="B78" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="C77" s="13" t="s">
+      <c r="C78" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="13"/>
-      <c r="B78" s="13"/>
-      <c r="C78" s="13"/>
-      <c r="D78" s="1" t="s">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="14"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="14"/>
+      <c r="D79" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="13"/>
-      <c r="B79" s="13"/>
-      <c r="C79" s="13"/>
-      <c r="D79" s="1" t="s">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="14"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="13"/>
-      <c r="B80" s="13"/>
-      <c r="C80" s="13"/>
-      <c r="D80" s="1" t="s">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="14"/>
+      <c r="B81" s="14"/>
+      <c r="C81" s="14"/>
+      <c r="D81" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="13"/>
-      <c r="B81" s="13"/>
-      <c r="C81" s="13"/>
-      <c r="D81" s="1" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="14"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="14"/>
+      <c r="D82" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="13"/>
-      <c r="B82" s="13"/>
-      <c r="C82" s="13"/>
-      <c r="D82" s="1" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="14"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="14"/>
+      <c r="D83" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="13"/>
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
-      <c r="D83" s="1" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="14"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="14"/>
+      <c r="D84" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="13"/>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="1" t="s">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="14"/>
+      <c r="B85" s="14"/>
+      <c r="C85" s="14"/>
+      <c r="D85" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="13"/>
-      <c r="B85" s="13"/>
-      <c r="C85" s="13"/>
-      <c r="D85" s="1" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="14"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B87" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C87" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="D87" s="1" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -2930,13 +3114,13 @@
         <v>214</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
@@ -2944,57 +3128,55 @@
         <v>214</v>
       </c>
       <c r="B89" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C90" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D90" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D91" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="E90" s="12" t="s">
+      <c r="E91" s="12" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B91" s="11" t="s">
-        <v>299</v>
-      </c>
-      <c r="C91" s="11" t="s">
-        <v>302</v>
-      </c>
-      <c r="D91" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="E91" s="12"/>
-      <c r="F91"/>
     </row>
     <row r="92" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
         <v>162</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E92" s="12"/>
       <c r="F92"/>
@@ -3004,129 +3186,128 @@
         <v>162</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E93" s="12"/>
       <c r="F93"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" s="13" t="s">
+    <row r="94" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="C94" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="D94" s="11" t="s">
+        <v>307</v>
+      </c>
+      <c r="E94" s="12"/>
+      <c r="F94"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C95" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="D94" s="13" t="s">
+      <c r="D95" s="14" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="13"/>
-      <c r="B95" s="1" t="s">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="14"/>
+      <c r="B96" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D95" s="13"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="13"/>
-      <c r="B96" s="1" t="s">
+      <c r="D96" s="14"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="14"/>
+      <c r="B97" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="D96" s="13"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="13" t="s">
+      <c r="D97" s="14"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="B97" s="13" t="s">
+      <c r="B98" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C98" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="D98" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98" s="13"/>
-      <c r="B98" s="13"/>
-      <c r="C98" s="10" t="s">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="14"/>
+      <c r="B99" s="14"/>
+      <c r="C99" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="D99" s="1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="99" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="11" t="s">
+    <row r="100" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="B99" s="11" t="s">
+      <c r="B100" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="C99" s="11" t="s">
+      <c r="C100" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="D99" s="11" t="s">
+      <c r="D100" s="11" t="s">
         <v>323</v>
       </c>
-      <c r="F99"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="13" t="s">
+      <c r="F100"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="B100" s="13" t="s">
+      <c r="B101" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C101" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="D101" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="13"/>
-      <c r="B101" s="13"/>
-      <c r="C101" s="10" t="s">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="14"/>
+      <c r="B102" s="14"/>
+      <c r="C102" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="D102" s="1" t="s">
         <v>264</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="E102" s="12" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
@@ -3134,27 +3315,30 @@
         <v>162</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>314</v>
+        <v>328</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>317</v>
+        <v>310</v>
+      </c>
+      <c r="E103" s="12" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="B104" s="11" t="s">
-        <v>311</v>
+      <c r="B104" s="1" t="s">
+        <v>313</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -3162,147 +3346,242 @@
         <v>162</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B106" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="C107" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="D107" s="1" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A107" s="13" t="s">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B108" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C108" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="D107" s="13" t="s">
+      <c r="D108" s="14" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108" s="13"/>
-      <c r="B108" s="1" t="s">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" s="14"/>
+      <c r="B109" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="C108" s="11" t="s">
+      <c r="C109" s="11" t="s">
         <v>333</v>
       </c>
-      <c r="D108" s="13"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A109" s="13"/>
-      <c r="B109" s="1" t="s">
+      <c r="D109" s="14"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" s="14"/>
+      <c r="B110" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="C109" s="11" t="s">
+      <c r="C110" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="D109" s="13"/>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A110" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C110" s="11" t="s">
-        <v>340</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>339</v>
-      </c>
+      <c r="D110" s="14"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
         <v>162</v>
       </c>
       <c r="B111" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C111" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C112" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="D111" s="1" t="s">
+      <c r="D112" s="1" t="s">
         <v>342</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="B115" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>392</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A107:A109"/>
-    <mergeCell ref="D107:D109"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="D54:D56"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C25:C29"/>
-    <mergeCell ref="D25:D29"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="C77:C85"/>
-    <mergeCell ref="B77:B85"/>
-    <mergeCell ref="A77:A85"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="A94:A96"/>
-    <mergeCell ref="D94:D96"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="B100:B101"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="A101:A102"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="A108:A110"/>
+    <mergeCell ref="D108:D110"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="D55:D57"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="C78:C86"/>
+    <mergeCell ref="B78:B86"/>
+    <mergeCell ref="A78:A86"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="A95:A97"/>
+    <mergeCell ref="D95:D97"/>
+    <mergeCell ref="B98:B99"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E10" r:id="rId1"/>
-    <hyperlink ref="E90" r:id="rId2"/>
-    <hyperlink ref="E102" r:id="rId3"/>
+    <hyperlink ref="E11" r:id="rId1"/>
+    <hyperlink ref="E91" r:id="rId2"/>
+    <hyperlink ref="E103" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3355,7 +3634,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="14" t="s">
         <v>107</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -3366,7 +3645,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="3" t="s">
         <v>125</v>
       </c>
@@ -3402,7 +3681,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="14" t="s">
         <v>117</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -3413,7 +3692,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="2" t="s">
         <v>120</v>
       </c>
@@ -3435,33 +3714,147 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="10.83203125" style="13"/>
+    <col min="2" max="2" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="B6" s="13">
+        <v>0</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="18" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20181121.2331 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="403">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1611,6 +1611,46 @@
   </si>
   <si>
     <t>open Var1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nrow()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nrow(Data frame A)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get the rows of A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ncol()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ncol(Data frame A)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get the columns of A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: reshape2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>melt()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mtcars$car &lt;- rownames(mtcars); mtcarsMelt &lt;- melt(mtcars)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reshape data frame mtcars into 3 columns: [id, variables, value]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2004,10 +2044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F118"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -3524,6 +3564,48 @@
       </c>
       <c r="D118" s="1" t="s">
         <v>392</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update on 20181123.1043 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -2046,8 +2046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:C30"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A38" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update on 20181124.0942 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="RCommands" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="ShellCommands" sheetId="3" r:id="rId3"/>
     <sheet name="PythonCommands" sheetId="4" r:id="rId4"/>
     <sheet name="Date Source Link" sheetId="5" r:id="rId5"/>
+    <sheet name="HPCCommands" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RCommands!$A$1:$A$74</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="406">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1651,6 +1652,18 @@
   </si>
   <si>
     <t>reshape data frame mtcars into 3 columns: [id, variables, value]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mail -s "YOUR EMAIL SUBJECT" YOUR EMAIL ADDRESS &lt;&lt;&lt; 'YOUR EMAIL CONTENT'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">send an email </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mail</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1716,7 +1729,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1761,10 +1774,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2046,7 +2062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A53" workbookViewId="0">
       <selection activeCell="A38" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -2197,10 +2213,10 @@
       <c r="F10"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -2214,8 +2230,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
@@ -2240,10 +2256,10 @@
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -2255,8 +2271,8 @@
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="4" t="s">
         <v>26</v>
       </c>
@@ -2266,8 +2282,8 @@
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="4" t="s">
         <v>28</v>
       </c>
@@ -2277,10 +2293,10 @@
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="15" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -2292,8 +2308,8 @@
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="4" t="s">
         <v>34</v>
       </c>
@@ -2303,10 +2319,10 @@
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -2318,8 +2334,8 @@
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="4" t="s">
         <v>39</v>
       </c>
@@ -2329,8 +2345,8 @@
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="4" t="s">
         <v>41</v>
       </c>
@@ -2340,8 +2356,8 @@
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="4" t="s">
         <v>44</v>
       </c>
@@ -2351,10 +2367,10 @@
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="15" t="s">
         <v>45</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -2366,8 +2382,8 @@
       <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="4" t="s">
         <v>47</v>
       </c>
@@ -2392,46 +2408,46 @@
       <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="17" t="s">
         <v>61</v>
       </c>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="14"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="15"/>
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="14"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="15"/>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="14"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="15"/>
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="14"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="15"/>
       <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -2494,25 +2510,25 @@
       <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="17" t="s">
         <v>82</v>
       </c>
       <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
       <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -2632,10 +2648,10 @@
       <c r="E44" s="4"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="15" t="s">
         <v>136</v>
       </c>
       <c r="C45" s="4" t="s">
@@ -2647,8 +2663,8 @@
       <c r="E45" s="4"/>
     </row>
     <row r="46" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="14"/>
-      <c r="B46" s="14"/>
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
       <c r="C46" s="4" t="s">
         <v>142</v>
       </c>
@@ -2673,10 +2689,10 @@
       <c r="E47" s="4"/>
     </row>
     <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="14" t="s">
+      <c r="A48" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="15" t="s">
         <v>171</v>
       </c>
       <c r="C48" s="9" t="s">
@@ -2688,8 +2704,8 @@
       <c r="F48"/>
     </row>
     <row r="49" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="14"/>
-      <c r="B49" s="14"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="15"/>
       <c r="C49" s="9" t="s">
         <v>179</v>
       </c>
@@ -2714,10 +2730,10 @@
       <c r="F50"/>
     </row>
     <row r="51" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="14" t="s">
+      <c r="A51" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="15" t="s">
         <v>175</v>
       </c>
       <c r="C51" s="8" t="s">
@@ -2729,8 +2745,8 @@
       <c r="F51"/>
     </row>
     <row r="52" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="14"/>
-      <c r="B52" s="14"/>
+      <c r="A52" s="15"/>
+      <c r="B52" s="15"/>
       <c r="C52" s="9" t="s">
         <v>183</v>
       </c>
@@ -2740,13 +2756,13 @@
       <c r="F52"/>
     </row>
     <row r="53" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="C53" s="15" t="s">
+      <c r="C53" s="17" t="s">
         <v>191</v>
       </c>
       <c r="D53" s="8" t="s">
@@ -2755,50 +2771,50 @@
       <c r="F53"/>
     </row>
     <row r="54" spans="1:6" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A54" s="14"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="15"/>
+      <c r="A54" s="15"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="17"/>
       <c r="D54" s="9" t="s">
         <v>192</v>
       </c>
       <c r="F54"/>
     </row>
     <row r="55" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="14" t="s">
+      <c r="A55" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="15" t="s">
         <v>186</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D55" s="15" t="s">
         <v>193</v>
       </c>
       <c r="F55"/>
     </row>
     <row r="56" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="14"/>
-      <c r="B56" s="14"/>
+      <c r="A56" s="15"/>
+      <c r="B56" s="15"/>
       <c r="C56" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="D56" s="14"/>
+      <c r="D56" s="15"/>
       <c r="F56"/>
     </row>
     <row r="57" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="14"/>
-      <c r="B57" s="14"/>
+      <c r="A57" s="15"/>
+      <c r="B57" s="15"/>
       <c r="C57" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="D57" s="14"/>
+      <c r="D57" s="15"/>
       <c r="F57"/>
     </row>
     <row r="58" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="14"/>
-      <c r="B58" s="14"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="15"/>
       <c r="C58" s="8" t="s">
         <v>195</v>
       </c>
@@ -2853,10 +2869,10 @@
       <c r="F61"/>
     </row>
     <row r="62" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="14" t="s">
+      <c r="A62" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="15" t="s">
         <v>203</v>
       </c>
       <c r="C62" s="8" t="s">
@@ -2868,8 +2884,8 @@
       <c r="F62"/>
     </row>
     <row r="63" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="14"/>
-      <c r="B63" s="14"/>
+      <c r="A63" s="15"/>
+      <c r="B63" s="15"/>
       <c r="C63" s="8" t="s">
         <v>208</v>
       </c>
@@ -2879,8 +2895,8 @@
       <c r="F63"/>
     </row>
     <row r="64" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="14"/>
-      <c r="B64" s="14"/>
+      <c r="A64" s="15"/>
+      <c r="B64" s="15"/>
       <c r="C64" s="8" t="s">
         <v>209</v>
       </c>
@@ -2933,10 +2949,10 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="14" t="s">
+      <c r="A68" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="B68" s="14" t="s">
+      <c r="B68" s="15" t="s">
         <v>151</v>
       </c>
       <c r="C68" s="1" t="s">
@@ -2947,8 +2963,8 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="14"/>
-      <c r="B69" s="14"/>
+      <c r="A69" s="15"/>
+      <c r="B69" s="15"/>
       <c r="C69" s="4" t="s">
         <v>155</v>
       </c>
@@ -2985,10 +3001,10 @@
       </c>
     </row>
     <row r="72" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="14" t="s">
+      <c r="A72" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B72" s="14" t="s">
+      <c r="B72" s="15" t="s">
         <v>163</v>
       </c>
       <c r="C72" s="6" t="s">
@@ -3000,8 +3016,8 @@
       <c r="F72"/>
     </row>
     <row r="73" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="14"/>
-      <c r="B73" s="14"/>
+      <c r="A73" s="15"/>
+      <c r="B73" s="15"/>
       <c r="C73" s="10" t="s">
         <v>234</v>
       </c>
@@ -3058,13 +3074,13 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="14" t="s">
+      <c r="A78" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="B78" s="14" t="s">
+      <c r="B78" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="C78" s="14" t="s">
+      <c r="C78" s="15" t="s">
         <v>231</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -3072,65 +3088,65 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="14"/>
-      <c r="B79" s="14"/>
-      <c r="C79" s="14"/>
+      <c r="A79" s="15"/>
+      <c r="B79" s="15"/>
+      <c r="C79" s="15"/>
       <c r="D79" s="1" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="14"/>
-      <c r="B80" s="14"/>
-      <c r="C80" s="14"/>
+      <c r="A80" s="15"/>
+      <c r="B80" s="15"/>
+      <c r="C80" s="15"/>
       <c r="D80" s="1" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="14"/>
-      <c r="B81" s="14"/>
-      <c r="C81" s="14"/>
+      <c r="A81" s="15"/>
+      <c r="B81" s="15"/>
+      <c r="C81" s="15"/>
       <c r="D81" s="1" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="14"/>
-      <c r="B82" s="14"/>
-      <c r="C82" s="14"/>
+      <c r="A82" s="15"/>
+      <c r="B82" s="15"/>
+      <c r="C82" s="15"/>
       <c r="D82" s="1" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="14"/>
-      <c r="B83" s="14"/>
-      <c r="C83" s="14"/>
+      <c r="A83" s="15"/>
+      <c r="B83" s="15"/>
+      <c r="C83" s="15"/>
       <c r="D83" s="1" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="14"/>
-      <c r="B84" s="14"/>
-      <c r="C84" s="14"/>
+      <c r="A84" s="15"/>
+      <c r="B84" s="15"/>
+      <c r="C84" s="15"/>
       <c r="D84" s="1" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="14"/>
-      <c r="B85" s="14"/>
-      <c r="C85" s="14"/>
+      <c r="A85" s="15"/>
+      <c r="B85" s="15"/>
+      <c r="C85" s="15"/>
       <c r="D85" s="1" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="14"/>
-      <c r="B86" s="14"/>
-      <c r="C86" s="14"/>
+      <c r="A86" s="15"/>
+      <c r="B86" s="15"/>
+      <c r="C86" s="15"/>
       <c r="D86" s="1" t="s">
         <v>230</v>
       </c>
@@ -3254,7 +3270,7 @@
       <c r="F94"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="14" t="s">
+      <c r="A95" s="15" t="s">
         <v>162</v>
       </c>
       <c r="B95" s="1" t="s">
@@ -3263,35 +3279,35 @@
       <c r="C95" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="D95" s="14" t="s">
+      <c r="D95" s="15" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="14"/>
+      <c r="A96" s="15"/>
       <c r="B96" s="1" t="s">
         <v>252</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D96" s="14"/>
+      <c r="D96" s="15"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="14"/>
+      <c r="A97" s="15"/>
       <c r="B97" s="1" t="s">
         <v>254</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="D97" s="14"/>
+      <c r="D97" s="15"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98" s="14" t="s">
+      <c r="A98" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="B98" s="14" t="s">
+      <c r="B98" s="15" t="s">
         <v>255</v>
       </c>
       <c r="C98" s="1" t="s">
@@ -3302,8 +3318,8 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99" s="14"/>
-      <c r="B99" s="14"/>
+      <c r="A99" s="15"/>
+      <c r="B99" s="15"/>
       <c r="C99" s="10" t="s">
         <v>258</v>
       </c>
@@ -3327,10 +3343,10 @@
       <c r="F100"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="14" t="s">
+      <c r="A101" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="B101" s="14" t="s">
+      <c r="B101" s="15" t="s">
         <v>260</v>
       </c>
       <c r="C101" s="1" t="s">
@@ -3341,8 +3357,8 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102" s="14"/>
-      <c r="B102" s="14"/>
+      <c r="A102" s="15"/>
+      <c r="B102" s="15"/>
       <c r="C102" s="10" t="s">
         <v>263</v>
       </c>
@@ -3424,7 +3440,7 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108" s="14" t="s">
+      <c r="A108" s="15" t="s">
         <v>162</v>
       </c>
       <c r="B108" s="1" t="s">
@@ -3433,29 +3449,29 @@
       <c r="C108" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="D108" s="14" t="s">
+      <c r="D108" s="15" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A109" s="14"/>
+      <c r="A109" s="15"/>
       <c r="B109" s="1" t="s">
         <v>330</v>
       </c>
       <c r="C109" s="11" t="s">
         <v>333</v>
       </c>
-      <c r="D109" s="14"/>
+      <c r="D109" s="15"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A110" s="14"/>
+      <c r="A110" s="15"/>
       <c r="B110" s="1" t="s">
         <v>331</v>
       </c>
       <c r="C110" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="D110" s="14"/>
+      <c r="D110" s="15"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
@@ -3610,6 +3626,38 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A108:A110"/>
+    <mergeCell ref="D108:D110"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="D55:D57"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="C78:C86"/>
+    <mergeCell ref="B78:B86"/>
+    <mergeCell ref="A78:A86"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="A95:A97"/>
+    <mergeCell ref="D95:D97"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A45:A46"/>
     <mergeCell ref="A98:A99"/>
     <mergeCell ref="A101:A102"/>
     <mergeCell ref="B101:B102"/>
@@ -3626,38 +3674,6 @@
     <mergeCell ref="B19:B22"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="C26:C30"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="A108:A110"/>
-    <mergeCell ref="D108:D110"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="D55:D57"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="C78:C86"/>
-    <mergeCell ref="B78:B86"/>
-    <mergeCell ref="A78:A86"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="A95:A97"/>
-    <mergeCell ref="D95:D97"/>
-    <mergeCell ref="B98:B99"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -3716,7 +3732,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>107</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -3727,7 +3743,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="3" t="s">
         <v>125</v>
       </c>
@@ -3763,7 +3779,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
         <v>117</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -3774,7 +3790,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="2" t="s">
         <v>120</v>
       </c>
@@ -4159,4 +4175,57 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="15.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>405</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update on 20181124.1735 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RCommands" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="HPCCommands" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RCommands!$A$1:$A$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RCommands!$A$1:$A$78</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="463">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -405,14 +405,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>bind_rows(A, B)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>return [A; B]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>read.csv()</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1647,14 +1639,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>mtcars$car &lt;- rownames(mtcars); mtcarsMelt &lt;- melt(mtcars)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reshape data frame mtcars into 3 columns: [id, variables, value]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>mail -s "YOUR EMAIL SUBJECT" YOUR EMAIL ADDRESS &lt;&lt;&lt; 'YOUR EMAIL CONTENT'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1664,6 +1648,256 @@
   </si>
   <si>
     <t>mail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mtcarsMelt &lt;- melt(mtcars, id.vars = c('cyl', 'gear'),
+variable.name = 'carVariable', value.name = 'carValue')</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: reshape2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dcast()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>turn long format to wide format - reshape data frame into 3 columns: [id, variables, value]
+id.vars: set id; variable.name, value.name: rename variable and value columns</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dcast(mtcarsMelt, cyl + gear ~ variable)
+dcast(mtcarsMelt,cyl+gear~variable,fun.aggregate=mean)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>turn wide format to long format - cyl and gear are id
+the mean of all variables for each combination of cyl and gear by using the fun.aggregate parameter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git diff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git diff file</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>check any changes have been made to the file</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>write.table(IdXY_All2, file = "TidyDataset.txt", row.name=FALSE)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>write.table()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>output data frame IdXY_All2 to txt file: TidyDataset.txt without row names</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mkdir</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create a new directory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>touch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create a new file</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>copy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete and cannot be retrieved</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>move to another directory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>print the current date and time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>echo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>General</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>print</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>open .</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>show the current directory in a folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>General</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enter VISUAL mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cut</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paste</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>i</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enter INSERT mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>summarize_all()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unzip()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>read.table()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>read.table("Filename", colClasses = c("integer", "character"), 
+col.names = c("activity.code", "activity"))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>load the file and assign the class of the 2 columns as interger and character
+assign column names as activity.code and activity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unzip("ProjectData.zip")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unzip the zip file ProjectData.zip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>File Operation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: dplyr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bind_cols()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bind_cols(A,B,C)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bind_rows(A,B,C)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return [A; B; C]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return [A B C]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inner_join</t>
+  </si>
+  <si>
+    <t>by_species &lt;- group_by(iris, Species)
+temp &lt;- summarise_all(by_species, funs(min, max))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>perform min and max on all the columns except column Species</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inner_join(band_members, band_instruments, by = "name")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>merge band_members and band_instruments by column name, drop rows with uncommon name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1729,7 +1963,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1776,11 +2010,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2060,10 +2300,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A38" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2071,7 +2311,7 @@
     <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="74" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="99.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="101.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -2111,10 +2351,10 @@
         <v>56</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F3"/>
     </row>
@@ -2164,13 +2404,13 @@
     </row>
     <row r="7" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>238</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>240</v>
       </c>
       <c r="F7"/>
     </row>
@@ -2205,18 +2445,18 @@
         <v>18</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F10"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B11" s="15" t="s">
+      <c r="A11" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -2225,20 +2465,20 @@
       <c r="D11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="19" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="16"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
@@ -2257,210 +2497,211 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
+        <v>452</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>458</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B15" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="4" t="s">
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="4" t="s">
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B18" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="4" t="s">
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="15" t="s">
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B20" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="4" t="s">
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="4" t="s">
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="4" t="s">
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="15" t="s">
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B24" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="4" t="s">
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="15" t="s">
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B27" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C27" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D27" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="15"/>
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="15"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="17"/>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="15"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="17"/>
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="15"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="17"/>
       <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="17"/>
       <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -2468,1218 +2709,1343 @@
         <v>62</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>72</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E33" s="4"/>
-      <c r="F33"/>
-    </row>
-    <row r="34" spans="1:6" ht="54" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+      <c r="C34" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34"/>
+    </row>
+    <row r="35" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>453</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>457</v>
+      </c>
+      <c r="F35"/>
+    </row>
+    <row r="36" spans="1:6" ht="54" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D36" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="15" t="s">
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B37" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C37" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="D37" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="E37" s="4"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>88</v>
-      </c>
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
       <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="15" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A43" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>446</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>447</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>448</v>
+      </c>
+      <c r="F43"/>
+    </row>
+    <row r="44" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C39" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="C44" s="4"/>
+      <c r="D44" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E39" s="4"/>
-    </row>
-    <row r="40" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B40" s="4" t="s">
+      <c r="E44" s="4"/>
+      <c r="F44"/>
+    </row>
+    <row r="45" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4" t="s">
+      <c r="C45" s="4"/>
+      <c r="D45" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E40" s="4"/>
-      <c r="F40"/>
-    </row>
-    <row r="41" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E41" s="4"/>
-      <c r="F41"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B42" s="4" t="s">
+      <c r="E45" s="4"/>
+      <c r="F45"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E42" s="4"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E43" s="7"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E44" s="4"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="E45" s="4"/>
-    </row>
-    <row r="46" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="15"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="F46"/>
+      <c r="E46" s="4"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B47" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="17"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="E47" s="4"/>
-    </row>
-    <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="15" t="s">
+      <c r="E51" s="4"/>
+    </row>
+    <row r="52" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D52" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="F52"/>
+    </row>
+    <row r="53" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="17"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="F53"/>
+    </row>
+    <row r="54" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B54" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C54" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="F54"/>
+    </row>
+    <row r="55" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="F55"/>
+    </row>
+    <row r="56" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="17"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="D48" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="F48"/>
-    </row>
-    <row r="49" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="15"/>
-      <c r="B49" s="15"/>
-      <c r="C49" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="F49"/>
-    </row>
-    <row r="50" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="C50" s="9" t="s">
+      <c r="D56" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="F56"/>
+    </row>
+    <row r="57" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B57" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="D50" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="F50"/>
-    </row>
-    <row r="51" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="F51"/>
-    </row>
-    <row r="52" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="15"/>
-      <c r="B52" s="15"/>
-      <c r="C52" s="9" t="s">
+      <c r="C57" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="D57" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="D52" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="F52"/>
-    </row>
-    <row r="53" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="B53" s="15" t="s">
+      <c r="F57"/>
+    </row>
+    <row r="58" spans="1:6" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+      <c r="A58" s="17"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="F58"/>
+    </row>
+    <row r="59" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B59" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C59" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D59" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="D53" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="F53"/>
-    </row>
-    <row r="54" spans="1:6" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A54" s="15"/>
-      <c r="B54" s="15"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="9" t="s">
+      <c r="F59"/>
+    </row>
+    <row r="60" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="17"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D60" s="17"/>
+      <c r="F60"/>
+    </row>
+    <row r="61" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="17"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="F54"/>
-    </row>
-    <row r="55" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="C55" s="8" t="s">
+      <c r="D61" s="17"/>
+      <c r="F61"/>
+    </row>
+    <row r="62" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="17"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="F62"/>
+    </row>
+    <row r="63" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B63" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="D55" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="F55"/>
-    </row>
-    <row r="56" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="15"/>
-      <c r="B56" s="15"/>
-      <c r="C56" s="8" t="s">
+      <c r="C63" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D63" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="D56" s="15"/>
-      <c r="F56"/>
-    </row>
-    <row r="57" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="15"/>
-      <c r="B57" s="15"/>
-      <c r="C57" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="D57" s="15"/>
-      <c r="F57"/>
-    </row>
-    <row r="58" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="15"/>
-      <c r="B58" s="15"/>
-      <c r="C58" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="D58" s="8" t="s">
+      <c r="F63"/>
+    </row>
+    <row r="64" spans="1:6" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A64" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B64" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="F58"/>
-    </row>
-    <row r="59" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="F59"/>
-    </row>
-    <row r="60" spans="1:6" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A60" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="F60"/>
-    </row>
-    <row r="61" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="D61" s="8" t="s">
+      <c r="C64" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="F61"/>
-    </row>
-    <row r="62" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="F62"/>
-    </row>
-    <row r="63" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="15"/>
-      <c r="B63" s="15"/>
-      <c r="C63" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="F63"/>
-    </row>
-    <row r="64" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="15"/>
-      <c r="B64" s="15"/>
-      <c r="C64" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>207</v>
+      <c r="D64" s="9" t="s">
+        <v>211</v>
       </c>
       <c r="F64"/>
     </row>
     <row r="65" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B65" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="F65"/>
+    </row>
+    <row r="66" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F66"/>
+    </row>
+    <row r="67" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="17"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="F67"/>
+    </row>
+    <row r="68" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="17"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="F68"/>
+    </row>
+    <row r="69" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="D69" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="C65" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="F65"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="B68" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="15"/>
-      <c r="B69" s="15"/>
-      <c r="C69" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>154</v>
-      </c>
+      <c r="F69"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>157</v>
+      <c r="D70" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B72" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="F72"/>
-    </row>
-    <row r="73" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="15"/>
-      <c r="B73" s="15"/>
-      <c r="C73" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="D73" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="F73"/>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="17"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B76" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="F76"/>
+    </row>
+    <row r="77" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="17"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D77" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="F77"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D75" s="1" t="s">
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="B82" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="C82" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="B78" s="15" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="17"/>
+      <c r="B83" s="17"/>
+      <c r="C83" s="17"/>
+      <c r="D83" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C78" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="D78" s="1" t="s">
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="17"/>
+      <c r="B84" s="17"/>
+      <c r="C84" s="17"/>
+      <c r="D84" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="15"/>
-      <c r="B79" s="15"/>
-      <c r="C79" s="15"/>
-      <c r="D79" s="1" t="s">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="17"/>
+      <c r="B85" s="17"/>
+      <c r="C85" s="17"/>
+      <c r="D85" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="15"/>
-      <c r="B80" s="15"/>
-      <c r="C80" s="15"/>
-      <c r="D80" s="1" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="17"/>
+      <c r="B86" s="17"/>
+      <c r="C86" s="17"/>
+      <c r="D86" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="15"/>
-      <c r="B81" s="15"/>
-      <c r="C81" s="15"/>
-      <c r="D81" s="1" t="s">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="17"/>
+      <c r="B87" s="17"/>
+      <c r="C87" s="17"/>
+      <c r="D87" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="15"/>
-      <c r="B82" s="15"/>
-      <c r="C82" s="15"/>
-      <c r="D82" s="1" t="s">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="17"/>
+      <c r="B88" s="17"/>
+      <c r="C88" s="17"/>
+      <c r="D88" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="15"/>
-      <c r="B83" s="15"/>
-      <c r="C83" s="15"/>
-      <c r="D83" s="1" t="s">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="17"/>
+      <c r="B89" s="17"/>
+      <c r="C89" s="17"/>
+      <c r="D89" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="15"/>
-      <c r="B84" s="15"/>
-      <c r="C84" s="15"/>
-      <c r="D84" s="1" t="s">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="17"/>
+      <c r="B90" s="17"/>
+      <c r="C90" s="17"/>
+      <c r="D90" s="1" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="15"/>
-      <c r="B85" s="15"/>
-      <c r="C85" s="15"/>
-      <c r="D85" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="15"/>
-      <c r="B86" s="15"/>
-      <c r="C86" s="15"/>
-      <c r="D86" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>162</v>
+        <v>212</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>169</v>
+        <v>230</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>234</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="E91" s="12" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B92" s="11" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="E95" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B96" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="D96" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="E96" s="12"/>
+      <c r="F96"/>
+    </row>
+    <row r="97" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B97" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="C97" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="D97" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="E97" s="12"/>
+      <c r="F97"/>
+    </row>
+    <row r="98" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B98" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="C92" s="11" t="s">
-        <v>302</v>
-      </c>
-      <c r="D92" s="11" t="s">
+      <c r="C98" s="11" t="s">
         <v>303</v>
       </c>
-      <c r="E92" s="12"/>
-      <c r="F92"/>
-    </row>
-    <row r="93" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B93" s="11" t="s">
-        <v>300</v>
-      </c>
-      <c r="C93" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="D93" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="E93" s="12"/>
-      <c r="F93"/>
-    </row>
-    <row r="94" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B94" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="C94" s="11" t="s">
+      <c r="D98" s="11" t="s">
         <v>305</v>
       </c>
-      <c r="D94" s="11" t="s">
-        <v>307</v>
-      </c>
-      <c r="E94" s="12"/>
-      <c r="F94"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="B95" s="1" t="s">
+      <c r="E98" s="12"/>
+      <c r="F98"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D99" s="17" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" s="17"/>
+      <c r="B100" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="D95" s="15" t="s">
+      <c r="C100" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="15"/>
-      <c r="B96" s="1" t="s">
+      <c r="D100" s="17"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="17"/>
+      <c r="B101" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C101" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D101" s="17"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B102" s="17" t="s">
         <v>253</v>
       </c>
-      <c r="D96" s="15"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="15"/>
-      <c r="B97" s="1" t="s">
+      <c r="C102" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C97" s="1" t="s">
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" s="17"/>
+      <c r="B103" s="17"/>
+      <c r="C103" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B104" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="C104" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="D97" s="15"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="B98" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99" s="15"/>
-      <c r="B99" s="15"/>
-      <c r="C99" s="10" t="s">
+      <c r="D104" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="F104"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B105" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="C105" s="1" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B100" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="C100" s="11" t="s">
-        <v>322</v>
-      </c>
-      <c r="D100" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="F100"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="B101" s="15" t="s">
+      <c r="D105" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="C101" s="1" t="s">
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" s="17"/>
+      <c r="B106" s="17"/>
+      <c r="C106" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="D106" s="1" t="s">
         <v>262</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102" s="15"/>
-      <c r="B102" s="15"/>
-      <c r="C102" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="E103" s="12" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B105" s="11" t="s">
-        <v>311</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B106" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>324</v>
+        <v>306</v>
       </c>
       <c r="C107" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E107" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="D107" s="1" t="s">
-        <v>326</v>
-      </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108" s="15" t="s">
-        <v>162</v>
+      <c r="A108" s="11" t="s">
+        <v>160</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="D108" s="15" t="s">
-        <v>335</v>
+        <v>312</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A109" s="15"/>
-      <c r="B109" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="C109" s="11" t="s">
-        <v>333</v>
-      </c>
-      <c r="D109" s="15"/>
+      <c r="A109" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B109" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A110" s="15"/>
-      <c r="B110" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="C110" s="11" t="s">
-        <v>334</v>
-      </c>
-      <c r="D110" s="15"/>
+      <c r="A110" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B110" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B111" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D112" s="17" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" s="17"/>
+      <c r="B113" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C113" s="11" t="s">
+        <v>331</v>
+      </c>
+      <c r="D113" s="17"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" s="17"/>
+      <c r="B114" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C114" s="11" t="s">
+        <v>332</v>
+      </c>
+      <c r="D114" s="17"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C115" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="C111" s="11" t="s">
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D116" s="1" t="s">
         <v>340</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A112" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A113" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A114" s="13" t="s">
-        <v>372</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A115" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="B115" s="13" t="s">
-        <v>379</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A116" s="13" t="s">
-        <v>372</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C117" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="B117" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>388</v>
-      </c>
       <c r="D117" s="1" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>391</v>
+        <v>376</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>392</v>
+        <v>375</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="13" t="s">
-        <v>372</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>394</v>
+        <v>379</v>
+      </c>
+      <c r="B119" s="13" t="s">
+        <v>377</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>395</v>
+        <v>378</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>396</v>
+        <v>380</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>399</v>
+        <v>370</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
       <c r="D121" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" s="17" t="s">
+        <v>397</v>
+      </c>
+      <c r="B125" s="17" t="s">
+        <v>398</v>
+      </c>
+      <c r="C125" s="18" t="s">
         <v>402</v>
       </c>
+      <c r="D125" s="18" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" s="17"/>
+      <c r="B126" s="17"/>
+      <c r="C126" s="17"/>
+      <c r="D126" s="17"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" s="17" t="s">
+        <v>403</v>
+      </c>
+      <c r="B127" s="17" t="s">
+        <v>404</v>
+      </c>
+      <c r="C127" s="18" t="s">
+        <v>406</v>
+      </c>
+      <c r="D127" s="18" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" s="17"/>
+      <c r="B128" s="17"/>
+      <c r="C128" s="17"/>
+      <c r="D128" s="17"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" s="17"/>
+      <c r="B129" s="17"/>
+      <c r="C129" s="17"/>
+      <c r="D129" s="17"/>
+    </row>
+    <row r="130" spans="1:4" ht="36" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C130" s="16" t="s">
+        <v>459</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>450</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="48">
-    <mergeCell ref="A108:A110"/>
-    <mergeCell ref="D108:D110"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="D55:D57"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="C78:C86"/>
-    <mergeCell ref="B78:B86"/>
-    <mergeCell ref="A78:A86"/>
+  <mergeCells count="56">
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="D125:D126"/>
+    <mergeCell ref="B125:B126"/>
+    <mergeCell ref="A125:A126"/>
+    <mergeCell ref="D127:D129"/>
+    <mergeCell ref="C127:C129"/>
+    <mergeCell ref="B127:B129"/>
+    <mergeCell ref="A127:A129"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="A105:A106"/>
+    <mergeCell ref="B105:B106"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="D27:D31"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="A49:A50"/>
     <mergeCell ref="B72:B73"/>
     <mergeCell ref="A72:A73"/>
-    <mergeCell ref="A95:A97"/>
-    <mergeCell ref="D95:D97"/>
-    <mergeCell ref="B98:B99"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="A68:A69"/>
     <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="A101:A102"/>
-    <mergeCell ref="B101:B102"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A112:A114"/>
+    <mergeCell ref="D112:D114"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="D59:D61"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="C82:C90"/>
+    <mergeCell ref="B82:B90"/>
+    <mergeCell ref="A82:A90"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="D99:D101"/>
+    <mergeCell ref="B102:B103"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E11" r:id="rId1"/>
-    <hyperlink ref="E91" r:id="rId2"/>
-    <hyperlink ref="E103" r:id="rId3"/>
+    <hyperlink ref="E95" r:id="rId2"/>
+    <hyperlink ref="E107" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3690,7 +4056,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -3703,99 +4069,110 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="C4" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="C9" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B9" s="2" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="17"/>
+      <c r="B10" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
-      <c r="B10" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>121</v>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="25" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3812,15 +4189,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="13"/>
+    <col min="1" max="1" width="16" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="68.6640625" style="2" bestFit="1" customWidth="1"/>
@@ -3832,127 +4209,258 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B6" s="13">
         <v>0</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>357</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B8" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>365</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B9" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>366</v>
       </c>
-      <c r="D9" s="13" t="s">
+    </row>
+    <row r="10" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>434</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>433</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>436</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>437</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
+        <v>439</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>440</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>442</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+      <c r="D15" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
+      <c r="B18" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="18" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B19" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
+        <v>424</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3977,13 +4485,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4011,82 +4519,82 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -4094,63 +4602,63 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" s="12" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -4181,7 +4689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -4202,10 +4710,10 @@
         <v>4</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4213,13 +4721,13 @@
         <v>56</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update on 20181221.1459 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="6080" yWindow="6820" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="RCommands" sheetId="1" r:id="rId1"/>
     <sheet name="GitCommands" sheetId="2" r:id="rId2"/>
     <sheet name="ShellCommands" sheetId="3" r:id="rId3"/>
     <sheet name="PythonCommands" sheetId="4" r:id="rId4"/>
-    <sheet name="Date Source Link" sheetId="5" r:id="rId5"/>
-    <sheet name="HPCCommands" sheetId="6" r:id="rId6"/>
+    <sheet name="HPCCommands" sheetId="6" r:id="rId5"/>
+    <sheet name="Date Source Link" sheetId="5" r:id="rId6"/>
+    <sheet name="Learning Sources" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RCommands!$A$1:$A$78</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="478">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1898,6 +1899,66 @@
   </si>
   <si>
     <t>merge band_members and band_instruments by column name, drop rows with uncommon name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.edwardtufte.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beautiful Evidence, Graphics Press LLC.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subset()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>General</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subset(iris, Sepal.Length&gt;5)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get a subset of iris: column Sepal.Length &gt; 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Graphs Principles</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R Graph Gallery</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.r-graph-gallery.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R Bloggers</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1963,7 +2024,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2018,6 +2079,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2300,10 +2364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+    <sheetView topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2453,10 +2517,10 @@
       <c r="F10"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -2465,20 +2529,20 @@
       <c r="D11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="19"/>
+      <c r="E12" s="20"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
@@ -2510,10 +2574,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="19" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -2525,8 +2589,8 @@
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="4" t="s">
         <v>26</v>
       </c>
@@ -2536,8 +2600,8 @@
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="4" t="s">
         <v>28</v>
       </c>
@@ -2547,10 +2611,10 @@
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -2562,8 +2626,8 @@
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="4" t="s">
         <v>34</v>
       </c>
@@ -2573,10 +2637,10 @@
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="19" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -2588,8 +2652,8 @@
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="4" t="s">
         <v>39</v>
       </c>
@@ -2599,8 +2663,8 @@
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="4" t="s">
         <v>41</v>
       </c>
@@ -2610,8 +2674,8 @@
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="4" t="s">
         <v>44</v>
       </c>
@@ -2621,10 +2685,10 @@
       <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="19" t="s">
         <v>45</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -2636,8 +2700,8 @@
       <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
       <c r="C25" s="4" t="s">
         <v>47</v>
       </c>
@@ -2662,10 +2726,10 @@
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="19" t="s">
         <v>50</v>
       </c>
       <c r="C27" s="18" t="s">
@@ -2677,31 +2741,31 @@
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="18"/>
-      <c r="D28" s="17"/>
+      <c r="D28" s="19"/>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="18"/>
-      <c r="D29" s="17"/>
+      <c r="D29" s="19"/>
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
       <c r="C30" s="18"/>
-      <c r="D30" s="17"/>
+      <c r="D30" s="19"/>
       <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="18"/>
-      <c r="D31" s="17"/>
+      <c r="D31" s="19"/>
       <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -2779,13 +2843,13 @@
       <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C37" s="17" t="s">
+      <c r="C37" s="19" t="s">
         <v>81</v>
       </c>
       <c r="D37" s="18" t="s">
@@ -2794,10 +2858,10 @@
       <c r="E37" s="4"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
+      <c r="A38" s="19"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
       <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -2946,10 +3010,10 @@
       <c r="E48" s="4"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="19" t="s">
         <v>134</v>
       </c>
       <c r="C49" s="4" t="s">
@@ -2961,8 +3025,8 @@
       <c r="E49" s="4"/>
     </row>
     <row r="50" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="17"/>
-      <c r="B50" s="17"/>
+      <c r="A50" s="19"/>
+      <c r="B50" s="19"/>
       <c r="C50" s="4" t="s">
         <v>140</v>
       </c>
@@ -2987,10 +3051,10 @@
       <c r="E51" s="4"/>
     </row>
     <row r="52" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="19" t="s">
         <v>169</v>
       </c>
       <c r="C52" s="9" t="s">
@@ -3002,8 +3066,8 @@
       <c r="F52"/>
     </row>
     <row r="53" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="17"/>
-      <c r="B53" s="17"/>
+      <c r="A53" s="19"/>
+      <c r="B53" s="19"/>
       <c r="C53" s="9" t="s">
         <v>177</v>
       </c>
@@ -3028,10 +3092,10 @@
       <c r="F54"/>
     </row>
     <row r="55" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="17" t="s">
+      <c r="A55" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="19" t="s">
         <v>173</v>
       </c>
       <c r="C55" s="8" t="s">
@@ -3043,8 +3107,8 @@
       <c r="F55"/>
     </row>
     <row r="56" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
+      <c r="A56" s="19"/>
+      <c r="B56" s="19"/>
       <c r="C56" s="9" t="s">
         <v>181</v>
       </c>
@@ -3054,10 +3118,10 @@
       <c r="F56"/>
     </row>
     <row r="57" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="17" t="s">
+      <c r="A57" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="19" t="s">
         <v>182</v>
       </c>
       <c r="C57" s="18" t="s">
@@ -3069,8 +3133,8 @@
       <c r="F57"/>
     </row>
     <row r="58" spans="1:6" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A58" s="17"/>
-      <c r="B58" s="17"/>
+      <c r="A58" s="19"/>
+      <c r="B58" s="19"/>
       <c r="C58" s="18"/>
       <c r="D58" s="9" t="s">
         <v>190</v>
@@ -3078,41 +3142,41 @@
       <c r="F58"/>
     </row>
     <row r="59" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="17" t="s">
+      <c r="A59" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B59" s="19" t="s">
         <v>184</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="D59" s="19" t="s">
         <v>191</v>
       </c>
       <c r="F59"/>
     </row>
     <row r="60" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="17"/>
-      <c r="B60" s="17"/>
+      <c r="A60" s="19"/>
+      <c r="B60" s="19"/>
       <c r="C60" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="D60" s="17"/>
+      <c r="D60" s="19"/>
       <c r="F60"/>
     </row>
     <row r="61" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="17"/>
-      <c r="B61" s="17"/>
+      <c r="A61" s="19"/>
+      <c r="B61" s="19"/>
       <c r="C61" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="D61" s="17"/>
+      <c r="D61" s="19"/>
       <c r="F61"/>
     </row>
     <row r="62" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="17"/>
-      <c r="B62" s="17"/>
+      <c r="A62" s="19"/>
+      <c r="B62" s="19"/>
       <c r="C62" s="8" t="s">
         <v>193</v>
       </c>
@@ -3167,10 +3231,10 @@
       <c r="F65"/>
     </row>
     <row r="66" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="17" t="s">
+      <c r="A66" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="B66" s="17" t="s">
+      <c r="B66" s="19" t="s">
         <v>201</v>
       </c>
       <c r="C66" s="8" t="s">
@@ -3182,8 +3246,8 @@
       <c r="F66"/>
     </row>
     <row r="67" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="17"/>
-      <c r="B67" s="17"/>
+      <c r="A67" s="19"/>
+      <c r="B67" s="19"/>
       <c r="C67" s="8" t="s">
         <v>206</v>
       </c>
@@ -3193,8 +3257,8 @@
       <c r="F67"/>
     </row>
     <row r="68" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="17"/>
-      <c r="B68" s="17"/>
+      <c r="A68" s="19"/>
+      <c r="B68" s="19"/>
       <c r="C68" s="8" t="s">
         <v>207</v>
       </c>
@@ -3247,10 +3311,10 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="17" t="s">
+      <c r="A72" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="B72" s="17" t="s">
+      <c r="B72" s="19" t="s">
         <v>149</v>
       </c>
       <c r="C72" s="1" t="s">
@@ -3261,8 +3325,8 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="17"/>
-      <c r="B73" s="17"/>
+      <c r="A73" s="19"/>
+      <c r="B73" s="19"/>
       <c r="C73" s="4" t="s">
         <v>153</v>
       </c>
@@ -3299,10 +3363,10 @@
       </c>
     </row>
     <row r="76" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="17" t="s">
+      <c r="A76" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B76" s="17" t="s">
+      <c r="B76" s="19" t="s">
         <v>161</v>
       </c>
       <c r="C76" s="6" t="s">
@@ -3314,8 +3378,8 @@
       <c r="F76"/>
     </row>
     <row r="77" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="17"/>
-      <c r="B77" s="17"/>
+      <c r="A77" s="19"/>
+      <c r="B77" s="19"/>
       <c r="C77" s="10" t="s">
         <v>232</v>
       </c>
@@ -3372,13 +3436,13 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="17" t="s">
+      <c r="A82" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="B82" s="17" t="s">
+      <c r="B82" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C82" s="17" t="s">
+      <c r="C82" s="19" t="s">
         <v>229</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -3386,65 +3450,65 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="17"/>
-      <c r="B83" s="17"/>
-      <c r="C83" s="17"/>
+      <c r="A83" s="19"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="19"/>
       <c r="D83" s="1" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="17"/>
-      <c r="B84" s="17"/>
-      <c r="C84" s="17"/>
+      <c r="A84" s="19"/>
+      <c r="B84" s="19"/>
+      <c r="C84" s="19"/>
       <c r="D84" s="1" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="17"/>
-      <c r="B85" s="17"/>
-      <c r="C85" s="17"/>
+      <c r="A85" s="19"/>
+      <c r="B85" s="19"/>
+      <c r="C85" s="19"/>
       <c r="D85" s="1" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="17"/>
-      <c r="B86" s="17"/>
-      <c r="C86" s="17"/>
+      <c r="A86" s="19"/>
+      <c r="B86" s="19"/>
+      <c r="C86" s="19"/>
       <c r="D86" s="1" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="17"/>
-      <c r="B87" s="17"/>
-      <c r="C87" s="17"/>
+      <c r="A87" s="19"/>
+      <c r="B87" s="19"/>
+      <c r="C87" s="19"/>
       <c r="D87" s="1" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="17"/>
-      <c r="B88" s="17"/>
-      <c r="C88" s="17"/>
+      <c r="A88" s="19"/>
+      <c r="B88" s="19"/>
+      <c r="C88" s="19"/>
       <c r="D88" s="1" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="17"/>
-      <c r="B89" s="17"/>
-      <c r="C89" s="17"/>
+      <c r="A89" s="19"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="19"/>
       <c r="D89" s="1" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="17"/>
-      <c r="B90" s="17"/>
-      <c r="C90" s="17"/>
+      <c r="A90" s="19"/>
+      <c r="B90" s="19"/>
+      <c r="C90" s="19"/>
       <c r="D90" s="1" t="s">
         <v>228</v>
       </c>
@@ -3568,7 +3632,7 @@
       <c r="F98"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99" s="17" t="s">
+      <c r="A99" s="19" t="s">
         <v>160</v>
       </c>
       <c r="B99" s="1" t="s">
@@ -3577,35 +3641,35 @@
       <c r="C99" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="D99" s="17" t="s">
+      <c r="D99" s="19" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="17"/>
+      <c r="A100" s="19"/>
       <c r="B100" s="1" t="s">
         <v>250</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D100" s="17"/>
+      <c r="D100" s="19"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="17"/>
+      <c r="A101" s="19"/>
       <c r="B101" s="1" t="s">
         <v>252</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="D101" s="17"/>
+      <c r="D101" s="19"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102" s="17" t="s">
+      <c r="A102" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="B102" s="17" t="s">
+      <c r="B102" s="19" t="s">
         <v>253</v>
       </c>
       <c r="C102" s="1" t="s">
@@ -3616,8 +3680,8 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" s="17"/>
-      <c r="B103" s="17"/>
+      <c r="A103" s="19"/>
+      <c r="B103" s="19"/>
       <c r="C103" s="10" t="s">
         <v>256</v>
       </c>
@@ -3641,10 +3705,10 @@
       <c r="F104"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105" s="17" t="s">
+      <c r="A105" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="B105" s="17" t="s">
+      <c r="B105" s="19" t="s">
         <v>258</v>
       </c>
       <c r="C105" s="1" t="s">
@@ -3655,8 +3719,8 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106" s="17"/>
-      <c r="B106" s="17"/>
+      <c r="A106" s="19"/>
+      <c r="B106" s="19"/>
       <c r="C106" s="10" t="s">
         <v>261</v>
       </c>
@@ -3738,7 +3802,7 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A112" s="17" t="s">
+      <c r="A112" s="19" t="s">
         <v>160</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -3747,29 +3811,29 @@
       <c r="C112" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="D112" s="17" t="s">
+      <c r="D112" s="19" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A113" s="17"/>
+      <c r="A113" s="19"/>
       <c r="B113" s="1" t="s">
         <v>328</v>
       </c>
       <c r="C113" s="11" t="s">
         <v>331</v>
       </c>
-      <c r="D113" s="17"/>
+      <c r="D113" s="19"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A114" s="17"/>
+      <c r="A114" s="19"/>
       <c r="B114" s="1" t="s">
         <v>329</v>
       </c>
       <c r="C114" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="D114" s="17"/>
+      <c r="D114" s="19"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="11" t="s">
@@ -3909,10 +3973,10 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A125" s="17" t="s">
+      <c r="A125" s="19" t="s">
         <v>397</v>
       </c>
-      <c r="B125" s="17" t="s">
+      <c r="B125" s="19" t="s">
         <v>398</v>
       </c>
       <c r="C125" s="18" t="s">
@@ -3923,16 +3987,16 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A126" s="17"/>
-      <c r="B126" s="17"/>
-      <c r="C126" s="17"/>
-      <c r="D126" s="17"/>
+      <c r="A126" s="19"/>
+      <c r="B126" s="19"/>
+      <c r="C126" s="19"/>
+      <c r="D126" s="19"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A127" s="17" t="s">
+      <c r="A127" s="19" t="s">
         <v>403</v>
       </c>
-      <c r="B127" s="17" t="s">
+      <c r="B127" s="19" t="s">
         <v>404</v>
       </c>
       <c r="C127" s="18" t="s">
@@ -3943,16 +4007,16 @@
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A128" s="17"/>
-      <c r="B128" s="17"/>
-      <c r="C128" s="17"/>
-      <c r="D128" s="17"/>
+      <c r="A128" s="19"/>
+      <c r="B128" s="19"/>
+      <c r="C128" s="19"/>
+      <c r="D128" s="19"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A129" s="17"/>
-      <c r="B129" s="17"/>
-      <c r="C129" s="17"/>
-      <c r="D129" s="17"/>
+      <c r="A129" s="19"/>
+      <c r="B129" s="19"/>
+      <c r="C129" s="19"/>
+      <c r="D129" s="19"/>
     </row>
     <row r="130" spans="1:4" ht="36" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
@@ -3982,16 +4046,54 @@
         <v>450</v>
       </c>
     </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>470</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="C125:C126"/>
-    <mergeCell ref="D125:D126"/>
-    <mergeCell ref="B125:B126"/>
-    <mergeCell ref="A125:A126"/>
-    <mergeCell ref="D127:D129"/>
-    <mergeCell ref="C127:C129"/>
-    <mergeCell ref="B127:B129"/>
-    <mergeCell ref="A127:A129"/>
+    <mergeCell ref="A112:A114"/>
+    <mergeCell ref="D112:D114"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="D59:D61"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="C82:C90"/>
+    <mergeCell ref="B82:B90"/>
+    <mergeCell ref="A82:A90"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="D99:D101"/>
+    <mergeCell ref="B102:B103"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="D27:D31"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="A49:A50"/>
     <mergeCell ref="A102:A103"/>
     <mergeCell ref="A105:A106"/>
     <mergeCell ref="B105:B106"/>
@@ -4008,38 +4110,14 @@
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="C27:C31"/>
-    <mergeCell ref="D27:D31"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A112:A114"/>
-    <mergeCell ref="D112:D114"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="D59:D61"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="C82:C90"/>
-    <mergeCell ref="B82:B90"/>
-    <mergeCell ref="A82:A90"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="D99:D101"/>
-    <mergeCell ref="B102:B103"/>
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="D125:D126"/>
+    <mergeCell ref="B125:B126"/>
+    <mergeCell ref="A125:A126"/>
+    <mergeCell ref="D127:D129"/>
+    <mergeCell ref="C127:C129"/>
+    <mergeCell ref="B127:B129"/>
+    <mergeCell ref="A127:A129"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -4098,7 +4176,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="19" t="s">
         <v>105</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -4109,7 +4187,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="3" t="s">
         <v>123</v>
       </c>
@@ -4145,7 +4223,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="19" t="s">
         <v>115</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -4156,7 +4234,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="2" t="s">
         <v>118</v>
       </c>
@@ -4504,6 +4582,59 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="15.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>401</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>399</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4685,55 +4816,69 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="14"/>
-    <col min="2" max="2" width="15.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="95.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="14"/>
+    <col min="1" max="1" width="19.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>401</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>399</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>471</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>463</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>472</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>465</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
+        <v>476</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>477</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update on 20181222.1633 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="6820" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RCommands" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="492">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -82,10 +82,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Package Operation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>total &lt;- merge(data frame A, data frame B, by = "ID")</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -110,10 +106,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Package Operation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>tbl_df()</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -259,10 +251,6 @@
   </si>
   <si>
     <t>same as length(unique(x))</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>General</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -302,14 +290,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>General</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>quantile()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>quantile(A, c(0.3, 0.5, 0.9))</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -438,14 +418,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Data Operation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>String Operation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Commands</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -690,19 +662,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sys.getlocale()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>view your locale, returns something like "zh_CN.UTF-8", "en_US.UTF-8"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>help()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>General</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -897,18 +861,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Time Operation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>date()</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sys.Date()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>return the current date, Date class</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -992,14 +948,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>General</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>as.numeric()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>transfer to numeric data</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1522,10 +1470,6 @@
   </si>
   <si>
     <t>move (not remove) all displays away, so as to leave a tidy screen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>General</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1854,10 +1798,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>File Operation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Package: dplyr</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1922,10 +1862,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>General</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>subset(iris, Sepal.Length&gt;5)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1959,6 +1895,127 @@
   </si>
   <si>
     <t>R Bloggers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot(cars$speed, cars$dist)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points (cars$speed, cars$dist)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: lattice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xyplot()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>state &lt;- data.frame(state.x77, region = state.region)
+xyplot(Life.Exp ~ Income | region, data = state, layout = c(4,1))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot 4 plots in 1 line, y-axis is state$Life.Exp, x-axis is state$Income
+4 plots are different based on state$region</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: ggplot2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qplot(displ, hwy, data = mpg)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qplot()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points (mpg$displ, mpg$hwy)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: graphics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hist()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hist(airquality$Ozone)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>make a histogram</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>with()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>with(airquality, plot(Wind, Ozone))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: base</t>
+  </si>
+  <si>
+    <t>Package: base</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: utils</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: base</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: dplyr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>quantile()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: stats</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>as.numeric()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: utils</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: base</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sys.getlocale()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: base</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sys.Date()</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2364,10 +2421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F132"/>
+  <dimension ref="A1:F138"/>
   <sheetViews>
-    <sheetView topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="D137" sqref="D137"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2399,7 +2456,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>56</v>
+        <v>482</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -2411,76 +2468,76 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
-        <v>56</v>
+      <c r="A3" s="17" t="s">
+        <v>482</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="F3"/>
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>56</v>
+      <c r="A4" s="17" t="s">
+        <v>482</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4"/>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>57</v>
+        <v>483</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5"/>
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>64</v>
+        <v>485</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>65</v>
+        <v>484</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6"/>
     </row>
     <row r="7" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>236</v>
+      <c r="A7" s="17" t="s">
+        <v>482</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>237</v>
+        <v>486</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="F7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>11</v>
+        <v>487</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>2</v>
@@ -2492,42 +2549,42 @@
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>18</v>
+      <c r="A9" s="17" t="s">
+        <v>487</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>18</v>
+      <c r="A10" s="17" t="s">
+        <v>482</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="F10"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>98</v>
+        <v>479</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>9</v>
@@ -2537,54 +2594,54 @@
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="E12" s="20"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>458</v>
+        <v>443</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>461</v>
+        <v>446</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="D15" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="E15" s="4"/>
     </row>
@@ -2592,10 +2649,10 @@
       <c r="A16" s="19"/>
       <c r="B16" s="19"/>
       <c r="C16" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E16" s="4"/>
     </row>
@@ -2603,25 +2660,25 @@
       <c r="A17" s="19"/>
       <c r="B17" s="19"/>
       <c r="C17" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="E18" s="4"/>
     </row>
@@ -2629,25 +2686,25 @@
       <c r="A19" s="19"/>
       <c r="B19" s="19"/>
       <c r="C19" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B20" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="E20" s="4"/>
     </row>
@@ -2655,10 +2712,10 @@
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E21" s="4"/>
     </row>
@@ -2666,10 +2723,10 @@
       <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E22" s="4"/>
     </row>
@@ -2677,25 +2734,25 @@
       <c r="A23" s="19"/>
       <c r="B23" s="19"/>
       <c r="C23" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="E24" s="4"/>
     </row>
@@ -2703,40 +2760,40 @@
       <c r="A25" s="19"/>
       <c r="B25" s="19"/>
       <c r="C25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E27" s="4"/>
     </row>
@@ -2770,90 +2827,90 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E33" s="4"/>
     </row>
     <row r="34" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34"/>
     </row>
     <row r="35" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>457</v>
+        <v>442</v>
       </c>
       <c r="F35"/>
     </row>
     <row r="36" spans="1:6" ht="54" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>80</v>
-      </c>
       <c r="C37" s="19" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E37" s="4"/>
     </row>
@@ -2866,161 +2923,161 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E40" s="4"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>97</v>
+        <v>487</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E41" s="4"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="15" t="s">
-        <v>97</v>
+      <c r="A42" s="17" t="s">
+        <v>487</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="15" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A43" s="15" t="s">
-        <v>97</v>
+      <c r="A43" s="17" t="s">
+        <v>487</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>447</v>
+        <v>433</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>448</v>
+        <v>434</v>
       </c>
       <c r="F43"/>
     </row>
     <row r="44" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>99</v>
+        <v>488</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44"/>
     </row>
     <row r="45" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
-        <v>99</v>
+      <c r="A45" s="17" t="s">
+        <v>488</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
-        <v>99</v>
+      <c r="A46" s="17" t="s">
+        <v>488</v>
       </c>
       <c r="B46" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="17" t="s">
+        <v>488</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="17" t="s">
+        <v>488</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="D48" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E46" s="4"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E47" s="7"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>133</v>
       </c>
       <c r="E48" s="4"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="19" t="s">
-        <v>99</v>
+        <v>479</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E49" s="4"/>
     </row>
@@ -3028,40 +3085,40 @@
       <c r="A50" s="19"/>
       <c r="B50" s="19"/>
       <c r="C50" s="4" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F50"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
-        <v>99</v>
+      <c r="A51" s="17" t="s">
+        <v>488</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E51" s="4"/>
     </row>
     <row r="52" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="F52"/>
     </row>
@@ -3069,40 +3126,40 @@
       <c r="A53" s="19"/>
       <c r="B53" s="19"/>
       <c r="C53" s="9" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="F53"/>
     </row>
     <row r="54" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B54" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C54" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C54" s="9" t="s">
-        <v>180</v>
-      </c>
       <c r="D54" s="8" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="F54"/>
     </row>
     <row r="55" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="F55"/>
     </row>
@@ -3110,25 +3167,25 @@
       <c r="A56" s="19"/>
       <c r="B56" s="19"/>
       <c r="C56" s="9" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="F56"/>
     </row>
     <row r="57" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F57"/>
     </row>
@@ -3137,22 +3194,22 @@
       <c r="B58" s="19"/>
       <c r="C58" s="18"/>
       <c r="D58" s="9" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="F58"/>
     </row>
     <row r="59" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="D59" s="19" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="F59"/>
     </row>
@@ -3160,7 +3217,7 @@
       <c r="A60" s="19"/>
       <c r="B60" s="19"/>
       <c r="C60" s="8" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D60" s="19"/>
       <c r="F60"/>
@@ -3169,7 +3226,7 @@
       <c r="A61" s="19"/>
       <c r="B61" s="19"/>
       <c r="C61" s="8" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D61" s="19"/>
       <c r="F61"/>
@@ -3178,70 +3235,70 @@
       <c r="A62" s="19"/>
       <c r="B62" s="19"/>
       <c r="C62" s="8" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="F62"/>
     </row>
     <row r="63" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="F63"/>
     </row>
     <row r="64" spans="1:6" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="F64"/>
     </row>
     <row r="65" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="F65"/>
     </row>
     <row r="66" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="19" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="F66"/>
     </row>
@@ -3249,10 +3306,10 @@
       <c r="A67" s="19"/>
       <c r="B67" s="19"/>
       <c r="C67" s="8" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="F67"/>
     </row>
@@ -3260,120 +3317,120 @@
       <c r="A68" s="19"/>
       <c r="B68" s="19"/>
       <c r="C68" s="8" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="F68"/>
     </row>
     <row r="69" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="F69"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B72" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="B72" s="19" t="s">
-        <v>149</v>
-      </c>
       <c r="C72" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="19"/>
       <c r="B73" s="19"/>
       <c r="C73" s="4" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="76" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="19" t="s">
-        <v>56</v>
+        <v>488</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>161</v>
+        <v>489</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="F76"/>
     </row>
@@ -3381,72 +3438,72 @@
       <c r="A77" s="19"/>
       <c r="B77" s="19"/>
       <c r="C77" s="10" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="F77"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>164</v>
+        <v>487</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>212</v>
+        <v>490</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="10" t="s">
-        <v>212</v>
+      <c r="A80" s="17" t="s">
+        <v>490</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>214</v>
+        <v>491</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
-        <v>212</v>
+        <v>488</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="19" t="s">
-        <v>212</v>
+        <v>488</v>
       </c>
       <c r="B82" s="19" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="C82" s="19" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -3454,7 +3511,7 @@
       <c r="B83" s="19"/>
       <c r="C83" s="19"/>
       <c r="D83" s="1" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -3462,7 +3519,7 @@
       <c r="B84" s="19"/>
       <c r="C84" s="19"/>
       <c r="D84" s="1" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -3470,7 +3527,7 @@
       <c r="B85" s="19"/>
       <c r="C85" s="19"/>
       <c r="D85" s="1" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -3478,7 +3535,7 @@
       <c r="B86" s="19"/>
       <c r="C86" s="19"/>
       <c r="D86" s="1" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -3486,7 +3543,7 @@
       <c r="B87" s="19"/>
       <c r="C87" s="19"/>
       <c r="D87" s="1" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -3494,7 +3551,7 @@
       <c r="B88" s="19"/>
       <c r="C88" s="19"/>
       <c r="D88" s="1" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
@@ -3502,7 +3559,7 @@
       <c r="B89" s="19"/>
       <c r="C89" s="19"/>
       <c r="D89" s="1" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -3510,480 +3567,480 @@
       <c r="B90" s="19"/>
       <c r="C90" s="19"/>
       <c r="D90" s="1" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>212</v>
+        <v>488</v>
       </c>
       <c r="B91" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="17" t="s">
+        <v>488</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="17" t="s">
+        <v>488</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="D93" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="17" t="s">
+        <v>488</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D94" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
     </row>
     <row r="96" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="11" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="E96" s="12"/>
       <c r="F96"/>
     </row>
     <row r="97" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="11" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="E97" s="12"/>
       <c r="F97"/>
     </row>
     <row r="98" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="11" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="E98" s="12"/>
       <c r="F98"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="19" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="D99" s="19" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="19"/>
       <c r="B100" s="1" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="D100" s="19"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="19"/>
       <c r="B101" s="1" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="D101" s="19"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="19" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="19"/>
       <c r="B103" s="19"/>
       <c r="C103" s="10" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
     </row>
     <row r="104" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="11" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B104" s="11" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="D104" s="11" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="F104"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="19" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B105" s="19" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="19"/>
       <c r="B106" s="19"/>
       <c r="C106" s="10" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="11" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="E107" s="12" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="11" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="11" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="11" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="19" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="D112" s="19" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="19"/>
       <c r="B113" s="1" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="D113" s="19"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="19"/>
       <c r="B114" s="1" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="D114" s="19"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="11" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="11" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>370</v>
+        <v>487</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="13" t="s">
-        <v>370</v>
+        <v>488</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="13" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="B119" s="13" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A120" s="13" t="s">
-        <v>370</v>
+      <c r="A120" s="17" t="s">
+        <v>487</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A121" s="1" t="s">
-        <v>370</v>
+      <c r="A121" s="17" t="s">
+        <v>488</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A122" s="13" t="s">
-        <v>370</v>
+      <c r="A122" s="17" t="s">
+        <v>487</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="13" t="s">
-        <v>370</v>
+        <v>482</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A124" s="13" t="s">
-        <v>370</v>
+      <c r="A124" s="17" t="s">
+        <v>482</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="19" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="B125" s="19" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="C125" s="18" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="D125" s="18" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -3994,16 +4051,16 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="19" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="B127" s="19" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="C127" s="18" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="D127" s="18" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -4012,56 +4069,137 @@
       <c r="C128" s="19"/>
       <c r="D128" s="19"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" s="19"/>
       <c r="B129" s="19"/>
       <c r="C129" s="19"/>
       <c r="D129" s="19"/>
     </row>
-    <row r="130" spans="1:4" ht="36" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="C130" s="16" t="s">
+        <v>444</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" s="17" t="s">
+        <v>480</v>
+      </c>
+      <c r="B132" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="B130" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="C130" s="16" t="s">
-        <v>459</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A131" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A132" s="1" t="s">
+      <c r="C132" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="17" t="s">
+        <v>480</v>
+      </c>
+      <c r="B134" s="17" t="s">
+        <v>477</v>
+      </c>
+      <c r="C134" s="17" t="s">
+        <v>478</v>
+      </c>
+      <c r="F134"/>
+    </row>
+    <row r="135" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="B135" s="17" t="s">
+        <v>474</v>
+      </c>
+      <c r="C135" s="17" t="s">
+        <v>475</v>
+      </c>
+      <c r="D135" s="17" t="s">
+        <v>476</v>
+      </c>
+      <c r="F135"/>
+    </row>
+    <row r="136" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="19" t="s">
+        <v>465</v>
+      </c>
+      <c r="B136" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="C136" s="18" t="s">
+        <v>467</v>
+      </c>
+      <c r="D136" s="18" t="s">
         <v>468</v>
       </c>
-      <c r="B132" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="C132" s="1" t="s">
+      <c r="E136" s="1"/>
+      <c r="F136"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A137" s="19"/>
+      <c r="B137" s="19"/>
+      <c r="C137" s="19"/>
+      <c r="D137" s="19"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="D132" s="1" t="s">
+      <c r="B138" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="C138" s="1" t="s">
         <v>470</v>
       </c>
+      <c r="D138" s="1" t="s">
+        <v>472</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="56">
+  <mergeCells count="60">
+    <mergeCell ref="A136:A137"/>
+    <mergeCell ref="B136:B137"/>
+    <mergeCell ref="C136:C137"/>
+    <mergeCell ref="D136:D137"/>
     <mergeCell ref="A112:A114"/>
     <mergeCell ref="D112:D114"/>
     <mergeCell ref="C57:C58"/>
@@ -4147,110 +4285,110 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="19"/>
       <c r="B5" s="3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
     </row>
     <row r="25" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4287,255 +4425,255 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>350</v>
+        <v>337</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>352</v>
+        <v>339</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>348</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="B6" s="13">
         <v>0</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>356</v>
+        <v>343</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>357</v>
+        <v>344</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>366</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>434</v>
+        <v>420</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>435</v>
+        <v>421</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>437</v>
+        <v>423</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>440</v>
+        <v>426</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>441</v>
+        <v>427</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>442</v>
+        <v>428</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4563,13 +4701,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4605,24 +4743,24 @@
         <v>4</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4650,82 +4788,82 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -4733,63 +4871,63 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" s="12" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -4820,7 +4958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -4834,43 +4972,43 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>464</v>
+        <v>449</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>466</v>
+        <v>451</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>475</v>
+        <v>459</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>476</v>
+        <v>460</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>477</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update on 20181222.1853 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="2360" yWindow="6780" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RCommands" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="501">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2016,6 +2016,43 @@
   </si>
   <si>
     <t>Sys.Date()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transform()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>airquality &lt;- transform(airquality, Month = factor(Month))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transform airquality's column Month to be factor(Month)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boxplot()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>airquality &lt;- transform(airquality, Month = factor(Month))
+boxplot(Ozone ~ Month, airquality, xlab = "Month", ylab = "Ozone")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>make a boxplot with multiple subplot, each has a different month</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>par()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>par("lty")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the default line type for global graphics parameters</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2421,10 +2458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F138"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="A143" sqref="A143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -4194,12 +4231,64 @@
         <v>472</v>
       </c>
     </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A140" s="19" t="s">
+        <v>473</v>
+      </c>
+      <c r="B140" s="19" t="s">
+        <v>495</v>
+      </c>
+      <c r="C140" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="D140" s="19" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A141" s="19"/>
+      <c r="B141" s="19"/>
+      <c r="C141" s="19"/>
+      <c r="D141" s="19"/>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="60">
+  <mergeCells count="64">
     <mergeCell ref="A136:A137"/>
     <mergeCell ref="B136:B137"/>
     <mergeCell ref="C136:C137"/>
     <mergeCell ref="D136:D137"/>
+    <mergeCell ref="A140:A141"/>
+    <mergeCell ref="B140:B141"/>
+    <mergeCell ref="C140:C141"/>
+    <mergeCell ref="D140:D141"/>
     <mergeCell ref="A112:A114"/>
     <mergeCell ref="D112:D114"/>
     <mergeCell ref="C57:C58"/>

</xml_diff>

<commit_message>
Update on 20181223.1435 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="6780" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="1780" yWindow="780" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RCommands" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="535">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2053,6 +2053,169 @@
   </si>
   <si>
     <t>return the default line type for global graphics parameters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>with(airquality, plot(Wind, Ozone))
+title(main = "Ozone and Wind in New York City")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add a title to the plot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: graphics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>points()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>with(airquality, plot(Wind, Ozone, main = "Ozone and Wind in New York City"))
+with(subset(airquality, Month == 5), points(Wind, Ozone, col = "blue"))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create the title with one call with plot function;
+get a subset of airquality whose Month is May, and re-add the point (Wind, Ozone) of May in blue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>legend()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>with(airquality, plot(Wind, Ozone, main = "Ozone and Wind in New York City", type = "n"))
+with(subset(airquality, Month == 5), points(wind, Ozone, col = "blue"))
+with(subset(airquality, Month != 5), points(Wind, Ozone, col = "red"))
+legend("topright", pch = 1, col = c("blue","red"), legend = c("May", "Other Months"))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type = "n" means do not plot anything but just setup the graphic device
+so the scales are set but no points are plotted;
+add blue points and red points to the gragh;
+add legends to the graph on the top right, shown as rings, with colors and annotation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: stats</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lm()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model &lt;- lm(Ozone ~ Wind, airquality)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>do linear regression on airquality$Ozone and airquality$Wind, just create this model, no plot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>abline()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>with(airquality, plot(Wind, Ozone, main = "Ozone and Wind in New York City", pch = 20))
+model &lt;- lm(Ozone ~ Wind, airquality)
+abline(model, lwd = 2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scatter plot points (Wind, Ozone), points showns as solid circles;
+create a linear regression on (Wind, Ozone);
+add the regression line to the plot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>par(mfrow = c(1, 2))
+with(airquality, {
+plot(Wind, Ozone, main = "Ozone and Wind")
+plot(Solar.R, Ozone, main = "Ozone and Solar Radiation")
+})</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mtext()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>par(mfrow = c(1,3), mar = c(4,4,2,1), oma = c(0,0,2,0))
+with(airquality, {
+plot(Wind, Ozone, main = "Ozone and Wind")
+plot(Solar.R, Ozone, main = "Ozone and Solar Radiation")
+plot(Temp, Ozone, main = "Ozone and Temperature")
+mtext("Ozone and Weather in New York City", outer = TRUE)
+})</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set mar to adjust the distance between the 3 plots;
+set oma to adjust the outer margin, default: c(0,0,0,0). Oma = c(0,0,2,0) leaves space on the top
+mtext add outer title for all 3 plots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>par(mar = c(2,2,2,2))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set the margin of 4 sides to be all 2, the default is c(4,4,2,1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title("Ozone and Wind in New York City")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: graphics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>text()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x &lt;- rnorm(100); y &lt;- rnorm(100); plot(x,y,pch=20); text(0,0, "label")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add text: "label" in the location of (0,0) in the plot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create 2 graphic devices, placed in 1 row of 2 columns;
+scatter plot (Wind, Ozone) on the left graphic device;
+scatter plot (Solar.R, Ozone) on the right graphic device</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gl()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gl(2,3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create a factor object with 2 levels, specified as 1 and 2, each repeats for 3 times</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gl(2,3, labels = c("Male","Female"))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create a factor object with 2 levels, specified as Male and Female, each repeats for 3 times</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2458,17 +2621,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F142"/>
+  <dimension ref="A1:F170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="A143" sqref="A143"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="C181" sqref="C181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="101.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
@@ -4266,21 +4429,296 @@
       <c r="D141" s="19"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A142" s="1" t="s">
+      <c r="A142" s="19" t="s">
         <v>473</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="B142" s="19" t="s">
+        <v>501</v>
+      </c>
+      <c r="C142" s="18" t="s">
+        <v>502</v>
+      </c>
+      <c r="D142" s="19" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A143" s="19"/>
+      <c r="B143" s="19"/>
+      <c r="C143" s="19"/>
+      <c r="D143" s="19"/>
+    </row>
+    <row r="144" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="19"/>
+      <c r="B144" s="19"/>
+      <c r="C144" s="17" t="s">
+        <v>524</v>
+      </c>
+      <c r="D144" s="19"/>
+      <c r="F144"/>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A145" s="19" t="s">
+        <v>504</v>
+      </c>
+      <c r="B145" s="19" t="s">
+        <v>505</v>
+      </c>
+      <c r="C145" s="18" t="s">
+        <v>506</v>
+      </c>
+      <c r="D145" s="18" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A146" s="19"/>
+      <c r="B146" s="19"/>
+      <c r="C146" s="19"/>
+      <c r="D146" s="19"/>
+    </row>
+    <row r="147" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="19" t="s">
+        <v>504</v>
+      </c>
+      <c r="B147" s="19" t="s">
+        <v>508</v>
+      </c>
+      <c r="C147" s="18" t="s">
+        <v>509</v>
+      </c>
+      <c r="D147" s="18" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A148" s="19"/>
+      <c r="B148" s="19"/>
+      <c r="C148" s="18"/>
+      <c r="D148" s="19"/>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A149" s="19"/>
+      <c r="B149" s="19"/>
+      <c r="C149" s="18"/>
+      <c r="D149" s="19"/>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A150" s="19"/>
+      <c r="B150" s="19"/>
+      <c r="C150" s="18"/>
+      <c r="D150" s="19"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A151" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="19" t="s">
+        <v>473</v>
+      </c>
+      <c r="B152" s="19" t="s">
+        <v>515</v>
+      </c>
+      <c r="C152" s="18" t="s">
+        <v>516</v>
+      </c>
+      <c r="D152" s="18" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A153" s="19"/>
+      <c r="B153" s="19"/>
+      <c r="C153" s="18"/>
+      <c r="D153" s="19"/>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A154" s="19" t="s">
+        <v>473</v>
+      </c>
+      <c r="B154" s="19" t="s">
         <v>498</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="C154" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="D142" s="1" t="s">
+      <c r="D154" s="1" t="s">
         <v>500</v>
       </c>
     </row>
+    <row r="155" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="19"/>
+      <c r="B155" s="19"/>
+      <c r="C155" s="17" t="s">
+        <v>522</v>
+      </c>
+      <c r="D155" s="17" t="s">
+        <v>523</v>
+      </c>
+      <c r="F155"/>
+    </row>
+    <row r="156" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="19"/>
+      <c r="B156" s="19"/>
+      <c r="C156" s="18" t="s">
+        <v>518</v>
+      </c>
+      <c r="D156" s="18" t="s">
+        <v>529</v>
+      </c>
+      <c r="F156"/>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A157" s="19"/>
+      <c r="B157" s="19"/>
+      <c r="C157" s="19"/>
+      <c r="D157" s="19"/>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A158" s="19"/>
+      <c r="B158" s="19"/>
+      <c r="C158" s="19"/>
+      <c r="D158" s="19"/>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A159" s="19"/>
+      <c r="B159" s="19"/>
+      <c r="C159" s="19"/>
+      <c r="D159" s="19"/>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A160" s="19"/>
+      <c r="B160" s="19"/>
+      <c r="C160" s="19"/>
+      <c r="D160" s="19"/>
+    </row>
+    <row r="161" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="19" t="s">
+        <v>504</v>
+      </c>
+      <c r="B161" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="C161" s="18" t="s">
+        <v>520</v>
+      </c>
+      <c r="D161" s="18" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" s="19"/>
+      <c r="B162" s="19"/>
+      <c r="C162" s="18"/>
+      <c r="D162" s="19"/>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" s="19"/>
+      <c r="B163" s="19"/>
+      <c r="C163" s="18"/>
+      <c r="D163" s="19"/>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" s="19"/>
+      <c r="B164" s="19"/>
+      <c r="C164" s="18"/>
+      <c r="D164" s="19"/>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165" s="19"/>
+      <c r="B165" s="19"/>
+      <c r="C165" s="18"/>
+      <c r="D165" s="19"/>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166" s="19"/>
+      <c r="B166" s="19"/>
+      <c r="C166" s="18"/>
+      <c r="D166" s="19"/>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167" s="19"/>
+      <c r="B167" s="19"/>
+      <c r="C167" s="18"/>
+      <c r="D167" s="19"/>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169" s="19" t="s">
+        <v>482</v>
+      </c>
+      <c r="B169" s="19" t="s">
+        <v>530</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170" s="19"/>
+      <c r="B170" s="19"/>
+      <c r="C170" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>534</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="64">
+  <mergeCells count="90">
+    <mergeCell ref="B169:B170"/>
+    <mergeCell ref="A169:A170"/>
+    <mergeCell ref="D156:D160"/>
+    <mergeCell ref="C161:C167"/>
+    <mergeCell ref="A161:A167"/>
+    <mergeCell ref="B161:B167"/>
+    <mergeCell ref="D161:D167"/>
+    <mergeCell ref="C156:C160"/>
+    <mergeCell ref="B154:B160"/>
+    <mergeCell ref="A154:A160"/>
+    <mergeCell ref="D147:D150"/>
+    <mergeCell ref="A152:A153"/>
+    <mergeCell ref="B152:B153"/>
+    <mergeCell ref="C152:C153"/>
+    <mergeCell ref="D152:D153"/>
+    <mergeCell ref="C147:C150"/>
+    <mergeCell ref="B147:B150"/>
+    <mergeCell ref="A147:A150"/>
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="A145:A146"/>
+    <mergeCell ref="B145:B146"/>
+    <mergeCell ref="C145:C146"/>
+    <mergeCell ref="D145:D146"/>
+    <mergeCell ref="B142:B144"/>
+    <mergeCell ref="A142:A144"/>
+    <mergeCell ref="D142:D144"/>
     <mergeCell ref="A136:A137"/>
     <mergeCell ref="B136:B137"/>
     <mergeCell ref="C136:C137"/>

</xml_diff>

<commit_message>
Update on 20181224.1605 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="780" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RCommands" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Learning Sources" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RCommands!$A$1:$A$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RCommands!$A$1:$A$172</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="568">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1949,14 +1949,6 @@
   </si>
   <si>
     <t>hist()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hist(airquality$Ozone)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>make a histogram</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2216,6 +2208,153 @@
   </si>
   <si>
     <t>create a factor object with 2 levels, specified as Male and Female, each repeats for 3 times</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: grDevices</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pdf()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pdf(file = "myplot.pdf")
+with(faithful, plot(eruptions, waiting))
+title(main = "Old Faithful Geyser data")
+dev.off()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>open PDF device; create 'myplot.pdf' in my working directory
+create plot and send to the myplot.pdf file, no plot appears on screen
+dev.off() closes the PDF file device, it is very important to close the file device</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: grDevices</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dev.off()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>close the file device</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dev.cur()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the currently active graphics device; every graphics device is assigned as an integer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dev.set()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dev.set(3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set the graphics device 3 to be the currently active graphics device</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: grDevices</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dev.copy()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>with(faithful, plot(eruptions, waiting))
+title(main = "Old Faithful Geyser data")
+dev.copy(png, file="geyserplot.png")
+dev.off()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>copy the plot on screen device to png device</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R.version.string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the R version</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R General</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dim()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dim(iris)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the dimension of iris</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>abline(h=12)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw a horizontal line (y = 12) onto the currently active plot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rug()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hist(airquality$Ozone); rug(airquality$Ozone)</t>
+  </si>
+  <si>
+    <t>gives how many data points are in each bucket and where they lie within the bucket.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hist(airquality$Ozone, breaks = 30)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>make a histogram, argument breaks is set to adjust the number or widths of the buckets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>table()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a &lt;- rep(c(NA, 1/0:3), 10); table(a)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>counts the number of each element of a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>barplot()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a &lt;- rep(c(NA, 1/0:3), 10); ta &lt;- table(a); barplot(ta, col = "wheat", main = "Counts")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>represent a table with bars</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2281,7 +2420,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2333,6 +2472,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2621,10 +2763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F170"/>
+  <dimension ref="A1:F187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="C181" sqref="C181"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2656,7 +2798,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -2669,7 +2811,7 @@
     </row>
     <row r="3" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>369</v>
@@ -2681,7 +2823,7 @@
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>55</v>
@@ -2695,7 +2837,7 @@
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>52</v>
@@ -2709,10 +2851,10 @@
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>61</v>
@@ -2725,10 +2867,10 @@
     </row>
     <row r="7" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>225</v>
@@ -2737,7 +2879,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>2</v>
@@ -2750,7 +2892,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>15</v>
@@ -2763,7 +2905,7 @@
     </row>
     <row r="10" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>328</v>
@@ -2774,10 +2916,10 @@
       <c r="F10"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
-        <v>479</v>
-      </c>
-      <c r="B11" s="19" t="s">
+      <c r="A11" s="20" t="s">
+        <v>477</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -2786,20 +2928,20 @@
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="21" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="20"/>
+      <c r="E12" s="21"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
@@ -2831,10 +2973,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -2846,8 +2988,8 @@
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="4" t="s">
         <v>24</v>
       </c>
@@ -2857,8 +2999,8 @@
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="4" t="s">
         <v>26</v>
       </c>
@@ -2868,10 +3010,10 @@
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="20" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -2883,8 +3025,8 @@
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="4" t="s">
         <v>32</v>
       </c>
@@ -2894,10 +3036,10 @@
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="20" t="s">
         <v>34</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -2909,8 +3051,8 @@
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="4" t="s">
         <v>37</v>
       </c>
@@ -2920,8 +3062,8 @@
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="4" t="s">
         <v>39</v>
       </c>
@@ -2931,8 +3073,8 @@
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
       <c r="C23" s="4" t="s">
         <v>42</v>
       </c>
@@ -2942,10 +3084,10 @@
       <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="20" t="s">
         <v>43</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -2957,8 +3099,8 @@
       <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
       <c r="C25" s="4" t="s">
         <v>45</v>
       </c>
@@ -2983,46 +3125,46 @@
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="19" t="s">
         <v>58</v>
       </c>
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="19"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="20"/>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="19"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="20"/>
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="20"/>
       <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="19"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="20"/>
       <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -3100,25 +3242,25 @@
       <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D37" s="18" t="s">
+      <c r="D37" s="19" t="s">
         <v>77</v>
       </c>
       <c r="E37" s="4"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="19"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
+      <c r="A38" s="20"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
       <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -3151,7 +3293,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>85</v>
@@ -3166,7 +3308,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>398</v>
@@ -3180,7 +3322,7 @@
     </row>
     <row r="43" spans="1:6" s="15" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>432</v>
@@ -3195,7 +3337,7 @@
     </row>
     <row r="44" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>88</v>
@@ -3209,7 +3351,7 @@
     </row>
     <row r="45" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>90</v>
@@ -3223,7 +3365,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>118</v>
@@ -3238,7 +3380,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>121</v>
@@ -3253,7 +3395,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>124</v>
@@ -3267,10 +3409,10 @@
       <c r="E48" s="4"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="19" t="s">
-        <v>479</v>
-      </c>
-      <c r="B49" s="19" t="s">
+      <c r="A49" s="20" t="s">
+        <v>477</v>
+      </c>
+      <c r="B49" s="20" t="s">
         <v>127</v>
       </c>
       <c r="C49" s="4" t="s">
@@ -3282,8 +3424,8 @@
       <c r="E49" s="4"/>
     </row>
     <row r="50" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="19"/>
-      <c r="B50" s="19"/>
+      <c r="A50" s="20"/>
+      <c r="B50" s="20"/>
       <c r="C50" s="4" t="s">
         <v>133</v>
       </c>
@@ -3294,7 +3436,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>130</v>
@@ -3308,10 +3450,10 @@
       <c r="E51" s="4"/>
     </row>
     <row r="52" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="B52" s="19" t="s">
+      <c r="B52" s="20" t="s">
         <v>160</v>
       </c>
       <c r="C52" s="9" t="s">
@@ -3323,8 +3465,8 @@
       <c r="F52"/>
     </row>
     <row r="53" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="19"/>
-      <c r="B53" s="19"/>
+      <c r="A53" s="20"/>
+      <c r="B53" s="20"/>
       <c r="C53" s="9" t="s">
         <v>168</v>
       </c>
@@ -3349,10 +3491,10 @@
       <c r="F54"/>
     </row>
     <row r="55" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="19" t="s">
+      <c r="A55" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="B55" s="19" t="s">
+      <c r="B55" s="20" t="s">
         <v>164</v>
       </c>
       <c r="C55" s="8" t="s">
@@ -3364,8 +3506,8 @@
       <c r="F55"/>
     </row>
     <row r="56" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="19"/>
-      <c r="B56" s="19"/>
+      <c r="A56" s="20"/>
+      <c r="B56" s="20"/>
       <c r="C56" s="9" t="s">
         <v>172</v>
       </c>
@@ -3375,13 +3517,13 @@
       <c r="F56"/>
     </row>
     <row r="57" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="19" t="s">
+      <c r="A57" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="B57" s="19" t="s">
+      <c r="B57" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="C57" s="18" t="s">
+      <c r="C57" s="19" t="s">
         <v>180</v>
       </c>
       <c r="D57" s="8" t="s">
@@ -3390,50 +3532,50 @@
       <c r="F57"/>
     </row>
     <row r="58" spans="1:6" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A58" s="19"/>
-      <c r="B58" s="19"/>
-      <c r="C58" s="18"/>
+      <c r="A58" s="20"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="19"/>
       <c r="D58" s="9" t="s">
         <v>181</v>
       </c>
       <c r="F58"/>
     </row>
     <row r="59" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="19" t="s">
+      <c r="A59" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="B59" s="19" t="s">
+      <c r="B59" s="20" t="s">
         <v>175</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="D59" s="19" t="s">
+      <c r="D59" s="20" t="s">
         <v>182</v>
       </c>
       <c r="F59"/>
     </row>
     <row r="60" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="19"/>
-      <c r="B60" s="19"/>
+      <c r="A60" s="20"/>
+      <c r="B60" s="20"/>
       <c r="C60" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="D60" s="19"/>
+      <c r="D60" s="20"/>
       <c r="F60"/>
     </row>
     <row r="61" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="19"/>
-      <c r="B61" s="19"/>
+      <c r="A61" s="20"/>
+      <c r="B61" s="20"/>
       <c r="C61" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="D61" s="19"/>
+      <c r="D61" s="20"/>
       <c r="F61"/>
     </row>
     <row r="62" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="19"/>
-      <c r="B62" s="19"/>
+      <c r="A62" s="20"/>
+      <c r="B62" s="20"/>
       <c r="C62" s="8" t="s">
         <v>184</v>
       </c>
@@ -3488,10 +3630,10 @@
       <c r="F65"/>
     </row>
     <row r="66" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="19" t="s">
+      <c r="A66" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="B66" s="19" t="s">
+      <c r="B66" s="20" t="s">
         <v>192</v>
       </c>
       <c r="C66" s="8" t="s">
@@ -3503,8 +3645,8 @@
       <c r="F66"/>
     </row>
     <row r="67" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="19"/>
-      <c r="B67" s="19"/>
+      <c r="A67" s="20"/>
+      <c r="B67" s="20"/>
       <c r="C67" s="8" t="s">
         <v>197</v>
       </c>
@@ -3514,8 +3656,8 @@
       <c r="F67"/>
     </row>
     <row r="68" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="19"/>
-      <c r="B68" s="19"/>
+      <c r="A68" s="20"/>
+      <c r="B68" s="20"/>
       <c r="C68" s="8" t="s">
         <v>198</v>
       </c>
@@ -3568,10 +3710,10 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="19" t="s">
+      <c r="A72" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="B72" s="19" t="s">
+      <c r="B72" s="20" t="s">
         <v>142</v>
       </c>
       <c r="C72" s="1" t="s">
@@ -3582,8 +3724,8 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="19"/>
-      <c r="B73" s="19"/>
+      <c r="A73" s="20"/>
+      <c r="B73" s="20"/>
       <c r="C73" s="4" t="s">
         <v>146</v>
       </c>
@@ -3620,11 +3762,11 @@
       </c>
     </row>
     <row r="76" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="19" t="s">
-        <v>488</v>
-      </c>
-      <c r="B76" s="19" t="s">
-        <v>489</v>
+      <c r="A76" s="20" t="s">
+        <v>486</v>
+      </c>
+      <c r="B76" s="20" t="s">
+        <v>487</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>220</v>
@@ -3635,8 +3777,8 @@
       <c r="F76"/>
     </row>
     <row r="77" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="19"/>
-      <c r="B77" s="19"/>
+      <c r="A77" s="20"/>
+      <c r="B77" s="20"/>
       <c r="C77" s="10" t="s">
         <v>221</v>
       </c>
@@ -3647,7 +3789,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>155</v>
@@ -3661,7 +3803,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>203</v>
@@ -3672,10 +3814,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="17" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>204</v>
@@ -3683,7 +3825,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>205</v>
@@ -3693,13 +3835,13 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="19" t="s">
-        <v>488</v>
-      </c>
-      <c r="B82" s="19" t="s">
+      <c r="A82" s="20" t="s">
+        <v>486</v>
+      </c>
+      <c r="B82" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="C82" s="19" t="s">
+      <c r="C82" s="20" t="s">
         <v>218</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -3707,72 +3849,72 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="19"/>
-      <c r="B83" s="19"/>
-      <c r="C83" s="19"/>
+      <c r="A83" s="20"/>
+      <c r="B83" s="20"/>
+      <c r="C83" s="20"/>
       <c r="D83" s="1" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="19"/>
-      <c r="B84" s="19"/>
-      <c r="C84" s="19"/>
+      <c r="A84" s="20"/>
+      <c r="B84" s="20"/>
+      <c r="C84" s="20"/>
       <c r="D84" s="1" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="19"/>
-      <c r="B85" s="19"/>
-      <c r="C85" s="19"/>
+      <c r="A85" s="20"/>
+      <c r="B85" s="20"/>
+      <c r="C85" s="20"/>
       <c r="D85" s="1" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="19"/>
-      <c r="B86" s="19"/>
-      <c r="C86" s="19"/>
+      <c r="A86" s="20"/>
+      <c r="B86" s="20"/>
+      <c r="C86" s="20"/>
       <c r="D86" s="1" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="19"/>
-      <c r="B87" s="19"/>
-      <c r="C87" s="19"/>
+      <c r="A87" s="20"/>
+      <c r="B87" s="20"/>
+      <c r="C87" s="20"/>
       <c r="D87" s="1" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="19"/>
-      <c r="B88" s="19"/>
-      <c r="C88" s="19"/>
+      <c r="A88" s="20"/>
+      <c r="B88" s="20"/>
+      <c r="C88" s="20"/>
       <c r="D88" s="1" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="19"/>
-      <c r="B89" s="19"/>
-      <c r="C89" s="19"/>
+      <c r="A89" s="20"/>
+      <c r="B89" s="20"/>
+      <c r="C89" s="20"/>
       <c r="D89" s="1" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="19"/>
-      <c r="B90" s="19"/>
-      <c r="C90" s="19"/>
+      <c r="A90" s="20"/>
+      <c r="B90" s="20"/>
+      <c r="C90" s="20"/>
       <c r="D90" s="1" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>219</v>
@@ -3786,7 +3928,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="17" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>226</v>
@@ -3800,7 +3942,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="17" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>229</v>
@@ -3814,7 +3956,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="17" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>232</v>
@@ -3889,7 +4031,7 @@
       <c r="F98"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99" s="19" t="s">
+      <c r="A99" s="20" t="s">
         <v>153</v>
       </c>
       <c r="B99" s="1" t="s">
@@ -3898,35 +4040,35 @@
       <c r="C99" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="D99" s="19" t="s">
+      <c r="D99" s="20" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="19"/>
+      <c r="A100" s="20"/>
       <c r="B100" s="1" t="s">
         <v>237</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D100" s="19"/>
+      <c r="D100" s="20"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="19"/>
+      <c r="A101" s="20"/>
       <c r="B101" s="1" t="s">
         <v>239</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="D101" s="19"/>
+      <c r="D101" s="20"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102" s="19" t="s">
+      <c r="A102" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="B102" s="19" t="s">
+      <c r="B102" s="20" t="s">
         <v>240</v>
       </c>
       <c r="C102" s="1" t="s">
@@ -3937,8 +4079,8 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" s="19"/>
-      <c r="B103" s="19"/>
+      <c r="A103" s="20"/>
+      <c r="B103" s="20"/>
       <c r="C103" s="10" t="s">
         <v>243</v>
       </c>
@@ -3962,10 +4104,10 @@
       <c r="F104"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105" s="19" t="s">
+      <c r="A105" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="B105" s="19" t="s">
+      <c r="B105" s="20" t="s">
         <v>245</v>
       </c>
       <c r="C105" s="1" t="s">
@@ -3976,8 +4118,8 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106" s="19"/>
-      <c r="B106" s="19"/>
+      <c r="A106" s="20"/>
+      <c r="B106" s="20"/>
       <c r="C106" s="10" t="s">
         <v>248</v>
       </c>
@@ -4059,7 +4201,7 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A112" s="19" t="s">
+      <c r="A112" s="20" t="s">
         <v>153</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -4068,29 +4210,29 @@
       <c r="C112" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="D112" s="19" t="s">
+      <c r="D112" s="20" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A113" s="19"/>
+      <c r="A113" s="20"/>
       <c r="B113" s="1" t="s">
         <v>315</v>
       </c>
       <c r="C113" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="D113" s="19"/>
+      <c r="D113" s="20"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A114" s="19"/>
+      <c r="A114" s="20"/>
       <c r="B114" s="1" t="s">
         <v>316</v>
       </c>
       <c r="C114" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="D114" s="19"/>
+      <c r="D114" s="20"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="11" t="s">
@@ -4122,7 +4264,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>357</v>
@@ -4136,7 +4278,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="13" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>360</v>
@@ -4161,7 +4303,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="17" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>366</v>
@@ -4175,7 +4317,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="17" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>371</v>
@@ -4189,7 +4331,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="17" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>374</v>
@@ -4203,7 +4345,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>377</v>
@@ -4217,7 +4359,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="17" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>380</v>
@@ -4230,50 +4372,50 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A125" s="19" t="s">
+      <c r="A125" s="20" t="s">
         <v>383</v>
       </c>
-      <c r="B125" s="19" t="s">
+      <c r="B125" s="20" t="s">
         <v>384</v>
       </c>
-      <c r="C125" s="18" t="s">
+      <c r="C125" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="D125" s="18" t="s">
+      <c r="D125" s="19" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A126" s="19"/>
-      <c r="B126" s="19"/>
-      <c r="C126" s="19"/>
-      <c r="D126" s="19"/>
+      <c r="A126" s="20"/>
+      <c r="B126" s="20"/>
+      <c r="C126" s="20"/>
+      <c r="D126" s="20"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A127" s="19" t="s">
+      <c r="A127" s="20" t="s">
         <v>389</v>
       </c>
-      <c r="B127" s="19" t="s">
+      <c r="B127" s="20" t="s">
         <v>390</v>
       </c>
-      <c r="C127" s="18" t="s">
+      <c r="C127" s="19" t="s">
         <v>392</v>
       </c>
-      <c r="D127" s="18" t="s">
+      <c r="D127" s="19" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A128" s="19"/>
-      <c r="B128" s="19"/>
-      <c r="C128" s="19"/>
-      <c r="D128" s="19"/>
+      <c r="A128" s="20"/>
+      <c r="B128" s="20"/>
+      <c r="C128" s="20"/>
+      <c r="D128" s="20"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A129" s="19"/>
-      <c r="B129" s="19"/>
-      <c r="C129" s="19"/>
-      <c r="D129" s="19"/>
+      <c r="A129" s="20"/>
+      <c r="B129" s="20"/>
+      <c r="C129" s="20"/>
+      <c r="D129" s="20"/>
     </row>
     <row r="130" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
@@ -4291,7 +4433,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>431</v>
@@ -4305,7 +4447,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="17" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>452</v>
@@ -4333,13 +4475,13 @@
     </row>
     <row r="134" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="17" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B134" s="17" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C134" s="17" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="F134"/>
     </row>
@@ -4351,382 +4493,569 @@
         <v>474</v>
       </c>
       <c r="C135" s="17" t="s">
-        <v>475</v>
+        <v>560</v>
       </c>
       <c r="D135" s="17" t="s">
-        <v>476</v>
+        <v>561</v>
       </c>
       <c r="F135"/>
     </row>
     <row r="136" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="19" t="s">
+      <c r="A136" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="B136" s="17" t="s">
+        <v>557</v>
+      </c>
+      <c r="C136" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="D136" s="18" t="s">
+        <v>559</v>
+      </c>
+      <c r="F136"/>
+    </row>
+    <row r="137" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="20" t="s">
         <v>465</v>
       </c>
-      <c r="B136" s="19" t="s">
+      <c r="B137" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="C136" s="18" t="s">
+      <c r="C137" s="19" t="s">
         <v>467</v>
       </c>
-      <c r="D136" s="18" t="s">
+      <c r="D137" s="19" t="s">
         <v>468</v>
       </c>
-      <c r="E136" s="1"/>
-      <c r="F136"/>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A137" s="19"/>
-      <c r="B137" s="19"/>
-      <c r="C137" s="19"/>
-      <c r="D137" s="19"/>
+      <c r="E137" s="1"/>
+      <c r="F137"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A138" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>472</v>
-      </c>
+      <c r="A138" s="20"/>
+      <c r="B138" s="20"/>
+      <c r="C138" s="20"/>
+      <c r="D138" s="20"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>488</v>
+        <v>469</v>
       </c>
       <c r="B139" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A140" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="D140" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="C139" s="1" t="s">
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A141" s="20" t="s">
+        <v>473</v>
+      </c>
+      <c r="B141" s="20" t="s">
         <v>493</v>
       </c>
-      <c r="D139" s="1" t="s">
+      <c r="C141" s="19" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A140" s="19" t="s">
+      <c r="D141" s="20" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A142" s="20"/>
+      <c r="B142" s="20"/>
+      <c r="C142" s="20"/>
+      <c r="D142" s="20"/>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A143" s="20" t="s">
         <v>473</v>
       </c>
-      <c r="B140" s="19" t="s">
-        <v>495</v>
-      </c>
-      <c r="C140" s="18" t="s">
+      <c r="B143" s="20" t="s">
+        <v>499</v>
+      </c>
+      <c r="C143" s="19" t="s">
+        <v>500</v>
+      </c>
+      <c r="D143" s="20" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A144" s="20"/>
+      <c r="B144" s="20"/>
+      <c r="C144" s="20"/>
+      <c r="D144" s="20"/>
+    </row>
+    <row r="145" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="20"/>
+      <c r="B145" s="20"/>
+      <c r="C145" s="17" t="s">
+        <v>522</v>
+      </c>
+      <c r="D145" s="20"/>
+      <c r="F145"/>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A146" s="20" t="s">
+        <v>502</v>
+      </c>
+      <c r="B146" s="20" t="s">
+        <v>503</v>
+      </c>
+      <c r="C146" s="19" t="s">
+        <v>504</v>
+      </c>
+      <c r="D146" s="19" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A147" s="20"/>
+      <c r="B147" s="20"/>
+      <c r="C147" s="20"/>
+      <c r="D147" s="20"/>
+    </row>
+    <row r="148" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="20" t="s">
+        <v>502</v>
+      </c>
+      <c r="B148" s="20" t="s">
+        <v>506</v>
+      </c>
+      <c r="C148" s="19" t="s">
+        <v>507</v>
+      </c>
+      <c r="D148" s="19" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A149" s="20"/>
+      <c r="B149" s="20"/>
+      <c r="C149" s="19"/>
+      <c r="D149" s="20"/>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A150" s="20"/>
+      <c r="B150" s="20"/>
+      <c r="C150" s="19"/>
+      <c r="D150" s="20"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A151" s="20"/>
+      <c r="B151" s="20"/>
+      <c r="C151" s="19"/>
+      <c r="D151" s="20"/>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="20" t="s">
+        <v>473</v>
+      </c>
+      <c r="B153" s="20" t="s">
+        <v>513</v>
+      </c>
+      <c r="C153" s="19" t="s">
+        <v>514</v>
+      </c>
+      <c r="D153" s="19" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A154" s="20"/>
+      <c r="B154" s="20"/>
+      <c r="C154" s="19"/>
+      <c r="D154" s="20"/>
+    </row>
+    <row r="155" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="20"/>
+      <c r="B155" s="20"/>
+      <c r="C155" s="18" t="s">
+        <v>555</v>
+      </c>
+      <c r="D155" s="17" t="s">
+        <v>556</v>
+      </c>
+      <c r="F155"/>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A156" s="20" t="s">
+        <v>473</v>
+      </c>
+      <c r="B156" s="20" t="s">
         <v>496</v>
       </c>
-      <c r="D140" s="19" t="s">
+      <c r="C156" s="1" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A141" s="19"/>
-      <c r="B141" s="19"/>
-      <c r="C141" s="19"/>
-      <c r="D141" s="19"/>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A142" s="19" t="s">
-        <v>473</v>
-      </c>
-      <c r="B142" s="19" t="s">
-        <v>501</v>
-      </c>
-      <c r="C142" s="18" t="s">
+      <c r="D156" s="1" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="20"/>
+      <c r="B157" s="20"/>
+      <c r="C157" s="17" t="s">
+        <v>520</v>
+      </c>
+      <c r="D157" s="17" t="s">
+        <v>521</v>
+      </c>
+      <c r="F157"/>
+    </row>
+    <row r="158" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="20"/>
+      <c r="B158" s="20"/>
+      <c r="C158" s="19" t="s">
+        <v>516</v>
+      </c>
+      <c r="D158" s="19" t="s">
+        <v>527</v>
+      </c>
+      <c r="F158"/>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A159" s="20"/>
+      <c r="B159" s="20"/>
+      <c r="C159" s="20"/>
+      <c r="D159" s="20"/>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A160" s="20"/>
+      <c r="B160" s="20"/>
+      <c r="C160" s="20"/>
+      <c r="D160" s="20"/>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" s="20"/>
+      <c r="B161" s="20"/>
+      <c r="C161" s="20"/>
+      <c r="D161" s="20"/>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" s="20"/>
+      <c r="B162" s="20"/>
+      <c r="C162" s="20"/>
+      <c r="D162" s="20"/>
+    </row>
+    <row r="163" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="20" t="s">
         <v>502</v>
       </c>
-      <c r="D142" s="19" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A143" s="19"/>
-      <c r="B143" s="19"/>
-      <c r="C143" s="19"/>
-      <c r="D143" s="19"/>
-    </row>
-    <row r="144" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="19"/>
-      <c r="B144" s="19"/>
-      <c r="C144" s="17" t="s">
+      <c r="B163" s="20" t="s">
+        <v>517</v>
+      </c>
+      <c r="C163" s="19" t="s">
+        <v>518</v>
+      </c>
+      <c r="D163" s="19" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" s="20"/>
+      <c r="B164" s="20"/>
+      <c r="C164" s="19"/>
+      <c r="D164" s="20"/>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165" s="20"/>
+      <c r="B165" s="20"/>
+      <c r="C165" s="19"/>
+      <c r="D165" s="20"/>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166" s="20"/>
+      <c r="B166" s="20"/>
+      <c r="C166" s="19"/>
+      <c r="D166" s="20"/>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167" s="20"/>
+      <c r="B167" s="20"/>
+      <c r="C167" s="19"/>
+      <c r="D167" s="20"/>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168" s="20"/>
+      <c r="B168" s="20"/>
+      <c r="C168" s="19"/>
+      <c r="D168" s="20"/>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169" s="20"/>
+      <c r="B169" s="20"/>
+      <c r="C169" s="19"/>
+      <c r="D169" s="20"/>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="B170" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="D144" s="19"/>
-      <c r="F144"/>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A145" s="19" t="s">
-        <v>504</v>
-      </c>
-      <c r="B145" s="19" t="s">
-        <v>505</v>
-      </c>
-      <c r="C145" s="18" t="s">
-        <v>506</v>
-      </c>
-      <c r="D145" s="18" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A146" s="19"/>
-      <c r="B146" s="19"/>
-      <c r="C146" s="19"/>
-      <c r="D146" s="19"/>
-    </row>
-    <row r="147" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="19" t="s">
-        <v>504</v>
-      </c>
-      <c r="B147" s="19" t="s">
-        <v>508</v>
-      </c>
-      <c r="C147" s="18" t="s">
-        <v>509</v>
-      </c>
-      <c r="D147" s="18" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A148" s="19"/>
-      <c r="B148" s="19"/>
-      <c r="C148" s="18"/>
-      <c r="D148" s="19"/>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A149" s="19"/>
-      <c r="B149" s="19"/>
-      <c r="C149" s="18"/>
-      <c r="D149" s="19"/>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A150" s="19"/>
-      <c r="B150" s="19"/>
-      <c r="C150" s="18"/>
-      <c r="D150" s="19"/>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A151" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="19" t="s">
-        <v>473</v>
-      </c>
-      <c r="B152" s="19" t="s">
-        <v>515</v>
-      </c>
-      <c r="C152" s="18" t="s">
-        <v>516</v>
-      </c>
-      <c r="D152" s="18" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A153" s="19"/>
-      <c r="B153" s="19"/>
-      <c r="C153" s="18"/>
-      <c r="D153" s="19"/>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A154" s="19" t="s">
-        <v>473</v>
-      </c>
-      <c r="B154" s="19" t="s">
-        <v>498</v>
-      </c>
-      <c r="C154" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="19"/>
-      <c r="B155" s="19"/>
-      <c r="C155" s="17" t="s">
-        <v>522</v>
-      </c>
-      <c r="D155" s="17" t="s">
-        <v>523</v>
-      </c>
-      <c r="F155"/>
-    </row>
-    <row r="156" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="19"/>
-      <c r="B156" s="19"/>
-      <c r="C156" s="18" t="s">
-        <v>518</v>
-      </c>
-      <c r="D156" s="18" t="s">
+      <c r="C170" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" s="20" t="s">
+        <v>480</v>
+      </c>
+      <c r="B171" s="20" t="s">
+        <v>528</v>
+      </c>
+      <c r="C171" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="F156"/>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A157" s="19"/>
-      <c r="B157" s="19"/>
-      <c r="C157" s="19"/>
-      <c r="D157" s="19"/>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A158" s="19"/>
-      <c r="B158" s="19"/>
-      <c r="C158" s="19"/>
-      <c r="D158" s="19"/>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A159" s="19"/>
-      <c r="B159" s="19"/>
-      <c r="C159" s="19"/>
-      <c r="D159" s="19"/>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A160" s="19"/>
-      <c r="B160" s="19"/>
-      <c r="C160" s="19"/>
-      <c r="D160" s="19"/>
-    </row>
-    <row r="161" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="19" t="s">
-        <v>504</v>
-      </c>
-      <c r="B161" s="19" t="s">
-        <v>519</v>
-      </c>
-      <c r="C161" s="18" t="s">
-        <v>520</v>
-      </c>
-      <c r="D161" s="18" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A162" s="19"/>
-      <c r="B162" s="19"/>
-      <c r="C162" s="18"/>
-      <c r="D162" s="19"/>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A163" s="19"/>
-      <c r="B163" s="19"/>
-      <c r="C163" s="18"/>
-      <c r="D163" s="19"/>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A164" s="19"/>
-      <c r="B164" s="19"/>
-      <c r="C164" s="18"/>
-      <c r="D164" s="19"/>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A165" s="19"/>
-      <c r="B165" s="19"/>
-      <c r="C165" s="18"/>
-      <c r="D165" s="19"/>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A166" s="19"/>
-      <c r="B166" s="19"/>
-      <c r="C166" s="18"/>
-      <c r="D166" s="19"/>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A167" s="19"/>
-      <c r="B167" s="19"/>
-      <c r="C167" s="18"/>
-      <c r="D167" s="19"/>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A168" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="D168" s="1" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A169" s="19" t="s">
-        <v>482</v>
-      </c>
-      <c r="B169" s="19" t="s">
+      <c r="D171" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="C169" s="1" t="s">
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172" s="20"/>
+      <c r="B172" s="20"/>
+      <c r="C172" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D169" s="1" t="s">
+      <c r="D172" s="1" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A170" s="19"/>
-      <c r="B170" s="19"/>
-      <c r="C170" s="1" t="s">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173" s="20" t="s">
         <v>533</v>
       </c>
-      <c r="D170" s="1" t="s">
+      <c r="B173" s="20" t="s">
         <v>534</v>
       </c>
+      <c r="C173" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="D173" s="19" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174" s="20"/>
+      <c r="B174" s="20"/>
+      <c r="C174" s="20"/>
+      <c r="D174" s="20"/>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175" s="20"/>
+      <c r="B175" s="20"/>
+      <c r="C175" s="20"/>
+      <c r="D175" s="20"/>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176" s="20"/>
+      <c r="B176" s="20"/>
+      <c r="C176" s="20"/>
+      <c r="D176" s="20"/>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178" s="17" t="s">
+        <v>537</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179" s="17" t="s">
+        <v>537</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180" s="20" t="s">
+        <v>545</v>
+      </c>
+      <c r="B180" s="20" t="s">
+        <v>546</v>
+      </c>
+      <c r="C180" s="19" t="s">
+        <v>547</v>
+      </c>
+      <c r="D180" s="20" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181" s="20"/>
+      <c r="B181" s="20"/>
+      <c r="C181" s="20"/>
+      <c r="D181" s="20"/>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182" s="20"/>
+      <c r="B182" s="20"/>
+      <c r="C182" s="20"/>
+      <c r="D182" s="20"/>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183" s="20"/>
+      <c r="B183" s="20"/>
+      <c r="C183" s="20"/>
+      <c r="D183" s="20"/>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A186" s="17" t="s">
+        <v>480</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A187" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>567</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="90">
-    <mergeCell ref="B169:B170"/>
-    <mergeCell ref="A169:A170"/>
-    <mergeCell ref="D156:D160"/>
-    <mergeCell ref="C161:C167"/>
-    <mergeCell ref="A161:A167"/>
-    <mergeCell ref="B161:B167"/>
-    <mergeCell ref="D161:D167"/>
-    <mergeCell ref="C156:C160"/>
-    <mergeCell ref="B154:B160"/>
-    <mergeCell ref="A154:A160"/>
-    <mergeCell ref="D147:D150"/>
-    <mergeCell ref="A152:A153"/>
-    <mergeCell ref="B152:B153"/>
-    <mergeCell ref="C152:C153"/>
-    <mergeCell ref="D152:D153"/>
-    <mergeCell ref="C147:C150"/>
-    <mergeCell ref="B147:B150"/>
-    <mergeCell ref="A147:A150"/>
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="A145:A146"/>
-    <mergeCell ref="B145:B146"/>
-    <mergeCell ref="C145:C146"/>
-    <mergeCell ref="D145:D146"/>
-    <mergeCell ref="B142:B144"/>
-    <mergeCell ref="A142:A144"/>
-    <mergeCell ref="D142:D144"/>
-    <mergeCell ref="A136:A137"/>
-    <mergeCell ref="B136:B137"/>
-    <mergeCell ref="C136:C137"/>
-    <mergeCell ref="D136:D137"/>
-    <mergeCell ref="A140:A141"/>
-    <mergeCell ref="B140:B141"/>
-    <mergeCell ref="C140:C141"/>
-    <mergeCell ref="D140:D141"/>
+  <mergeCells count="98">
+    <mergeCell ref="D173:D176"/>
+    <mergeCell ref="C180:C183"/>
+    <mergeCell ref="B180:B183"/>
+    <mergeCell ref="A180:A183"/>
+    <mergeCell ref="D180:D183"/>
+    <mergeCell ref="B171:B172"/>
+    <mergeCell ref="A171:A172"/>
+    <mergeCell ref="C173:C176"/>
+    <mergeCell ref="B173:B176"/>
+    <mergeCell ref="A173:A176"/>
+    <mergeCell ref="D158:D162"/>
+    <mergeCell ref="C163:C169"/>
+    <mergeCell ref="A163:A169"/>
+    <mergeCell ref="B163:B169"/>
+    <mergeCell ref="D163:D169"/>
+    <mergeCell ref="C158:C162"/>
+    <mergeCell ref="B156:B162"/>
+    <mergeCell ref="A156:A162"/>
+    <mergeCell ref="B153:B155"/>
+    <mergeCell ref="A153:A155"/>
+    <mergeCell ref="D148:D151"/>
+    <mergeCell ref="C153:C154"/>
+    <mergeCell ref="D153:D154"/>
+    <mergeCell ref="C148:C151"/>
+    <mergeCell ref="B148:B151"/>
+    <mergeCell ref="A148:A151"/>
+    <mergeCell ref="C143:C144"/>
+    <mergeCell ref="A146:A147"/>
+    <mergeCell ref="B146:B147"/>
+    <mergeCell ref="C146:C147"/>
+    <mergeCell ref="D146:D147"/>
+    <mergeCell ref="B143:B145"/>
+    <mergeCell ref="A143:A145"/>
+    <mergeCell ref="D143:D145"/>
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="B137:B138"/>
+    <mergeCell ref="C137:C138"/>
+    <mergeCell ref="D137:D138"/>
+    <mergeCell ref="A141:A142"/>
+    <mergeCell ref="B141:B142"/>
+    <mergeCell ref="C141:C142"/>
+    <mergeCell ref="D141:D142"/>
     <mergeCell ref="A112:A114"/>
     <mergeCell ref="D112:D114"/>
     <mergeCell ref="C57:C58"/>
@@ -4841,7 +5170,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="20" t="s">
         <v>98</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -4852,7 +5181,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="3" t="s">
         <v>116</v>
       </c>
@@ -4888,7 +5217,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="20" t="s">
         <v>108</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -4899,7 +5228,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="2" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
Update on 20181227.1225 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RCommands" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Learning Sources" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RCommands!$A$1:$A$172</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RCommands!$A$1:$A$170</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="579">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -940,10 +940,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>as.Date(c("1jan1960","2jan1960"), "%d%b%y")</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>turn date in character format to Date class</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1902,10 +1898,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>plot(cars$speed, cars$dist)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>plot points (cars$speed, cars$dist)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2080,13 +2072,6 @@
   </si>
   <si>
     <t>legend()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>with(airquality, plot(Wind, Ozone, main = "Ozone and Wind in New York City", type = "n"))
-with(subset(airquality, Month == 5), points(wind, Ozone, col = "blue"))
-with(subset(airquality, Month != 5), points(Wind, Ozone, col = "red"))
-legend("topright", pch = 1, col = c("blue","red"), legend = c("May", "Other Months"))</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2355,6 +2340,76 @@
   </si>
   <si>
     <t>represent a table with bars</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>as.Date(c("1jan1960","2jan1960"), "%d%b%Y")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>strptime()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>strptime(c("2006-01-08 10:07:52", "2006-08-07 19:33:02"),
+"%Y-%m-%d %H:%M:%S", tz = "EST5EDT"))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>convert character date time to Date/Time Classes
+tz means timezone, EST for the first date time and EDT for the second date time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lines()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot(x, y); lines(x, y)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add lines to the scatter plot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot(cars$speed, cars$dist)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot(cars$speed, cars$dist, type = "l")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot lines instead of points</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>with(airquality, plot(Wind, Ozone, main = "Ozone and Wind in New York City", type = "n"))
+with(subset(airquality, Month == 5), points(Wind, Ozone, col = "blue"))
+with(subset(airquality, Month != 5), points(Wind, Ozone, col = "red"))
+legend("topright", pch = 1, col = c("blue","red"), legend = c("May", "Other Months"))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set.seed(10)
+x &lt;- rnorm(100)
+f &lt;- rep(0:1, each = 50)
+y &lt;- x + f - f * x + rnorm(100, sd = 0.5)
+f &lt;- factor(f, labels = c("Group 1", "Group 2"))
+xyplot(y ~ x | f, panel = function(x, y, ...){
+panel.xyplot(x, y, ...)
+panel.abline(h = median(y), lty = 2)})</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>panel argument allows for operations on each panel:
+panel.xyplot(x,y, ...) create points (x,y) in each panel
+panel.abline(h=median(y), lty=2) add horizontal line (median of y) in each panel</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2763,10 +2818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F187"/>
+  <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="C201" sqref="C201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2798,7 +2853,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -2811,19 +2866,19 @@
     </row>
     <row r="3" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>369</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>370</v>
       </c>
       <c r="F3"/>
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>55</v>
@@ -2837,7 +2892,7 @@
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>52</v>
@@ -2851,10 +2906,10 @@
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>61</v>
@@ -2867,19 +2922,19 @@
     </row>
     <row r="7" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>2</v>
@@ -2892,7 +2947,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>15</v>
@@ -2905,19 +2960,19 @@
     </row>
     <row r="10" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B10" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>328</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>329</v>
       </c>
       <c r="F10"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B11" s="20" t="s">
         <v>10</v>
@@ -2960,16 +3015,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>446</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -3203,10 +3258,10 @@
         <v>84</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>440</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>441</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34"/>
@@ -3216,13 +3271,13 @@
         <v>19</v>
       </c>
       <c r="B35" s="15" t="s">
+        <v>437</v>
+      </c>
+      <c r="C35" s="15" t="s">
         <v>438</v>
       </c>
-      <c r="C35" s="15" t="s">
-        <v>439</v>
-      </c>
       <c r="D35" s="15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F35"/>
     </row>
@@ -3293,7 +3348,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>85</v>
@@ -3308,36 +3363,36 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="15" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B43" s="15" t="s">
+        <v>431</v>
+      </c>
+      <c r="C43" s="16" t="s">
         <v>432</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="D43" s="16" t="s">
         <v>433</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>434</v>
       </c>
       <c r="F43"/>
     </row>
     <row r="44" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>88</v>
@@ -3351,7 +3406,7 @@
     </row>
     <row r="45" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>90</v>
@@ -3365,7 +3420,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>118</v>
@@ -3380,7 +3435,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>121</v>
@@ -3395,7 +3450,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>124</v>
@@ -3410,7 +3465,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B49" s="20" t="s">
         <v>127</v>
@@ -3436,7 +3491,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>130</v>
@@ -3763,10 +3818,10 @@
     </row>
     <row r="76" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="20" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B76" s="20" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>220</v>
@@ -3789,7 +3844,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>155</v>
@@ -3803,7 +3858,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>203</v>
@@ -3814,10 +3869,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="17" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>204</v>
@@ -3825,7 +3880,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>205</v>
@@ -3836,7 +3891,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="20" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B82" s="20" t="s">
         <v>208</v>
@@ -3914,58 +3969,58 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>219</v>
       </c>
       <c r="C91" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="17" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B92" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="D92" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="17" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B93" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="D93" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="17" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B94" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="D94" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
@@ -3976,10 +4031,10 @@
         <v>158</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="96" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3987,13 +4042,13 @@
         <v>153</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C96" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="D96" s="11" t="s">
         <v>287</v>
-      </c>
-      <c r="D96" s="11" t="s">
-        <v>288</v>
       </c>
       <c r="E96" s="12"/>
       <c r="F96"/>
@@ -4003,13 +4058,13 @@
         <v>153</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E97" s="12"/>
       <c r="F97"/>
@@ -4019,13 +4074,13 @@
         <v>153</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E98" s="12"/>
       <c r="F98"/>
@@ -4035,32 +4090,32 @@
         <v>153</v>
       </c>
       <c r="B99" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D99" s="20" t="s">
         <v>235</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="D99" s="20" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="20"/>
       <c r="B100" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="D100" s="20"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="20"/>
       <c r="B101" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D101" s="20"/>
     </row>
@@ -4069,23 +4124,23 @@
         <v>153</v>
       </c>
       <c r="B102" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="20"/>
       <c r="B103" s="20"/>
       <c r="C103" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="104" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -4093,13 +4148,13 @@
         <v>153</v>
       </c>
       <c r="B104" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="C104" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="C104" s="11" t="s">
+      <c r="D104" s="11" t="s">
         <v>307</v>
-      </c>
-      <c r="D104" s="11" t="s">
-        <v>308</v>
       </c>
       <c r="F104"/>
     </row>
@@ -4108,23 +4163,23 @@
         <v>153</v>
       </c>
       <c r="B105" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="D105" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="20"/>
       <c r="B106" s="20"/>
       <c r="C106" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="D106" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
@@ -4132,16 +4187,16 @@
         <v>153</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E107" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
@@ -4149,13 +4204,13 @@
         <v>153</v>
       </c>
       <c r="B108" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>299</v>
-      </c>
       <c r="D108" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
@@ -4163,13 +4218,13 @@
         <v>153</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
@@ -4177,13 +4232,13 @@
         <v>153</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
@@ -4191,13 +4246,13 @@
         <v>153</v>
       </c>
       <c r="B111" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C111" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="D111" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -4205,32 +4260,32 @@
         <v>153</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D112" s="20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="20"/>
       <c r="B113" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D113" s="20"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="20"/>
       <c r="B114" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D114" s="20"/>
     </row>
@@ -4239,13 +4294,13 @@
         <v>153</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -4253,136 +4308,136 @@
         <v>153</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C116" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D116" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B117" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C117" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="D117" s="1" t="s">
         <v>358</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="13" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B118" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D118" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B119" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="D119" s="1" t="s">
         <v>363</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B120" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C120" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="D120" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="17" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B121" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C121" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="D121" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B122" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="D122" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B123" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="D123" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="17" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B124" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C124" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="D124" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="B125" s="20" t="s">
         <v>383</v>
       </c>
-      <c r="B125" s="20" t="s">
-        <v>384</v>
-      </c>
       <c r="C125" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D125" s="19" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -4393,16 +4448,16 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="20" t="s">
+        <v>388</v>
+      </c>
+      <c r="B127" s="20" t="s">
         <v>389</v>
       </c>
-      <c r="B127" s="20" t="s">
-        <v>390</v>
-      </c>
       <c r="C127" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="D127" s="19" t="s">
         <v>392</v>
-      </c>
-      <c r="D127" s="19" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -4419,164 +4474,162 @@
     </row>
     <row r="130" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C130" s="16" t="s">
+        <v>443</v>
+      </c>
+      <c r="D130" s="1" t="s">
         <v>444</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C131" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="D131" s="1" t="s">
         <v>435</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="17" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B132" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C132" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="C132" s="1" t="s">
+      <c r="D132" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="D132" s="1" t="s">
-        <v>454</v>
-      </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A133" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="B133" s="1" t="s">
+      <c r="A133" s="20" t="s">
+        <v>471</v>
+      </c>
+      <c r="B133" s="20" t="s">
+        <v>461</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="D133" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="C133" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>464</v>
-      </c>
     </row>
     <row r="134" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="17" t="s">
-        <v>478</v>
-      </c>
-      <c r="B134" s="17" t="s">
-        <v>475</v>
-      </c>
+      <c r="A134" s="20"/>
+      <c r="B134" s="20"/>
       <c r="C134" s="17" t="s">
-        <v>476</v>
+        <v>573</v>
+      </c>
+      <c r="D134" s="17" t="s">
+        <v>574</v>
       </c>
       <c r="F134"/>
     </row>
     <row r="135" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="17" t="s">
+        <v>476</v>
+      </c>
+      <c r="B135" s="17" t="s">
         <v>473</v>
       </c>
-      <c r="B135" s="17" t="s">
+      <c r="C135" s="17" t="s">
         <v>474</v>
       </c>
-      <c r="C135" s="17" t="s">
-        <v>560</v>
-      </c>
       <c r="D135" s="17" t="s">
-        <v>561</v>
+        <v>575</v>
       </c>
       <c r="F135"/>
     </row>
     <row r="136" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="17" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B136" s="17" t="s">
+        <v>472</v>
+      </c>
+      <c r="C136" s="17" t="s">
         <v>557</v>
       </c>
-      <c r="C136" s="17" t="s">
+      <c r="D136" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D136" s="18" t="s">
-        <v>559</v>
-      </c>
       <c r="F136"/>
     </row>
     <row r="137" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="20" t="s">
-        <v>465</v>
-      </c>
-      <c r="B137" s="20" t="s">
-        <v>466</v>
-      </c>
-      <c r="C137" s="19" t="s">
-        <v>467</v>
-      </c>
-      <c r="D137" s="19" t="s">
-        <v>468</v>
-      </c>
-      <c r="E137" s="1"/>
+      <c r="A137" s="17" t="s">
+        <v>471</v>
+      </c>
+      <c r="B137" s="17" t="s">
+        <v>554</v>
+      </c>
+      <c r="C137" s="17" t="s">
+        <v>555</v>
+      </c>
+      <c r="D137" s="18" t="s">
+        <v>556</v>
+      </c>
       <c r="F137"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A138" s="20"/>
-      <c r="B138" s="20"/>
-      <c r="C138" s="20"/>
-      <c r="D138" s="20"/>
+      <c r="A138" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A139" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="B139" s="1" t="s">
+      <c r="A139" s="20" t="s">
         <v>471</v>
       </c>
-      <c r="C139" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>472</v>
+      <c r="B139" s="20" t="s">
+        <v>491</v>
+      </c>
+      <c r="C139" s="19" t="s">
+        <v>492</v>
+      </c>
+      <c r="D139" s="20" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A140" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>492</v>
-      </c>
+      <c r="A140" s="20"/>
+      <c r="B140" s="20"/>
+      <c r="C140" s="20"/>
+      <c r="D140" s="20"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" s="20" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B141" s="20" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="C141" s="19" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="D141" s="20" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
@@ -4585,44 +4638,44 @@
       <c r="C142" s="20"/>
       <c r="D142" s="20"/>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A143" s="20" t="s">
-        <v>473</v>
-      </c>
-      <c r="B143" s="20" t="s">
-        <v>499</v>
-      </c>
-      <c r="C143" s="19" t="s">
+    <row r="143" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="20"/>
+      <c r="B143" s="20"/>
+      <c r="C143" s="17" t="s">
+        <v>519</v>
+      </c>
+      <c r="D143" s="20"/>
+      <c r="F143"/>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A144" s="20" t="s">
         <v>500</v>
       </c>
-      <c r="D143" s="20" t="s">
+      <c r="B144" s="20" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A144" s="20"/>
-      <c r="B144" s="20"/>
-      <c r="C144" s="20"/>
-      <c r="D144" s="20"/>
-    </row>
-    <row r="145" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C144" s="19" t="s">
+        <v>502</v>
+      </c>
+      <c r="D144" s="19" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="20"/>
       <c r="B145" s="20"/>
-      <c r="C145" s="17" t="s">
-        <v>522</v>
-      </c>
+      <c r="C145" s="20"/>
       <c r="D145" s="20"/>
-      <c r="F145"/>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="146" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="20" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B146" s="20" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C146" s="19" t="s">
-        <v>504</v>
+        <v>576</v>
       </c>
       <c r="D146" s="19" t="s">
         <v>505</v>
@@ -4631,22 +4684,14 @@
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="20"/>
       <c r="B147" s="20"/>
-      <c r="C147" s="20"/>
+      <c r="C147" s="19"/>
       <c r="D147" s="20"/>
     </row>
-    <row r="148" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A148" s="20" t="s">
-        <v>502</v>
-      </c>
-      <c r="B148" s="20" t="s">
-        <v>506</v>
-      </c>
-      <c r="C148" s="19" t="s">
-        <v>507</v>
-      </c>
-      <c r="D148" s="19" t="s">
-        <v>508</v>
-      </c>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A148" s="20"/>
+      <c r="B148" s="20"/>
+      <c r="C148" s="19"/>
+      <c r="D148" s="20"/>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="20"/>
@@ -4655,97 +4700,97 @@
       <c r="D149" s="20"/>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A150" s="20"/>
-      <c r="B150" s="20"/>
-      <c r="C150" s="19"/>
-      <c r="D150" s="20"/>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A151" s="20"/>
-      <c r="B151" s="20"/>
-      <c r="C151" s="19"/>
-      <c r="D151" s="20"/>
+      <c r="A150" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="20" t="s">
+        <v>471</v>
+      </c>
+      <c r="B151" s="20" t="s">
+        <v>510</v>
+      </c>
+      <c r="C151" s="19" t="s">
+        <v>511</v>
+      </c>
+      <c r="D151" s="19" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A152" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="20" t="s">
-        <v>473</v>
-      </c>
-      <c r="B153" s="20" t="s">
-        <v>513</v>
-      </c>
-      <c r="C153" s="19" t="s">
-        <v>514</v>
-      </c>
-      <c r="D153" s="19" t="s">
-        <v>515</v>
-      </c>
+      <c r="A152" s="20"/>
+      <c r="B152" s="20"/>
+      <c r="C152" s="19"/>
+      <c r="D152" s="20"/>
+    </row>
+    <row r="153" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="20"/>
+      <c r="B153" s="20"/>
+      <c r="C153" s="18" t="s">
+        <v>552</v>
+      </c>
+      <c r="D153" s="17" t="s">
+        <v>553</v>
+      </c>
+      <c r="F153"/>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A154" s="20"/>
-      <c r="B154" s="20"/>
-      <c r="C154" s="19"/>
-      <c r="D154" s="20"/>
+      <c r="A154" s="20" t="s">
+        <v>471</v>
+      </c>
+      <c r="B154" s="20" t="s">
+        <v>494</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="155" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155" s="20"/>
       <c r="B155" s="20"/>
-      <c r="C155" s="18" t="s">
-        <v>555</v>
+      <c r="C155" s="17" t="s">
+        <v>517</v>
       </c>
       <c r="D155" s="17" t="s">
-        <v>556</v>
+        <v>518</v>
       </c>
       <c r="F155"/>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A156" s="20" t="s">
-        <v>473</v>
-      </c>
-      <c r="B156" s="20" t="s">
-        <v>496</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="20"/>
+      <c r="B156" s="20"/>
+      <c r="C156" s="19" t="s">
+        <v>513</v>
+      </c>
+      <c r="D156" s="19" t="s">
+        <v>524</v>
+      </c>
+      <c r="F156"/>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="20"/>
       <c r="B157" s="20"/>
-      <c r="C157" s="17" t="s">
-        <v>520</v>
-      </c>
-      <c r="D157" s="17" t="s">
-        <v>521</v>
-      </c>
-      <c r="F157"/>
-    </row>
-    <row r="158" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C157" s="20"/>
+      <c r="D157" s="20"/>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="20"/>
       <c r="B158" s="20"/>
-      <c r="C158" s="19" t="s">
-        <v>516</v>
-      </c>
-      <c r="D158" s="19" t="s">
-        <v>527</v>
-      </c>
-      <c r="F158"/>
+      <c r="C158" s="20"/>
+      <c r="D158" s="20"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" s="20"/>
@@ -4759,31 +4804,31 @@
       <c r="C160" s="20"/>
       <c r="D160" s="20"/>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A161" s="20"/>
-      <c r="B161" s="20"/>
-      <c r="C161" s="20"/>
-      <c r="D161" s="20"/>
+    <row r="161" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="20" t="s">
+        <v>500</v>
+      </c>
+      <c r="B161" s="20" t="s">
+        <v>514</v>
+      </c>
+      <c r="C161" s="19" t="s">
+        <v>515</v>
+      </c>
+      <c r="D161" s="19" t="s">
+        <v>516</v>
+      </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="20"/>
       <c r="B162" s="20"/>
-      <c r="C162" s="20"/>
+      <c r="C162" s="19"/>
       <c r="D162" s="20"/>
     </row>
-    <row r="163" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="20" t="s">
-        <v>502</v>
-      </c>
-      <c r="B163" s="20" t="s">
-        <v>517</v>
-      </c>
-      <c r="C163" s="19" t="s">
-        <v>518</v>
-      </c>
-      <c r="D163" s="19" t="s">
-        <v>519</v>
-      </c>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" s="20"/>
+      <c r="B163" s="20"/>
+      <c r="C163" s="19"/>
+      <c r="D163" s="20"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="20"/>
@@ -4810,68 +4855,68 @@
       <c r="D167" s="20"/>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A168" s="20"/>
-      <c r="B168" s="20"/>
-      <c r="C168" s="19"/>
-      <c r="D168" s="20"/>
+      <c r="A168" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A169" s="20"/>
-      <c r="B169" s="20"/>
-      <c r="C169" s="19"/>
-      <c r="D169" s="20"/>
+      <c r="A169" s="20" t="s">
+        <v>478</v>
+      </c>
+      <c r="B169" s="20" t="s">
+        <v>525</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>527</v>
+      </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A170" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>524</v>
-      </c>
+      <c r="A170" s="20"/>
+      <c r="B170" s="20"/>
       <c r="C170" s="1" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" s="20" t="s">
-        <v>480</v>
+        <v>530</v>
       </c>
       <c r="B171" s="20" t="s">
-        <v>528</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>530</v>
+        <v>531</v>
+      </c>
+      <c r="C171" s="19" t="s">
+        <v>532</v>
+      </c>
+      <c r="D171" s="19" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="20"/>
       <c r="B172" s="20"/>
-      <c r="C172" s="1" t="s">
-        <v>531</v>
-      </c>
-      <c r="D172" s="1" t="s">
-        <v>532</v>
-      </c>
+      <c r="C172" s="20"/>
+      <c r="D172" s="20"/>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A173" s="20" t="s">
-        <v>533</v>
-      </c>
-      <c r="B173" s="20" t="s">
-        <v>534</v>
-      </c>
-      <c r="C173" s="19" t="s">
-        <v>535</v>
-      </c>
-      <c r="D173" s="19" t="s">
-        <v>536</v>
-      </c>
+      <c r="A173" s="20"/>
+      <c r="B173" s="20"/>
+      <c r="C173" s="20"/>
+      <c r="D173" s="20"/>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="20"/>
@@ -4880,182 +4925,300 @@
       <c r="D174" s="20"/>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A175" s="20"/>
-      <c r="B175" s="20"/>
-      <c r="C175" s="20"/>
-      <c r="D175" s="20"/>
+      <c r="A175" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>536</v>
+      </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A176" s="20"/>
-      <c r="B176" s="20"/>
-      <c r="C176" s="20"/>
-      <c r="D176" s="20"/>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A177" s="1" t="s">
+      <c r="A176" s="17" t="s">
+        <v>534</v>
+      </c>
+      <c r="B176" s="1" t="s">
         <v>537</v>
       </c>
+      <c r="D176" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A177" s="17" t="s">
+        <v>534</v>
+      </c>
       <c r="B177" s="1" t="s">
-        <v>538</v>
+        <v>539</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>540</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A178" s="17" t="s">
-        <v>537</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>540</v>
-      </c>
-      <c r="D178" s="1" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A179" s="17" t="s">
-        <v>537</v>
-      </c>
-      <c r="B179" s="1" t="s">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A178" s="20" t="s">
         <v>542</v>
       </c>
-      <c r="C179" s="1" t="s">
+      <c r="B178" s="20" t="s">
         <v>543</v>
       </c>
-      <c r="D179" s="1" t="s">
+      <c r="C178" s="19" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A180" s="20" t="s">
+      <c r="D178" s="20" t="s">
         <v>545</v>
       </c>
-      <c r="B180" s="20" t="s">
-        <v>546</v>
-      </c>
-      <c r="C180" s="19" t="s">
-        <v>547</v>
-      </c>
-      <c r="D180" s="20" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A179" s="20"/>
+      <c r="B179" s="20"/>
+      <c r="C179" s="20"/>
+      <c r="D179" s="20"/>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A180" s="20"/>
+      <c r="B180" s="20"/>
+      <c r="C180" s="20"/>
+      <c r="D180" s="20"/>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" s="20"/>
       <c r="B181" s="20"/>
       <c r="C181" s="20"/>
       <c r="D181" s="20"/>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A182" s="20"/>
-      <c r="B182" s="20"/>
-      <c r="C182" s="20"/>
-      <c r="D182" s="20"/>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A183" s="20"/>
-      <c r="B183" s="20"/>
-      <c r="C183" s="20"/>
-      <c r="D183" s="20"/>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A184" s="1" t="s">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A182" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A183" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="D183" s="1" t="s">
         <v>551</v>
       </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A184" s="17" t="s">
+        <v>478</v>
+      </c>
       <c r="B184" s="1" t="s">
-        <v>549</v>
+        <v>559</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>560</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>480</v>
+        <v>500</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>552</v>
+        <v>562</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>553</v>
+        <v>563</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A186" s="17" t="s">
-        <v>480</v>
-      </c>
-      <c r="B186" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="C186" s="1" t="s">
-        <v>563</v>
-      </c>
-      <c r="D186" s="1" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A187" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="B187" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="C187" s="1" t="s">
+    <row r="186" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A186" s="20" t="s">
+        <v>478</v>
+      </c>
+      <c r="B186" s="20" t="s">
         <v>566</v>
       </c>
-      <c r="D187" s="1" t="s">
+      <c r="C186" s="19" t="s">
         <v>567</v>
       </c>
+      <c r="D186" s="19" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A187" s="20"/>
+      <c r="B187" s="20"/>
+      <c r="C187" s="19"/>
+      <c r="D187" s="20"/>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A188" s="17" t="s">
+        <v>500</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="C188" s="18" t="s">
+        <v>570</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="20" t="s">
+        <v>463</v>
+      </c>
+      <c r="B189" s="20" t="s">
+        <v>464</v>
+      </c>
+      <c r="C189" s="19" t="s">
+        <v>465</v>
+      </c>
+      <c r="D189" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="E189" s="1"/>
+      <c r="F189"/>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A190" s="20"/>
+      <c r="B190" s="20"/>
+      <c r="C190" s="20"/>
+      <c r="D190" s="20"/>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A191" s="20"/>
+      <c r="B191" s="20"/>
+      <c r="C191" s="19" t="s">
+        <v>577</v>
+      </c>
+      <c r="D191" s="19" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A192" s="20"/>
+      <c r="B192" s="20"/>
+      <c r="C192" s="20"/>
+      <c r="D192" s="20"/>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A193" s="20"/>
+      <c r="B193" s="20"/>
+      <c r="C193" s="20"/>
+      <c r="D193" s="20"/>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A194" s="20"/>
+      <c r="B194" s="20"/>
+      <c r="C194" s="20"/>
+      <c r="D194" s="20"/>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A195" s="20"/>
+      <c r="B195" s="20"/>
+      <c r="C195" s="20"/>
+      <c r="D195" s="20"/>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A196" s="20"/>
+      <c r="B196" s="20"/>
+      <c r="C196" s="20"/>
+      <c r="D196" s="20"/>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197" s="20"/>
+      <c r="B197" s="20"/>
+      <c r="C197" s="20"/>
+      <c r="D197" s="20"/>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A198" s="20"/>
+      <c r="B198" s="20"/>
+      <c r="C198" s="20"/>
+      <c r="D198" s="20"/>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A199" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>470</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="98">
-    <mergeCell ref="D173:D176"/>
-    <mergeCell ref="C180:C183"/>
-    <mergeCell ref="B180:B183"/>
-    <mergeCell ref="A180:A183"/>
-    <mergeCell ref="D180:D183"/>
-    <mergeCell ref="B171:B172"/>
-    <mergeCell ref="A171:A172"/>
-    <mergeCell ref="C173:C176"/>
-    <mergeCell ref="B173:B176"/>
-    <mergeCell ref="A173:A176"/>
-    <mergeCell ref="D158:D162"/>
-    <mergeCell ref="C163:C169"/>
-    <mergeCell ref="A163:A169"/>
-    <mergeCell ref="B163:B169"/>
-    <mergeCell ref="D163:D169"/>
-    <mergeCell ref="C158:C162"/>
-    <mergeCell ref="B156:B162"/>
-    <mergeCell ref="A156:A162"/>
-    <mergeCell ref="B153:B155"/>
-    <mergeCell ref="A153:A155"/>
-    <mergeCell ref="D148:D151"/>
-    <mergeCell ref="C153:C154"/>
-    <mergeCell ref="D153:D154"/>
-    <mergeCell ref="C148:C151"/>
-    <mergeCell ref="B148:B151"/>
-    <mergeCell ref="A148:A151"/>
-    <mergeCell ref="C143:C144"/>
-    <mergeCell ref="A146:A147"/>
-    <mergeCell ref="B146:B147"/>
-    <mergeCell ref="C146:C147"/>
-    <mergeCell ref="D146:D147"/>
-    <mergeCell ref="B143:B145"/>
-    <mergeCell ref="A143:A145"/>
-    <mergeCell ref="D143:D145"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="B137:B138"/>
-    <mergeCell ref="C137:C138"/>
-    <mergeCell ref="D137:D138"/>
-    <mergeCell ref="A141:A142"/>
-    <mergeCell ref="B141:B142"/>
+  <mergeCells count="106">
+    <mergeCell ref="A133:A134"/>
+    <mergeCell ref="B133:B134"/>
+    <mergeCell ref="C191:C198"/>
+    <mergeCell ref="D191:D198"/>
+    <mergeCell ref="B189:B198"/>
+    <mergeCell ref="A189:A198"/>
+    <mergeCell ref="C186:C187"/>
+    <mergeCell ref="B186:B187"/>
+    <mergeCell ref="A186:A187"/>
+    <mergeCell ref="D186:D187"/>
+    <mergeCell ref="D171:D174"/>
+    <mergeCell ref="C178:C181"/>
+    <mergeCell ref="B178:B181"/>
+    <mergeCell ref="A178:A181"/>
+    <mergeCell ref="D178:D181"/>
+    <mergeCell ref="B169:B170"/>
+    <mergeCell ref="A169:A170"/>
+    <mergeCell ref="C171:C174"/>
+    <mergeCell ref="B171:B174"/>
+    <mergeCell ref="A171:A174"/>
+    <mergeCell ref="D156:D160"/>
+    <mergeCell ref="C161:C167"/>
+    <mergeCell ref="A161:A167"/>
+    <mergeCell ref="B161:B167"/>
+    <mergeCell ref="D161:D167"/>
+    <mergeCell ref="C156:C160"/>
+    <mergeCell ref="B154:B160"/>
+    <mergeCell ref="A154:A160"/>
+    <mergeCell ref="B151:B153"/>
+    <mergeCell ref="A151:A153"/>
+    <mergeCell ref="D146:D149"/>
+    <mergeCell ref="C151:C152"/>
+    <mergeCell ref="D151:D152"/>
+    <mergeCell ref="C146:C149"/>
+    <mergeCell ref="B146:B149"/>
+    <mergeCell ref="A146:A149"/>
     <mergeCell ref="C141:C142"/>
-    <mergeCell ref="D141:D142"/>
+    <mergeCell ref="A144:A145"/>
+    <mergeCell ref="B144:B145"/>
+    <mergeCell ref="C144:C145"/>
+    <mergeCell ref="D144:D145"/>
+    <mergeCell ref="B141:B143"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="D141:D143"/>
+    <mergeCell ref="C189:C190"/>
+    <mergeCell ref="D189:D190"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="B139:B140"/>
+    <mergeCell ref="C139:C140"/>
+    <mergeCell ref="D139:D140"/>
     <mergeCell ref="A112:A114"/>
     <mergeCell ref="D112:D114"/>
     <mergeCell ref="C57:C58"/>
@@ -5238,13 +5401,13 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>395</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="25" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5292,134 +5455,134 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B6" s="13">
         <v>0</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="D7" s="13" t="s">
         <v>343</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>350</v>
-      </c>
       <c r="D8" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>418</v>
+      </c>
+      <c r="D10" s="15" t="s">
         <v>420</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>419</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
+        <v>421</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>422</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="D11" s="15" t="s">
         <v>423</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>425</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="D12" s="15" t="s">
         <v>426</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B13" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="D13" s="15" t="s">
         <v>428</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -5427,10 +5590,10 @@
         <v>54</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>340</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -5438,10 +5601,10 @@
         <v>54</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>355</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -5449,10 +5612,10 @@
         <v>92</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -5460,10 +5623,10 @@
         <v>92</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>402</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -5471,10 +5634,10 @@
         <v>54</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -5482,10 +5645,10 @@
         <v>54</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>406</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -5493,43 +5656,43 @@
         <v>54</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>408</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
+        <v>409</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>411</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
+        <v>413</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>414</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5610,13 +5773,13 @@
         <v>54</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>385</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5644,82 +5807,82 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>251</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>253</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>255</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>257</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>259</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>261</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>263</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>265</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>267</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>269</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -5727,63 +5890,63 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>276</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>278</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="B19" s="12" t="s">
         <v>282</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>280</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -5828,43 +5991,43 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>447</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>448</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>450</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
+        <v>456</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>458</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>457</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>459</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
+        <v>459</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>460</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>461</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update on 20181227.1456 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RCommands" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="629">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1930,6 +1930,9 @@
   <si>
     <t>qplot()</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points (mpg$displ, mpg$hwy)</t>
   </si>
   <si>
     <t>plot points (mpg$displ, mpg$hwy)</t>
@@ -2410,6 +2413,253 @@
     <t>panel argument allows for operations on each panel:
 panel.xyplot(x,y, ...) create points (x,y) in each panel
 panel.abline(h=median(y), lty=2) add horizontal line (median of y) in each panel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>panel.lmline(x, y, col=2) add linear regression line in each panel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set.seed(10)
+x &lt;- rnorm(100)
+f &lt;- rep(0:1, each = 50)
+y &lt;- x + f - f * x + rnorm(100, sd = 0.5)
+f &lt;- factor(f, labels = c("Group 1", "Group 2"))
+xyplot(y ~ x | f, panel = function(x, y, ...){
+panel.xyplot(x, y, ...)
+panel.lmline(x, y, col = 2)})</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://ggplot2.org</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qplot(displ, hwy, data = mpg, color = drv)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qplot(displ, hwy, data = mpg, geom = c("point", "smooth"))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points (mpg$displ, mpg$hwy),
+and add a smooth geom to this plot with the gray field as 95% confidence interval</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qplot(hwy, data = mpg, fill = drv)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot a histogram of mpg$hwy,
+and fill in the bar different colors based on what the mpg$drv they are</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qplot(displ, hwy, data = mpg, facets = .~ drv)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qplot(hwy, data = mpg, facets = drv ~., binwidth = 2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qplot(displ, hwy, data = mpg, facets = drv ~.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points (mpg$displ, mpg$hwy),
+separate the points into different panels based on their mpg$drv, all panels in one row</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points (mpg$displ, mpg$hwy),
+separate the points into different panels based on their mpg$drv, all panels in one column</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot a histogram of mpg$hwy,
+separate into different panels based on their mpg$drv, all panels in one column
+binwidth = 2 set the width of the bars</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qplot(hwy, data = mpg, geom = "density")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rather than plot a histogram, a density smooth is plotted</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qplot(hwy, data = mpg, geom = "density", color = drv)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot a density smooth for mpg$hwy,
+seperated into different density smooth based on mpg$drv, and each has different color</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qplot(displ, hwy, data = mpg, shape = drv)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points (mpg$displ, mpg$hwy),
+and display the points in different symbols according to mpg$drv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points (mpg$displ, mpg$hwy),
+and display the points in different colors according to mpg$drv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qplot(displ, hwy, data = mpg, color = drv) + geom_smooth(method = "lm")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points (mpg$displ, mpg$hwy),
+and display the points in different colors according to mpg$drv,
+and add linear regression lines for different groups of points seperated by mpg$drv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points (mpg$displ, mpg$hwy),
+separate into different panels according to mpg$drv,
+and add linear regression lines for different groups of points seperated by mpg$drv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qplot(displ, hwy, data = mpg, facets = .~ drv) + geom_smooth(method = "lm")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ggplot()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g &lt;- ggplot(mpg, aes(displ, hwy))
+summary(g)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set up for plot, but nothing plotted
+summary(g) shows the summary of the setting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: ggplot2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g &lt;- ggplot(mpg, aes(displ, hwy))
+print(g)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set up for plot, but nothing plotted
+print(g) just displays the graph without points plottted</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g &lt;- ggplot(mpg, aes(displ, hwy))
+g + geom_point()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g &lt;- ggplot(mpg, aes(displ, hwy))
+p &lt;- g + geom_point()
+print(p)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g &lt;- ggplot(mpg, aes(displ, hwy))
+g + geom_point() + geom_smooth()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g &lt;- ggplot(mpg, aes(displ, hwy))
+g + geom_point() + geom_smooth(method = "lm")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points (mpg$displ, mpg$hwy)
+and add a smooth curve</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points (mpg$displ, mpg$hwy)
+and add a linear regression line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g &lt;- ggplot(mpg, aes(displ, hwy))
+g + geom_point() + facet_grid(.~ drv) + geom_smooth(method = "lm")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g &lt;- ggplot(mpg, aes(displ, hwy))
+g + geom_point(color = "steelblue", size = 4, alpha = 1/2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g &lt;- ggplot(mpg, aes(displ, hwy))
+g + geom_point(aes(color = drv), size = 4, alpha = 1/2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points (mpg$displ, mpg$hwy)
+separated into different panels based on mpg$drv in on row
+and add a linear regression line to each panel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points (mpg$displ, mpg$hwy)
+the points are set to be in size 4 (default = 1) and in color steelblue and half transparent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points (mpg$displ, mpg$hwy)
+the points are set to be in size 4 (default = 1) and half transparent
+separated into different colors based on mpg$drv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g &lt;- ggplot(mpg, aes(displ, hwy))
+g + geom_point(aes(color = drv)) + labs(title = "mpg cohort")
++ labs(x="DISPL", y="HWY")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points (mpg$displ, mpg$hwy)
+separated into different colors based on mpg$drv
+add x-axis label and y-axis label and title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g &lt;- ggplot(mpg, aes(displ, hwy))
+g + geom_point(aes(color = drv), size = 4, alpha = 1/2) + 
+geom_smooth(size = 4, linetype = 3, method = "lm", se = FALSE)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points (mpg$displ, mpg$hwy)
+the points are set to be in size 4 (default = 1) and half transparent
+separated into different colors based on mpg$drv
+add regression line (dotted line, and se = FALSE turn off confidence interval)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g &lt;- ggplot(mpg, aes(displ, hwy))
+g + geom_point(aes(color = drv)) + theme_bw(base_family = "Times")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points (mpg$displ, mpg$hwy)
+separated into different colors based on mpg$drv
+change the background into normal black and white, change the font to "Times"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2818,10 +3068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F199"/>
+  <dimension ref="A1:F263"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="C201" sqref="C201"/>
+    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="C266" sqref="C266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2853,7 +3103,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -2866,7 +3116,7 @@
     </row>
     <row r="3" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>368</v>
@@ -2878,7 +3128,7 @@
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>55</v>
@@ -2892,7 +3142,7 @@
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>52</v>
@@ -2906,10 +3156,10 @@
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>481</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>480</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>61</v>
@@ -2922,10 +3172,10 @@
     </row>
     <row r="7" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>224</v>
@@ -2934,7 +3184,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>2</v>
@@ -2947,7 +3197,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>15</v>
@@ -2960,7 +3210,7 @@
     </row>
     <row r="10" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>327</v>
@@ -2972,7 +3222,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B11" s="20" t="s">
         <v>10</v>
@@ -3348,7 +3598,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>85</v>
@@ -3363,7 +3613,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>397</v>
@@ -3377,7 +3627,7 @@
     </row>
     <row r="43" spans="1:6" s="15" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>431</v>
@@ -3392,7 +3642,7 @@
     </row>
     <row r="44" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>88</v>
@@ -3406,7 +3656,7 @@
     </row>
     <row r="45" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>90</v>
@@ -3420,7 +3670,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>118</v>
@@ -3435,7 +3685,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>121</v>
@@ -3450,7 +3700,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>124</v>
@@ -3465,7 +3715,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B49" s="20" t="s">
         <v>127</v>
@@ -3491,7 +3741,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>130</v>
@@ -3818,10 +4068,10 @@
     </row>
     <row r="76" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="20" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B76" s="20" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>220</v>
@@ -3844,7 +4094,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>155</v>
@@ -3858,7 +4108,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>203</v>
@@ -3869,10 +4119,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="17" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>204</v>
@@ -3880,7 +4130,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>205</v>
@@ -3891,7 +4141,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="20" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B82" s="20" t="s">
         <v>208</v>
@@ -3969,13 +4219,13 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>219</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>223</v>
@@ -3983,7 +4233,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="17" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>225</v>
@@ -3997,7 +4247,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="17" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>228</v>
@@ -4011,7 +4261,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="17" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>231</v>
@@ -4319,7 +4569,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>356</v>
@@ -4333,7 +4583,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="13" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>359</v>
@@ -4358,7 +4608,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="17" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>365</v>
@@ -4372,7 +4622,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="17" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>370</v>
@@ -4386,7 +4636,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="17" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>373</v>
@@ -4400,7 +4650,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="13" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>376</v>
@@ -4414,7 +4664,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="17" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>379</v>
@@ -4488,7 +4738,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>430</v>
@@ -4502,7 +4752,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="17" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>451</v>
@@ -4516,13 +4766,13 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="20" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B133" s="20" t="s">
         <v>461</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>462</v>
@@ -4532,84 +4782,84 @@
       <c r="A134" s="20"/>
       <c r="B134" s="20"/>
       <c r="C134" s="17" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="D134" s="17" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="F134"/>
     </row>
     <row r="135" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="17" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B135" s="17" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C135" s="17" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D135" s="17" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="F135"/>
     </row>
     <row r="136" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="17" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B136" s="17" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C136" s="17" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="D136" s="17" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="F136"/>
     </row>
     <row r="137" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137" s="17" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B137" s="17" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C137" s="17" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="D137" s="18" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="F137"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="20" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B139" s="20" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C139" s="19" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="D139" s="20" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
@@ -4620,16 +4870,16 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" s="20" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B141" s="20" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C141" s="19" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D141" s="20" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
@@ -4642,23 +4892,23 @@
       <c r="A143" s="20"/>
       <c r="B143" s="20"/>
       <c r="C143" s="17" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="D143" s="20"/>
       <c r="F143"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="20" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B144" s="20" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C144" s="19" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="D144" s="19" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
@@ -4669,16 +4919,16 @@
     </row>
     <row r="146" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="20" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B146" s="20" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C146" s="19" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="D146" s="19" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
@@ -4701,30 +4951,30 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="151" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="20" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B151" s="20" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C151" s="19" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="D151" s="19" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
@@ -4737,35 +4987,35 @@
       <c r="A153" s="20"/>
       <c r="B153" s="20"/>
       <c r="C153" s="18" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="D153" s="17" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="F153"/>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="20" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B154" s="20" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="155" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155" s="20"/>
       <c r="B155" s="20"/>
       <c r="C155" s="17" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="D155" s="17" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="F155"/>
     </row>
@@ -4773,10 +5023,10 @@
       <c r="A156" s="20"/>
       <c r="B156" s="20"/>
       <c r="C156" s="19" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="D156" s="19" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="F156"/>
     </row>
@@ -4806,16 +5056,16 @@
     </row>
     <row r="161" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="20" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B161" s="20" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C161" s="19" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="D161" s="19" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
@@ -4856,54 +5106,54 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" s="20" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B169" s="20" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" s="20"/>
       <c r="B170" s="20"/>
       <c r="C170" s="1" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" s="20" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B171" s="20" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C171" s="19" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D171" s="19" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
@@ -4926,52 +5176,52 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" s="17" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" s="17" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" s="20" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B178" s="20" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C178" s="19" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D178" s="20" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
@@ -4994,69 +5244,69 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="D182" s="1" t="s">
         <v>548</v>
-      </c>
-      <c r="B182" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="D182" s="1" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" s="17" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="20" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B186" s="20" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C186" s="19" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D186" s="19" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
@@ -5067,16 +5317,16 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" s="17" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C188" s="18" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="189" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
@@ -5105,10 +5355,10 @@
       <c r="A191" s="20"/>
       <c r="B191" s="20"/>
       <c r="C191" s="19" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="D191" s="19" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
@@ -5117,64 +5367,613 @@
       <c r="C192" s="20"/>
       <c r="D192" s="20"/>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" s="20"/>
       <c r="B193" s="20"/>
       <c r="C193" s="20"/>
       <c r="D193" s="20"/>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" s="20"/>
       <c r="B194" s="20"/>
       <c r="C194" s="20"/>
       <c r="D194" s="20"/>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" s="20"/>
       <c r="B195" s="20"/>
       <c r="C195" s="20"/>
       <c r="D195" s="20"/>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" s="20"/>
       <c r="B196" s="20"/>
       <c r="C196" s="20"/>
       <c r="D196" s="20"/>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" s="20"/>
       <c r="B197" s="20"/>
       <c r="C197" s="20"/>
       <c r="D197" s="20"/>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" s="20"/>
       <c r="B198" s="20"/>
       <c r="C198" s="20"/>
       <c r="D198" s="20"/>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A199" s="1" t="s">
+    <row r="199" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A199" s="20"/>
+      <c r="B199" s="20"/>
+      <c r="C199" s="19" t="s">
+        <v>581</v>
+      </c>
+      <c r="D199" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="F199"/>
+    </row>
+    <row r="200" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A200" s="20"/>
+      <c r="B200" s="20"/>
+      <c r="C200" s="20"/>
+      <c r="D200" s="20"/>
+      <c r="F200"/>
+    </row>
+    <row r="201" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A201" s="20"/>
+      <c r="B201" s="20"/>
+      <c r="C201" s="20"/>
+      <c r="D201" s="20"/>
+      <c r="F201"/>
+    </row>
+    <row r="202" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="20"/>
+      <c r="B202" s="20"/>
+      <c r="C202" s="20"/>
+      <c r="D202" s="20"/>
+      <c r="F202"/>
+    </row>
+    <row r="203" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A203" s="20"/>
+      <c r="B203" s="20"/>
+      <c r="C203" s="20"/>
+      <c r="D203" s="20"/>
+      <c r="F203"/>
+    </row>
+    <row r="204" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A204" s="20"/>
+      <c r="B204" s="20"/>
+      <c r="C204" s="20"/>
+      <c r="D204" s="20"/>
+      <c r="F204"/>
+    </row>
+    <row r="205" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A205" s="20"/>
+      <c r="B205" s="20"/>
+      <c r="C205" s="20"/>
+      <c r="D205" s="20"/>
+      <c r="F205"/>
+    </row>
+    <row r="206" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A206" s="20"/>
+      <c r="B206" s="20"/>
+      <c r="C206" s="20"/>
+      <c r="D206" s="20"/>
+      <c r="F206"/>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A207" s="20" t="s">
         <v>467</v>
       </c>
-      <c r="B199" s="1" t="s">
+      <c r="B207" s="20" t="s">
         <v>469</v>
       </c>
-      <c r="C199" s="1" t="s">
+      <c r="C207" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="D199" s="1" t="s">
+      <c r="D207" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="E207" s="12" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A208" s="20"/>
+      <c r="B208" s="20"/>
+      <c r="C208" s="20" t="s">
+        <v>583</v>
+      </c>
+      <c r="D208" s="19" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A209" s="20"/>
+      <c r="B209" s="20"/>
+      <c r="C209" s="20"/>
+      <c r="D209" s="20"/>
+      <c r="F209"/>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A210" s="20"/>
+      <c r="B210" s="20"/>
+      <c r="C210" s="20" t="s">
+        <v>584</v>
+      </c>
+      <c r="D210" s="19" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A211" s="20"/>
+      <c r="B211" s="20"/>
+      <c r="C211" s="20"/>
+      <c r="D211" s="20"/>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A212" s="20"/>
+      <c r="B212" s="20"/>
+      <c r="C212" s="20" t="s">
+        <v>586</v>
+      </c>
+      <c r="D212" s="19" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A213" s="20"/>
+      <c r="B213" s="20"/>
+      <c r="C213" s="20"/>
+      <c r="D213" s="20"/>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A214" s="20"/>
+      <c r="B214" s="20"/>
+      <c r="C214" s="20" t="s">
+        <v>588</v>
+      </c>
+      <c r="D214" s="19" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A215" s="20"/>
+      <c r="B215" s="20"/>
+      <c r="C215" s="20"/>
+      <c r="D215" s="20"/>
+    </row>
+    <row r="216" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A216" s="20"/>
+      <c r="B216" s="20"/>
+      <c r="C216" s="20" t="s">
+        <v>590</v>
+      </c>
+      <c r="D216" s="19" t="s">
+        <v>592</v>
+      </c>
+      <c r="F216"/>
+    </row>
+    <row r="217" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A217" s="20"/>
+      <c r="B217" s="20"/>
+      <c r="C217" s="20"/>
+      <c r="D217" s="20"/>
+      <c r="F217"/>
+    </row>
+    <row r="218" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A218" s="20"/>
+      <c r="B218" s="20"/>
+      <c r="C218" s="20" t="s">
+        <v>589</v>
+      </c>
+      <c r="D218" s="19" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A219" s="20"/>
+      <c r="B219" s="20"/>
+      <c r="C219" s="20"/>
+      <c r="D219" s="19"/>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A220" s="20"/>
+      <c r="B220" s="20"/>
+      <c r="C220" s="20"/>
+      <c r="D220" s="19"/>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A221" s="20"/>
+      <c r="B221" s="20"/>
+      <c r="C221" s="17" t="s">
+        <v>594</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A222" s="20"/>
+      <c r="B222" s="20"/>
+      <c r="C222" s="20" t="s">
+        <v>596</v>
+      </c>
+      <c r="D222" s="19" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A223" s="20"/>
+      <c r="B223" s="20"/>
+      <c r="C223" s="20"/>
+      <c r="D223" s="20"/>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A224" s="20"/>
+      <c r="B224" s="20"/>
+      <c r="C224" s="20" t="s">
+        <v>598</v>
+      </c>
+      <c r="D224" s="19" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A225" s="20"/>
+      <c r="B225" s="20"/>
+      <c r="C225" s="20"/>
+      <c r="D225" s="20"/>
+    </row>
+    <row r="226" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A226" s="20"/>
+      <c r="B226" s="20"/>
+      <c r="C226" s="20" t="s">
+        <v>601</v>
+      </c>
+      <c r="D226" s="19" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A227" s="20"/>
+      <c r="B227" s="20"/>
+      <c r="C227" s="20"/>
+      <c r="D227" s="19"/>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A228" s="20"/>
+      <c r="B228" s="20"/>
+      <c r="C228" s="20"/>
+      <c r="D228" s="19"/>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A229" s="20"/>
+      <c r="B229" s="20"/>
+      <c r="C229" s="20" t="s">
+        <v>604</v>
+      </c>
+      <c r="D229" s="19" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A230" s="20"/>
+      <c r="B230" s="20"/>
+      <c r="C230" s="20"/>
+      <c r="D230" s="19"/>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A231" s="20"/>
+      <c r="B231" s="20"/>
+      <c r="C231" s="20"/>
+      <c r="D231" s="19"/>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A232" s="20" t="s">
+        <v>608</v>
+      </c>
+      <c r="B232" s="20" t="s">
+        <v>605</v>
+      </c>
+      <c r="C232" s="19" t="s">
+        <v>606</v>
+      </c>
+      <c r="D232" s="19" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A233" s="20"/>
+      <c r="B233" s="20"/>
+      <c r="C233" s="20"/>
+      <c r="D233" s="20"/>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A234" s="20"/>
+      <c r="B234" s="20"/>
+      <c r="C234" s="19" t="s">
+        <v>609</v>
+      </c>
+      <c r="D234" s="19" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A235" s="20"/>
+      <c r="B235" s="20"/>
+      <c r="C235" s="20"/>
+      <c r="D235" s="20"/>
+    </row>
+    <row r="236" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A236" s="20"/>
+      <c r="B236" s="20"/>
+      <c r="C236" s="19" t="s">
+        <v>612</v>
+      </c>
+      <c r="D236" s="20" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A237" s="20"/>
+      <c r="B237" s="20"/>
+      <c r="C237" s="19"/>
+      <c r="D237" s="20"/>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A238" s="20"/>
+      <c r="B238" s="20"/>
+      <c r="C238" s="19"/>
+      <c r="D238" s="20"/>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A239" s="20"/>
+      <c r="B239" s="20"/>
+      <c r="C239" s="19" t="s">
+        <v>611</v>
+      </c>
+      <c r="D239" s="20" t="s">
         <v>470</v>
       </c>
     </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A240" s="20"/>
+      <c r="B240" s="20"/>
+      <c r="C240" s="20"/>
+      <c r="D240" s="20"/>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A241" s="20"/>
+      <c r="B241" s="20"/>
+      <c r="C241" s="19" t="s">
+        <v>613</v>
+      </c>
+      <c r="D241" s="19" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A242" s="20"/>
+      <c r="B242" s="20"/>
+      <c r="C242" s="20"/>
+      <c r="D242" s="20"/>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A243" s="20"/>
+      <c r="B243" s="20"/>
+      <c r="C243" s="19" t="s">
+        <v>614</v>
+      </c>
+      <c r="D243" s="19" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A244" s="20"/>
+      <c r="B244" s="20"/>
+      <c r="C244" s="20"/>
+      <c r="D244" s="20"/>
+    </row>
+    <row r="245" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A245" s="20"/>
+      <c r="B245" s="20"/>
+      <c r="C245" s="19" t="s">
+        <v>617</v>
+      </c>
+      <c r="D245" s="19" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A246" s="20"/>
+      <c r="B246" s="20"/>
+      <c r="C246" s="19"/>
+      <c r="D246" s="19"/>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A247" s="20"/>
+      <c r="B247" s="20"/>
+      <c r="C247" s="19"/>
+      <c r="D247" s="19"/>
+    </row>
+    <row r="248" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A248" s="20"/>
+      <c r="B248" s="20"/>
+      <c r="C248" s="19" t="s">
+        <v>618</v>
+      </c>
+      <c r="D248" s="19" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A249" s="20"/>
+      <c r="B249" s="20"/>
+      <c r="C249" s="19"/>
+      <c r="D249" s="19"/>
+    </row>
+    <row r="250" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A250" s="20"/>
+      <c r="B250" s="20"/>
+      <c r="C250" s="19"/>
+      <c r="D250" s="19"/>
+      <c r="F250"/>
+    </row>
+    <row r="251" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A251" s="20"/>
+      <c r="B251" s="20"/>
+      <c r="C251" s="19" t="s">
+        <v>619</v>
+      </c>
+      <c r="D251" s="19" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A252" s="20"/>
+      <c r="B252" s="20"/>
+      <c r="C252" s="19"/>
+      <c r="D252" s="19"/>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A253" s="20"/>
+      <c r="B253" s="20"/>
+      <c r="C253" s="19"/>
+      <c r="D253" s="19"/>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A254" s="20"/>
+      <c r="B254" s="20"/>
+      <c r="C254" s="19" t="s">
+        <v>623</v>
+      </c>
+      <c r="D254" s="19" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A255" s="20"/>
+      <c r="B255" s="20"/>
+      <c r="C255" s="19"/>
+      <c r="D255" s="19"/>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A256" s="20"/>
+      <c r="B256" s="20"/>
+      <c r="C256" s="19"/>
+      <c r="D256" s="19"/>
+    </row>
+    <row r="257" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A257" s="20"/>
+      <c r="B257" s="20"/>
+      <c r="C257" s="19" t="s">
+        <v>625</v>
+      </c>
+      <c r="D257" s="19" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A258" s="20"/>
+      <c r="B258" s="20"/>
+      <c r="C258" s="19"/>
+      <c r="D258" s="19"/>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A259" s="20"/>
+      <c r="B259" s="20"/>
+      <c r="C259" s="19"/>
+      <c r="D259" s="19"/>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A260" s="20"/>
+      <c r="B260" s="20"/>
+      <c r="C260" s="19"/>
+      <c r="D260" s="19"/>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A261" s="20"/>
+      <c r="B261" s="20"/>
+      <c r="C261" s="19" t="s">
+        <v>627</v>
+      </c>
+      <c r="D261" s="19" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A262" s="20"/>
+      <c r="B262" s="20"/>
+      <c r="C262" s="19"/>
+      <c r="D262" s="19"/>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A263" s="20"/>
+      <c r="B263" s="20"/>
+      <c r="C263" s="19"/>
+      <c r="D263" s="19"/>
+    </row>
   </sheetData>
-  <mergeCells count="106">
+  <mergeCells count="156">
+    <mergeCell ref="C261:C263"/>
+    <mergeCell ref="D261:D263"/>
+    <mergeCell ref="B232:B263"/>
+    <mergeCell ref="A232:A263"/>
+    <mergeCell ref="C254:C256"/>
+    <mergeCell ref="D254:D256"/>
+    <mergeCell ref="C257:C260"/>
+    <mergeCell ref="D257:D260"/>
+    <mergeCell ref="C245:C247"/>
+    <mergeCell ref="D245:D247"/>
+    <mergeCell ref="C251:C253"/>
+    <mergeCell ref="D251:D253"/>
+    <mergeCell ref="C248:C250"/>
+    <mergeCell ref="D248:D250"/>
+    <mergeCell ref="C239:C240"/>
+    <mergeCell ref="D236:D238"/>
+    <mergeCell ref="D239:D240"/>
+    <mergeCell ref="C241:C242"/>
+    <mergeCell ref="C243:C244"/>
+    <mergeCell ref="D241:D242"/>
+    <mergeCell ref="D243:D244"/>
+    <mergeCell ref="C232:C233"/>
+    <mergeCell ref="D232:D233"/>
+    <mergeCell ref="C234:C235"/>
+    <mergeCell ref="D234:D235"/>
+    <mergeCell ref="C236:C238"/>
+    <mergeCell ref="C226:C228"/>
+    <mergeCell ref="D226:D228"/>
+    <mergeCell ref="C229:C231"/>
+    <mergeCell ref="D229:D231"/>
+    <mergeCell ref="C222:C223"/>
+    <mergeCell ref="D222:D223"/>
+    <mergeCell ref="C224:C225"/>
+    <mergeCell ref="D224:D225"/>
+    <mergeCell ref="C212:C213"/>
+    <mergeCell ref="D212:D213"/>
+    <mergeCell ref="C214:C215"/>
+    <mergeCell ref="D214:D215"/>
+    <mergeCell ref="C216:C217"/>
+    <mergeCell ref="D216:D217"/>
+    <mergeCell ref="C218:C220"/>
+    <mergeCell ref="D218:D220"/>
+    <mergeCell ref="C199:C206"/>
+    <mergeCell ref="B189:B206"/>
+    <mergeCell ref="A189:A206"/>
+    <mergeCell ref="D199:D206"/>
+    <mergeCell ref="C210:C211"/>
+    <mergeCell ref="D210:D211"/>
+    <mergeCell ref="C208:C209"/>
+    <mergeCell ref="D208:D209"/>
+    <mergeCell ref="B207:B231"/>
+    <mergeCell ref="A207:A231"/>
     <mergeCell ref="A133:A134"/>
     <mergeCell ref="B133:B134"/>
     <mergeCell ref="C191:C198"/>
     <mergeCell ref="D191:D198"/>
-    <mergeCell ref="B189:B198"/>
-    <mergeCell ref="A189:A198"/>
     <mergeCell ref="C186:C187"/>
     <mergeCell ref="B186:B187"/>
     <mergeCell ref="A186:A187"/>
@@ -5281,6 +6080,7 @@
     <hyperlink ref="E11" r:id="rId1"/>
     <hyperlink ref="E95" r:id="rId2"/>
     <hyperlink ref="E107" r:id="rId3"/>
+    <hyperlink ref="E207" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update on 20181227.1546 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="641">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2660,6 +2660,73 @@
     <t>plot points (mpg$displ, mpg$hwy)
 separated into different colors based on mpg$drv
 change the background into normal black and white, change the font to "Times"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>testdat &lt;- data.frame(x = 1:100, y = rnorm(100))
+testdat[50,2] &lt;- 100
+g &lt;- ggplot(testdat, aes(x = x, y = y))
+g + geom_line()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot lines of all points (testdat$x, testdat$y)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>testdat &lt;- data.frame(x = 1:100, y = rnorm(100))
+testdat[50,2] &lt;- 100
+g &lt;- ggplot(testdat, aes(x = x, y = y))
+g + geom_line() + ylim(-3, 3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>remove all points whose y is not in the range of (-3, 3) and then plot the lines</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>testdat &lt;- data.frame(x = 1:100, y = rnorm(100))
+testdat[50,2] &lt;- 100
+g &lt;- ggplot(testdat, aes(x = x, y = y))
+g + geom_line() + coord_cartesian(ylim = c(-3, 3))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot the line of all points (testdat$x, testdat$y)
+ and then only show those whose y is in the range of (-3, 3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mpg$New &lt;- rnorm(nrow(mpg))
+cutpoints &lt;- quantile(mpg$New, seq(0,1,length=4),na.rm=TRUE)
+mpg$Cut &lt;- cut(mpg$New, cutpoints)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cut()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: base</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>separate continuous variable mpg$New into 3 levels, mpg$Cut is a factor variable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mpg$New &lt;- rnorm(nrow(mpg))
+cutpoints &lt;- quantile(mpg$New, seq(0,1,length=4),na.rm=TRUE)
+mpg$Cut &lt;- cut(mpg$New, cutpoints)
+g &lt;- ggplot(mpg, aes(displ, hwy))
+g+geom_point()+facet_wrap(drv ~ Cut, nrow = 3, ncol = 4) +
+theme_bw(base_family = "Avenir", base_size = 10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>separate continuous variable mpg$New into 3 levels, mpg$Cut is a factor variable
+facet_wrap(drv ~ Cut, nrow = 3, ncol = 4): creates 3*4 panels for points (mpg$displ, mpg$hwy) with different (mpg$drv, mpg$Cut)
+theme_bw(base_family = "Avenir", base_size = 10): set the background as normal black and white, set the font as "Avenir" and letter size as 10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3068,10 +3135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F263"/>
+  <dimension ref="A1:F285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="C266" sqref="C266"/>
+    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
+      <selection activeCell="C291" sqref="C291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -5916,12 +5983,180 @@
       <c r="C263" s="19"/>
       <c r="D263" s="19"/>
     </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A264" s="20"/>
+      <c r="B264" s="20"/>
+      <c r="C264" s="19" t="s">
+        <v>629</v>
+      </c>
+      <c r="D264" s="20" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A265" s="20"/>
+      <c r="B265" s="20"/>
+      <c r="C265" s="20"/>
+      <c r="D265" s="20"/>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A266" s="20"/>
+      <c r="B266" s="20"/>
+      <c r="C266" s="20"/>
+      <c r="D266" s="20"/>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A267" s="20"/>
+      <c r="B267" s="20"/>
+      <c r="C267" s="20"/>
+      <c r="D267" s="20"/>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A268" s="20"/>
+      <c r="B268" s="20"/>
+      <c r="C268" s="19" t="s">
+        <v>631</v>
+      </c>
+      <c r="D268" s="20" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A269" s="20"/>
+      <c r="B269" s="20"/>
+      <c r="C269" s="20"/>
+      <c r="D269" s="20"/>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A270" s="20"/>
+      <c r="B270" s="20"/>
+      <c r="C270" s="20"/>
+      <c r="D270" s="20"/>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A271" s="20"/>
+      <c r="B271" s="20"/>
+      <c r="C271" s="20"/>
+      <c r="D271" s="20"/>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A272" s="20"/>
+      <c r="B272" s="20"/>
+      <c r="C272" s="19" t="s">
+        <v>633</v>
+      </c>
+      <c r="D272" s="19" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A273" s="20"/>
+      <c r="B273" s="20"/>
+      <c r="C273" s="20"/>
+      <c r="D273" s="20"/>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A274" s="20"/>
+      <c r="B274" s="20"/>
+      <c r="C274" s="20"/>
+      <c r="D274" s="20"/>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A275" s="20"/>
+      <c r="B275" s="20"/>
+      <c r="C275" s="20"/>
+      <c r="D275" s="20"/>
+    </row>
+    <row r="276" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A276" s="20"/>
+      <c r="B276" s="20"/>
+      <c r="C276" s="19" t="s">
+        <v>639</v>
+      </c>
+      <c r="D276" s="19" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A277" s="20"/>
+      <c r="B277" s="20"/>
+      <c r="C277" s="19"/>
+      <c r="D277" s="20"/>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A278" s="20"/>
+      <c r="B278" s="20"/>
+      <c r="C278" s="19"/>
+      <c r="D278" s="20"/>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A279" s="20"/>
+      <c r="B279" s="20"/>
+      <c r="C279" s="19"/>
+      <c r="D279" s="20"/>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A280" s="20"/>
+      <c r="B280" s="20"/>
+      <c r="C280" s="19"/>
+      <c r="D280" s="20"/>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A281" s="20"/>
+      <c r="B281" s="20"/>
+      <c r="C281" s="19"/>
+      <c r="D281" s="20"/>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A282" s="20"/>
+      <c r="B282" s="20"/>
+      <c r="C282" s="19"/>
+      <c r="D282" s="20"/>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A283" s="20" t="s">
+        <v>637</v>
+      </c>
+      <c r="B283" s="20" t="s">
+        <v>636</v>
+      </c>
+      <c r="C283" s="19" t="s">
+        <v>635</v>
+      </c>
+      <c r="D283" s="20" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A284" s="20"/>
+      <c r="B284" s="20"/>
+      <c r="C284" s="20"/>
+      <c r="D284" s="20"/>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A285" s="20"/>
+      <c r="B285" s="20"/>
+      <c r="C285" s="20"/>
+      <c r="D285" s="20"/>
+    </row>
   </sheetData>
-  <mergeCells count="156">
+  <mergeCells count="168">
+    <mergeCell ref="A232:A282"/>
+    <mergeCell ref="B232:B282"/>
+    <mergeCell ref="C276:C282"/>
+    <mergeCell ref="D283:D285"/>
+    <mergeCell ref="D276:D282"/>
+    <mergeCell ref="C283:C285"/>
+    <mergeCell ref="B283:B285"/>
+    <mergeCell ref="A283:A285"/>
+    <mergeCell ref="C264:C267"/>
+    <mergeCell ref="D264:D267"/>
+    <mergeCell ref="C268:C271"/>
+    <mergeCell ref="D268:D271"/>
+    <mergeCell ref="C272:C275"/>
+    <mergeCell ref="D272:D275"/>
     <mergeCell ref="C261:C263"/>
     <mergeCell ref="D261:D263"/>
-    <mergeCell ref="B232:B263"/>
-    <mergeCell ref="A232:A263"/>
     <mergeCell ref="C254:C256"/>
     <mergeCell ref="D254:D256"/>
     <mergeCell ref="C257:C260"/>

</xml_diff>

<commit_message>
Update on 20181227.2344 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="820" yWindow="5620" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RCommands" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="664">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2727,6 +2727,107 @@
     <t>separate continuous variable mpg$New into 3 levels, mpg$Cut is a factor variable
 facet_wrap(drv ~ Cut, nrow = 3, ncol = 4): creates 3*4 panels for points (mpg$displ, mpg$hwy) with different (mpg$drv, mpg$Cut)
 theme_bw(base_family = "Avenir", base_size = 10): set the background as normal black and white, set the font as "Avenir" and letter size as 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xyplot(Ozone ~ Wind, data = airquality, col = "red", pch = 8, main = "Big Apple Data")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points(airquality$Wind, airquality$Ozone) in red and snowflake shape, set the title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>table(mpg$drv, mpg$displ)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>counts the number of each combination of (mpg$drv, mpg$displ)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot points(airquality$Wind, airquality$Ozone) in different panels based on (Month, Day)
+strip = FALSE turn off the titles of all panels</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xyplot(Ozone ~ Wind | as.factor(Month) * as.factor(Day), data = airquality, strip = FALSE)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colorRamp()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: grDevices</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colorRampPalette()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p1 &lt;- colorRampPalette(c("red","blue"))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>creats the function pal which we can call with a number between 0 and 1
+The 0 and 1 correspond to the extremes of the color palette.
+ Arguments between 0 and 1 return blends of these extremes.
+pal(0.4) would return a 3-long vector, because it is based on RGB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>creats the function p1 which we can call with an integer
+the integer represents how may colors you want
+p1(4) would return 4-element vector, each element represents a color, also based on RGB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rgb()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rgb(0,0.5,0.5,0.3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create a mix color of red, green, blue;
+first 3 arguments represent the density of red, green, blue; the 4th argument set the transparency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot(x,y,pch=19,col=rgb(0,0.5,0.5,0.3))</t>
+  </si>
+  <si>
+    <t>pal &lt;- colorRamp(c("red","blue"))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qplot(y = hwy, data = mpg, color = drv)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>specifying the y parameter only, without an x argument,
+plots the values of the y argument in the order in which they occur in the data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qplot(drv, hwy, data=mpg, geom="boxplot")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mpg$drv is a factor variable, and this makes boxplot on mpg$hwy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g &lt;- ggplot(mpg, aes(x=displ,y=hwy,color=factor(year)))
+g+geom_point()+facet_grid(drv~cyl,margins=TRUE)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The margins argument tells ggplot to display the marginal totals over each row and column
+that is combination of all drv and all cyl</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3135,10 +3236,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F285"/>
+  <dimension ref="A1:F303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
-      <selection activeCell="C291" sqref="C291"/>
+    <sheetView tabSelected="1" topLeftCell="B246" workbookViewId="0">
+      <selection activeCell="C250" sqref="C250:C251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -5335,10 +5436,10 @@
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A184" s="17" t="s">
+      <c r="A184" s="20" t="s">
         <v>479</v>
       </c>
-      <c r="B184" s="1" t="s">
+      <c r="B184" s="20" t="s">
         <v>560</v>
       </c>
       <c r="C184" s="1" t="s">
@@ -5348,109 +5449,125 @@
         <v>562</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A185" s="1" t="s">
+    <row r="185" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A185" s="20"/>
+      <c r="B185" s="20"/>
+      <c r="C185" s="17" t="s">
+        <v>643</v>
+      </c>
+      <c r="D185" s="17" t="s">
+        <v>644</v>
+      </c>
+      <c r="F185"/>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A186" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="B185" s="1" t="s">
+      <c r="B186" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="C185" s="1" t="s">
+      <c r="C186" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="D185" s="1" t="s">
+      <c r="D186" s="1" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A186" s="20" t="s">
+    <row r="187" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A187" s="20" t="s">
         <v>479</v>
       </c>
-      <c r="B186" s="20" t="s">
+      <c r="B187" s="20" t="s">
         <v>567</v>
       </c>
-      <c r="C186" s="19" t="s">
+      <c r="C187" s="19" t="s">
         <v>568</v>
       </c>
-      <c r="D186" s="19" t="s">
+      <c r="D187" s="19" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A187" s="20"/>
-      <c r="B187" s="20"/>
-      <c r="C187" s="19"/>
-      <c r="D187" s="20"/>
-    </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A188" s="17" t="s">
+      <c r="A188" s="20"/>
+      <c r="B188" s="20"/>
+      <c r="C188" s="19"/>
+      <c r="D188" s="20"/>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A189" s="17" t="s">
         <v>501</v>
       </c>
-      <c r="B188" s="1" t="s">
+      <c r="B189" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="C188" s="18" t="s">
+      <c r="C189" s="18" t="s">
         <v>571</v>
       </c>
-      <c r="D188" s="1" t="s">
+      <c r="D189" s="1" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="189" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A189" s="20" t="s">
+    <row r="190" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A190" s="20" t="s">
         <v>463</v>
       </c>
-      <c r="B189" s="20" t="s">
+      <c r="B190" s="20" t="s">
         <v>464</v>
       </c>
-      <c r="C189" s="19" t="s">
+      <c r="C190" s="19" t="s">
         <v>465</v>
       </c>
-      <c r="D189" s="19" t="s">
+      <c r="D190" s="19" t="s">
         <v>466</v>
       </c>
-      <c r="E189" s="1"/>
-      <c r="F189"/>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A190" s="20"/>
-      <c r="B190" s="20"/>
-      <c r="C190" s="20"/>
-      <c r="D190" s="20"/>
+      <c r="E190" s="1"/>
+      <c r="F190"/>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" s="20"/>
       <c r="B191" s="20"/>
-      <c r="C191" s="19" t="s">
-        <v>578</v>
-      </c>
-      <c r="D191" s="19" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C191" s="20"/>
+      <c r="D191" s="20"/>
+    </row>
+    <row r="192" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A192" s="20"/>
       <c r="B192" s="20"/>
-      <c r="C192" s="20"/>
-      <c r="D192" s="20"/>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C192" s="17" t="s">
+        <v>641</v>
+      </c>
+      <c r="D192" s="17" t="s">
+        <v>642</v>
+      </c>
+      <c r="F192"/>
+    </row>
+    <row r="193" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A193" s="20"/>
       <c r="B193" s="20"/>
-      <c r="C193" s="20"/>
-      <c r="D193" s="20"/>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C193" s="20" t="s">
+        <v>646</v>
+      </c>
+      <c r="D193" s="19" t="s">
+        <v>645</v>
+      </c>
+      <c r="F193"/>
+    </row>
+    <row r="194" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A194" s="20"/>
       <c r="B194" s="20"/>
       <c r="C194" s="20"/>
       <c r="D194" s="20"/>
+      <c r="F194"/>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" s="20"/>
       <c r="B195" s="20"/>
-      <c r="C195" s="20"/>
-      <c r="D195" s="20"/>
+      <c r="C195" s="19" t="s">
+        <v>578</v>
+      </c>
+      <c r="D195" s="19" t="s">
+        <v>579</v>
+      </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" s="20"/>
@@ -5470,43 +5587,39 @@
       <c r="C198" s="20"/>
       <c r="D198" s="20"/>
     </row>
-    <row r="199" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" s="20"/>
       <c r="B199" s="20"/>
-      <c r="C199" s="19" t="s">
-        <v>581</v>
-      </c>
-      <c r="D199" s="20" t="s">
-        <v>580</v>
-      </c>
-      <c r="F199"/>
-    </row>
-    <row r="200" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C199" s="20"/>
+      <c r="D199" s="20"/>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" s="20"/>
       <c r="B200" s="20"/>
       <c r="C200" s="20"/>
       <c r="D200" s="20"/>
-      <c r="F200"/>
-    </row>
-    <row r="201" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" s="20"/>
       <c r="B201" s="20"/>
       <c r="C201" s="20"/>
       <c r="D201" s="20"/>
-      <c r="F201"/>
-    </row>
-    <row r="202" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" s="20"/>
       <c r="B202" s="20"/>
       <c r="C202" s="20"/>
       <c r="D202" s="20"/>
-      <c r="F202"/>
     </row>
     <row r="203" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A203" s="20"/>
       <c r="B203" s="20"/>
-      <c r="C203" s="20"/>
-      <c r="D203" s="20"/>
+      <c r="C203" s="19" t="s">
+        <v>581</v>
+      </c>
+      <c r="D203" s="20" t="s">
+        <v>580</v>
+      </c>
       <c r="F203"/>
     </row>
     <row r="204" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
@@ -5530,32 +5643,19 @@
       <c r="D206" s="20"/>
       <c r="F206"/>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A207" s="20" t="s">
-        <v>467</v>
-      </c>
-      <c r="B207" s="20" t="s">
-        <v>469</v>
-      </c>
-      <c r="C207" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="D207" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="E207" s="12" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="20"/>
+      <c r="B207" s="20"/>
+      <c r="C207" s="20"/>
+      <c r="D207" s="20"/>
+      <c r="F207"/>
+    </row>
+    <row r="208" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A208" s="20"/>
       <c r="B208" s="20"/>
-      <c r="C208" s="20" t="s">
-        <v>583</v>
-      </c>
-      <c r="D208" s="19" t="s">
-        <v>600</v>
-      </c>
+      <c r="C208" s="20"/>
+      <c r="D208" s="20"/>
+      <c r="F208"/>
     </row>
     <row r="209" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A209" s="20"/>
@@ -5564,46 +5664,55 @@
       <c r="D209" s="20"/>
       <c r="F209"/>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A210" s="20"/>
       <c r="B210" s="20"/>
-      <c r="C210" s="20" t="s">
-        <v>584</v>
-      </c>
-      <c r="D210" s="19" t="s">
-        <v>585</v>
-      </c>
+      <c r="C210" s="20"/>
+      <c r="D210" s="20"/>
+      <c r="F210"/>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A211" s="20"/>
-      <c r="B211" s="20"/>
-      <c r="C211" s="20"/>
-      <c r="D211" s="20"/>
+      <c r="A211" s="20" t="s">
+        <v>467</v>
+      </c>
+      <c r="B211" s="20" t="s">
+        <v>469</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="E211" s="12" t="s">
+        <v>582</v>
+      </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212" s="20"/>
       <c r="B212" s="20"/>
       <c r="C212" s="20" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D212" s="19" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A213" s="20"/>
       <c r="B213" s="20"/>
       <c r="C213" s="20"/>
       <c r="D213" s="20"/>
+      <c r="F213"/>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214" s="20"/>
       <c r="B214" s="20"/>
       <c r="C214" s="20" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="D214" s="19" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.2">
@@ -5616,10 +5725,10 @@
       <c r="A216" s="20"/>
       <c r="B216" s="20"/>
       <c r="C216" s="20" t="s">
-        <v>590</v>
+        <v>658</v>
       </c>
       <c r="D216" s="19" t="s">
-        <v>592</v>
+        <v>659</v>
       </c>
       <c r="F216"/>
     </row>
@@ -5630,79 +5739,82 @@
       <c r="D217" s="20"/>
       <c r="F217"/>
     </row>
-    <row r="218" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A218" s="20"/>
       <c r="B218" s="20"/>
-      <c r="C218" s="20" t="s">
-        <v>589</v>
-      </c>
-      <c r="D218" s="19" t="s">
-        <v>593</v>
-      </c>
+      <c r="C218" s="17" t="s">
+        <v>660</v>
+      </c>
+      <c r="D218" s="17" t="s">
+        <v>661</v>
+      </c>
+      <c r="F218"/>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219" s="20"/>
       <c r="B219" s="20"/>
-      <c r="C219" s="20"/>
-      <c r="D219" s="19"/>
+      <c r="C219" s="20" t="s">
+        <v>586</v>
+      </c>
+      <c r="D219" s="19" t="s">
+        <v>587</v>
+      </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220" s="20"/>
       <c r="B220" s="20"/>
       <c r="C220" s="20"/>
-      <c r="D220" s="19"/>
+      <c r="D220" s="20"/>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221" s="20"/>
       <c r="B221" s="20"/>
-      <c r="C221" s="17" t="s">
-        <v>594</v>
-      </c>
-      <c r="D221" s="1" t="s">
-        <v>595</v>
+      <c r="C221" s="20" t="s">
+        <v>588</v>
+      </c>
+      <c r="D221" s="19" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A222" s="20"/>
       <c r="B222" s="20"/>
-      <c r="C222" s="20" t="s">
-        <v>596</v>
-      </c>
-      <c r="D222" s="19" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C222" s="20"/>
+      <c r="D222" s="20"/>
+    </row>
+    <row r="223" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A223" s="20"/>
       <c r="B223" s="20"/>
-      <c r="C223" s="20"/>
-      <c r="D223" s="20"/>
-    </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C223" s="20" t="s">
+        <v>590</v>
+      </c>
+      <c r="D223" s="19" t="s">
+        <v>592</v>
+      </c>
+      <c r="F223"/>
+    </row>
+    <row r="224" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A224" s="20"/>
       <c r="B224" s="20"/>
-      <c r="C224" s="20" t="s">
-        <v>598</v>
-      </c>
-      <c r="D224" s="19" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C224" s="20"/>
+      <c r="D224" s="20"/>
+      <c r="F224"/>
+    </row>
+    <row r="225" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="20"/>
       <c r="B225" s="20"/>
-      <c r="C225" s="20"/>
-      <c r="D225" s="20"/>
-    </row>
-    <row r="226" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C225" s="20" t="s">
+        <v>589</v>
+      </c>
+      <c r="D225" s="19" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226" s="20"/>
       <c r="B226" s="20"/>
-      <c r="C226" s="20" t="s">
-        <v>601</v>
-      </c>
-      <c r="D226" s="19" t="s">
-        <v>602</v>
-      </c>
+      <c r="C226" s="20"/>
+      <c r="D226" s="19"/>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" s="20"/>
@@ -5713,97 +5825,101 @@
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" s="20"/>
       <c r="B228" s="20"/>
-      <c r="C228" s="20"/>
-      <c r="D228" s="19"/>
+      <c r="C228" s="17" t="s">
+        <v>594</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>595</v>
+      </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" s="20"/>
       <c r="B229" s="20"/>
       <c r="C229" s="20" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
       <c r="D229" s="19" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" s="20"/>
       <c r="B230" s="20"/>
       <c r="C230" s="20"/>
-      <c r="D230" s="19"/>
+      <c r="D230" s="20"/>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" s="20"/>
       <c r="B231" s="20"/>
-      <c r="C231" s="20"/>
-      <c r="D231" s="19"/>
+      <c r="C231" s="20" t="s">
+        <v>598</v>
+      </c>
+      <c r="D231" s="19" t="s">
+        <v>599</v>
+      </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A232" s="20" t="s">
-        <v>608</v>
-      </c>
-      <c r="B232" s="20" t="s">
-        <v>605</v>
-      </c>
-      <c r="C232" s="19" t="s">
-        <v>606</v>
-      </c>
-      <c r="D232" s="19" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A232" s="20"/>
+      <c r="B232" s="20"/>
+      <c r="C232" s="20"/>
+      <c r="D232" s="20"/>
+    </row>
+    <row r="233" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="20"/>
       <c r="B233" s="20"/>
-      <c r="C233" s="20"/>
-      <c r="D233" s="20"/>
+      <c r="C233" s="20" t="s">
+        <v>601</v>
+      </c>
+      <c r="D233" s="19" t="s">
+        <v>602</v>
+      </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" s="20"/>
       <c r="B234" s="20"/>
-      <c r="C234" s="19" t="s">
-        <v>609</v>
-      </c>
-      <c r="D234" s="19" t="s">
-        <v>610</v>
-      </c>
+      <c r="C234" s="20"/>
+      <c r="D234" s="19"/>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" s="20"/>
       <c r="B235" s="20"/>
       <c r="C235" s="20"/>
-      <c r="D235" s="20"/>
-    </row>
-    <row r="236" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D235" s="19"/>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" s="20"/>
       <c r="B236" s="20"/>
-      <c r="C236" s="19" t="s">
-        <v>612</v>
-      </c>
-      <c r="D236" s="20" t="s">
-        <v>471</v>
+      <c r="C236" s="20" t="s">
+        <v>604</v>
+      </c>
+      <c r="D236" s="19" t="s">
+        <v>603</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" s="20"/>
       <c r="B237" s="20"/>
-      <c r="C237" s="19"/>
-      <c r="D237" s="20"/>
+      <c r="C237" s="20"/>
+      <c r="D237" s="19"/>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" s="20"/>
       <c r="B238" s="20"/>
-      <c r="C238" s="19"/>
-      <c r="D238" s="20"/>
+      <c r="C238" s="20"/>
+      <c r="D238" s="19"/>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A239" s="20"/>
-      <c r="B239" s="20"/>
+      <c r="A239" s="20" t="s">
+        <v>608</v>
+      </c>
+      <c r="B239" s="20" t="s">
+        <v>605</v>
+      </c>
       <c r="C239" s="19" t="s">
-        <v>611</v>
-      </c>
-      <c r="D239" s="20" t="s">
-        <v>470</v>
+        <v>606</v>
+      </c>
+      <c r="D239" s="19" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
@@ -5812,242 +5928,246 @@
       <c r="C240" s="20"/>
       <c r="D240" s="20"/>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" s="20"/>
       <c r="B241" s="20"/>
       <c r="C241" s="19" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="D241" s="19" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" s="20"/>
       <c r="B242" s="20"/>
       <c r="C242" s="20"/>
       <c r="D242" s="20"/>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="20"/>
       <c r="B243" s="20"/>
       <c r="C243" s="19" t="s">
-        <v>614</v>
-      </c>
-      <c r="D243" s="19" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+        <v>612</v>
+      </c>
+      <c r="D243" s="20" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" s="20"/>
       <c r="B244" s="20"/>
-      <c r="C244" s="20"/>
+      <c r="C244" s="19"/>
       <c r="D244" s="20"/>
     </row>
-    <row r="245" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" s="20"/>
       <c r="B245" s="20"/>
-      <c r="C245" s="19" t="s">
-        <v>617</v>
-      </c>
-      <c r="D245" s="19" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C245" s="19"/>
+      <c r="D245" s="20"/>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" s="20"/>
       <c r="B246" s="20"/>
-      <c r="C246" s="19"/>
-      <c r="D246" s="19"/>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C246" s="19" t="s">
+        <v>611</v>
+      </c>
+      <c r="D246" s="20" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" s="20"/>
       <c r="B247" s="20"/>
-      <c r="C247" s="19"/>
-      <c r="D247" s="19"/>
-    </row>
-    <row r="248" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C247" s="20"/>
+      <c r="D247" s="20"/>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" s="20"/>
       <c r="B248" s="20"/>
       <c r="C248" s="19" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="D248" s="19" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" s="20"/>
       <c r="B249" s="20"/>
-      <c r="C249" s="19"/>
-      <c r="D249" s="19"/>
-    </row>
-    <row r="250" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C249" s="20"/>
+      <c r="D249" s="20"/>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" s="20"/>
       <c r="B250" s="20"/>
-      <c r="C250" s="19"/>
-      <c r="D250" s="19"/>
-      <c r="F250"/>
-    </row>
-    <row r="251" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C250" s="19" t="s">
+        <v>614</v>
+      </c>
+      <c r="D250" s="19" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" s="20"/>
       <c r="B251" s="20"/>
-      <c r="C251" s="19" t="s">
-        <v>619</v>
-      </c>
-      <c r="D251" s="19" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C251" s="20"/>
+      <c r="D251" s="20"/>
+    </row>
+    <row r="252" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="20"/>
       <c r="B252" s="20"/>
-      <c r="C252" s="19"/>
-      <c r="D252" s="19"/>
-    </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C252" s="19" t="s">
+        <v>617</v>
+      </c>
+      <c r="D252" s="19" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" s="20"/>
       <c r="B253" s="20"/>
       <c r="C253" s="19"/>
       <c r="D253" s="19"/>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" s="20"/>
       <c r="B254" s="20"/>
-      <c r="C254" s="19" t="s">
-        <v>623</v>
-      </c>
-      <c r="D254" s="19" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C254" s="19"/>
+      <c r="D254" s="19"/>
+    </row>
+    <row r="255" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="20"/>
       <c r="B255" s="20"/>
-      <c r="C255" s="19"/>
-      <c r="D255" s="19"/>
-    </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C255" s="19" t="s">
+        <v>618</v>
+      </c>
+      <c r="D255" s="19" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" s="20"/>
       <c r="B256" s="20"/>
       <c r="C256" s="19"/>
       <c r="D256" s="19"/>
     </row>
-    <row r="257" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A257" s="20"/>
       <c r="B257" s="20"/>
-      <c r="C257" s="19" t="s">
-        <v>625</v>
-      </c>
-      <c r="D257" s="19" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C257" s="19"/>
+      <c r="D257" s="19"/>
+      <c r="F257"/>
+    </row>
+    <row r="258" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="20"/>
       <c r="B258" s="20"/>
-      <c r="C258" s="19"/>
-      <c r="D258" s="19"/>
-    </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C258" s="19" t="s">
+        <v>619</v>
+      </c>
+      <c r="D258" s="19" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A259" s="20"/>
       <c r="B259" s="20"/>
       <c r="C259" s="19"/>
       <c r="D259" s="19"/>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A260" s="20"/>
       <c r="B260" s="20"/>
       <c r="C260" s="19"/>
       <c r="D260" s="19"/>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A261" s="20"/>
       <c r="B261" s="20"/>
       <c r="C261" s="19" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="D261" s="19" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A262" s="20"/>
       <c r="B262" s="20"/>
       <c r="C262" s="19"/>
       <c r="D262" s="19"/>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A263" s="20"/>
       <c r="B263" s="20"/>
       <c r="C263" s="19"/>
       <c r="D263" s="19"/>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A264" s="20"/>
       <c r="B264" s="20"/>
       <c r="C264" s="19" t="s">
-        <v>629</v>
-      </c>
-      <c r="D264" s="20" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+        <v>625</v>
+      </c>
+      <c r="D264" s="19" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A265" s="20"/>
       <c r="B265" s="20"/>
-      <c r="C265" s="20"/>
-      <c r="D265" s="20"/>
-    </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C265" s="19"/>
+      <c r="D265" s="19"/>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A266" s="20"/>
       <c r="B266" s="20"/>
-      <c r="C266" s="20"/>
-      <c r="D266" s="20"/>
-    </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C266" s="19"/>
+      <c r="D266" s="19"/>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A267" s="20"/>
       <c r="B267" s="20"/>
-      <c r="C267" s="20"/>
-      <c r="D267" s="20"/>
-    </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C267" s="19"/>
+      <c r="D267" s="19"/>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A268" s="20"/>
       <c r="B268" s="20"/>
       <c r="C268" s="19" t="s">
-        <v>631</v>
-      </c>
-      <c r="D268" s="20" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
+        <v>627</v>
+      </c>
+      <c r="D268" s="19" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A269" s="20"/>
       <c r="B269" s="20"/>
-      <c r="C269" s="20"/>
-      <c r="D269" s="20"/>
-    </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C269" s="19"/>
+      <c r="D269" s="19"/>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A270" s="20"/>
       <c r="B270" s="20"/>
-      <c r="C270" s="20"/>
-      <c r="D270" s="20"/>
-    </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C270" s="19"/>
+      <c r="D270" s="19"/>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A271" s="20"/>
       <c r="B271" s="20"/>
-      <c r="C271" s="20"/>
-      <c r="D271" s="20"/>
-    </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C271" s="19" t="s">
+        <v>629</v>
+      </c>
+      <c r="D271" s="20" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A272" s="20"/>
       <c r="B272" s="20"/>
-      <c r="C272" s="19" t="s">
-        <v>633</v>
-      </c>
-      <c r="D272" s="19" t="s">
-        <v>634</v>
-      </c>
+      <c r="C272" s="20"/>
+      <c r="D272" s="20"/>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" s="20"/>
@@ -6064,155 +6184,323 @@
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275" s="20"/>
       <c r="B275" s="20"/>
-      <c r="C275" s="20"/>
-      <c r="D275" s="20"/>
-    </row>
-    <row r="276" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C275" s="19" t="s">
+        <v>631</v>
+      </c>
+      <c r="D275" s="20" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276" s="20"/>
       <c r="B276" s="20"/>
-      <c r="C276" s="19" t="s">
-        <v>639</v>
-      </c>
-      <c r="D276" s="19" t="s">
-        <v>640</v>
-      </c>
+      <c r="C276" s="20"/>
+      <c r="D276" s="20"/>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277" s="20"/>
       <c r="B277" s="20"/>
-      <c r="C277" s="19"/>
+      <c r="C277" s="20"/>
       <c r="D277" s="20"/>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278" s="20"/>
       <c r="B278" s="20"/>
-      <c r="C278" s="19"/>
+      <c r="C278" s="20"/>
       <c r="D278" s="20"/>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" s="20"/>
       <c r="B279" s="20"/>
-      <c r="C279" s="19"/>
-      <c r="D279" s="20"/>
+      <c r="C279" s="19" t="s">
+        <v>633</v>
+      </c>
+      <c r="D279" s="19" t="s">
+        <v>634</v>
+      </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" s="20"/>
       <c r="B280" s="20"/>
-      <c r="C280" s="19"/>
+      <c r="C280" s="20"/>
       <c r="D280" s="20"/>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281" s="20"/>
       <c r="B281" s="20"/>
-      <c r="C281" s="19"/>
+      <c r="C281" s="20"/>
       <c r="D281" s="20"/>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282" s="20"/>
       <c r="B282" s="20"/>
-      <c r="C282" s="19"/>
+      <c r="C282" s="20"/>
       <c r="D282" s="20"/>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A283" s="20" t="s">
-        <v>637</v>
-      </c>
-      <c r="B283" s="20" t="s">
-        <v>636</v>
-      </c>
+    <row r="283" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A283" s="20"/>
+      <c r="B283" s="20"/>
       <c r="C283" s="19" t="s">
-        <v>635</v>
-      </c>
-      <c r="D283" s="20" t="s">
-        <v>638</v>
+        <v>639</v>
+      </c>
+      <c r="D283" s="19" t="s">
+        <v>640</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" s="20"/>
       <c r="B284" s="20"/>
-      <c r="C284" s="20"/>
+      <c r="C284" s="19"/>
       <c r="D284" s="20"/>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285" s="20"/>
       <c r="B285" s="20"/>
-      <c r="C285" s="20"/>
+      <c r="C285" s="19"/>
       <c r="D285" s="20"/>
     </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A286" s="20"/>
+      <c r="B286" s="20"/>
+      <c r="C286" s="19"/>
+      <c r="D286" s="20"/>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A287" s="20"/>
+      <c r="B287" s="20"/>
+      <c r="C287" s="19"/>
+      <c r="D287" s="20"/>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A288" s="20"/>
+      <c r="B288" s="20"/>
+      <c r="C288" s="19"/>
+      <c r="D288" s="20"/>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A289" s="20"/>
+      <c r="B289" s="20"/>
+      <c r="C289" s="19"/>
+      <c r="D289" s="20"/>
+    </row>
+    <row r="290" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A290" s="20"/>
+      <c r="B290" s="20"/>
+      <c r="C290" s="19" t="s">
+        <v>662</v>
+      </c>
+      <c r="D290" s="19" t="s">
+        <v>663</v>
+      </c>
+      <c r="F290"/>
+    </row>
+    <row r="291" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A291" s="20"/>
+      <c r="B291" s="20"/>
+      <c r="C291" s="19"/>
+      <c r="D291" s="20"/>
+      <c r="F291"/>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A292" s="20" t="s">
+        <v>637</v>
+      </c>
+      <c r="B292" s="20" t="s">
+        <v>636</v>
+      </c>
+      <c r="C292" s="19" t="s">
+        <v>635</v>
+      </c>
+      <c r="D292" s="20" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A293" s="20"/>
+      <c r="B293" s="20"/>
+      <c r="C293" s="20"/>
+      <c r="D293" s="20"/>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A294" s="20"/>
+      <c r="B294" s="20"/>
+      <c r="C294" s="20"/>
+      <c r="D294" s="20"/>
+    </row>
+    <row r="295" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A295" s="20" t="s">
+        <v>531</v>
+      </c>
+      <c r="B295" s="20" t="s">
+        <v>647</v>
+      </c>
+      <c r="C295" s="20" t="s">
+        <v>657</v>
+      </c>
+      <c r="D295" s="19" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A296" s="20"/>
+      <c r="B296" s="20"/>
+      <c r="C296" s="20"/>
+      <c r="D296" s="19"/>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A297" s="20"/>
+      <c r="B297" s="20"/>
+      <c r="C297" s="20"/>
+      <c r="D297" s="19"/>
+    </row>
+    <row r="298" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A298" s="20"/>
+      <c r="B298" s="20"/>
+      <c r="C298" s="20"/>
+      <c r="D298" s="19"/>
+      <c r="F298"/>
+    </row>
+    <row r="299" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A299" s="20" t="s">
+        <v>648</v>
+      </c>
+      <c r="B299" s="20" t="s">
+        <v>649</v>
+      </c>
+      <c r="C299" s="20" t="s">
+        <v>650</v>
+      </c>
+      <c r="D299" s="19" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A300" s="20"/>
+      <c r="B300" s="20"/>
+      <c r="C300" s="20"/>
+      <c r="D300" s="19"/>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A301" s="20"/>
+      <c r="B301" s="20"/>
+      <c r="C301" s="20"/>
+      <c r="D301" s="19"/>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A302" s="20" t="s">
+        <v>531</v>
+      </c>
+      <c r="B302" s="20" t="s">
+        <v>653</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="D302" s="19" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A303" s="20"/>
+      <c r="B303" s="20"/>
+      <c r="C303" s="17" t="s">
+        <v>656</v>
+      </c>
+      <c r="D303" s="20"/>
+    </row>
   </sheetData>
-  <mergeCells count="168">
-    <mergeCell ref="A232:A282"/>
-    <mergeCell ref="B232:B282"/>
-    <mergeCell ref="C276:C282"/>
-    <mergeCell ref="D283:D285"/>
-    <mergeCell ref="D276:D282"/>
-    <mergeCell ref="C283:C285"/>
-    <mergeCell ref="B283:B285"/>
-    <mergeCell ref="A283:A285"/>
+  <mergeCells count="187">
+    <mergeCell ref="A299:A301"/>
+    <mergeCell ref="D302:D303"/>
+    <mergeCell ref="B302:B303"/>
+    <mergeCell ref="A302:A303"/>
+    <mergeCell ref="C216:C217"/>
+    <mergeCell ref="D216:D217"/>
+    <mergeCell ref="C290:C291"/>
+    <mergeCell ref="D290:D291"/>
+    <mergeCell ref="B239:B291"/>
+    <mergeCell ref="A239:A291"/>
+    <mergeCell ref="D295:D298"/>
+    <mergeCell ref="C295:C298"/>
+    <mergeCell ref="B295:B298"/>
+    <mergeCell ref="D299:D301"/>
+    <mergeCell ref="C299:C301"/>
+    <mergeCell ref="B299:B301"/>
+    <mergeCell ref="A295:A298"/>
+    <mergeCell ref="A184:A185"/>
+    <mergeCell ref="B184:B185"/>
+    <mergeCell ref="C283:C289"/>
+    <mergeCell ref="D292:D294"/>
+    <mergeCell ref="D283:D289"/>
+    <mergeCell ref="C292:C294"/>
+    <mergeCell ref="B292:B294"/>
+    <mergeCell ref="A292:A294"/>
+    <mergeCell ref="C271:C274"/>
+    <mergeCell ref="D271:D274"/>
+    <mergeCell ref="C275:C278"/>
+    <mergeCell ref="D275:D278"/>
+    <mergeCell ref="C279:C282"/>
+    <mergeCell ref="D279:D282"/>
+    <mergeCell ref="C268:C270"/>
+    <mergeCell ref="D268:D270"/>
+    <mergeCell ref="C261:C263"/>
+    <mergeCell ref="D261:D263"/>
     <mergeCell ref="C264:C267"/>
     <mergeCell ref="D264:D267"/>
-    <mergeCell ref="C268:C271"/>
-    <mergeCell ref="D268:D271"/>
-    <mergeCell ref="C272:C275"/>
-    <mergeCell ref="D272:D275"/>
-    <mergeCell ref="C261:C263"/>
-    <mergeCell ref="D261:D263"/>
-    <mergeCell ref="C254:C256"/>
-    <mergeCell ref="D254:D256"/>
-    <mergeCell ref="C257:C260"/>
-    <mergeCell ref="D257:D260"/>
-    <mergeCell ref="C245:C247"/>
-    <mergeCell ref="D245:D247"/>
-    <mergeCell ref="C251:C253"/>
-    <mergeCell ref="D251:D253"/>
-    <mergeCell ref="C248:C250"/>
-    <mergeCell ref="D248:D250"/>
+    <mergeCell ref="C252:C254"/>
+    <mergeCell ref="D252:D254"/>
+    <mergeCell ref="C258:C260"/>
+    <mergeCell ref="D258:D260"/>
+    <mergeCell ref="C255:C257"/>
+    <mergeCell ref="D255:D257"/>
+    <mergeCell ref="C246:C247"/>
+    <mergeCell ref="D243:D245"/>
+    <mergeCell ref="D246:D247"/>
+    <mergeCell ref="C248:C249"/>
+    <mergeCell ref="C250:C251"/>
+    <mergeCell ref="D248:D249"/>
+    <mergeCell ref="D250:D251"/>
     <mergeCell ref="C239:C240"/>
-    <mergeCell ref="D236:D238"/>
     <mergeCell ref="D239:D240"/>
     <mergeCell ref="C241:C242"/>
-    <mergeCell ref="C243:C244"/>
     <mergeCell ref="D241:D242"/>
-    <mergeCell ref="D243:D244"/>
-    <mergeCell ref="C232:C233"/>
-    <mergeCell ref="D232:D233"/>
-    <mergeCell ref="C234:C235"/>
-    <mergeCell ref="D234:D235"/>
+    <mergeCell ref="C243:C245"/>
+    <mergeCell ref="C233:C235"/>
+    <mergeCell ref="D233:D235"/>
     <mergeCell ref="C236:C238"/>
-    <mergeCell ref="C226:C228"/>
-    <mergeCell ref="D226:D228"/>
-    <mergeCell ref="C229:C231"/>
-    <mergeCell ref="D229:D231"/>
-    <mergeCell ref="C222:C223"/>
-    <mergeCell ref="D222:D223"/>
-    <mergeCell ref="C224:C225"/>
-    <mergeCell ref="D224:D225"/>
+    <mergeCell ref="D236:D238"/>
+    <mergeCell ref="C229:C230"/>
+    <mergeCell ref="D229:D230"/>
+    <mergeCell ref="C231:C232"/>
+    <mergeCell ref="D231:D232"/>
+    <mergeCell ref="C219:C220"/>
+    <mergeCell ref="D219:D220"/>
+    <mergeCell ref="C221:C222"/>
+    <mergeCell ref="D221:D222"/>
+    <mergeCell ref="C223:C224"/>
+    <mergeCell ref="D223:D224"/>
+    <mergeCell ref="C225:C227"/>
+    <mergeCell ref="D225:D227"/>
+    <mergeCell ref="C203:C210"/>
+    <mergeCell ref="B190:B210"/>
+    <mergeCell ref="A190:A210"/>
+    <mergeCell ref="D203:D210"/>
+    <mergeCell ref="C214:C215"/>
+    <mergeCell ref="D214:D215"/>
     <mergeCell ref="C212:C213"/>
     <mergeCell ref="D212:D213"/>
-    <mergeCell ref="C214:C215"/>
-    <mergeCell ref="D214:D215"/>
-    <mergeCell ref="C216:C217"/>
-    <mergeCell ref="D216:D217"/>
-    <mergeCell ref="C218:C220"/>
-    <mergeCell ref="D218:D220"/>
-    <mergeCell ref="C199:C206"/>
-    <mergeCell ref="B189:B206"/>
-    <mergeCell ref="A189:A206"/>
-    <mergeCell ref="D199:D206"/>
-    <mergeCell ref="C210:C211"/>
-    <mergeCell ref="D210:D211"/>
-    <mergeCell ref="C208:C209"/>
-    <mergeCell ref="D208:D209"/>
-    <mergeCell ref="B207:B231"/>
-    <mergeCell ref="A207:A231"/>
+    <mergeCell ref="B211:B238"/>
+    <mergeCell ref="A211:A238"/>
+    <mergeCell ref="C193:C194"/>
+    <mergeCell ref="D193:D194"/>
     <mergeCell ref="A133:A134"/>
     <mergeCell ref="B133:B134"/>
-    <mergeCell ref="C191:C198"/>
-    <mergeCell ref="D191:D198"/>
-    <mergeCell ref="C186:C187"/>
-    <mergeCell ref="B186:B187"/>
-    <mergeCell ref="A186:A187"/>
-    <mergeCell ref="D186:D187"/>
+    <mergeCell ref="C195:C202"/>
+    <mergeCell ref="D195:D202"/>
+    <mergeCell ref="C187:C188"/>
+    <mergeCell ref="B187:B188"/>
+    <mergeCell ref="A187:A188"/>
+    <mergeCell ref="D187:D188"/>
     <mergeCell ref="D171:D174"/>
     <mergeCell ref="C178:C181"/>
     <mergeCell ref="B178:B181"/>
@@ -6247,8 +6535,8 @@
     <mergeCell ref="B141:B143"/>
     <mergeCell ref="A141:A143"/>
     <mergeCell ref="D141:D143"/>
-    <mergeCell ref="C189:C190"/>
-    <mergeCell ref="D189:D190"/>
+    <mergeCell ref="C190:C191"/>
+    <mergeCell ref="D190:D191"/>
     <mergeCell ref="A139:A140"/>
     <mergeCell ref="B139:B140"/>
     <mergeCell ref="C139:C140"/>
@@ -6315,7 +6603,7 @@
     <hyperlink ref="E11" r:id="rId1"/>
     <hyperlink ref="E95" r:id="rId2"/>
     <hyperlink ref="E107" r:id="rId3"/>
-    <hyperlink ref="E207" r:id="rId4"/>
+    <hyperlink ref="E211" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update on 20181229.2332 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="820" yWindow="5620" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="400" yWindow="6040" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RCommands" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="709">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2828,6 +2828,237 @@
   <si>
     <t>The margins argument tells ggplot to display the marginal totals over each row and column
 that is combination of all drv and all cyl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dist()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set.seed(1234)
+par(mar=c(0,0,0,0))
+x &lt;- rnorm(12,mean=rep(1:3,each=4),sd=0.2)
+y &lt;- rnorm(12,mean=rep(c(1,2,1),each=4),sd=0.2)
+plot(x,y,col = "blue", pch = 19, cex = 2)
+text(x+0.05, y+0.05, labels = as.character(1:12))
+dataFrame &lt;- data.frame(x=x,y=y)
+dist(dataFrame)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get the pairwise distances between all the points (x,y)
+that is the distances between all the different rows of the data frame
+the default is to calculate the Euclidean distance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hclust()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: stats</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>make the Cluster Dendrogram of all the points (x,y)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set.seed(1234)
+x &lt;- rnorm(12,mean=rep(1:3,each=4),sd=0.2)
+y &lt;- rnorm(12,mean=rep(c(1,2,1),each=4),sd=0.2)
+plot(x,y,col = "blue", pch = 19, cex = 2)
+text(x+0.05, y+0.05, labels = as.character(1:12))
+dataFrame &lt;- data.frame(x=x,y=y)
+distxy &lt;- dist(dataFrame)
+hClustering &lt;- hclust(distxy)
+plot(hClustering)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://gallery.r-enthusiasts.com/RGraphGallery.php?graph=79</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set.seed(1234)
+x &lt;- rnorm(12,mean=rep(1:3,each=4),sd=0.2)
+y &lt;- rnorm(12,mean=rep(c(1,2,1),each=4),sd=0.2)
+dataFrame &lt;- data.frame(x=x,y=y)
+set.seed(143)
+dataMatrix &lt;- as.matrix(dataFrame)[sample(1:12),]
+heatmap(dataMatrix)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>heatmap()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>heatmap() a way to visualize high dimension data:
+add a clustering dendrogram to the left and another on the top</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kmeans()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set.seed(1234)
+x &lt;- rnorm(12,mean=rep(1:3,each=4),sd=0.2)
+y &lt;- rnorm(12,mean=rep(c(1,2,1),each=4),sd=0.2)
+dataFrame &lt;- data.frame(x=x,y=y)
+kmeansObj &lt;- kmeans(dataFrame, centers = 3)
+par(mar = rep(0.2, 4))
+plot(x, y, col = kmeansObj$cluster, pch = 19, cex = 2)
+points(kmeansObj$centers, col = 1:3, pch = 3,lwd = 3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>run kmeans algorithm on all the points (x,y)
+plot(x, y, col=kmeansObject$cluster) plots the clusters in different colors
+points(kmeansObj$centers, col = 1:3) plots the centers of the clusters in different colors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>as.dendrogram()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set.seed(1234)
+x &lt;- rnorm(12,mean=rep(1:3,each=4),sd=0.2)
+y &lt;- rnorm(12,mean=rep(c(1,2,1),each=4),sd=0.2)
+dataFrame &lt;- data.frame(x=x,y=y)
+distxy &lt;- dist(dataFrame)
+hClustering &lt;- hclust(distxy)
+plot(as.dendrogram(hClustering))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transfer a hclust object to a dendrogram</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://sebastianraschka.com/Articles/heatmaps_in_r.html#clustering</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>which.min()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>apply()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>col.sums &lt;- apply(x, 2, sum)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calculate the column sum, 2 means column-wise, (1 means row-wise)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>which.min(x)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the location of the min in x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n &lt;- 17; fac &lt;- factor(rep_len(1:3, n), levels = 1:5)
+table(fac)
+tapply(1:n, fac, sum)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>apply function sum to different groups assigned by the factor object fac</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tapply()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>svd()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scale()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x &lt;- c(1,2,3,6,3); scale(x, center=T, scale=F)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x &lt;- c(1,2,3,6,3); scale(x, center=T, scale=T)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>center x: all elements of x minus mean(x)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>center and scale x: all elements of x minus mean(x), then the diffs divide by std(x)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>outer()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>outer product of A and B: column vector A * row vector B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A &lt;- c(1, 2, 3); B &lt;- c(4, 5, 6, 7); outer(A,B,"*")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A &lt;- c(1, 2, 3); B &lt;- c(4, 5, 6, 7); outer(A,B,"+")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the same as outer product of A and B, except that elements are not multipled but plussed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get the transpose of matrix A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t(matrix A)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Singular Value Decomposition of a Matirx: X = U*D*V'
+U: orthogonal (left singular vectors)
+V: orthogonal (right singular vectors)
+D: diagonal matirx (singular values)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prcomp()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Principal Components Analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hilbert &lt;- function(n) { i &lt;- 1:n; 1 / outer(i - 1, i, "+") }
+X &lt;- hilbert(9)[, 1:6]
+(s &lt;- svd(X))
+D &lt;- diag(s$d)
+s$u %*% D %*% t(s$v) #  X = U D V'
+t(s$u) %*% X %*% s$v #  D = U' X V
+plot(s$d, xlab="Column",ylab="Singular value",pch=19)
+plot(s$d^2/sum(s$d^2),xlab="Column",ylab="Prop. of variance explained", pch=19)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2893,7 +3124,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2956,6 +3187,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3236,10 +3470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F303"/>
+  <dimension ref="A1:F373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B246" workbookViewId="0">
-      <selection activeCell="C250" sqref="C250:C251"/>
+    <sheetView tabSelected="1" topLeftCell="A354" workbookViewId="0">
+      <selection activeCell="C367" sqref="C367"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -6408,8 +6642,585 @@
       </c>
       <c r="D303" s="20"/>
     </row>
+    <row r="304" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A304" s="20" t="s">
+        <v>507</v>
+      </c>
+      <c r="B304" s="20" t="s">
+        <v>664</v>
+      </c>
+      <c r="C304" s="19" t="s">
+        <v>665</v>
+      </c>
+      <c r="D304" s="19" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A305" s="20"/>
+      <c r="B305" s="20"/>
+      <c r="C305" s="19"/>
+      <c r="D305" s="20"/>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A306" s="20"/>
+      <c r="B306" s="20"/>
+      <c r="C306" s="19"/>
+      <c r="D306" s="20"/>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A307" s="20"/>
+      <c r="B307" s="20"/>
+      <c r="C307" s="19"/>
+      <c r="D307" s="20"/>
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A308" s="20"/>
+      <c r="B308" s="20"/>
+      <c r="C308" s="19"/>
+      <c r="D308" s="20"/>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A309" s="20"/>
+      <c r="B309" s="20"/>
+      <c r="C309" s="19"/>
+      <c r="D309" s="20"/>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A310" s="20"/>
+      <c r="B310" s="20"/>
+      <c r="C310" s="19"/>
+      <c r="D310" s="20"/>
+    </row>
+    <row r="311" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A311" s="20"/>
+      <c r="B311" s="20"/>
+      <c r="C311" s="19"/>
+      <c r="D311" s="20"/>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A312" s="20"/>
+      <c r="B312" s="20"/>
+      <c r="C312" s="19"/>
+      <c r="D312" s="20"/>
+    </row>
+    <row r="313" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A313" s="20" t="s">
+        <v>668</v>
+      </c>
+      <c r="B313" s="20" t="s">
+        <v>667</v>
+      </c>
+      <c r="C313" s="19" t="s">
+        <v>670</v>
+      </c>
+      <c r="D313" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="E313" s="22" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A314" s="20"/>
+      <c r="B314" s="20"/>
+      <c r="C314" s="19"/>
+      <c r="D314" s="20"/>
+      <c r="E314" s="20"/>
+    </row>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A315" s="20"/>
+      <c r="B315" s="20"/>
+      <c r="C315" s="19"/>
+      <c r="D315" s="20"/>
+      <c r="E315" s="20"/>
+    </row>
+    <row r="316" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A316" s="20"/>
+      <c r="B316" s="20"/>
+      <c r="C316" s="19"/>
+      <c r="D316" s="20"/>
+      <c r="E316" s="20"/>
+    </row>
+    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A317" s="20"/>
+      <c r="B317" s="20"/>
+      <c r="C317" s="19"/>
+      <c r="D317" s="20"/>
+      <c r="E317" s="20"/>
+    </row>
+    <row r="318" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A318" s="20"/>
+      <c r="B318" s="20"/>
+      <c r="C318" s="19"/>
+      <c r="D318" s="20"/>
+      <c r="E318" s="20"/>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A319" s="20"/>
+      <c r="B319" s="20"/>
+      <c r="C319" s="19"/>
+      <c r="D319" s="20"/>
+      <c r="E319" s="20"/>
+    </row>
+    <row r="320" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A320" s="20"/>
+      <c r="B320" s="20"/>
+      <c r="C320" s="19"/>
+      <c r="D320" s="20"/>
+      <c r="E320" s="20"/>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A321" s="20"/>
+      <c r="B321" s="20"/>
+      <c r="C321" s="19"/>
+      <c r="D321" s="20"/>
+      <c r="E321" s="20"/>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A322" s="20"/>
+      <c r="B322" s="20"/>
+      <c r="C322" s="19"/>
+      <c r="D322" s="20"/>
+      <c r="E322" s="20"/>
+    </row>
+    <row r="323" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A323" s="20" t="s">
+        <v>507</v>
+      </c>
+      <c r="B323" s="20" t="s">
+        <v>678</v>
+      </c>
+      <c r="C323" s="19" t="s">
+        <v>679</v>
+      </c>
+      <c r="D323" s="20" t="s">
+        <v>680</v>
+      </c>
+      <c r="F323"/>
+    </row>
+    <row r="324" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A324" s="20"/>
+      <c r="B324" s="20"/>
+      <c r="C324" s="19"/>
+      <c r="D324" s="20"/>
+      <c r="F324"/>
+    </row>
+    <row r="325" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A325" s="20"/>
+      <c r="B325" s="20"/>
+      <c r="C325" s="19"/>
+      <c r="D325" s="20"/>
+      <c r="F325"/>
+    </row>
+    <row r="326" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A326" s="20"/>
+      <c r="B326" s="20"/>
+      <c r="C326" s="19"/>
+      <c r="D326" s="20"/>
+      <c r="F326"/>
+    </row>
+    <row r="327" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A327" s="20"/>
+      <c r="B327" s="20"/>
+      <c r="C327" s="19"/>
+      <c r="D327" s="20"/>
+      <c r="F327"/>
+    </row>
+    <row r="328" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A328" s="20"/>
+      <c r="B328" s="20"/>
+      <c r="C328" s="19"/>
+      <c r="D328" s="20"/>
+      <c r="F328"/>
+    </row>
+    <row r="329" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A329" s="20"/>
+      <c r="B329" s="20"/>
+      <c r="C329" s="19"/>
+      <c r="D329" s="20"/>
+      <c r="F329"/>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A330" s="20" t="s">
+        <v>507</v>
+      </c>
+      <c r="B330" s="20" t="s">
+        <v>673</v>
+      </c>
+      <c r="C330" s="19" t="s">
+        <v>672</v>
+      </c>
+      <c r="D330" s="19" t="s">
+        <v>674</v>
+      </c>
+      <c r="E330" s="22" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A331" s="20"/>
+      <c r="B331" s="20"/>
+      <c r="C331" s="19"/>
+      <c r="D331" s="20"/>
+      <c r="E331" s="20"/>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A332" s="20"/>
+      <c r="B332" s="20"/>
+      <c r="C332" s="19"/>
+      <c r="D332" s="20"/>
+      <c r="E332" s="20"/>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A333" s="20"/>
+      <c r="B333" s="20"/>
+      <c r="C333" s="19"/>
+      <c r="D333" s="20"/>
+      <c r="E333" s="20"/>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A334" s="20"/>
+      <c r="B334" s="20"/>
+      <c r="C334" s="19"/>
+      <c r="D334" s="20"/>
+      <c r="E334" s="20"/>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A335" s="20"/>
+      <c r="B335" s="20"/>
+      <c r="C335" s="19"/>
+      <c r="D335" s="20"/>
+      <c r="E335" s="20"/>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A336" s="20"/>
+      <c r="B336" s="20"/>
+      <c r="C336" s="19"/>
+      <c r="D336" s="20"/>
+      <c r="E336" s="20"/>
+    </row>
+    <row r="337" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A337" s="20"/>
+      <c r="B337" s="20"/>
+      <c r="C337" s="19"/>
+      <c r="D337" s="20"/>
+      <c r="E337" s="20"/>
+    </row>
+    <row r="338" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A338" s="20" t="s">
+        <v>668</v>
+      </c>
+      <c r="B338" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="C338" s="19" t="s">
+        <v>676</v>
+      </c>
+      <c r="D338" s="19" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A339" s="20"/>
+      <c r="B339" s="20"/>
+      <c r="C339" s="19"/>
+      <c r="D339" s="20"/>
+    </row>
+    <row r="340" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A340" s="20"/>
+      <c r="B340" s="20"/>
+      <c r="C340" s="19"/>
+      <c r="D340" s="20"/>
+    </row>
+    <row r="341" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A341" s="20"/>
+      <c r="B341" s="20"/>
+      <c r="C341" s="19"/>
+      <c r="D341" s="20"/>
+    </row>
+    <row r="342" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A342" s="20"/>
+      <c r="B342" s="20"/>
+      <c r="C342" s="19"/>
+      <c r="D342" s="20"/>
+    </row>
+    <row r="343" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A343" s="20"/>
+      <c r="B343" s="20"/>
+      <c r="C343" s="19"/>
+      <c r="D343" s="20"/>
+    </row>
+    <row r="344" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A344" s="20"/>
+      <c r="B344" s="20"/>
+      <c r="C344" s="19"/>
+      <c r="D344" s="20"/>
+    </row>
+    <row r="345" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A345" s="20"/>
+      <c r="B345" s="20"/>
+      <c r="C345" s="19"/>
+      <c r="D345" s="20"/>
+    </row>
+    <row r="346" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A346" s="20"/>
+      <c r="B346" s="20"/>
+      <c r="C346" s="19"/>
+      <c r="D346" s="20"/>
+    </row>
+    <row r="347" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A347" s="20"/>
+      <c r="B347" s="20"/>
+      <c r="C347" s="19"/>
+      <c r="D347" s="20"/>
+    </row>
+    <row r="348" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A348" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B348" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="C348" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="D348" s="1" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="349" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A349" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B349" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="C349" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="D349" s="1" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="350" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A350" s="20" t="s">
+        <v>479</v>
+      </c>
+      <c r="B350" s="20" t="s">
+        <v>690</v>
+      </c>
+      <c r="C350" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="D350" s="20" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="351" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A351" s="20"/>
+      <c r="B351" s="20"/>
+      <c r="C351" s="19"/>
+      <c r="D351" s="20"/>
+    </row>
+    <row r="352" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A352" s="20"/>
+      <c r="B352" s="20"/>
+      <c r="C352" s="19"/>
+      <c r="D352" s="20"/>
+    </row>
+    <row r="353" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A353" s="20" t="s">
+        <v>485</v>
+      </c>
+      <c r="B353" s="20" t="s">
+        <v>692</v>
+      </c>
+      <c r="C353" s="18" t="s">
+        <v>693</v>
+      </c>
+      <c r="D353" s="17" t="s">
+        <v>695</v>
+      </c>
+      <c r="F353"/>
+    </row>
+    <row r="354" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A354" s="20"/>
+      <c r="B354" s="20"/>
+      <c r="C354" s="18" t="s">
+        <v>694</v>
+      </c>
+      <c r="D354" s="17" t="s">
+        <v>696</v>
+      </c>
+      <c r="F354"/>
+    </row>
+    <row r="355" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A355" s="20" t="s">
+        <v>485</v>
+      </c>
+      <c r="B355" s="20" t="s">
+        <v>697</v>
+      </c>
+      <c r="C355" s="18" t="s">
+        <v>699</v>
+      </c>
+      <c r="D355" s="17" t="s">
+        <v>698</v>
+      </c>
+      <c r="F355"/>
+    </row>
+    <row r="356" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A356" s="20"/>
+      <c r="B356" s="20"/>
+      <c r="C356" s="18" t="s">
+        <v>700</v>
+      </c>
+      <c r="D356" s="17" t="s">
+        <v>701</v>
+      </c>
+      <c r="F356"/>
+    </row>
+    <row r="357" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A357" s="17" t="s">
+        <v>485</v>
+      </c>
+      <c r="B357" s="17" t="s">
+        <v>702</v>
+      </c>
+      <c r="C357" s="18" t="s">
+        <v>704</v>
+      </c>
+      <c r="D357" s="17" t="s">
+        <v>703</v>
+      </c>
+      <c r="F357"/>
+    </row>
+    <row r="358" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A358" s="20" t="s">
+        <v>485</v>
+      </c>
+      <c r="B358" s="20" t="s">
+        <v>691</v>
+      </c>
+      <c r="C358" s="19" t="s">
+        <v>708</v>
+      </c>
+      <c r="D358" s="19" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A359" s="20"/>
+      <c r="B359" s="20"/>
+      <c r="C359" s="19"/>
+      <c r="D359" s="20"/>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A360" s="20"/>
+      <c r="B360" s="20"/>
+      <c r="C360" s="19"/>
+      <c r="D360" s="20"/>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A361" s="20"/>
+      <c r="B361" s="20"/>
+      <c r="C361" s="19"/>
+      <c r="D361" s="20"/>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A362" s="20"/>
+      <c r="B362" s="20"/>
+      <c r="C362" s="19"/>
+      <c r="D362" s="20"/>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A363" s="20"/>
+      <c r="B363" s="20"/>
+      <c r="C363" s="19"/>
+      <c r="D363" s="20"/>
+    </row>
+    <row r="364" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A364" s="20"/>
+      <c r="B364" s="20"/>
+      <c r="C364" s="19"/>
+      <c r="F364"/>
+    </row>
+    <row r="365" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A365" s="20"/>
+      <c r="B365" s="20"/>
+      <c r="C365" s="19"/>
+      <c r="F365"/>
+    </row>
+    <row r="366" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A366" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B366" s="17" t="s">
+        <v>706</v>
+      </c>
+      <c r="C366" s="18"/>
+      <c r="D366" s="1" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C367" s="18"/>
+    </row>
+    <row r="368" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C368" s="18"/>
+    </row>
+    <row r="369" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C369" s="17"/>
+    </row>
+    <row r="370" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C370" s="17"/>
+    </row>
+    <row r="371" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C371" s="17"/>
+    </row>
+    <row r="372" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C372" s="17"/>
+    </row>
+    <row r="373" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C373" s="17"/>
+    </row>
   </sheetData>
-  <mergeCells count="187">
+  <mergeCells count="221">
+    <mergeCell ref="D358:D363"/>
+    <mergeCell ref="C358:C365"/>
+    <mergeCell ref="B358:B365"/>
+    <mergeCell ref="A358:A365"/>
+    <mergeCell ref="B353:B354"/>
+    <mergeCell ref="A353:A354"/>
+    <mergeCell ref="B355:B356"/>
+    <mergeCell ref="A355:A356"/>
+    <mergeCell ref="C350:C352"/>
+    <mergeCell ref="D350:D352"/>
+    <mergeCell ref="B350:B352"/>
+    <mergeCell ref="A350:A352"/>
+    <mergeCell ref="C338:C347"/>
+    <mergeCell ref="B338:B347"/>
+    <mergeCell ref="A338:A347"/>
+    <mergeCell ref="D338:D347"/>
+    <mergeCell ref="E313:E322"/>
+    <mergeCell ref="C330:C337"/>
+    <mergeCell ref="B330:B337"/>
+    <mergeCell ref="A330:A337"/>
+    <mergeCell ref="D330:D337"/>
+    <mergeCell ref="C323:C329"/>
+    <mergeCell ref="B323:B329"/>
+    <mergeCell ref="A323:A329"/>
+    <mergeCell ref="D323:D329"/>
+    <mergeCell ref="E330:E337"/>
+    <mergeCell ref="C313:C322"/>
+    <mergeCell ref="B313:B322"/>
+    <mergeCell ref="A313:A322"/>
+    <mergeCell ref="D313:D322"/>
+    <mergeCell ref="C304:C312"/>
+    <mergeCell ref="B304:B312"/>
+    <mergeCell ref="A304:A312"/>
+    <mergeCell ref="D304:D312"/>
     <mergeCell ref="A299:A301"/>
     <mergeCell ref="D302:D303"/>
     <mergeCell ref="B302:B303"/>
@@ -6604,6 +7415,8 @@
     <hyperlink ref="E95" r:id="rId2"/>
     <hyperlink ref="E107" r:id="rId3"/>
     <hyperlink ref="E211" r:id="rId4"/>
+    <hyperlink ref="E313" r:id="rId5"/>
+    <hyperlink ref="E330" r:id="rId6" location="clustering"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update on 20181230.1523 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="730">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2894,11 +2894,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>heatmap() a way to visualize high dimension data:
-add a clustering dendrogram to the left and another on the top</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>kmeans()</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2996,14 +2991,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>center x: all elements of x minus mean(x)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>center and scale x: all elements of x minus mean(x), then the diffs divide by std(x)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>outer()</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3059,6 +3046,107 @@
 t(s$u) %*% X %*% s$v #  D = U' X V
 plot(s$d, xlab="Column",ylab="Singular value",pch=19)
 plot(s$d^2/sum(s$d^2),xlab="Column",ylab="Prop. of variance explained", pch=19)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%*%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Matrix Multiplication</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.stat.cmu.edu/~cshalizi/ADAfaEPoV/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colors()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Returns the built-in color names which R knows about.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: RColorBrewer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brewer.pal()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cols &lt;- brewer.pal(3, "BuGn")
+pal &lt;- colorRampPalette(cols)
+image(volcano, col = pal(20))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"BuGn" is the name of palette: blue-green palette, 3 means create 3 primary colors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>combining cols and colorRampPalette to create a color-creating function pal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>show a volcano-like image using 20 different colors created by function pal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>smoothScatter()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x &lt;- rnorm(10000)
+y &lt;- rnorm(10000)
+smoothScatter(x, y)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>smoothScatter() create a 2D histogram of points (x, y)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>heatmap() is a way to visualize high dimension data:
+add a clustering dendrogram to the left and another on the top</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>center x: each column of x minus their column mean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>center and scale x: each column of x minus their column mean, then the diffs divide by their column std</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>diag()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>diag(c(1,2,3))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create a diagonal matrix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>readLines()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: base</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>readLines("Filename.txt", 10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>read at most the first 10 lines of Filename.txt</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3470,18 +3558,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F373"/>
+  <dimension ref="A1:F379"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A354" workbookViewId="0">
-      <selection activeCell="C367" sqref="C367"/>
+    <sheetView tabSelected="1" topLeftCell="C370" workbookViewId="0">
+      <selection activeCell="D379" sqref="D379"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="93.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="101.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="107.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -6642,128 +6730,148 @@
       </c>
       <c r="D303" s="20"/>
     </row>
-    <row r="304" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A304" s="20" t="s">
-        <v>507</v>
+        <v>711</v>
       </c>
       <c r="B304" s="20" t="s">
-        <v>664</v>
+        <v>712</v>
       </c>
       <c r="C304" s="19" t="s">
-        <v>665</v>
-      </c>
-      <c r="D304" s="19" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
+        <v>713</v>
+      </c>
+      <c r="D304" s="17" t="s">
+        <v>714</v>
+      </c>
+      <c r="F304"/>
+    </row>
+    <row r="305" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A305" s="20"/>
       <c r="B305" s="20"/>
-      <c r="C305" s="19"/>
-      <c r="D305" s="20"/>
-    </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C305" s="20"/>
+      <c r="D305" s="17" t="s">
+        <v>715</v>
+      </c>
+      <c r="F305"/>
+    </row>
+    <row r="306" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A306" s="20"/>
       <c r="B306" s="20"/>
-      <c r="C306" s="19"/>
-      <c r="D306" s="20"/>
-    </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A307" s="20"/>
-      <c r="B307" s="20"/>
-      <c r="C307" s="19"/>
-      <c r="D307" s="20"/>
-    </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C306" s="20"/>
+      <c r="D306" s="17" t="s">
+        <v>716</v>
+      </c>
+      <c r="F306"/>
+    </row>
+    <row r="307" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A307" s="20" t="s">
+        <v>501</v>
+      </c>
+      <c r="B307" s="20" t="s">
+        <v>717</v>
+      </c>
+      <c r="C307" s="19" t="s">
+        <v>718</v>
+      </c>
+      <c r="D307" s="20" t="s">
+        <v>719</v>
+      </c>
+      <c r="F307"/>
+    </row>
+    <row r="308" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A308" s="20"/>
       <c r="B308" s="20"/>
-      <c r="C308" s="19"/>
+      <c r="C308" s="20"/>
       <c r="D308" s="20"/>
-    </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F308"/>
+    </row>
+    <row r="309" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A309" s="20"/>
       <c r="B309" s="20"/>
-      <c r="C309" s="19"/>
+      <c r="C309" s="20"/>
       <c r="D309" s="20"/>
-    </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A310" s="20"/>
-      <c r="B310" s="20"/>
-      <c r="C310" s="19"/>
-      <c r="D310" s="20"/>
-    </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F309"/>
+    </row>
+    <row r="310" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A310" s="20" t="s">
+        <v>507</v>
+      </c>
+      <c r="B310" s="20" t="s">
+        <v>664</v>
+      </c>
+      <c r="C310" s="19" t="s">
+        <v>665</v>
+      </c>
+      <c r="D310" s="19" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A311" s="20"/>
       <c r="B311" s="20"/>
       <c r="C311" s="19"/>
       <c r="D311" s="20"/>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A312" s="20"/>
       <c r="B312" s="20"/>
       <c r="C312" s="19"/>
       <c r="D312" s="20"/>
     </row>
-    <row r="313" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A313" s="20" t="s">
-        <v>668</v>
-      </c>
-      <c r="B313" s="20" t="s">
-        <v>667</v>
-      </c>
-      <c r="C313" s="19" t="s">
-        <v>670</v>
-      </c>
-      <c r="D313" s="20" t="s">
-        <v>669</v>
-      </c>
-      <c r="E313" s="22" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A313" s="20"/>
+      <c r="B313" s="20"/>
+      <c r="C313" s="19"/>
+      <c r="D313" s="20"/>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A314" s="20"/>
       <c r="B314" s="20"/>
       <c r="C314" s="19"/>
       <c r="D314" s="20"/>
-      <c r="E314" s="20"/>
-    </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A315" s="20"/>
       <c r="B315" s="20"/>
       <c r="C315" s="19"/>
       <c r="D315" s="20"/>
-      <c r="E315" s="20"/>
-    </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A316" s="20"/>
       <c r="B316" s="20"/>
       <c r="C316" s="19"/>
       <c r="D316" s="20"/>
-      <c r="E316" s="20"/>
-    </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A317" s="20"/>
       <c r="B317" s="20"/>
       <c r="C317" s="19"/>
       <c r="D317" s="20"/>
-      <c r="E317" s="20"/>
-    </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A318" s="20"/>
       <c r="B318" s="20"/>
       <c r="C318" s="19"/>
       <c r="D318" s="20"/>
-      <c r="E318" s="20"/>
-    </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A319" s="20"/>
-      <c r="B319" s="20"/>
-      <c r="C319" s="19"/>
-      <c r="D319" s="20"/>
-      <c r="E319" s="20"/>
-    </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="319" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A319" s="20" t="s">
+        <v>668</v>
+      </c>
+      <c r="B319" s="20" t="s">
+        <v>667</v>
+      </c>
+      <c r="C319" s="19" t="s">
+        <v>670</v>
+      </c>
+      <c r="D319" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="E319" s="22" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A320" s="20"/>
       <c r="B320" s="20"/>
       <c r="C320" s="19"/>
@@ -6784,121 +6892,121 @@
       <c r="D322" s="20"/>
       <c r="E322" s="20"/>
     </row>
-    <row r="323" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A323" s="20" t="s">
-        <v>507</v>
-      </c>
-      <c r="B323" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="C323" s="19" t="s">
-        <v>679</v>
-      </c>
-      <c r="D323" s="20" t="s">
-        <v>680</v>
-      </c>
-      <c r="F323"/>
-    </row>
-    <row r="324" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A323" s="20"/>
+      <c r="B323" s="20"/>
+      <c r="C323" s="19"/>
+      <c r="D323" s="20"/>
+      <c r="E323" s="20"/>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A324" s="20"/>
       <c r="B324" s="20"/>
       <c r="C324" s="19"/>
       <c r="D324" s="20"/>
-      <c r="F324"/>
-    </row>
-    <row r="325" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E324" s="20"/>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A325" s="20"/>
       <c r="B325" s="20"/>
       <c r="C325" s="19"/>
       <c r="D325" s="20"/>
-      <c r="F325"/>
-    </row>
-    <row r="326" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E325" s="20"/>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A326" s="20"/>
       <c r="B326" s="20"/>
       <c r="C326" s="19"/>
       <c r="D326" s="20"/>
-      <c r="F326"/>
-    </row>
-    <row r="327" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E326" s="20"/>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A327" s="20"/>
       <c r="B327" s="20"/>
       <c r="C327" s="19"/>
       <c r="D327" s="20"/>
-      <c r="F327"/>
-    </row>
-    <row r="328" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E327" s="20"/>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A328" s="20"/>
       <c r="B328" s="20"/>
       <c r="C328" s="19"/>
       <c r="D328" s="20"/>
-      <c r="F328"/>
+      <c r="E328" s="20"/>
     </row>
     <row r="329" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A329" s="20"/>
-      <c r="B329" s="20"/>
-      <c r="C329" s="19"/>
-      <c r="D329" s="20"/>
+      <c r="A329" s="20" t="s">
+        <v>507</v>
+      </c>
+      <c r="B329" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="C329" s="19" t="s">
+        <v>678</v>
+      </c>
+      <c r="D329" s="20" t="s">
+        <v>679</v>
+      </c>
       <c r="F329"/>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A330" s="20" t="s">
-        <v>507</v>
-      </c>
-      <c r="B330" s="20" t="s">
-        <v>673</v>
-      </c>
-      <c r="C330" s="19" t="s">
-        <v>672</v>
-      </c>
-      <c r="D330" s="19" t="s">
-        <v>674</v>
-      </c>
-      <c r="E330" s="22" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A330" s="20"/>
+      <c r="B330" s="20"/>
+      <c r="C330" s="19"/>
+      <c r="D330" s="20"/>
+      <c r="F330"/>
+    </row>
+    <row r="331" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A331" s="20"/>
       <c r="B331" s="20"/>
       <c r="C331" s="19"/>
       <c r="D331" s="20"/>
-      <c r="E331" s="20"/>
-    </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F331"/>
+    </row>
+    <row r="332" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A332" s="20"/>
       <c r="B332" s="20"/>
       <c r="C332" s="19"/>
       <c r="D332" s="20"/>
-      <c r="E332" s="20"/>
-    </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F332"/>
+    </row>
+    <row r="333" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A333" s="20"/>
       <c r="B333" s="20"/>
       <c r="C333" s="19"/>
       <c r="D333" s="20"/>
-      <c r="E333" s="20"/>
-    </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F333"/>
+    </row>
+    <row r="334" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A334" s="20"/>
       <c r="B334" s="20"/>
       <c r="C334" s="19"/>
       <c r="D334" s="20"/>
-      <c r="E334" s="20"/>
-    </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F334"/>
+    </row>
+    <row r="335" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A335" s="20"/>
       <c r="B335" s="20"/>
       <c r="C335" s="19"/>
       <c r="D335" s="20"/>
-      <c r="E335" s="20"/>
+      <c r="F335"/>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A336" s="20"/>
-      <c r="B336" s="20"/>
-      <c r="C336" s="19"/>
-      <c r="D336" s="20"/>
-      <c r="E336" s="20"/>
+      <c r="A336" s="20" t="s">
+        <v>507</v>
+      </c>
+      <c r="B336" s="20" t="s">
+        <v>673</v>
+      </c>
+      <c r="C336" s="19" t="s">
+        <v>672</v>
+      </c>
+      <c r="D336" s="19" t="s">
+        <v>720</v>
+      </c>
+      <c r="E336" s="22" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A337" s="20"/>
@@ -6907,55 +7015,61 @@
       <c r="D337" s="20"/>
       <c r="E337" s="20"/>
     </row>
-    <row r="338" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A338" s="20" t="s">
-        <v>668</v>
-      </c>
-      <c r="B338" s="20" t="s">
-        <v>675</v>
-      </c>
-      <c r="C338" s="19" t="s">
-        <v>676</v>
-      </c>
-      <c r="D338" s="19" t="s">
-        <v>677</v>
-      </c>
+    <row r="338" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A338" s="20"/>
+      <c r="B338" s="20"/>
+      <c r="C338" s="19"/>
+      <c r="D338" s="20"/>
+      <c r="E338" s="20"/>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A339" s="20"/>
       <c r="B339" s="20"/>
       <c r="C339" s="19"/>
       <c r="D339" s="20"/>
+      <c r="E339" s="20"/>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A340" s="20"/>
       <c r="B340" s="20"/>
       <c r="C340" s="19"/>
       <c r="D340" s="20"/>
+      <c r="E340" s="20"/>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A341" s="20"/>
       <c r="B341" s="20"/>
       <c r="C341" s="19"/>
       <c r="D341" s="20"/>
+      <c r="E341" s="20"/>
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A342" s="20"/>
       <c r="B342" s="20"/>
       <c r="C342" s="19"/>
       <c r="D342" s="20"/>
+      <c r="E342" s="20"/>
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A343" s="20"/>
       <c r="B343" s="20"/>
       <c r="C343" s="19"/>
       <c r="D343" s="20"/>
-    </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A344" s="20"/>
-      <c r="B344" s="20"/>
-      <c r="C344" s="19"/>
-      <c r="D344" s="20"/>
+      <c r="E343" s="20"/>
+    </row>
+    <row r="344" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A344" s="20" t="s">
+        <v>668</v>
+      </c>
+      <c r="B344" s="20" t="s">
+        <v>674</v>
+      </c>
+      <c r="C344" s="19" t="s">
+        <v>675</v>
+      </c>
+      <c r="D344" s="19" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A345" s="20"/>
@@ -6976,46 +7090,22 @@
       <c r="D347" s="20"/>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A348" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B348" s="1" t="s">
-        <v>682</v>
-      </c>
-      <c r="C348" s="1" t="s">
-        <v>686</v>
-      </c>
-      <c r="D348" s="1" t="s">
-        <v>687</v>
-      </c>
+      <c r="A348" s="20"/>
+      <c r="B348" s="20"/>
+      <c r="C348" s="19"/>
+      <c r="D348" s="20"/>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A349" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="B349" s="1" t="s">
-        <v>683</v>
-      </c>
-      <c r="C349" s="1" t="s">
-        <v>684</v>
-      </c>
-      <c r="D349" s="1" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="350" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A350" s="20" t="s">
-        <v>479</v>
-      </c>
-      <c r="B350" s="20" t="s">
-        <v>690</v>
-      </c>
-      <c r="C350" s="19" t="s">
-        <v>688</v>
-      </c>
-      <c r="D350" s="20" t="s">
-        <v>689</v>
-      </c>
+      <c r="A349" s="20"/>
+      <c r="B349" s="20"/>
+      <c r="C349" s="19"/>
+      <c r="D349" s="20"/>
+    </row>
+    <row r="350" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A350" s="20"/>
+      <c r="B350" s="20"/>
+      <c r="C350" s="19"/>
+      <c r="D350" s="20"/>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A351" s="20"/>
@@ -7029,198 +7119,308 @@
       <c r="C352" s="19"/>
       <c r="D352" s="20"/>
     </row>
-    <row r="353" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A353" s="20" t="s">
+    <row r="353" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A353" s="20"/>
+      <c r="B353" s="20"/>
+      <c r="C353" s="19"/>
+      <c r="D353" s="20"/>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A354" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="C354" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="D354" s="1" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A355" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="B353" s="20" t="s">
+      <c r="B355" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="C355" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="D355" s="1" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A356" s="20" t="s">
+        <v>479</v>
+      </c>
+      <c r="B356" s="20" t="s">
+        <v>689</v>
+      </c>
+      <c r="C356" s="19" t="s">
+        <v>687</v>
+      </c>
+      <c r="D356" s="20" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A357" s="20"/>
+      <c r="B357" s="20"/>
+      <c r="C357" s="19"/>
+      <c r="D357" s="20"/>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A358" s="20"/>
+      <c r="B358" s="20"/>
+      <c r="C358" s="19"/>
+      <c r="D358" s="20"/>
+    </row>
+    <row r="359" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A359" s="20" t="s">
+        <v>485</v>
+      </c>
+      <c r="B359" s="20" t="s">
+        <v>691</v>
+      </c>
+      <c r="C359" s="18" t="s">
         <v>692</v>
       </c>
-      <c r="C353" s="18" t="s">
-        <v>693</v>
-      </c>
-      <c r="D353" s="17" t="s">
-        <v>695</v>
-      </c>
-      <c r="F353"/>
-    </row>
-    <row r="354" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A354" s="20"/>
-      <c r="B354" s="20"/>
-      <c r="C354" s="18" t="s">
-        <v>694</v>
-      </c>
-      <c r="D354" s="17" t="s">
-        <v>696</v>
-      </c>
-      <c r="F354"/>
-    </row>
-    <row r="355" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A355" s="20" t="s">
-        <v>485</v>
-      </c>
-      <c r="B355" s="20" t="s">
-        <v>697</v>
-      </c>
-      <c r="C355" s="18" t="s">
-        <v>699</v>
-      </c>
-      <c r="D355" s="17" t="s">
-        <v>698</v>
-      </c>
-      <c r="F355"/>
-    </row>
-    <row r="356" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A356" s="20"/>
-      <c r="B356" s="20"/>
-      <c r="C356" s="18" t="s">
-        <v>700</v>
-      </c>
-      <c r="D356" s="17" t="s">
-        <v>701</v>
-      </c>
-      <c r="F356"/>
-    </row>
-    <row r="357" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A357" s="17" t="s">
-        <v>485</v>
-      </c>
-      <c r="B357" s="17" t="s">
-        <v>702</v>
-      </c>
-      <c r="C357" s="18" t="s">
-        <v>704</v>
-      </c>
-      <c r="D357" s="17" t="s">
-        <v>703</v>
-      </c>
-      <c r="F357"/>
-    </row>
-    <row r="358" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A358" s="20" t="s">
-        <v>485</v>
-      </c>
-      <c r="B358" s="20" t="s">
-        <v>691</v>
-      </c>
-      <c r="C358" s="19" t="s">
-        <v>708</v>
-      </c>
-      <c r="D358" s="19" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A359" s="20"/>
-      <c r="B359" s="20"/>
-      <c r="C359" s="19"/>
-      <c r="D359" s="20"/>
-    </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D359" s="17" t="s">
+        <v>721</v>
+      </c>
+      <c r="F359"/>
+    </row>
+    <row r="360" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A360" s="20"/>
       <c r="B360" s="20"/>
-      <c r="C360" s="19"/>
-      <c r="D360" s="20"/>
-    </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A361" s="20"/>
-      <c r="B361" s="20"/>
-      <c r="C361" s="19"/>
-      <c r="D361" s="20"/>
-    </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C360" s="18" t="s">
+        <v>693</v>
+      </c>
+      <c r="D360" s="17" t="s">
+        <v>722</v>
+      </c>
+      <c r="F360"/>
+    </row>
+    <row r="361" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A361" s="20" t="s">
+        <v>485</v>
+      </c>
+      <c r="B361" s="20" t="s">
+        <v>694</v>
+      </c>
+      <c r="C361" s="18" t="s">
+        <v>696</v>
+      </c>
+      <c r="D361" s="17" t="s">
+        <v>695</v>
+      </c>
+      <c r="F361"/>
+    </row>
+    <row r="362" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A362" s="20"/>
       <c r="B362" s="20"/>
-      <c r="C362" s="19"/>
-      <c r="D362" s="20"/>
-    </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A363" s="20"/>
-      <c r="B363" s="20"/>
-      <c r="C363" s="19"/>
-      <c r="D363" s="20"/>
-    </row>
-    <row r="364" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A364" s="20"/>
-      <c r="B364" s="20"/>
-      <c r="C364" s="19"/>
-      <c r="F364"/>
-    </row>
-    <row r="365" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C362" s="18" t="s">
+        <v>697</v>
+      </c>
+      <c r="D362" s="17" t="s">
+        <v>698</v>
+      </c>
+      <c r="F362"/>
+    </row>
+    <row r="363" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A363" s="17" t="s">
+        <v>485</v>
+      </c>
+      <c r="B363" s="17" t="s">
+        <v>699</v>
+      </c>
+      <c r="C363" s="18" t="s">
+        <v>701</v>
+      </c>
+      <c r="D363" s="17" t="s">
+        <v>700</v>
+      </c>
+      <c r="F363"/>
+    </row>
+    <row r="364" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A364" s="20" t="s">
+        <v>485</v>
+      </c>
+      <c r="B364" s="20" t="s">
+        <v>690</v>
+      </c>
+      <c r="C364" s="19" t="s">
+        <v>705</v>
+      </c>
+      <c r="D364" s="19" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A365" s="20"/>
       <c r="B365" s="20"/>
       <c r="C365" s="19"/>
-      <c r="F365"/>
+      <c r="D365" s="20"/>
     </row>
     <row r="366" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A366" s="1" t="s">
+      <c r="A366" s="20"/>
+      <c r="B366" s="20"/>
+      <c r="C366" s="19"/>
+      <c r="D366" s="20"/>
+    </row>
+    <row r="367" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A367" s="20"/>
+      <c r="B367" s="20"/>
+      <c r="C367" s="19"/>
+      <c r="D367" s="20"/>
+    </row>
+    <row r="368" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A368" s="20"/>
+      <c r="B368" s="20"/>
+      <c r="C368" s="19"/>
+      <c r="D368" s="20"/>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A369" s="20"/>
+      <c r="B369" s="20"/>
+      <c r="C369" s="19"/>
+      <c r="D369" s="20"/>
+    </row>
+    <row r="370" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A370" s="20"/>
+      <c r="B370" s="20"/>
+      <c r="C370" s="19"/>
+      <c r="F370"/>
+    </row>
+    <row r="371" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A371" s="20"/>
+      <c r="B371" s="20"/>
+      <c r="C371" s="19"/>
+      <c r="F371"/>
+    </row>
+    <row r="372" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A372" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="B366" s="17" t="s">
+      <c r="B372" s="17" t="s">
+        <v>703</v>
+      </c>
+      <c r="C372" s="18"/>
+      <c r="D372" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="E372" s="12" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A373" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B373" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="C366" s="18"/>
-      <c r="D366" s="1" t="s">
+      <c r="C373" s="18"/>
+      <c r="D373" s="1" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C367" s="18"/>
-    </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C368" s="18"/>
-    </row>
-    <row r="369" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C369" s="17"/>
-    </row>
-    <row r="370" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C370" s="17"/>
-    </row>
-    <row r="371" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C371" s="17"/>
-    </row>
-    <row r="372" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C372" s="17"/>
-    </row>
-    <row r="373" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C373" s="17"/>
+    <row r="374" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A374" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B374" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="C374" s="18"/>
+      <c r="D374" s="1" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A375" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B375" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="C375" s="17" t="s">
+        <v>724</v>
+      </c>
+      <c r="D375" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A376" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="B376" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="C376" s="17" t="s">
+        <v>728</v>
+      </c>
+      <c r="D376" s="1" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C377" s="17"/>
+    </row>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C378" s="17"/>
+    </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C379" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="221">
-    <mergeCell ref="D358:D363"/>
-    <mergeCell ref="C358:C365"/>
-    <mergeCell ref="B358:B365"/>
-    <mergeCell ref="A358:A365"/>
-    <mergeCell ref="B353:B354"/>
-    <mergeCell ref="A353:A354"/>
-    <mergeCell ref="B355:B356"/>
-    <mergeCell ref="A355:A356"/>
-    <mergeCell ref="C350:C352"/>
-    <mergeCell ref="D350:D352"/>
-    <mergeCell ref="B350:B352"/>
-    <mergeCell ref="A350:A352"/>
-    <mergeCell ref="C338:C347"/>
-    <mergeCell ref="B338:B347"/>
-    <mergeCell ref="A338:A347"/>
-    <mergeCell ref="D338:D347"/>
-    <mergeCell ref="E313:E322"/>
-    <mergeCell ref="C330:C337"/>
-    <mergeCell ref="B330:B337"/>
-    <mergeCell ref="A330:A337"/>
-    <mergeCell ref="D330:D337"/>
-    <mergeCell ref="C323:C329"/>
-    <mergeCell ref="B323:B329"/>
-    <mergeCell ref="A323:A329"/>
-    <mergeCell ref="D323:D329"/>
-    <mergeCell ref="E330:E337"/>
-    <mergeCell ref="C313:C322"/>
-    <mergeCell ref="B313:B322"/>
-    <mergeCell ref="A313:A322"/>
-    <mergeCell ref="D313:D322"/>
-    <mergeCell ref="C304:C312"/>
-    <mergeCell ref="B304:B312"/>
-    <mergeCell ref="A304:A312"/>
-    <mergeCell ref="D304:D312"/>
+  <mergeCells count="228">
+    <mergeCell ref="D364:D369"/>
+    <mergeCell ref="C364:C371"/>
+    <mergeCell ref="B364:B371"/>
+    <mergeCell ref="A364:A371"/>
+    <mergeCell ref="B359:B360"/>
+    <mergeCell ref="A359:A360"/>
+    <mergeCell ref="B361:B362"/>
+    <mergeCell ref="A361:A362"/>
+    <mergeCell ref="C356:C358"/>
+    <mergeCell ref="D356:D358"/>
+    <mergeCell ref="B356:B358"/>
+    <mergeCell ref="A356:A358"/>
+    <mergeCell ref="C344:C353"/>
+    <mergeCell ref="B344:B353"/>
+    <mergeCell ref="A344:A353"/>
+    <mergeCell ref="D344:D353"/>
+    <mergeCell ref="E319:E328"/>
+    <mergeCell ref="C336:C343"/>
+    <mergeCell ref="B336:B343"/>
+    <mergeCell ref="A336:A343"/>
+    <mergeCell ref="D336:D343"/>
+    <mergeCell ref="C329:C335"/>
+    <mergeCell ref="B329:B335"/>
+    <mergeCell ref="A329:A335"/>
+    <mergeCell ref="D329:D335"/>
+    <mergeCell ref="E336:E343"/>
+    <mergeCell ref="C319:C328"/>
+    <mergeCell ref="B319:B328"/>
+    <mergeCell ref="A319:A328"/>
+    <mergeCell ref="D319:D328"/>
+    <mergeCell ref="C310:C318"/>
+    <mergeCell ref="B310:B318"/>
+    <mergeCell ref="A310:A318"/>
+    <mergeCell ref="D310:D318"/>
+    <mergeCell ref="C304:C306"/>
+    <mergeCell ref="B304:B306"/>
+    <mergeCell ref="A304:A306"/>
+    <mergeCell ref="C307:C309"/>
+    <mergeCell ref="B307:B309"/>
+    <mergeCell ref="A307:A309"/>
+    <mergeCell ref="D307:D309"/>
     <mergeCell ref="A299:A301"/>
     <mergeCell ref="D302:D303"/>
     <mergeCell ref="B302:B303"/>
@@ -7415,8 +7615,9 @@
     <hyperlink ref="E95" r:id="rId2"/>
     <hyperlink ref="E107" r:id="rId3"/>
     <hyperlink ref="E211" r:id="rId4"/>
-    <hyperlink ref="E313" r:id="rId5"/>
-    <hyperlink ref="E330" r:id="rId6" location="clustering"/>
+    <hyperlink ref="E319" r:id="rId5"/>
+    <hyperlink ref="E336" r:id="rId6" location="clustering"/>
+    <hyperlink ref="E372" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update on 20181230.1818 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -21,7 +21,7 @@
     <sheet name="Learning Sources" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RCommands!$A$1:$A$170</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RCommands!$A$1:$A$388</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="745">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1855,14 +1855,6 @@
   </si>
   <si>
     <t>subset()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>subset(iris, Sepal.Length&gt;5)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>get a subset of iris: column Sepal.Length &gt; 5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2961,12 +2953,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>n &lt;- 17; fac &lt;- factor(rep_len(1:3, n), levels = 1:5)
-table(fac)
-tapply(1:n, fac, sum)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>apply function sum to different groups assigned by the factor object fac</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3147,6 +3133,88 @@
   </si>
   <si>
     <t>read at most the first 10 lines of Filename.txt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>make.names()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>names(data frame A) &lt;- make.names(cnames[[1]])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>make.names() take arbitrary names and make them valid: replace the space in names by dot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boxplot(x0, x1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>creates 2 boxplots based on x0 and x1, x0 and x1 are both vectors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subset(iris, Sepal.Length&gt;5, c(Sepal.Length&gt;,Petal.Length, Petal.Width))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get a subset of iris: column Sepal.Length &gt; 5, and only the specified 3 columns</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intersect()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intersect(A, B)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get the intersect of A and B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>split()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g &lt;- airquality$Month
+l &lt;- split(airquality, g)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>split the data frame according to g, which is ariquality$Month, and return a list
+can be used together with the "apply" function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n &lt;- 17; fac &lt;- factor(rep_len(1:3, n), levels = 1:5)
+table(fac)
+tapply(1:n, fac, sum, na.rm = T)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>segments()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: graphics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x0 &lt;- 1:10
+y0 &lt;- 1:10
+x1 &lt;- rep(1,10)
+y1 &lt;- 1:10
+plot(x0, y0)
+points(x1,y1)
+segments(x0, y0, x1, y1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add line segments: link points (x0, y0) and points(x1, y1)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3558,10 +3626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F379"/>
+  <dimension ref="A1:F388"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C370" workbookViewId="0">
-      <selection activeCell="D379" sqref="D379"/>
+    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -3593,7 +3661,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -3606,7 +3674,7 @@
     </row>
     <row r="3" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>368</v>
@@ -3618,7 +3686,7 @@
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>55</v>
@@ -3632,7 +3700,7 @@
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>52</v>
@@ -3646,10 +3714,10 @@
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>61</v>
@@ -3662,10 +3730,10 @@
     </row>
     <row r="7" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>224</v>
@@ -3674,7 +3742,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>2</v>
@@ -3687,7 +3755,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>15</v>
@@ -3700,7 +3768,7 @@
     </row>
     <row r="10" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>327</v>
@@ -3712,7 +3780,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B11" s="20" t="s">
         <v>10</v>
@@ -4088,7 +4156,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>85</v>
@@ -4103,7 +4171,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>397</v>
@@ -4117,7 +4185,7 @@
     </row>
     <row r="43" spans="1:6" s="15" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>431</v>
@@ -4132,7 +4200,7 @@
     </row>
     <row r="44" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>88</v>
@@ -4146,7 +4214,7 @@
     </row>
     <row r="45" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>90</v>
@@ -4160,7 +4228,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>118</v>
@@ -4175,7 +4243,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>121</v>
@@ -4190,7 +4258,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>124</v>
@@ -4205,7 +4273,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B49" s="20" t="s">
         <v>127</v>
@@ -4231,7 +4299,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>130</v>
@@ -4558,10 +4626,10 @@
     </row>
     <row r="76" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="20" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B76" s="20" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>220</v>
@@ -4584,7 +4652,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>155</v>
@@ -4598,7 +4666,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>203</v>
@@ -4609,10 +4677,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="17" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>204</v>
@@ -4620,7 +4688,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>205</v>
@@ -4631,7 +4699,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="20" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B82" s="20" t="s">
         <v>208</v>
@@ -4709,13 +4777,13 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>219</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>223</v>
@@ -4723,7 +4791,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>225</v>
@@ -4737,7 +4805,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>228</v>
@@ -4751,7 +4819,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>231</v>
@@ -5059,7 +5127,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>356</v>
@@ -5073,7 +5141,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="13" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>359</v>
@@ -5098,7 +5166,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="17" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>365</v>
@@ -5112,7 +5180,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>370</v>
@@ -5126,7 +5194,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="17" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>373</v>
@@ -5140,7 +5208,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>376</v>
@@ -5154,7 +5222,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="17" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>379</v>
@@ -5228,7 +5296,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>430</v>
@@ -5242,114 +5310,114 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="17" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>451</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>452</v>
+        <v>732</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>453</v>
+        <v>733</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="20" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B133" s="20" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="134" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="20"/>
       <c r="B134" s="20"/>
       <c r="C134" s="17" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D134" s="17" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="F134"/>
     </row>
     <row r="135" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="17" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B135" s="17" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C135" s="17" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D135" s="17" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F135"/>
     </row>
     <row r="136" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="17" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B136" s="17" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C136" s="17" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D136" s="17" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="F136"/>
     </row>
     <row r="137" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137" s="17" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B137" s="17" t="s">
+        <v>553</v>
+      </c>
+      <c r="C137" s="17" t="s">
+        <v>554</v>
+      </c>
+      <c r="D137" s="18" t="s">
         <v>555</v>
-      </c>
-      <c r="C137" s="17" t="s">
-        <v>556</v>
-      </c>
-      <c r="D137" s="18" t="s">
-        <v>557</v>
       </c>
       <c r="F137"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B138" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="D138" s="1" t="s">
         <v>489</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="20" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B139" s="20" t="s">
+        <v>490</v>
+      </c>
+      <c r="C139" s="19" t="s">
+        <v>491</v>
+      </c>
+      <c r="D139" s="20" t="s">
         <v>492</v>
-      </c>
-      <c r="C139" s="19" t="s">
-        <v>493</v>
-      </c>
-      <c r="D139" s="20" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
@@ -5358,74 +5426,79 @@
       <c r="C140" s="20"/>
       <c r="D140" s="20"/>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A141" s="20" t="s">
-        <v>472</v>
-      </c>
-      <c r="B141" s="20" t="s">
+    <row r="141" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="20"/>
+      <c r="B141" s="20"/>
+      <c r="C141" s="17" t="s">
+        <v>730</v>
+      </c>
+      <c r="D141" s="17" t="s">
+        <v>731</v>
+      </c>
+      <c r="F141"/>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A142" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="B142" s="20" t="s">
+        <v>496</v>
+      </c>
+      <c r="C142" s="19" t="s">
+        <v>497</v>
+      </c>
+      <c r="D142" s="20" t="s">
         <v>498</v>
       </c>
-      <c r="C141" s="19" t="s">
-        <v>499</v>
-      </c>
-      <c r="D141" s="20" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A142" s="20"/>
-      <c r="B142" s="20"/>
-      <c r="C142" s="20"/>
-      <c r="D142" s="20"/>
-    </row>
-    <row r="143" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="20"/>
       <c r="B143" s="20"/>
-      <c r="C143" s="17" t="s">
-        <v>520</v>
-      </c>
+      <c r="C143" s="20"/>
       <c r="D143" s="20"/>
-      <c r="F143"/>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A144" s="20" t="s">
+    </row>
+    <row r="144" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="20"/>
+      <c r="B144" s="20"/>
+      <c r="C144" s="17" t="s">
+        <v>518</v>
+      </c>
+      <c r="D144" s="20"/>
+      <c r="F144"/>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A145" s="20" t="s">
+        <v>499</v>
+      </c>
+      <c r="B145" s="20" t="s">
+        <v>500</v>
+      </c>
+      <c r="C145" s="19" t="s">
         <v>501</v>
       </c>
-      <c r="B144" s="20" t="s">
+      <c r="D145" s="19" t="s">
         <v>502</v>
       </c>
-      <c r="C144" s="19" t="s">
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A146" s="20"/>
+      <c r="B146" s="20"/>
+      <c r="C146" s="20"/>
+      <c r="D146" s="20"/>
+    </row>
+    <row r="147" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="20" t="s">
+        <v>499</v>
+      </c>
+      <c r="B147" s="20" t="s">
         <v>503</v>
       </c>
-      <c r="D144" s="19" t="s">
+      <c r="C147" s="19" t="s">
+        <v>575</v>
+      </c>
+      <c r="D147" s="19" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A145" s="20"/>
-      <c r="B145" s="20"/>
-      <c r="C145" s="20"/>
-      <c r="D145" s="20"/>
-    </row>
-    <row r="146" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="B146" s="20" t="s">
-        <v>505</v>
-      </c>
-      <c r="C146" s="19" t="s">
-        <v>577</v>
-      </c>
-      <c r="D146" s="19" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A147" s="20"/>
-      <c r="B147" s="20"/>
-      <c r="C147" s="19"/>
-      <c r="D147" s="20"/>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="20"/>
@@ -5440,91 +5513,91 @@
       <c r="D149" s="20"/>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A150" s="1" t="s">
+      <c r="A150" s="20"/>
+      <c r="B150" s="20"/>
+      <c r="C150" s="19"/>
+      <c r="D150" s="20"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A151" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="C151" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="B150" s="1" t="s">
+      <c r="D151" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="C150" s="1" t="s">
+    </row>
+    <row r="152" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="B152" s="20" t="s">
         <v>509</v>
       </c>
-      <c r="D150" s="1" t="s">
+      <c r="C152" s="19" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="20" t="s">
-        <v>472</v>
-      </c>
-      <c r="B151" s="20" t="s">
+      <c r="D152" s="19" t="s">
         <v>511</v>
       </c>
-      <c r="C151" s="19" t="s">
-        <v>512</v>
-      </c>
-      <c r="D151" s="19" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A152" s="20"/>
-      <c r="B152" s="20"/>
-      <c r="C152" s="19"/>
-      <c r="D152" s="20"/>
-    </row>
-    <row r="153" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="20"/>
       <c r="B153" s="20"/>
-      <c r="C153" s="18" t="s">
-        <v>553</v>
-      </c>
-      <c r="D153" s="17" t="s">
-        <v>554</v>
-      </c>
-      <c r="F153"/>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A154" s="20" t="s">
-        <v>472</v>
-      </c>
-      <c r="B154" s="20" t="s">
+      <c r="C153" s="19"/>
+      <c r="D153" s="20"/>
+    </row>
+    <row r="154" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="20"/>
+      <c r="B154" s="20"/>
+      <c r="C154" s="18" t="s">
+        <v>551</v>
+      </c>
+      <c r="D154" s="17" t="s">
+        <v>552</v>
+      </c>
+      <c r="F154"/>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A155" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="B155" s="20" t="s">
+        <v>493</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D155" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="C154" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="20"/>
-      <c r="B155" s="20"/>
-      <c r="C155" s="17" t="s">
-        <v>518</v>
-      </c>
-      <c r="D155" s="17" t="s">
-        <v>519</v>
-      </c>
-      <c r="F155"/>
     </row>
     <row r="156" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A156" s="20"/>
       <c r="B156" s="20"/>
-      <c r="C156" s="19" t="s">
-        <v>514</v>
-      </c>
-      <c r="D156" s="19" t="s">
-        <v>525</v>
+      <c r="C156" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="D156" s="17" t="s">
+        <v>517</v>
       </c>
       <c r="F156"/>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A157" s="20"/>
       <c r="B157" s="20"/>
-      <c r="C157" s="20"/>
-      <c r="D157" s="20"/>
+      <c r="C157" s="19" t="s">
+        <v>512</v>
+      </c>
+      <c r="D157" s="19" t="s">
+        <v>523</v>
+      </c>
+      <c r="F157"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="20"/>
@@ -5544,25 +5617,25 @@
       <c r="C160" s="20"/>
       <c r="D160" s="20"/>
     </row>
-    <row r="161" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="B161" s="20" t="s">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" s="20"/>
+      <c r="B161" s="20"/>
+      <c r="C161" s="20"/>
+      <c r="D161" s="20"/>
+    </row>
+    <row r="162" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="20" t="s">
+        <v>499</v>
+      </c>
+      <c r="B162" s="20" t="s">
+        <v>513</v>
+      </c>
+      <c r="C162" s="19" t="s">
+        <v>514</v>
+      </c>
+      <c r="D162" s="19" t="s">
         <v>515</v>
       </c>
-      <c r="C161" s="19" t="s">
-        <v>516</v>
-      </c>
-      <c r="D161" s="19" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A162" s="20"/>
-      <c r="B162" s="20"/>
-      <c r="C162" s="19"/>
-      <c r="D162" s="20"/>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="20"/>
@@ -5595,62 +5668,62 @@
       <c r="D167" s="20"/>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A168" s="1" t="s">
+      <c r="A168" s="20"/>
+      <c r="B168" s="20"/>
+      <c r="C168" s="19"/>
+      <c r="D168" s="20"/>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C169" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="B168" s="1" t="s">
+      <c r="D169" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C168" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="D168" s="1" t="s">
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170" s="20" t="s">
+        <v>477</v>
+      </c>
+      <c r="B170" s="20" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A169" s="20" t="s">
-        <v>479</v>
-      </c>
-      <c r="B169" s="20" t="s">
+      <c r="C170" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D170" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="C169" s="1" t="s">
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" s="20"/>
+      <c r="B171" s="20"/>
+      <c r="C171" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="D169" s="1" t="s">
+      <c r="D171" s="1" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A170" s="20"/>
-      <c r="B170" s="20"/>
-      <c r="C170" s="1" t="s">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172" s="20" t="s">
         <v>529</v>
       </c>
-      <c r="D170" s="1" t="s">
+      <c r="B172" s="20" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A171" s="20" t="s">
+      <c r="C172" s="19" t="s">
         <v>531</v>
       </c>
-      <c r="B171" s="20" t="s">
+      <c r="D172" s="19" t="s">
         <v>532</v>
       </c>
-      <c r="C171" s="19" t="s">
-        <v>533</v>
-      </c>
-      <c r="D171" s="19" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A172" s="20"/>
-      <c r="B172" s="20"/>
-      <c r="C172" s="20"/>
-      <c r="D172" s="20"/>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="20"/>
@@ -5665,60 +5738,60 @@
       <c r="D174" s="20"/>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A175" s="1" t="s">
+      <c r="A175" s="20"/>
+      <c r="B175" s="20"/>
+      <c r="C175" s="20"/>
+      <c r="D175" s="20"/>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="D176" s="1" t="s">
         <v>535</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="D175" s="1" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A176" s="17" t="s">
-        <v>535</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="D176" s="1" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" s="17" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B177" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A178" s="17" t="s">
+        <v>533</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="D178" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="C177" s="1" t="s">
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A179" s="20" t="s">
         <v>541</v>
       </c>
-      <c r="D177" s="1" t="s">
+      <c r="B179" s="20" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A178" s="20" t="s">
+      <c r="C179" s="19" t="s">
         <v>543</v>
       </c>
-      <c r="B178" s="20" t="s">
+      <c r="D179" s="20" t="s">
         <v>544</v>
       </c>
-      <c r="C178" s="19" t="s">
-        <v>545</v>
-      </c>
-      <c r="D178" s="20" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A179" s="20"/>
-      <c r="B179" s="20"/>
-      <c r="C179" s="20"/>
-      <c r="D179" s="20"/>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" s="20"/>
@@ -5733,169 +5806,169 @@
       <c r="D181" s="20"/>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A182" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="B182" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="D182" s="1" t="s">
-        <v>548</v>
-      </c>
+      <c r="A182" s="20"/>
+      <c r="B182" s="20"/>
+      <c r="C182" s="20"/>
+      <c r="D182" s="20"/>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>479</v>
+        <v>547</v>
       </c>
       <c r="B183" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A184" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="D184" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="C183" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="D183" s="1" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A184" s="20" t="s">
-        <v>479</v>
-      </c>
-      <c r="B184" s="20" t="s">
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A185" s="20" t="s">
+        <v>477</v>
+      </c>
+      <c r="B185" s="20" t="s">
+        <v>558</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="D185" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="C184" s="1" t="s">
+    </row>
+    <row r="186" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A186" s="20"/>
+      <c r="B186" s="20"/>
+      <c r="C186" s="17" t="s">
+        <v>641</v>
+      </c>
+      <c r="D186" s="17" t="s">
+        <v>642</v>
+      </c>
+      <c r="F186"/>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A187" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B187" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="D184" s="1" t="s">
+      <c r="C187" s="1" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="185" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A185" s="20"/>
-      <c r="B185" s="20"/>
-      <c r="C185" s="17" t="s">
-        <v>643</v>
-      </c>
-      <c r="D185" s="17" t="s">
-        <v>644</v>
-      </c>
-      <c r="F185"/>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A186" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="B186" s="1" t="s">
+      <c r="D187" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="C186" s="1" t="s">
-        <v>564</v>
-      </c>
-      <c r="D186" s="1" t="s">
+    </row>
+    <row r="188" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A188" s="20" t="s">
+        <v>477</v>
+      </c>
+      <c r="B188" s="20" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A187" s="20" t="s">
-        <v>479</v>
-      </c>
-      <c r="B187" s="20" t="s">
+      <c r="C188" s="19" t="s">
+        <v>566</v>
+      </c>
+      <c r="D188" s="19" t="s">
         <v>567</v>
       </c>
-      <c r="C187" s="19" t="s">
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A189" s="20"/>
+      <c r="B189" s="20"/>
+      <c r="C189" s="19"/>
+      <c r="D189" s="20"/>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A190" s="17" t="s">
+        <v>499</v>
+      </c>
+      <c r="B190" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="D187" s="19" t="s">
+      <c r="C190" s="18" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A188" s="20"/>
-      <c r="B188" s="20"/>
-      <c r="C188" s="19"/>
-      <c r="D188" s="20"/>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A189" s="17" t="s">
-        <v>501</v>
-      </c>
-      <c r="B189" s="1" t="s">
+      <c r="D190" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="C189" s="18" t="s">
-        <v>571</v>
-      </c>
-      <c r="D189" s="1" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A190" s="20" t="s">
+    </row>
+    <row r="191" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A191" s="20" t="s">
+        <v>461</v>
+      </c>
+      <c r="B191" s="20" t="s">
+        <v>462</v>
+      </c>
+      <c r="C191" s="19" t="s">
         <v>463</v>
       </c>
-      <c r="B190" s="20" t="s">
+      <c r="D191" s="19" t="s">
         <v>464</v>
       </c>
-      <c r="C190" s="19" t="s">
-        <v>465</v>
-      </c>
-      <c r="D190" s="19" t="s">
-        <v>466</v>
-      </c>
-      <c r="E190" s="1"/>
-      <c r="F190"/>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A191" s="20"/>
-      <c r="B191" s="20"/>
-      <c r="C191" s="20"/>
-      <c r="D191" s="20"/>
-    </row>
-    <row r="192" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E191" s="1"/>
+      <c r="F191"/>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" s="20"/>
       <c r="B192" s="20"/>
-      <c r="C192" s="17" t="s">
-        <v>641</v>
-      </c>
-      <c r="D192" s="17" t="s">
-        <v>642</v>
-      </c>
-      <c r="F192"/>
+      <c r="C192" s="20"/>
+      <c r="D192" s="20"/>
     </row>
     <row r="193" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A193" s="20"/>
       <c r="B193" s="20"/>
-      <c r="C193" s="20" t="s">
-        <v>646</v>
-      </c>
-      <c r="D193" s="19" t="s">
-        <v>645</v>
+      <c r="C193" s="17" t="s">
+        <v>639</v>
+      </c>
+      <c r="D193" s="17" t="s">
+        <v>640</v>
       </c>
       <c r="F193"/>
     </row>
     <row r="194" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A194" s="20"/>
       <c r="B194" s="20"/>
-      <c r="C194" s="20"/>
-      <c r="D194" s="20"/>
+      <c r="C194" s="20" t="s">
+        <v>644</v>
+      </c>
+      <c r="D194" s="19" t="s">
+        <v>643</v>
+      </c>
       <c r="F194"/>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A195" s="20"/>
       <c r="B195" s="20"/>
-      <c r="C195" s="19" t="s">
-        <v>578</v>
-      </c>
-      <c r="D195" s="19" t="s">
-        <v>579</v>
-      </c>
+      <c r="C195" s="20"/>
+      <c r="D195" s="20"/>
+      <c r="F195"/>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" s="20"/>
       <c r="B196" s="20"/>
-      <c r="C196" s="20"/>
-      <c r="D196" s="20"/>
+      <c r="C196" s="19" t="s">
+        <v>576</v>
+      </c>
+      <c r="D196" s="19" t="s">
+        <v>577</v>
+      </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" s="20"/>
@@ -5933,22 +6006,21 @@
       <c r="C202" s="20"/>
       <c r="D202" s="20"/>
     </row>
-    <row r="203" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" s="20"/>
       <c r="B203" s="20"/>
-      <c r="C203" s="19" t="s">
-        <v>581</v>
-      </c>
-      <c r="D203" s="20" t="s">
-        <v>580</v>
-      </c>
-      <c r="F203"/>
+      <c r="C203" s="20"/>
+      <c r="D203" s="20"/>
     </row>
     <row r="204" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A204" s="20"/>
       <c r="B204" s="20"/>
-      <c r="C204" s="20"/>
-      <c r="D204" s="20"/>
+      <c r="C204" s="19" t="s">
+        <v>579</v>
+      </c>
+      <c r="D204" s="20" t="s">
+        <v>578</v>
+      </c>
       <c r="F204"/>
     </row>
     <row r="205" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
@@ -5993,294 +6065,295 @@
       <c r="D210" s="20"/>
       <c r="F210"/>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A211" s="20" t="s">
+    <row r="211" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A211" s="20"/>
+      <c r="B211" s="20"/>
+      <c r="C211" s="20"/>
+      <c r="D211" s="20"/>
+      <c r="F211"/>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A212" s="20" t="s">
+        <v>465</v>
+      </c>
+      <c r="B212" s="20" t="s">
         <v>467</v>
       </c>
-      <c r="B211" s="20" t="s">
+      <c r="C212" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="D212" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="C211" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="D211" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="E211" s="12" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A212" s="20"/>
-      <c r="B212" s="20"/>
-      <c r="C212" s="20" t="s">
-        <v>583</v>
-      </c>
-      <c r="D212" s="19" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E212" s="12" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213" s="20"/>
       <c r="B213" s="20"/>
-      <c r="C213" s="20"/>
-      <c r="D213" s="20"/>
-      <c r="F213"/>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C213" s="20" t="s">
+        <v>581</v>
+      </c>
+      <c r="D213" s="19" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A214" s="20"/>
       <c r="B214" s="20"/>
-      <c r="C214" s="20" t="s">
-        <v>584</v>
-      </c>
-      <c r="D214" s="19" t="s">
-        <v>585</v>
-      </c>
+      <c r="C214" s="20"/>
+      <c r="D214" s="20"/>
+      <c r="F214"/>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215" s="20"/>
       <c r="B215" s="20"/>
-      <c r="C215" s="20"/>
-      <c r="D215" s="20"/>
-    </row>
-    <row r="216" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C215" s="20" t="s">
+        <v>582</v>
+      </c>
+      <c r="D215" s="19" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216" s="20"/>
       <c r="B216" s="20"/>
-      <c r="C216" s="20" t="s">
-        <v>658</v>
-      </c>
-      <c r="D216" s="19" t="s">
-        <v>659</v>
-      </c>
-      <c r="F216"/>
+      <c r="C216" s="20"/>
+      <c r="D216" s="20"/>
     </row>
     <row r="217" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A217" s="20"/>
       <c r="B217" s="20"/>
-      <c r="C217" s="20"/>
-      <c r="D217" s="20"/>
+      <c r="C217" s="20" t="s">
+        <v>656</v>
+      </c>
+      <c r="D217" s="19" t="s">
+        <v>657</v>
+      </c>
       <c r="F217"/>
     </row>
     <row r="218" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A218" s="20"/>
       <c r="B218" s="20"/>
-      <c r="C218" s="17" t="s">
-        <v>660</v>
-      </c>
-      <c r="D218" s="17" t="s">
-        <v>661</v>
-      </c>
+      <c r="C218" s="20"/>
+      <c r="D218" s="20"/>
       <c r="F218"/>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A219" s="20"/>
       <c r="B219" s="20"/>
-      <c r="C219" s="20" t="s">
-        <v>586</v>
-      </c>
-      <c r="D219" s="19" t="s">
-        <v>587</v>
-      </c>
+      <c r="C219" s="17" t="s">
+        <v>658</v>
+      </c>
+      <c r="D219" s="17" t="s">
+        <v>659</v>
+      </c>
+      <c r="F219"/>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220" s="20"/>
       <c r="B220" s="20"/>
-      <c r="C220" s="20"/>
-      <c r="D220" s="20"/>
+      <c r="C220" s="20" t="s">
+        <v>584</v>
+      </c>
+      <c r="D220" s="19" t="s">
+        <v>585</v>
+      </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221" s="20"/>
       <c r="B221" s="20"/>
-      <c r="C221" s="20" t="s">
-        <v>588</v>
-      </c>
-      <c r="D221" s="19" t="s">
-        <v>591</v>
-      </c>
+      <c r="C221" s="20"/>
+      <c r="D221" s="20"/>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A222" s="20"/>
       <c r="B222" s="20"/>
-      <c r="C222" s="20"/>
-      <c r="D222" s="20"/>
-    </row>
-    <row r="223" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C222" s="20" t="s">
+        <v>586</v>
+      </c>
+      <c r="D222" s="19" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223" s="20"/>
       <c r="B223" s="20"/>
-      <c r="C223" s="20" t="s">
-        <v>590</v>
-      </c>
-      <c r="D223" s="19" t="s">
-        <v>592</v>
-      </c>
-      <c r="F223"/>
+      <c r="C223" s="20"/>
+      <c r="D223" s="20"/>
     </row>
     <row r="224" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A224" s="20"/>
       <c r="B224" s="20"/>
-      <c r="C224" s="20"/>
-      <c r="D224" s="20"/>
+      <c r="C224" s="20" t="s">
+        <v>588</v>
+      </c>
+      <c r="D224" s="19" t="s">
+        <v>590</v>
+      </c>
       <c r="F224"/>
     </row>
-    <row r="225" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A225" s="20"/>
       <c r="B225" s="20"/>
-      <c r="C225" s="20" t="s">
-        <v>589</v>
-      </c>
-      <c r="D225" s="19" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C225" s="20"/>
+      <c r="D225" s="20"/>
+      <c r="F225"/>
+    </row>
+    <row r="226" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="20"/>
       <c r="B226" s="20"/>
-      <c r="C226" s="20"/>
-      <c r="D226" s="19"/>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C226" s="20" t="s">
+        <v>587</v>
+      </c>
+      <c r="D226" s="19" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" s="20"/>
       <c r="B227" s="20"/>
       <c r="C227" s="20"/>
       <c r="D227" s="19"/>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" s="20"/>
       <c r="B228" s="20"/>
-      <c r="C228" s="17" t="s">
-        <v>594</v>
-      </c>
-      <c r="D228" s="1" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C228" s="20"/>
+      <c r="D228" s="19"/>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" s="20"/>
       <c r="B229" s="20"/>
-      <c r="C229" s="20" t="s">
-        <v>596</v>
-      </c>
-      <c r="D229" s="19" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C229" s="17" t="s">
+        <v>592</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" s="20"/>
       <c r="B230" s="20"/>
-      <c r="C230" s="20"/>
-      <c r="D230" s="20"/>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C230" s="20" t="s">
+        <v>594</v>
+      </c>
+      <c r="D230" s="19" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" s="20"/>
       <c r="B231" s="20"/>
-      <c r="C231" s="20" t="s">
-        <v>598</v>
-      </c>
-      <c r="D231" s="19" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C231" s="20"/>
+      <c r="D231" s="20"/>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" s="20"/>
       <c r="B232" s="20"/>
-      <c r="C232" s="20"/>
-      <c r="D232" s="20"/>
-    </row>
-    <row r="233" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C232" s="20" t="s">
+        <v>596</v>
+      </c>
+      <c r="D232" s="19" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" s="20"/>
       <c r="B233" s="20"/>
-      <c r="C233" s="20" t="s">
-        <v>601</v>
-      </c>
-      <c r="D233" s="19" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C233" s="20"/>
+      <c r="D233" s="20"/>
+    </row>
+    <row r="234" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="20"/>
       <c r="B234" s="20"/>
-      <c r="C234" s="20"/>
-      <c r="D234" s="19"/>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C234" s="20" t="s">
+        <v>599</v>
+      </c>
+      <c r="D234" s="19" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" s="20"/>
       <c r="B235" s="20"/>
       <c r="C235" s="20"/>
       <c r="D235" s="19"/>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" s="20"/>
       <c r="B236" s="20"/>
-      <c r="C236" s="20" t="s">
-        <v>604</v>
-      </c>
-      <c r="D236" s="19" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C236" s="20"/>
+      <c r="D236" s="19"/>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237" s="20"/>
       <c r="B237" s="20"/>
-      <c r="C237" s="20"/>
-      <c r="D237" s="19"/>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C237" s="20" t="s">
+        <v>602</v>
+      </c>
+      <c r="D237" s="19" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238" s="20"/>
       <c r="B238" s="20"/>
       <c r="C238" s="20"/>
       <c r="D238" s="19"/>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A239" s="20" t="s">
-        <v>608</v>
-      </c>
-      <c r="B239" s="20" t="s">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A239" s="20"/>
+      <c r="B239" s="20"/>
+      <c r="C239" s="20"/>
+      <c r="D239" s="19"/>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A240" s="20" t="s">
+        <v>606</v>
+      </c>
+      <c r="B240" s="20" t="s">
+        <v>603</v>
+      </c>
+      <c r="C240" s="19" t="s">
+        <v>604</v>
+      </c>
+      <c r="D240" s="19" t="s">
         <v>605</v>
       </c>
-      <c r="C239" s="19" t="s">
-        <v>606</v>
-      </c>
-      <c r="D239" s="19" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A240" s="20"/>
-      <c r="B240" s="20"/>
-      <c r="C240" s="20"/>
-      <c r="D240" s="20"/>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" s="20"/>
       <c r="B241" s="20"/>
-      <c r="C241" s="19" t="s">
-        <v>609</v>
-      </c>
-      <c r="D241" s="19" t="s">
-        <v>610</v>
-      </c>
+      <c r="C241" s="20"/>
+      <c r="D241" s="20"/>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" s="20"/>
       <c r="B242" s="20"/>
-      <c r="C242" s="20"/>
-      <c r="D242" s="20"/>
-    </row>
-    <row r="243" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C242" s="19" t="s">
+        <v>607</v>
+      </c>
+      <c r="D242" s="19" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" s="20"/>
       <c r="B243" s="20"/>
-      <c r="C243" s="19" t="s">
-        <v>612</v>
-      </c>
-      <c r="D243" s="20" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C243" s="20"/>
+      <c r="D243" s="20"/>
+    </row>
+    <row r="244" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="20"/>
       <c r="B244" s="20"/>
-      <c r="C244" s="19"/>
-      <c r="D244" s="20"/>
+      <c r="C244" s="19" t="s">
+        <v>610</v>
+      </c>
+      <c r="D244" s="20" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" s="20"/>
@@ -6291,66 +6364,66 @@
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" s="20"/>
       <c r="B246" s="20"/>
-      <c r="C246" s="19" t="s">
-        <v>611</v>
-      </c>
-      <c r="D246" s="20" t="s">
-        <v>470</v>
-      </c>
+      <c r="C246" s="19"/>
+      <c r="D246" s="20"/>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" s="20"/>
       <c r="B247" s="20"/>
-      <c r="C247" s="20"/>
-      <c r="D247" s="20"/>
+      <c r="C247" s="19" t="s">
+        <v>609</v>
+      </c>
+      <c r="D247" s="20" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" s="20"/>
       <c r="B248" s="20"/>
-      <c r="C248" s="19" t="s">
-        <v>613</v>
-      </c>
-      <c r="D248" s="19" t="s">
-        <v>615</v>
-      </c>
+      <c r="C248" s="20"/>
+      <c r="D248" s="20"/>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" s="20"/>
       <c r="B249" s="20"/>
-      <c r="C249" s="20"/>
-      <c r="D249" s="20"/>
+      <c r="C249" s="19" t="s">
+        <v>611</v>
+      </c>
+      <c r="D249" s="19" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" s="20"/>
       <c r="B250" s="20"/>
-      <c r="C250" s="19" t="s">
-        <v>614</v>
-      </c>
-      <c r="D250" s="19" t="s">
-        <v>616</v>
-      </c>
+      <c r="C250" s="20"/>
+      <c r="D250" s="20"/>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" s="20"/>
       <c r="B251" s="20"/>
-      <c r="C251" s="20"/>
-      <c r="D251" s="20"/>
-    </row>
-    <row r="252" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C251" s="19" t="s">
+        <v>612</v>
+      </c>
+      <c r="D251" s="19" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" s="20"/>
       <c r="B252" s="20"/>
-      <c r="C252" s="19" t="s">
-        <v>617</v>
-      </c>
-      <c r="D252" s="19" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C252" s="20"/>
+      <c r="D252" s="20"/>
+    </row>
+    <row r="253" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="20"/>
       <c r="B253" s="20"/>
-      <c r="C253" s="19"/>
-      <c r="D253" s="19"/>
+      <c r="C253" s="19" t="s">
+        <v>615</v>
+      </c>
+      <c r="D253" s="19" t="s">
+        <v>618</v>
+      </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" s="20"/>
@@ -6358,44 +6431,44 @@
       <c r="C254" s="19"/>
       <c r="D254" s="19"/>
     </row>
-    <row r="255" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" s="20"/>
       <c r="B255" s="20"/>
-      <c r="C255" s="19" t="s">
-        <v>618</v>
-      </c>
-      <c r="D255" s="19" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C255" s="19"/>
+      <c r="D255" s="19"/>
+    </row>
+    <row r="256" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="20"/>
       <c r="B256" s="20"/>
-      <c r="C256" s="19"/>
-      <c r="D256" s="19"/>
-    </row>
-    <row r="257" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C256" s="19" t="s">
+        <v>616</v>
+      </c>
+      <c r="D256" s="19" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A257" s="20"/>
       <c r="B257" s="20"/>
       <c r="C257" s="19"/>
       <c r="D257" s="19"/>
-      <c r="F257"/>
-    </row>
-    <row r="258" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="258" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A258" s="20"/>
       <c r="B258" s="20"/>
-      <c r="C258" s="19" t="s">
-        <v>619</v>
-      </c>
-      <c r="D258" s="19" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C258" s="19"/>
+      <c r="D258" s="19"/>
+      <c r="F258"/>
+    </row>
+    <row r="259" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="20"/>
       <c r="B259" s="20"/>
-      <c r="C259" s="19"/>
-      <c r="D259" s="19"/>
+      <c r="C259" s="19" t="s">
+        <v>617</v>
+      </c>
+      <c r="D259" s="19" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A260" s="20"/>
@@ -6406,18 +6479,18 @@
     <row r="261" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A261" s="20"/>
       <c r="B261" s="20"/>
-      <c r="C261" s="19" t="s">
-        <v>623</v>
-      </c>
-      <c r="D261" s="19" t="s">
-        <v>624</v>
-      </c>
+      <c r="C261" s="19"/>
+      <c r="D261" s="19"/>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A262" s="20"/>
       <c r="B262" s="20"/>
-      <c r="C262" s="19"/>
-      <c r="D262" s="19"/>
+      <c r="C262" s="19" t="s">
+        <v>621</v>
+      </c>
+      <c r="D262" s="19" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A263" s="20"/>
@@ -6425,21 +6498,21 @@
       <c r="C263" s="19"/>
       <c r="D263" s="19"/>
     </row>
-    <row r="264" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A264" s="20"/>
       <c r="B264" s="20"/>
-      <c r="C264" s="19" t="s">
-        <v>625</v>
-      </c>
-      <c r="D264" s="19" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C264" s="19"/>
+      <c r="D264" s="19"/>
+    </row>
+    <row r="265" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A265" s="20"/>
       <c r="B265" s="20"/>
-      <c r="C265" s="19"/>
-      <c r="D265" s="19"/>
+      <c r="C265" s="19" t="s">
+        <v>623</v>
+      </c>
+      <c r="D265" s="19" t="s">
+        <v>624</v>
+      </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A266" s="20"/>
@@ -6456,18 +6529,18 @@
     <row r="268" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A268" s="20"/>
       <c r="B268" s="20"/>
-      <c r="C268" s="19" t="s">
-        <v>627</v>
-      </c>
-      <c r="D268" s="19" t="s">
-        <v>628</v>
-      </c>
+      <c r="C268" s="19"/>
+      <c r="D268" s="19"/>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A269" s="20"/>
       <c r="B269" s="20"/>
-      <c r="C269" s="19"/>
-      <c r="D269" s="19"/>
+      <c r="C269" s="19" t="s">
+        <v>625</v>
+      </c>
+      <c r="D269" s="19" t="s">
+        <v>626</v>
+      </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A270" s="20"/>
@@ -6478,18 +6551,18 @@
     <row r="271" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A271" s="20"/>
       <c r="B271" s="20"/>
-      <c r="C271" s="19" t="s">
-        <v>629</v>
-      </c>
-      <c r="D271" s="20" t="s">
-        <v>630</v>
-      </c>
+      <c r="C271" s="19"/>
+      <c r="D271" s="19"/>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A272" s="20"/>
       <c r="B272" s="20"/>
-      <c r="C272" s="20"/>
-      <c r="D272" s="20"/>
+      <c r="C272" s="19" t="s">
+        <v>627</v>
+      </c>
+      <c r="D272" s="20" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" s="20"/>
@@ -6506,18 +6579,18 @@
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275" s="20"/>
       <c r="B275" s="20"/>
-      <c r="C275" s="19" t="s">
-        <v>631</v>
-      </c>
-      <c r="D275" s="20" t="s">
-        <v>632</v>
-      </c>
+      <c r="C275" s="20"/>
+      <c r="D275" s="20"/>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276" s="20"/>
       <c r="B276" s="20"/>
-      <c r="C276" s="20"/>
-      <c r="D276" s="20"/>
+      <c r="C276" s="19" t="s">
+        <v>629</v>
+      </c>
+      <c r="D276" s="20" t="s">
+        <v>630</v>
+      </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277" s="20"/>
@@ -6534,18 +6607,18 @@
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" s="20"/>
       <c r="B279" s="20"/>
-      <c r="C279" s="19" t="s">
-        <v>633</v>
-      </c>
-      <c r="D279" s="19" t="s">
-        <v>634</v>
-      </c>
+      <c r="C279" s="20"/>
+      <c r="D279" s="20"/>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" s="20"/>
       <c r="B280" s="20"/>
-      <c r="C280" s="20"/>
-      <c r="D280" s="20"/>
+      <c r="C280" s="19" t="s">
+        <v>631</v>
+      </c>
+      <c r="D280" s="19" t="s">
+        <v>632</v>
+      </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281" s="20"/>
@@ -6559,21 +6632,21 @@
       <c r="C282" s="20"/>
       <c r="D282" s="20"/>
     </row>
-    <row r="283" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283" s="20"/>
       <c r="B283" s="20"/>
-      <c r="C283" s="19" t="s">
-        <v>639</v>
-      </c>
-      <c r="D283" s="19" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C283" s="20"/>
+      <c r="D283" s="20"/>
+    </row>
+    <row r="284" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A284" s="20"/>
       <c r="B284" s="20"/>
-      <c r="C284" s="19"/>
-      <c r="D284" s="20"/>
+      <c r="C284" s="19" t="s">
+        <v>637</v>
+      </c>
+      <c r="D284" s="19" t="s">
+        <v>638</v>
+      </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285" s="20"/>
@@ -6605,43 +6678,43 @@
       <c r="C289" s="19"/>
       <c r="D289" s="20"/>
     </row>
-    <row r="290" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A290" s="20"/>
       <c r="B290" s="20"/>
-      <c r="C290" s="19" t="s">
-        <v>662</v>
-      </c>
-      <c r="D290" s="19" t="s">
-        <v>663</v>
-      </c>
-      <c r="F290"/>
+      <c r="C290" s="19"/>
+      <c r="D290" s="20"/>
     </row>
     <row r="291" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A291" s="20"/>
       <c r="B291" s="20"/>
-      <c r="C291" s="19"/>
-      <c r="D291" s="20"/>
+      <c r="C291" s="19" t="s">
+        <v>660</v>
+      </c>
+      <c r="D291" s="19" t="s">
+        <v>661</v>
+      </c>
       <c r="F291"/>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A292" s="20" t="s">
-        <v>637</v>
-      </c>
-      <c r="B292" s="20" t="s">
+    <row r="292" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A292" s="20"/>
+      <c r="B292" s="20"/>
+      <c r="C292" s="19"/>
+      <c r="D292" s="20"/>
+      <c r="F292"/>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A293" s="20" t="s">
+        <v>635</v>
+      </c>
+      <c r="B293" s="20" t="s">
+        <v>634</v>
+      </c>
+      <c r="C293" s="19" t="s">
+        <v>633</v>
+      </c>
+      <c r="D293" s="20" t="s">
         <v>636</v>
       </c>
-      <c r="C292" s="19" t="s">
-        <v>635</v>
-      </c>
-      <c r="D292" s="20" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A293" s="20"/>
-      <c r="B293" s="20"/>
-      <c r="C293" s="20"/>
-      <c r="D293" s="20"/>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A294" s="20"/>
@@ -6649,25 +6722,25 @@
       <c r="C294" s="20"/>
       <c r="D294" s="20"/>
     </row>
-    <row r="295" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A295" s="20" t="s">
-        <v>531</v>
-      </c>
-      <c r="B295" s="20" t="s">
-        <v>647</v>
-      </c>
-      <c r="C295" s="20" t="s">
-        <v>657</v>
-      </c>
-      <c r="D295" s="19" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A296" s="20"/>
-      <c r="B296" s="20"/>
-      <c r="C296" s="20"/>
-      <c r="D296" s="19"/>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A295" s="20"/>
+      <c r="B295" s="20"/>
+      <c r="C295" s="20"/>
+      <c r="D295" s="20"/>
+    </row>
+    <row r="296" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A296" s="20" t="s">
+        <v>529</v>
+      </c>
+      <c r="B296" s="20" t="s">
+        <v>645</v>
+      </c>
+      <c r="C296" s="20" t="s">
+        <v>655</v>
+      </c>
+      <c r="D296" s="19" t="s">
+        <v>649</v>
+      </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A297" s="20"/>
@@ -6675,32 +6748,32 @@
       <c r="C297" s="20"/>
       <c r="D297" s="19"/>
     </row>
-    <row r="298" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A298" s="20"/>
       <c r="B298" s="20"/>
       <c r="C298" s="20"/>
       <c r="D298" s="19"/>
-      <c r="F298"/>
-    </row>
-    <row r="299" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A299" s="20" t="s">
+    </row>
+    <row r="299" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A299" s="20"/>
+      <c r="B299" s="20"/>
+      <c r="C299" s="20"/>
+      <c r="D299" s="19"/>
+      <c r="F299"/>
+    </row>
+    <row r="300" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A300" s="20" t="s">
+        <v>646</v>
+      </c>
+      <c r="B300" s="20" t="s">
+        <v>647</v>
+      </c>
+      <c r="C300" s="20" t="s">
         <v>648</v>
       </c>
-      <c r="B299" s="20" t="s">
-        <v>649</v>
-      </c>
-      <c r="C299" s="20" t="s">
+      <c r="D300" s="19" t="s">
         <v>650</v>
       </c>
-      <c r="D299" s="19" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A300" s="20"/>
-      <c r="B300" s="20"/>
-      <c r="C300" s="20"/>
-      <c r="D300" s="19"/>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A301" s="20"/>
@@ -6709,48 +6782,45 @@
       <c r="D301" s="19"/>
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A302" s="20" t="s">
-        <v>531</v>
-      </c>
-      <c r="B302" s="20" t="s">
+      <c r="A302" s="20"/>
+      <c r="B302" s="20"/>
+      <c r="C302" s="20"/>
+      <c r="D302" s="19"/>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A303" s="20" t="s">
+        <v>529</v>
+      </c>
+      <c r="B303" s="20" t="s">
+        <v>651</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="D303" s="19" t="s">
         <v>653</v>
       </c>
-      <c r="C302" s="1" t="s">
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A304" s="20"/>
+      <c r="B304" s="20"/>
+      <c r="C304" s="17" t="s">
         <v>654</v>
       </c>
-      <c r="D302" s="19" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A303" s="20"/>
-      <c r="B303" s="20"/>
-      <c r="C303" s="17" t="s">
-        <v>656</v>
-      </c>
-      <c r="D303" s="20"/>
-    </row>
-    <row r="304" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A304" s="20" t="s">
+      <c r="D304" s="20"/>
+    </row>
+    <row r="305" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A305" s="20" t="s">
+        <v>708</v>
+      </c>
+      <c r="B305" s="20" t="s">
+        <v>709</v>
+      </c>
+      <c r="C305" s="19" t="s">
+        <v>710</v>
+      </c>
+      <c r="D305" s="17" t="s">
         <v>711</v>
-      </c>
-      <c r="B304" s="20" t="s">
-        <v>712</v>
-      </c>
-      <c r="C304" s="19" t="s">
-        <v>713</v>
-      </c>
-      <c r="D304" s="17" t="s">
-        <v>714</v>
-      </c>
-      <c r="F304"/>
-    </row>
-    <row r="305" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A305" s="20"/>
-      <c r="B305" s="20"/>
-      <c r="C305" s="20"/>
-      <c r="D305" s="17" t="s">
-        <v>715</v>
       </c>
       <c r="F305"/>
     </row>
@@ -6759,30 +6829,32 @@
       <c r="B306" s="20"/>
       <c r="C306" s="20"/>
       <c r="D306" s="17" t="s">
+        <v>712</v>
+      </c>
+      <c r="F306"/>
+    </row>
+    <row r="307" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A307" s="20"/>
+      <c r="B307" s="20"/>
+      <c r="C307" s="20"/>
+      <c r="D307" s="17" t="s">
+        <v>713</v>
+      </c>
+      <c r="F307"/>
+    </row>
+    <row r="308" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A308" s="20" t="s">
+        <v>499</v>
+      </c>
+      <c r="B308" s="20" t="s">
+        <v>714</v>
+      </c>
+      <c r="C308" s="19" t="s">
+        <v>715</v>
+      </c>
+      <c r="D308" s="20" t="s">
         <v>716</v>
       </c>
-      <c r="F306"/>
-    </row>
-    <row r="307" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A307" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="B307" s="20" t="s">
-        <v>717</v>
-      </c>
-      <c r="C307" s="19" t="s">
-        <v>718</v>
-      </c>
-      <c r="D307" s="20" t="s">
-        <v>719</v>
-      </c>
-      <c r="F307"/>
-    </row>
-    <row r="308" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A308" s="20"/>
-      <c r="B308" s="20"/>
-      <c r="C308" s="20"/>
-      <c r="D308" s="20"/>
       <c r="F308"/>
     </row>
     <row r="309" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
@@ -6792,25 +6864,26 @@
       <c r="D309" s="20"/>
       <c r="F309"/>
     </row>
-    <row r="310" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A310" s="20" t="s">
-        <v>507</v>
-      </c>
-      <c r="B310" s="20" t="s">
+    <row r="310" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A310" s="20"/>
+      <c r="B310" s="20"/>
+      <c r="C310" s="20"/>
+      <c r="D310" s="20"/>
+      <c r="F310"/>
+    </row>
+    <row r="311" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A311" s="20" t="s">
+        <v>505</v>
+      </c>
+      <c r="B311" s="20" t="s">
+        <v>662</v>
+      </c>
+      <c r="C311" s="19" t="s">
+        <v>663</v>
+      </c>
+      <c r="D311" s="19" t="s">
         <v>664</v>
       </c>
-      <c r="C310" s="19" t="s">
-        <v>665</v>
-      </c>
-      <c r="D310" s="19" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A311" s="20"/>
-      <c r="B311" s="20"/>
-      <c r="C311" s="19"/>
-      <c r="D311" s="20"/>
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A312" s="20"/>
@@ -6854,29 +6927,28 @@
       <c r="C318" s="19"/>
       <c r="D318" s="20"/>
     </row>
-    <row r="319" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A319" s="20" t="s">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A319" s="20"/>
+      <c r="B319" s="20"/>
+      <c r="C319" s="19"/>
+      <c r="D319" s="20"/>
+    </row>
+    <row r="320" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A320" s="20" t="s">
+        <v>666</v>
+      </c>
+      <c r="B320" s="20" t="s">
+        <v>665</v>
+      </c>
+      <c r="C320" s="19" t="s">
         <v>668</v>
       </c>
-      <c r="B319" s="20" t="s">
+      <c r="D320" s="20" t="s">
         <v>667</v>
       </c>
-      <c r="C319" s="19" t="s">
-        <v>670</v>
-      </c>
-      <c r="D319" s="20" t="s">
+      <c r="E320" s="22" t="s">
         <v>669</v>
       </c>
-      <c r="E319" s="22" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A320" s="20"/>
-      <c r="B320" s="20"/>
-      <c r="C320" s="19"/>
-      <c r="D320" s="20"/>
-      <c r="E320" s="20"/>
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A321" s="20"/>
@@ -6934,26 +7006,26 @@
       <c r="D328" s="20"/>
       <c r="E328" s="20"/>
     </row>
-    <row r="329" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A329" s="20" t="s">
-        <v>507</v>
-      </c>
-      <c r="B329" s="20" t="s">
+    <row r="329" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A329" s="20"/>
+      <c r="B329" s="20"/>
+      <c r="C329" s="19"/>
+      <c r="D329" s="20"/>
+      <c r="E329" s="20"/>
+    </row>
+    <row r="330" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A330" s="20" t="s">
+        <v>505</v>
+      </c>
+      <c r="B330" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="C330" s="19" t="s">
+        <v>676</v>
+      </c>
+      <c r="D330" s="20" t="s">
         <v>677</v>
       </c>
-      <c r="C329" s="19" t="s">
-        <v>678</v>
-      </c>
-      <c r="D329" s="20" t="s">
-        <v>679</v>
-      </c>
-      <c r="F329"/>
-    </row>
-    <row r="330" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A330" s="20"/>
-      <c r="B330" s="20"/>
-      <c r="C330" s="19"/>
-      <c r="D330" s="20"/>
       <c r="F330"/>
     </row>
     <row r="331" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
@@ -6991,29 +7063,29 @@
       <c r="D335" s="20"/>
       <c r="F335"/>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A336" s="20" t="s">
-        <v>507</v>
-      </c>
-      <c r="B336" s="20" t="s">
-        <v>673</v>
-      </c>
-      <c r="C336" s="19" t="s">
-        <v>672</v>
-      </c>
-      <c r="D336" s="19" t="s">
-        <v>720</v>
-      </c>
-      <c r="E336" s="22" t="s">
-        <v>680</v>
-      </c>
+    <row r="336" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A336" s="20"/>
+      <c r="B336" s="20"/>
+      <c r="C336" s="19"/>
+      <c r="D336" s="20"/>
+      <c r="F336"/>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A337" s="20"/>
-      <c r="B337" s="20"/>
-      <c r="C337" s="19"/>
-      <c r="D337" s="20"/>
-      <c r="E337" s="20"/>
+      <c r="A337" s="20" t="s">
+        <v>505</v>
+      </c>
+      <c r="B337" s="20" t="s">
+        <v>671</v>
+      </c>
+      <c r="C337" s="19" t="s">
+        <v>670</v>
+      </c>
+      <c r="D337" s="19" t="s">
+        <v>717</v>
+      </c>
+      <c r="E337" s="22" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A338" s="20"/>
@@ -7057,25 +7129,26 @@
       <c r="D343" s="20"/>
       <c r="E343" s="20"/>
     </row>
-    <row r="344" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A344" s="20" t="s">
-        <v>668</v>
-      </c>
-      <c r="B344" s="20" t="s">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A344" s="20"/>
+      <c r="B344" s="20"/>
+      <c r="C344" s="19"/>
+      <c r="D344" s="20"/>
+      <c r="E344" s="20"/>
+    </row>
+    <row r="345" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A345" s="20" t="s">
+        <v>666</v>
+      </c>
+      <c r="B345" s="20" t="s">
+        <v>672</v>
+      </c>
+      <c r="C345" s="19" t="s">
+        <v>673</v>
+      </c>
+      <c r="D345" s="19" t="s">
         <v>674</v>
       </c>
-      <c r="C344" s="19" t="s">
-        <v>675</v>
-      </c>
-      <c r="D344" s="19" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A345" s="20"/>
-      <c r="B345" s="20"/>
-      <c r="C345" s="19"/>
-      <c r="D345" s="20"/>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A346" s="20"/>
@@ -7126,25 +7199,17 @@
       <c r="D353" s="20"/>
     </row>
     <row r="354" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A354" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B354" s="1" t="s">
-        <v>681</v>
-      </c>
-      <c r="C354" s="1" t="s">
-        <v>685</v>
-      </c>
-      <c r="D354" s="1" t="s">
-        <v>686</v>
-      </c>
+      <c r="A354" s="20"/>
+      <c r="B354" s="20"/>
+      <c r="C354" s="19"/>
+      <c r="D354" s="20"/>
     </row>
     <row r="355" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A355" s="1" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="C355" s="1" t="s">
         <v>683</v>
@@ -7153,25 +7218,33 @@
         <v>684</v>
       </c>
     </row>
-    <row r="356" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A356" s="20" t="s">
-        <v>479</v>
-      </c>
-      <c r="B356" s="20" t="s">
-        <v>689</v>
-      </c>
-      <c r="C356" s="19" t="s">
-        <v>687</v>
-      </c>
-      <c r="D356" s="20" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A357" s="20"/>
-      <c r="B357" s="20"/>
-      <c r="C357" s="19"/>
-      <c r="D357" s="20"/>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A356" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B356" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="C356" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="D356" s="1" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A357" s="20" t="s">
+        <v>477</v>
+      </c>
+      <c r="B357" s="20" t="s">
+        <v>686</v>
+      </c>
+      <c r="C357" s="19" t="s">
+        <v>740</v>
+      </c>
+      <c r="D357" s="20" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="358" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A358" s="20"/>
@@ -7179,92 +7252,92 @@
       <c r="C358" s="19"/>
       <c r="D358" s="20"/>
     </row>
-    <row r="359" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A359" s="20" t="s">
-        <v>485</v>
-      </c>
-      <c r="B359" s="20" t="s">
+    <row r="359" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A359" s="20"/>
+      <c r="B359" s="20"/>
+      <c r="C359" s="19"/>
+      <c r="D359" s="20"/>
+    </row>
+    <row r="360" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A360" s="20" t="s">
+        <v>483</v>
+      </c>
+      <c r="B360" s="20" t="s">
+        <v>688</v>
+      </c>
+      <c r="C360" s="18" t="s">
+        <v>689</v>
+      </c>
+      <c r="D360" s="17" t="s">
+        <v>718</v>
+      </c>
+      <c r="F360"/>
+    </row>
+    <row r="361" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A361" s="20"/>
+      <c r="B361" s="20"/>
+      <c r="C361" s="18" t="s">
+        <v>690</v>
+      </c>
+      <c r="D361" s="17" t="s">
+        <v>719</v>
+      </c>
+      <c r="F361"/>
+    </row>
+    <row r="362" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A362" s="20" t="s">
+        <v>483</v>
+      </c>
+      <c r="B362" s="20" t="s">
         <v>691</v>
       </c>
-      <c r="C359" s="18" t="s">
+      <c r="C362" s="18" t="s">
+        <v>693</v>
+      </c>
+      <c r="D362" s="17" t="s">
         <v>692</v>
       </c>
-      <c r="D359" s="17" t="s">
-        <v>721</v>
-      </c>
-      <c r="F359"/>
-    </row>
-    <row r="360" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A360" s="20"/>
-      <c r="B360" s="20"/>
-      <c r="C360" s="18" t="s">
-        <v>693</v>
-      </c>
-      <c r="D360" s="17" t="s">
-        <v>722</v>
-      </c>
-      <c r="F360"/>
-    </row>
-    <row r="361" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A361" s="20" t="s">
-        <v>485</v>
-      </c>
-      <c r="B361" s="20" t="s">
+      <c r="F362"/>
+    </row>
+    <row r="363" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A363" s="20"/>
+      <c r="B363" s="20"/>
+      <c r="C363" s="18" t="s">
         <v>694</v>
       </c>
-      <c r="C361" s="18" t="s">
+      <c r="D363" s="17" t="s">
+        <v>695</v>
+      </c>
+      <c r="F363"/>
+    </row>
+    <row r="364" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A364" s="17" t="s">
+        <v>483</v>
+      </c>
+      <c r="B364" s="17" t="s">
         <v>696</v>
       </c>
-      <c r="D361" s="17" t="s">
-        <v>695</v>
-      </c>
-      <c r="F361"/>
-    </row>
-    <row r="362" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A362" s="20"/>
-      <c r="B362" s="20"/>
-      <c r="C362" s="18" t="s">
+      <c r="C364" s="18" t="s">
+        <v>698</v>
+      </c>
+      <c r="D364" s="17" t="s">
         <v>697</v>
       </c>
-      <c r="D362" s="17" t="s">
-        <v>698</v>
-      </c>
-      <c r="F362"/>
-    </row>
-    <row r="363" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A363" s="17" t="s">
-        <v>485</v>
-      </c>
-      <c r="B363" s="17" t="s">
+      <c r="F364"/>
+    </row>
+    <row r="365" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A365" s="20" t="s">
+        <v>483</v>
+      </c>
+      <c r="B365" s="20" t="s">
+        <v>687</v>
+      </c>
+      <c r="C365" s="19" t="s">
+        <v>702</v>
+      </c>
+      <c r="D365" s="19" t="s">
         <v>699</v>
       </c>
-      <c r="C363" s="18" t="s">
-        <v>701</v>
-      </c>
-      <c r="D363" s="17" t="s">
-        <v>700</v>
-      </c>
-      <c r="F363"/>
-    </row>
-    <row r="364" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A364" s="20" t="s">
-        <v>485</v>
-      </c>
-      <c r="B364" s="20" t="s">
-        <v>690</v>
-      </c>
-      <c r="C364" s="19" t="s">
-        <v>705</v>
-      </c>
-      <c r="D364" s="19" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A365" s="20"/>
-      <c r="B365" s="20"/>
-      <c r="C365" s="19"/>
-      <c r="D365" s="20"/>
     </row>
     <row r="366" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A366" s="20"/>
@@ -7290,11 +7363,11 @@
       <c r="C369" s="19"/>
       <c r="D369" s="20"/>
     </row>
-    <row r="370" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A370" s="20"/>
       <c r="B370" s="20"/>
       <c r="C370" s="19"/>
-      <c r="F370"/>
+      <c r="D370" s="20"/>
     </row>
     <row r="371" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A371" s="20"/>
@@ -7302,254 +7375,357 @@
       <c r="C371" s="19"/>
       <c r="F371"/>
     </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A372" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="B372" s="17" t="s">
-        <v>703</v>
-      </c>
-      <c r="C372" s="18"/>
-      <c r="D372" s="1" t="s">
-        <v>704</v>
-      </c>
-      <c r="E372" s="12" t="s">
-        <v>708</v>
-      </c>
+    <row r="372" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A372" s="20"/>
+      <c r="B372" s="20"/>
+      <c r="C372" s="19"/>
+      <c r="F372"/>
     </row>
     <row r="373" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A373" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="B373" s="1" t="s">
-        <v>706</v>
+        <v>505</v>
+      </c>
+      <c r="B373" s="17" t="s">
+        <v>700</v>
       </c>
       <c r="C373" s="18"/>
       <c r="D373" s="1" t="s">
-        <v>707</v>
+        <v>701</v>
+      </c>
+      <c r="E373" s="12" t="s">
+        <v>705</v>
       </c>
     </row>
     <row r="374" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A374" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="B374" s="17" t="s">
-        <v>709</v>
+        <v>483</v>
+      </c>
+      <c r="B374" s="1" t="s">
+        <v>703</v>
       </c>
       <c r="C374" s="18"/>
       <c r="D374" s="1" t="s">
-        <v>710</v>
+        <v>704</v>
       </c>
     </row>
     <row r="375" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A375" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B375" s="1" t="s">
-        <v>723</v>
-      </c>
-      <c r="C375" s="17" t="s">
-        <v>724</v>
-      </c>
+        <v>541</v>
+      </c>
+      <c r="B375" s="17" t="s">
+        <v>706</v>
+      </c>
+      <c r="C375" s="18"/>
       <c r="D375" s="1" t="s">
-        <v>725</v>
+        <v>707</v>
       </c>
     </row>
     <row r="376" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A376" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B376" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="C376" s="17" t="s">
+        <v>721</v>
+      </c>
+      <c r="D376" s="1" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A377" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="B377" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="C377" s="17" t="s">
+        <v>725</v>
+      </c>
+      <c r="D377" s="1" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A378" s="17" t="s">
+        <v>724</v>
+      </c>
+      <c r="B378" s="1" t="s">
         <v>727</v>
       </c>
-      <c r="B376" s="1" t="s">
-        <v>726</v>
-      </c>
-      <c r="C376" s="17" t="s">
+      <c r="C378" s="17" t="s">
         <v>728</v>
       </c>
-      <c r="D376" s="1" t="s">
+      <c r="D378" s="1" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C377" s="17"/>
-    </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C378" s="17"/>
-    </row>
     <row r="379" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C379" s="17"/>
+      <c r="A379" s="17" t="s">
+        <v>724</v>
+      </c>
+      <c r="B379" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="C379" s="17" t="s">
+        <v>735</v>
+      </c>
+      <c r="D379" s="1" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A380" s="20" t="s">
+        <v>724</v>
+      </c>
+      <c r="B380" s="20" t="s">
+        <v>737</v>
+      </c>
+      <c r="C380" s="19" t="s">
+        <v>738</v>
+      </c>
+      <c r="D380" s="19" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A381" s="20"/>
+      <c r="B381" s="20"/>
+      <c r="C381" s="20"/>
+      <c r="D381" s="20"/>
+    </row>
+    <row r="382" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A382" s="20" t="s">
+        <v>742</v>
+      </c>
+      <c r="B382" s="20" t="s">
+        <v>741</v>
+      </c>
+      <c r="C382" s="19" t="s">
+        <v>743</v>
+      </c>
+      <c r="D382" s="20" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A383" s="20"/>
+      <c r="B383" s="20"/>
+      <c r="C383" s="19"/>
+      <c r="D383" s="20"/>
+    </row>
+    <row r="384" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A384" s="20"/>
+      <c r="B384" s="20"/>
+      <c r="C384" s="19"/>
+      <c r="D384" s="20"/>
+    </row>
+    <row r="385" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A385" s="20"/>
+      <c r="B385" s="20"/>
+      <c r="C385" s="19"/>
+      <c r="D385" s="20"/>
+    </row>
+    <row r="386" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A386" s="20"/>
+      <c r="B386" s="20"/>
+      <c r="C386" s="19"/>
+      <c r="D386" s="20"/>
+    </row>
+    <row r="387" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A387" s="20"/>
+      <c r="B387" s="20"/>
+      <c r="C387" s="19"/>
+      <c r="D387" s="20"/>
+    </row>
+    <row r="388" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A388" s="20"/>
+      <c r="B388" s="20"/>
+      <c r="C388" s="19"/>
+      <c r="D388" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="228">
-    <mergeCell ref="D364:D369"/>
-    <mergeCell ref="C364:C371"/>
-    <mergeCell ref="B364:B371"/>
-    <mergeCell ref="A364:A371"/>
-    <mergeCell ref="B359:B360"/>
-    <mergeCell ref="A359:A360"/>
-    <mergeCell ref="B361:B362"/>
-    <mergeCell ref="A361:A362"/>
-    <mergeCell ref="C356:C358"/>
-    <mergeCell ref="D356:D358"/>
-    <mergeCell ref="B356:B358"/>
-    <mergeCell ref="A356:A358"/>
-    <mergeCell ref="C344:C353"/>
-    <mergeCell ref="B344:B353"/>
-    <mergeCell ref="A344:A353"/>
-    <mergeCell ref="D344:D353"/>
-    <mergeCell ref="E319:E328"/>
-    <mergeCell ref="C336:C343"/>
-    <mergeCell ref="B336:B343"/>
-    <mergeCell ref="A336:A343"/>
-    <mergeCell ref="D336:D343"/>
-    <mergeCell ref="C329:C335"/>
-    <mergeCell ref="B329:B335"/>
-    <mergeCell ref="A329:A335"/>
-    <mergeCell ref="D329:D335"/>
-    <mergeCell ref="E336:E343"/>
-    <mergeCell ref="C319:C328"/>
-    <mergeCell ref="B319:B328"/>
-    <mergeCell ref="A319:A328"/>
-    <mergeCell ref="D319:D328"/>
-    <mergeCell ref="C310:C318"/>
-    <mergeCell ref="B310:B318"/>
-    <mergeCell ref="A310:A318"/>
-    <mergeCell ref="D310:D318"/>
-    <mergeCell ref="C304:C306"/>
-    <mergeCell ref="B304:B306"/>
-    <mergeCell ref="A304:A306"/>
-    <mergeCell ref="C307:C309"/>
-    <mergeCell ref="B307:B309"/>
-    <mergeCell ref="A307:A309"/>
-    <mergeCell ref="D307:D309"/>
-    <mergeCell ref="A299:A301"/>
-    <mergeCell ref="D302:D303"/>
-    <mergeCell ref="B302:B303"/>
-    <mergeCell ref="A302:A303"/>
-    <mergeCell ref="C216:C217"/>
-    <mergeCell ref="D216:D217"/>
-    <mergeCell ref="C290:C291"/>
-    <mergeCell ref="D290:D291"/>
-    <mergeCell ref="B239:B291"/>
-    <mergeCell ref="A239:A291"/>
-    <mergeCell ref="D295:D298"/>
-    <mergeCell ref="C295:C298"/>
-    <mergeCell ref="B295:B298"/>
-    <mergeCell ref="D299:D301"/>
-    <mergeCell ref="C299:C301"/>
-    <mergeCell ref="B299:B301"/>
-    <mergeCell ref="A295:A298"/>
-    <mergeCell ref="A184:A185"/>
-    <mergeCell ref="B184:B185"/>
-    <mergeCell ref="C283:C289"/>
-    <mergeCell ref="D292:D294"/>
-    <mergeCell ref="D283:D289"/>
-    <mergeCell ref="C292:C294"/>
-    <mergeCell ref="B292:B294"/>
-    <mergeCell ref="A292:A294"/>
-    <mergeCell ref="C271:C274"/>
-    <mergeCell ref="D271:D274"/>
-    <mergeCell ref="C275:C278"/>
-    <mergeCell ref="D275:D278"/>
-    <mergeCell ref="C279:C282"/>
-    <mergeCell ref="D279:D282"/>
-    <mergeCell ref="C268:C270"/>
-    <mergeCell ref="D268:D270"/>
-    <mergeCell ref="C261:C263"/>
-    <mergeCell ref="D261:D263"/>
-    <mergeCell ref="C264:C267"/>
-    <mergeCell ref="D264:D267"/>
-    <mergeCell ref="C252:C254"/>
-    <mergeCell ref="D252:D254"/>
-    <mergeCell ref="C258:C260"/>
-    <mergeCell ref="D258:D260"/>
-    <mergeCell ref="C255:C257"/>
-    <mergeCell ref="D255:D257"/>
-    <mergeCell ref="C246:C247"/>
-    <mergeCell ref="D243:D245"/>
-    <mergeCell ref="D246:D247"/>
-    <mergeCell ref="C248:C249"/>
-    <mergeCell ref="C250:C251"/>
-    <mergeCell ref="D248:D249"/>
-    <mergeCell ref="D250:D251"/>
-    <mergeCell ref="C239:C240"/>
-    <mergeCell ref="D239:D240"/>
-    <mergeCell ref="C241:C242"/>
-    <mergeCell ref="D241:D242"/>
-    <mergeCell ref="C243:C245"/>
-    <mergeCell ref="C233:C235"/>
-    <mergeCell ref="D233:D235"/>
-    <mergeCell ref="C236:C238"/>
-    <mergeCell ref="D236:D238"/>
-    <mergeCell ref="C229:C230"/>
-    <mergeCell ref="D229:D230"/>
-    <mergeCell ref="C231:C232"/>
-    <mergeCell ref="D231:D232"/>
-    <mergeCell ref="C219:C220"/>
-    <mergeCell ref="D219:D220"/>
-    <mergeCell ref="C221:C222"/>
-    <mergeCell ref="D221:D222"/>
-    <mergeCell ref="C223:C224"/>
-    <mergeCell ref="D223:D224"/>
-    <mergeCell ref="C225:C227"/>
-    <mergeCell ref="D225:D227"/>
-    <mergeCell ref="C203:C210"/>
-    <mergeCell ref="B190:B210"/>
-    <mergeCell ref="A190:A210"/>
-    <mergeCell ref="D203:D210"/>
-    <mergeCell ref="C214:C215"/>
-    <mergeCell ref="D214:D215"/>
-    <mergeCell ref="C212:C213"/>
-    <mergeCell ref="D212:D213"/>
-    <mergeCell ref="B211:B238"/>
-    <mergeCell ref="A211:A238"/>
-    <mergeCell ref="C193:C194"/>
-    <mergeCell ref="D193:D194"/>
+  <mergeCells count="236">
+    <mergeCell ref="C380:C381"/>
+    <mergeCell ref="B380:B381"/>
+    <mergeCell ref="A380:A381"/>
+    <mergeCell ref="D380:D381"/>
+    <mergeCell ref="C382:C388"/>
+    <mergeCell ref="A382:A388"/>
+    <mergeCell ref="B382:B388"/>
+    <mergeCell ref="D382:D388"/>
+    <mergeCell ref="D365:D370"/>
+    <mergeCell ref="C365:C372"/>
+    <mergeCell ref="B365:B372"/>
+    <mergeCell ref="A365:A372"/>
+    <mergeCell ref="B360:B361"/>
+    <mergeCell ref="A360:A361"/>
+    <mergeCell ref="B362:B363"/>
+    <mergeCell ref="A362:A363"/>
+    <mergeCell ref="C357:C359"/>
+    <mergeCell ref="D357:D359"/>
+    <mergeCell ref="B357:B359"/>
+    <mergeCell ref="A357:A359"/>
+    <mergeCell ref="C345:C354"/>
+    <mergeCell ref="B345:B354"/>
+    <mergeCell ref="A345:A354"/>
+    <mergeCell ref="D345:D354"/>
+    <mergeCell ref="E320:E329"/>
+    <mergeCell ref="C337:C344"/>
+    <mergeCell ref="B337:B344"/>
+    <mergeCell ref="A337:A344"/>
+    <mergeCell ref="D337:D344"/>
+    <mergeCell ref="C330:C336"/>
+    <mergeCell ref="B330:B336"/>
+    <mergeCell ref="A330:A336"/>
+    <mergeCell ref="D330:D336"/>
+    <mergeCell ref="E337:E344"/>
+    <mergeCell ref="C320:C329"/>
+    <mergeCell ref="B320:B329"/>
+    <mergeCell ref="A320:A329"/>
+    <mergeCell ref="D320:D329"/>
+    <mergeCell ref="C311:C319"/>
+    <mergeCell ref="B311:B319"/>
+    <mergeCell ref="A311:A319"/>
+    <mergeCell ref="D311:D319"/>
+    <mergeCell ref="C305:C307"/>
+    <mergeCell ref="B305:B307"/>
+    <mergeCell ref="A305:A307"/>
+    <mergeCell ref="C308:C310"/>
+    <mergeCell ref="B308:B310"/>
+    <mergeCell ref="A308:A310"/>
+    <mergeCell ref="D308:D310"/>
+    <mergeCell ref="A300:A302"/>
+    <mergeCell ref="D303:D304"/>
+    <mergeCell ref="B303:B304"/>
+    <mergeCell ref="A303:A304"/>
+    <mergeCell ref="C217:C218"/>
+    <mergeCell ref="D217:D218"/>
+    <mergeCell ref="C291:C292"/>
+    <mergeCell ref="D291:D292"/>
+    <mergeCell ref="B240:B292"/>
+    <mergeCell ref="A240:A292"/>
+    <mergeCell ref="D296:D299"/>
+    <mergeCell ref="C296:C299"/>
+    <mergeCell ref="B296:B299"/>
+    <mergeCell ref="D300:D302"/>
+    <mergeCell ref="C300:C302"/>
+    <mergeCell ref="B300:B302"/>
+    <mergeCell ref="A296:A299"/>
+    <mergeCell ref="A185:A186"/>
+    <mergeCell ref="B185:B186"/>
+    <mergeCell ref="C284:C290"/>
+    <mergeCell ref="D293:D295"/>
+    <mergeCell ref="D284:D290"/>
+    <mergeCell ref="C293:C295"/>
+    <mergeCell ref="B293:B295"/>
+    <mergeCell ref="A293:A295"/>
+    <mergeCell ref="C272:C275"/>
+    <mergeCell ref="D272:D275"/>
+    <mergeCell ref="C276:C279"/>
+    <mergeCell ref="D276:D279"/>
+    <mergeCell ref="C280:C283"/>
+    <mergeCell ref="D280:D283"/>
+    <mergeCell ref="C269:C271"/>
+    <mergeCell ref="D269:D271"/>
+    <mergeCell ref="C262:C264"/>
+    <mergeCell ref="D262:D264"/>
+    <mergeCell ref="C265:C268"/>
+    <mergeCell ref="D265:D268"/>
+    <mergeCell ref="C253:C255"/>
+    <mergeCell ref="D253:D255"/>
+    <mergeCell ref="C259:C261"/>
+    <mergeCell ref="D259:D261"/>
+    <mergeCell ref="C256:C258"/>
+    <mergeCell ref="D256:D258"/>
+    <mergeCell ref="C247:C248"/>
+    <mergeCell ref="D244:D246"/>
+    <mergeCell ref="D247:D248"/>
+    <mergeCell ref="C249:C250"/>
+    <mergeCell ref="C251:C252"/>
+    <mergeCell ref="D249:D250"/>
+    <mergeCell ref="D251:D252"/>
+    <mergeCell ref="C240:C241"/>
+    <mergeCell ref="D240:D241"/>
+    <mergeCell ref="C242:C243"/>
+    <mergeCell ref="D242:D243"/>
+    <mergeCell ref="C244:C246"/>
+    <mergeCell ref="C234:C236"/>
+    <mergeCell ref="D234:D236"/>
+    <mergeCell ref="C237:C239"/>
+    <mergeCell ref="D237:D239"/>
+    <mergeCell ref="C230:C231"/>
+    <mergeCell ref="D230:D231"/>
+    <mergeCell ref="C232:C233"/>
+    <mergeCell ref="D232:D233"/>
+    <mergeCell ref="C220:C221"/>
+    <mergeCell ref="D220:D221"/>
+    <mergeCell ref="C222:C223"/>
+    <mergeCell ref="D222:D223"/>
+    <mergeCell ref="C224:C225"/>
+    <mergeCell ref="D224:D225"/>
+    <mergeCell ref="C226:C228"/>
+    <mergeCell ref="D226:D228"/>
+    <mergeCell ref="C204:C211"/>
+    <mergeCell ref="B191:B211"/>
+    <mergeCell ref="A191:A211"/>
+    <mergeCell ref="D204:D211"/>
+    <mergeCell ref="C215:C216"/>
+    <mergeCell ref="D215:D216"/>
+    <mergeCell ref="C213:C214"/>
+    <mergeCell ref="D213:D214"/>
+    <mergeCell ref="B212:B239"/>
+    <mergeCell ref="A212:A239"/>
+    <mergeCell ref="C194:C195"/>
+    <mergeCell ref="D194:D195"/>
     <mergeCell ref="A133:A134"/>
     <mergeCell ref="B133:B134"/>
-    <mergeCell ref="C195:C202"/>
-    <mergeCell ref="D195:D202"/>
-    <mergeCell ref="C187:C188"/>
-    <mergeCell ref="B187:B188"/>
-    <mergeCell ref="A187:A188"/>
-    <mergeCell ref="D187:D188"/>
-    <mergeCell ref="D171:D174"/>
-    <mergeCell ref="C178:C181"/>
-    <mergeCell ref="B178:B181"/>
-    <mergeCell ref="A178:A181"/>
-    <mergeCell ref="D178:D181"/>
-    <mergeCell ref="B169:B170"/>
-    <mergeCell ref="A169:A170"/>
-    <mergeCell ref="C171:C174"/>
-    <mergeCell ref="B171:B174"/>
-    <mergeCell ref="A171:A174"/>
-    <mergeCell ref="D156:D160"/>
-    <mergeCell ref="C161:C167"/>
-    <mergeCell ref="A161:A167"/>
-    <mergeCell ref="B161:B167"/>
-    <mergeCell ref="D161:D167"/>
-    <mergeCell ref="C156:C160"/>
-    <mergeCell ref="B154:B160"/>
-    <mergeCell ref="A154:A160"/>
-    <mergeCell ref="B151:B153"/>
-    <mergeCell ref="A151:A153"/>
-    <mergeCell ref="D146:D149"/>
-    <mergeCell ref="C151:C152"/>
-    <mergeCell ref="D151:D152"/>
-    <mergeCell ref="C146:C149"/>
-    <mergeCell ref="B146:B149"/>
-    <mergeCell ref="A146:A149"/>
-    <mergeCell ref="C141:C142"/>
-    <mergeCell ref="A144:A145"/>
-    <mergeCell ref="B144:B145"/>
-    <mergeCell ref="C144:C145"/>
-    <mergeCell ref="D144:D145"/>
-    <mergeCell ref="B141:B143"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="D141:D143"/>
-    <mergeCell ref="C190:C191"/>
-    <mergeCell ref="D190:D191"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="B139:B140"/>
+    <mergeCell ref="C196:C203"/>
+    <mergeCell ref="D196:D203"/>
+    <mergeCell ref="A139:A141"/>
+    <mergeCell ref="B139:B141"/>
+    <mergeCell ref="C188:C189"/>
+    <mergeCell ref="B188:B189"/>
+    <mergeCell ref="A188:A189"/>
+    <mergeCell ref="D188:D189"/>
+    <mergeCell ref="D172:D175"/>
+    <mergeCell ref="C179:C182"/>
+    <mergeCell ref="B179:B182"/>
+    <mergeCell ref="A179:A182"/>
+    <mergeCell ref="D179:D182"/>
+    <mergeCell ref="B170:B171"/>
+    <mergeCell ref="A170:A171"/>
+    <mergeCell ref="C172:C175"/>
+    <mergeCell ref="B172:B175"/>
+    <mergeCell ref="A172:A175"/>
+    <mergeCell ref="D157:D161"/>
+    <mergeCell ref="C162:C168"/>
+    <mergeCell ref="A162:A168"/>
+    <mergeCell ref="B162:B168"/>
+    <mergeCell ref="D162:D168"/>
+    <mergeCell ref="C157:C161"/>
+    <mergeCell ref="B155:B161"/>
+    <mergeCell ref="A155:A161"/>
+    <mergeCell ref="B152:B154"/>
+    <mergeCell ref="A152:A154"/>
+    <mergeCell ref="D147:D150"/>
+    <mergeCell ref="C152:C153"/>
+    <mergeCell ref="D152:D153"/>
+    <mergeCell ref="C147:C150"/>
+    <mergeCell ref="B147:B150"/>
+    <mergeCell ref="A147:A150"/>
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="A145:A146"/>
+    <mergeCell ref="B145:B146"/>
+    <mergeCell ref="C145:C146"/>
+    <mergeCell ref="D145:D146"/>
+    <mergeCell ref="B142:B144"/>
+    <mergeCell ref="A142:A144"/>
+    <mergeCell ref="D142:D144"/>
+    <mergeCell ref="C191:C192"/>
+    <mergeCell ref="D191:D192"/>
     <mergeCell ref="C139:C140"/>
     <mergeCell ref="D139:D140"/>
     <mergeCell ref="A112:A114"/>
@@ -7614,10 +7790,10 @@
     <hyperlink ref="E11" r:id="rId1"/>
     <hyperlink ref="E95" r:id="rId2"/>
     <hyperlink ref="E107" r:id="rId3"/>
-    <hyperlink ref="E211" r:id="rId4"/>
-    <hyperlink ref="E319" r:id="rId5"/>
-    <hyperlink ref="E336" r:id="rId6" location="clustering"/>
-    <hyperlink ref="E372" r:id="rId7"/>
+    <hyperlink ref="E212" r:id="rId4"/>
+    <hyperlink ref="E320" r:id="rId5"/>
+    <hyperlink ref="E337" r:id="rId6" location="clustering"/>
+    <hyperlink ref="E373" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8328,7 +8504,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>447</v>
@@ -8339,7 +8515,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>449</v>
@@ -8350,21 +8526,21 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
+        <v>454</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>456</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>458</v>
-      </c>
       <c r="C3" s="17" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update on 20190103.2239 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="3120" yWindow="6640" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RCommands" sheetId="1" r:id="rId1"/>
-    <sheet name="GitCommands" sheetId="2" r:id="rId2"/>
-    <sheet name="ShellCommands" sheetId="3" r:id="rId3"/>
-    <sheet name="PythonCommands" sheetId="4" r:id="rId4"/>
-    <sheet name="HPCCommands" sheetId="6" r:id="rId5"/>
-    <sheet name="Date Source Link" sheetId="5" r:id="rId6"/>
-    <sheet name="Learning Sources" sheetId="7" r:id="rId7"/>
+    <sheet name="Markdown" sheetId="8" r:id="rId2"/>
+    <sheet name="GitCommands" sheetId="2" r:id="rId3"/>
+    <sheet name="ShellCommands" sheetId="3" r:id="rId4"/>
+    <sheet name="PythonCommands" sheetId="4" r:id="rId5"/>
+    <sheet name="HPCCommands" sheetId="6" r:id="rId6"/>
+    <sheet name="Date Source Link" sheetId="5" r:id="rId7"/>
+    <sheet name="Learning Sources" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RCommands!$A$1:$A$399</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RCommands!$A$1:$A$400</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="801">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3242,12 +3243,310 @@
     <t>summarize_all()</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Syntax</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Descriptions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Example</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*This text will appear italicized!*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">make text italic: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>This text will appear italicized!</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>**</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>**This text will appear bold!**</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">make text bold: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>This text will appear bold!</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>##</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>## This is a secondary heading</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>###</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>### This is a tertiary heading</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># This is a main heading</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">make a secondary heading (H2): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>This is a secondary heading</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">make a tertiary heading (H3): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>This is a tertiary head</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">make a main heading (H1): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>This is a main heading</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"- first item in list
+- second item in list
+- third item in list"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no quote when using this syntax, it returns an unordered list
+- first item in list
+- second item in list
+- third item in list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Font</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heading</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heading</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unordered list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ordered list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. first item in list
+2. second item in list
+3. third item in list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>returns an ordered list
+1. first item in list
+2. second item in list
+3. third item in list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>["text"]("link")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Rstudio](http://www.rstudio.com/)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rstudio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linking</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linking</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I spend so much time reading [R bloggers][1] and [Simply Statistics][2]!
+[1]: http://www.r-bloggers.com/ "R bloggers"
+[2]: http://simplystatistics.org/ "Simply statistics"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create multiple links:
+I spend so much time reading </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="14"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>R bloggers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="14"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Simply Statistics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>!</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Newlines</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[SPACE][SPACE]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>First line[SPACE][SPACE]Second line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>First line
+Second line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learning Sources</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Github's Markdown Guide: https://guides.github.com/features/mastering-markdown/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: knitr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R markdown can be converted to standard markdown using the knitr package in R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: markdown</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Markdown can be converted to HTML using the markdown package in R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: slidify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R markdown can be converted to slides using the slidify package</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3281,6 +3580,39 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color rgb="FF00B0F0"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -3645,10 +3977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F399"/>
+  <dimension ref="A1:F400"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A373" workbookViewId="0">
-      <selection activeCell="B399" sqref="B399"/>
+    <sheetView tabSelected="1" topLeftCell="A387" workbookViewId="0">
+      <selection activeCell="B391" sqref="B391:B397"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -7997,7 +8329,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="385" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A385" s="1" t="s">
         <v>466</v>
       </c>
@@ -8011,7 +8343,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="386" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A386" s="1" t="s">
         <v>710</v>
       </c>
@@ -8025,7 +8357,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="387" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A387" s="15" t="s">
         <v>710</v>
       </c>
@@ -8039,7 +8371,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="388" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A388" s="15" t="s">
         <v>710</v>
       </c>
@@ -8053,7 +8385,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="389" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A389" s="15" t="s">
         <v>710</v>
       </c>
@@ -8067,7 +8399,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="390" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A390" s="15" t="s">
         <v>710</v>
       </c>
@@ -8075,7 +8407,7 @@
       <c r="C390" s="18"/>
       <c r="D390" s="18"/>
     </row>
-    <row r="391" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A391" s="15" t="s">
         <v>727</v>
       </c>
@@ -8089,7 +8421,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="392" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A392" s="15" t="s">
         <v>727</v>
       </c>
@@ -8097,7 +8429,7 @@
       <c r="C392" s="17"/>
       <c r="D392" s="18"/>
     </row>
-    <row r="393" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A393" s="15" t="s">
         <v>727</v>
       </c>
@@ -8105,7 +8437,7 @@
       <c r="C393" s="17"/>
       <c r="D393" s="18"/>
     </row>
-    <row r="394" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A394" s="15" t="s">
         <v>727</v>
       </c>
@@ -8113,7 +8445,7 @@
       <c r="C394" s="17"/>
       <c r="D394" s="18"/>
     </row>
-    <row r="395" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A395" s="15" t="s">
         <v>727</v>
       </c>
@@ -8121,7 +8453,7 @@
       <c r="C395" s="17"/>
       <c r="D395" s="18"/>
     </row>
-    <row r="396" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A396" s="15" t="s">
         <v>727</v>
       </c>
@@ -8129,7 +8461,7 @@
       <c r="C396" s="17"/>
       <c r="D396" s="18"/>
     </row>
-    <row r="397" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A397" s="15" t="s">
         <v>727</v>
       </c>
@@ -8137,15 +8469,46 @@
       <c r="C397" s="17"/>
       <c r="D397" s="18"/>
     </row>
-    <row r="399" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C399" s="11" t="s">
+    <row r="398" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A398" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B398" s="18" t="s">
+        <v>796</v>
+      </c>
+      <c r="C398" s="18"/>
+      <c r="D398" s="18"/>
+      <c r="E398" s="11" t="s">
         <v>731</v>
       </c>
     </row>
+    <row r="399" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A399" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="B399" s="18" t="s">
+        <v>798</v>
+      </c>
+      <c r="C399" s="18"/>
+      <c r="D399" s="18"/>
+    </row>
+    <row r="400" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A400" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="B400" s="18" t="s">
+        <v>800</v>
+      </c>
+      <c r="C400" s="18"/>
+      <c r="D400" s="18"/>
+    </row>
   </sheetData>
-  <mergeCells count="194">
+  <mergeCells count="197">
     <mergeCell ref="D135:D136"/>
     <mergeCell ref="B135:B136"/>
+    <mergeCell ref="B398:D398"/>
+    <mergeCell ref="B399:D399"/>
+    <mergeCell ref="B400:D400"/>
     <mergeCell ref="D60:D62"/>
     <mergeCell ref="C60:C62"/>
     <mergeCell ref="B60:B62"/>
@@ -8348,13 +8711,284 @@
     <hyperlink ref="E329" r:id="rId5"/>
     <hyperlink ref="E346" r:id="rId6" location="clustering"/>
     <hyperlink ref="E382" r:id="rId7"/>
-    <hyperlink ref="C399" r:id="rId8"/>
+    <hyperlink ref="E398" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.1640625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="73.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>773</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>752</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>754</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>753</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>774</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>756</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>774</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>758</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>759</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>760</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="25" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>775</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>765</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>766</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>776</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>761</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>762</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>776</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>763</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>764</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>777</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>770</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>771</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>777</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>777</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>777</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>778</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>779</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>780</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
+        <v>778</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
+        <v>778</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
+        <v>778</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>785</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>782</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>783</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="17" t="s">
+        <v>787</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="15" t="s">
+        <v>789</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>790</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>791</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
+        <v>789</v>
+      </c>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="B7:B10"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D15" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
@@ -8490,7 +9124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
@@ -8770,7 +9404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -8805,7 +9439,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -8858,7 +9492,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
@@ -9041,7 +9675,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update on 20190120.1619 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2540" yWindow="1600" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="R" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="837">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3602,15 +3602,574 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Commands</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Example</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Description</t>
+    <t>Database Management System (DBMS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQLite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>retrive column prod_name, prod_id, prod_price from table Products</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>retrive all columns from table Products</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>retrive only the first 5 records' column prod_name from table Products</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oracle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> prod_name, prod_id, prod_price </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Products;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> * </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Products;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> prod_name </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Products </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>WHERE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>ROWNUM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;= 5;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> prod_name </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Products </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>FETCH FIRST 5 ROWS ONLY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> prod_name </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Products </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>LIMIT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> 5;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Statement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Explanation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>CREATE TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Shoes
+(
+ID        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>char(10)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>PRIMARY KEY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">,
+Brand  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>char(10)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>NOT NULL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">,
+Type    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>char(250)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>NOT NULL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">,
+color    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>char(250)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>NOT NULL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">,
+Price    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>decimal(8,2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>NOT NULL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">,
+Desc    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Varchar(750)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>NULL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">
+);</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create a table and assign the column names as well as the value type for each column
+Primary Key: must not be NULL or empty value
+NOT NULL: must not be NULL, but can be empty value
+NULL: NULL is accepted</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INSERT INTO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>INSERT INTO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Shoes
+              (Id
+              ,Brand
+              ,Type
+              ,Color
+              ,Price
+              Desc
+              )
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>VALUES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">
+              ('14535974'
+              ,'Gucci'
+              ,'Slippers'
+              ,'Pink'
+              ,'695.00'
+              NULL
+              );</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Insert a record into table Shoes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3618,7 +4177,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3687,6 +4246,11 @@
       <color rgb="FF00B0F0"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="5"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3709,7 +4273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3779,6 +4343,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8886,40 +9456,323 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="19"/>
-    <col min="2" max="2" width="13.33203125" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="19"/>
-    <col min="4" max="4" width="13.1640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.5" style="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" style="19" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>8</v>
+        <v>816</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>829</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>815</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>816</v>
-      </c>
       <c r="D1" s="19" t="s">
-        <v>817</v>
+        <v>830</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>818</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>824</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="19" t="s">
+        <v>825</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="19" t="s">
+        <v>828</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>822</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="19" t="s">
+        <v>826</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>823</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="19" t="s">
+        <v>827</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>831</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>832</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="20"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="20"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="20"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="20"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="20"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="20"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="20"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="20"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>834</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>835</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="20"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="20"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="20"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="20"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="20"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B22" s="20"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="20"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="20"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B24" s="20"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="20"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="20"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B26" s="20"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="20"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B27" s="20"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="20"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="20"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="20"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B30" s="20"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="20"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B31" s="20"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="20"/>
+    </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="C16:C31"/>
+    <mergeCell ref="B16:B31"/>
+    <mergeCell ref="D16:D31"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C7:C15"/>
+    <mergeCell ref="D7:D15"/>
+    <mergeCell ref="B7:B15"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update on 20190127.1410 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="R" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="868">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="878">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3635,245 +3635,6 @@
   </si>
   <si>
     <t>DB2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="5"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>SELECT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> prod_name, prod_id, prod_price </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="5"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>FROM</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Products;</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="5"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>SELECT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> * </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="5"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>FROM</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Products;</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="5"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>SELECT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> prod_name </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="5"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>FROM</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Products </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="5"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>WHERE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="5"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>ROWNUM</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;= 5;</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="5"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>SELECT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> prod_name </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="5"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>FROM</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Products </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="5"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>FETCH FIRST 5 ROWS ONLY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>;</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="5"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>SELECT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> prod_name </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="5"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>FROM</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Products </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="5"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>LIMIT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> 5;</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -4381,6 +4142,567 @@
     <t>objects()</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>SQLite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WHERE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> ProductName
+,UnitPrice
+,SupplierID
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Products
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>WHERE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> ProductName = 'Tofu';</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> prod_name
+,prod_id
+,prod_price
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Products;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> *
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Products;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> prod_name
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Products
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>LIMIT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> 5;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> prod_name
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Products
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>WHERE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>ROWNUM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;= 5;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> prod_name
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Products
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>FETCH FIRST 5 ROWS ONLY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> ProductName
+,UnitPrice
+,SupplierID
+,UnitsInStock
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Products
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>WHERE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> UnitsInStock </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>BETWEEN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> 15 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>AND</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> 80;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> ProductName
+,UnitPrice
+,SupplierID
+,UnitsInStock
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Products
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>WHERE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> ProductName </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>IS NULL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> ProductID
+,UnitPrice
+,SupplierID
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Products
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>WHERE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> SupplierID </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>IN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> (9, 10, 11);</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>only retrive column ProductName, UnitPrice, SuppliersID, UnitsInStock of the records whose ProductName is NULL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>only retrive column ProductName, UnitPrice, SuppliersID, UnitsInStock of the records whose UnitsInStock is between 15 and 80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>only retrive column ProductName, UnitPrice, SuppliersID
+of the records whose ProductName is 'Tofu'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>only retrive column ProductID, UnitPrice, SuppliersID
+of the records whose SuppliersID is equal to any number in (9,10,11)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -4469,10 +4791,80 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -4482,7 +4874,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4547,7 +4939,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4559,11 +4951,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4845,7 +5261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F416"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A402" workbookViewId="0">
+    <sheetView topLeftCell="A402" workbookViewId="0">
       <selection activeCell="A416" sqref="A416"/>
     </sheetView>
   </sheetViews>
@@ -5008,7 +5424,7 @@
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="26" t="s">
         <v>9</v>
       </c>
     </row>
@@ -5023,7 +5439,7 @@
       <c r="D12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="22"/>
+      <c r="E12" s="26"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
@@ -7317,13 +7733,13 @@
         <v>464</v>
       </c>
       <c r="B196" s="23" t="s">
-        <v>857</v>
+        <v>852</v>
       </c>
       <c r="C196" s="20" t="s">
-        <v>858</v>
+        <v>853</v>
       </c>
       <c r="D196" s="20" t="s">
-        <v>859</v>
+        <v>854</v>
       </c>
       <c r="F196"/>
     </row>
@@ -7333,10 +7749,10 @@
       </c>
       <c r="B197" s="23"/>
       <c r="C197" s="20" t="s">
-        <v>860</v>
+        <v>855</v>
       </c>
       <c r="D197" s="20" t="s">
-        <v>861</v>
+        <v>856</v>
       </c>
       <c r="F197"/>
     </row>
@@ -7346,10 +7762,10 @@
       </c>
       <c r="B198" s="23"/>
       <c r="C198" s="20" t="s">
-        <v>862</v>
+        <v>857</v>
       </c>
       <c r="D198" s="20" t="s">
-        <v>863</v>
+        <v>858</v>
       </c>
       <c r="F198"/>
     </row>
@@ -9488,84 +9904,264 @@
     </row>
     <row r="411" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A411" s="1" t="s">
-        <v>844</v>
+        <v>839</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>847</v>
+        <v>842</v>
       </c>
       <c r="C411" s="1" t="s">
-        <v>845</v>
+        <v>840</v>
       </c>
       <c r="D411" s="1" t="s">
-        <v>846</v>
+        <v>841</v>
       </c>
     </row>
     <row r="412" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A412" s="19" t="s">
+        <v>839</v>
+      </c>
+      <c r="B412" s="1" t="s">
         <v>844</v>
       </c>
-      <c r="B412" s="1" t="s">
-        <v>849</v>
-      </c>
       <c r="C412" s="1" t="s">
-        <v>851</v>
+        <v>846</v>
       </c>
       <c r="D412" s="1" t="s">
-        <v>852</v>
+        <v>847</v>
       </c>
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A413" s="19" t="s">
-        <v>844</v>
+        <v>839</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>850</v>
+        <v>845</v>
       </c>
       <c r="C413" s="1" t="s">
-        <v>853</v>
+        <v>848</v>
       </c>
       <c r="D413" s="1" t="s">
-        <v>854</v>
+        <v>849</v>
       </c>
     </row>
     <row r="414" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A414" s="19" t="s">
-        <v>844</v>
+        <v>839</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>848</v>
+        <v>843</v>
       </c>
       <c r="C414" s="1" t="s">
-        <v>855</v>
+        <v>850</v>
       </c>
       <c r="D414" s="1" t="s">
-        <v>856</v>
+        <v>851</v>
       </c>
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A415" s="1" t="s">
-        <v>864</v>
+        <v>859</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>865</v>
+        <v>860</v>
       </c>
       <c r="D415" s="1" t="s">
-        <v>866</v>
+        <v>861</v>
       </c>
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A416" s="21" t="s">
-        <v>864</v>
+        <v>859</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>867</v>
+        <v>862</v>
       </c>
       <c r="D416" s="21" t="s">
-        <v>866</v>
+        <v>861</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="204">
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="D27:D31"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D60:D62"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="C147:C148"/>
+    <mergeCell ref="D147:D148"/>
+    <mergeCell ref="D117:D119"/>
+    <mergeCell ref="D63:D65"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="C87:C95"/>
+    <mergeCell ref="B87:B95"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="D104:D106"/>
+    <mergeCell ref="B107:B108"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="B110:B111"/>
+    <mergeCell ref="C130:C131"/>
+    <mergeCell ref="D130:D131"/>
+    <mergeCell ref="B130:B131"/>
+    <mergeCell ref="D132:D134"/>
+    <mergeCell ref="C132:C134"/>
+    <mergeCell ref="B132:B134"/>
+    <mergeCell ref="B147:B149"/>
+    <mergeCell ref="B139:B142"/>
+    <mergeCell ref="C135:C136"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C150:C151"/>
+    <mergeCell ref="B153:B154"/>
+    <mergeCell ref="C153:C154"/>
+    <mergeCell ref="D153:D154"/>
+    <mergeCell ref="B150:B152"/>
+    <mergeCell ref="D150:D152"/>
+    <mergeCell ref="C203:C204"/>
+    <mergeCell ref="D203:D204"/>
+    <mergeCell ref="C160:C162"/>
+    <mergeCell ref="B160:B163"/>
+    <mergeCell ref="D160:D162"/>
+    <mergeCell ref="C200:C201"/>
+    <mergeCell ref="B200:B201"/>
+    <mergeCell ref="D200:D201"/>
+    <mergeCell ref="D181:D184"/>
+    <mergeCell ref="C188:C191"/>
+    <mergeCell ref="B188:B191"/>
+    <mergeCell ref="D188:D191"/>
+    <mergeCell ref="B179:B180"/>
+    <mergeCell ref="C181:C184"/>
+    <mergeCell ref="B181:B184"/>
+    <mergeCell ref="D166:D170"/>
+    <mergeCell ref="C171:C177"/>
+    <mergeCell ref="B171:B177"/>
+    <mergeCell ref="D171:D177"/>
+    <mergeCell ref="C166:C170"/>
+    <mergeCell ref="B164:B170"/>
+    <mergeCell ref="D155:D158"/>
+    <mergeCell ref="C155:C158"/>
+    <mergeCell ref="C216:C223"/>
+    <mergeCell ref="B203:B223"/>
+    <mergeCell ref="D216:D223"/>
+    <mergeCell ref="B194:B195"/>
+    <mergeCell ref="B155:B158"/>
+    <mergeCell ref="B196:B198"/>
+    <mergeCell ref="B224:B251"/>
+    <mergeCell ref="C206:C207"/>
+    <mergeCell ref="D206:D207"/>
+    <mergeCell ref="C208:C215"/>
+    <mergeCell ref="D208:D215"/>
+    <mergeCell ref="D246:D248"/>
+    <mergeCell ref="C249:C251"/>
+    <mergeCell ref="D249:D251"/>
+    <mergeCell ref="C242:C243"/>
+    <mergeCell ref="D242:D243"/>
+    <mergeCell ref="C244:C245"/>
+    <mergeCell ref="D244:D245"/>
+    <mergeCell ref="C232:C233"/>
+    <mergeCell ref="D232:D233"/>
+    <mergeCell ref="C234:C235"/>
+    <mergeCell ref="D234:D235"/>
+    <mergeCell ref="C236:C237"/>
+    <mergeCell ref="D236:D237"/>
+    <mergeCell ref="C238:C240"/>
+    <mergeCell ref="D238:D240"/>
+    <mergeCell ref="C284:C287"/>
+    <mergeCell ref="D284:D287"/>
+    <mergeCell ref="C288:C291"/>
+    <mergeCell ref="D288:D291"/>
+    <mergeCell ref="C292:C295"/>
+    <mergeCell ref="D292:D295"/>
+    <mergeCell ref="C227:C228"/>
+    <mergeCell ref="D227:D228"/>
+    <mergeCell ref="C225:C226"/>
+    <mergeCell ref="D225:D226"/>
+    <mergeCell ref="C246:C248"/>
+    <mergeCell ref="C281:C283"/>
+    <mergeCell ref="D281:D283"/>
+    <mergeCell ref="C274:C276"/>
+    <mergeCell ref="D274:D276"/>
+    <mergeCell ref="C277:C280"/>
+    <mergeCell ref="D277:D280"/>
+    <mergeCell ref="C265:C267"/>
+    <mergeCell ref="D265:D267"/>
+    <mergeCell ref="C271:C273"/>
+    <mergeCell ref="D271:D273"/>
+    <mergeCell ref="C268:C270"/>
+    <mergeCell ref="D268:D270"/>
+    <mergeCell ref="B252:B304"/>
+    <mergeCell ref="D308:D311"/>
+    <mergeCell ref="C308:C311"/>
+    <mergeCell ref="B308:B311"/>
+    <mergeCell ref="D312:D314"/>
+    <mergeCell ref="C312:C314"/>
+    <mergeCell ref="B312:B314"/>
+    <mergeCell ref="C259:C260"/>
+    <mergeCell ref="D256:D258"/>
+    <mergeCell ref="D259:D260"/>
+    <mergeCell ref="C261:C262"/>
+    <mergeCell ref="C263:C264"/>
+    <mergeCell ref="D261:D262"/>
+    <mergeCell ref="D263:D264"/>
+    <mergeCell ref="C252:C253"/>
+    <mergeCell ref="D252:D253"/>
+    <mergeCell ref="C254:C255"/>
+    <mergeCell ref="D254:D255"/>
+    <mergeCell ref="C256:C258"/>
+    <mergeCell ref="C296:C302"/>
+    <mergeCell ref="D305:D307"/>
+    <mergeCell ref="D296:D302"/>
+    <mergeCell ref="C305:C307"/>
+    <mergeCell ref="B305:B307"/>
+    <mergeCell ref="E332:E341"/>
+    <mergeCell ref="C349:C356"/>
+    <mergeCell ref="B349:B356"/>
+    <mergeCell ref="D349:D356"/>
+    <mergeCell ref="C342:C348"/>
+    <mergeCell ref="B342:B348"/>
+    <mergeCell ref="D342:D348"/>
+    <mergeCell ref="E349:E356"/>
+    <mergeCell ref="C332:C341"/>
+    <mergeCell ref="B332:B341"/>
+    <mergeCell ref="D332:D341"/>
+    <mergeCell ref="C317:C319"/>
+    <mergeCell ref="B407:B408"/>
+    <mergeCell ref="C407:C408"/>
+    <mergeCell ref="D407:D408"/>
+    <mergeCell ref="B404:B406"/>
+    <mergeCell ref="C404:C406"/>
+    <mergeCell ref="D404:D406"/>
+    <mergeCell ref="C392:C393"/>
+    <mergeCell ref="B392:B393"/>
+    <mergeCell ref="D392:D393"/>
+    <mergeCell ref="D377:D382"/>
+    <mergeCell ref="C377:C384"/>
+    <mergeCell ref="B377:B384"/>
+    <mergeCell ref="B372:B373"/>
+    <mergeCell ref="B374:B375"/>
+    <mergeCell ref="C369:C371"/>
+    <mergeCell ref="D369:D371"/>
+    <mergeCell ref="B369:B371"/>
     <mergeCell ref="D135:D136"/>
     <mergeCell ref="B135:B136"/>
     <mergeCell ref="B401:D401"/>
@@ -9590,186 +10186,6 @@
     <mergeCell ref="C323:C331"/>
     <mergeCell ref="B323:B331"/>
     <mergeCell ref="D323:D331"/>
-    <mergeCell ref="C317:C319"/>
-    <mergeCell ref="B407:B408"/>
-    <mergeCell ref="C407:C408"/>
-    <mergeCell ref="D407:D408"/>
-    <mergeCell ref="B404:B406"/>
-    <mergeCell ref="C404:C406"/>
-    <mergeCell ref="D404:D406"/>
-    <mergeCell ref="C392:C393"/>
-    <mergeCell ref="B392:B393"/>
-    <mergeCell ref="D392:D393"/>
-    <mergeCell ref="D377:D382"/>
-    <mergeCell ref="C377:C384"/>
-    <mergeCell ref="B377:B384"/>
-    <mergeCell ref="B372:B373"/>
-    <mergeCell ref="B374:B375"/>
-    <mergeCell ref="C369:C371"/>
-    <mergeCell ref="D369:D371"/>
-    <mergeCell ref="B369:B371"/>
-    <mergeCell ref="E332:E341"/>
-    <mergeCell ref="C349:C356"/>
-    <mergeCell ref="B349:B356"/>
-    <mergeCell ref="D349:D356"/>
-    <mergeCell ref="C342:C348"/>
-    <mergeCell ref="B342:B348"/>
-    <mergeCell ref="D342:D348"/>
-    <mergeCell ref="E349:E356"/>
-    <mergeCell ref="C332:C341"/>
-    <mergeCell ref="B332:B341"/>
-    <mergeCell ref="D332:D341"/>
-    <mergeCell ref="B252:B304"/>
-    <mergeCell ref="D308:D311"/>
-    <mergeCell ref="C308:C311"/>
-    <mergeCell ref="B308:B311"/>
-    <mergeCell ref="D312:D314"/>
-    <mergeCell ref="C312:C314"/>
-    <mergeCell ref="B312:B314"/>
-    <mergeCell ref="C259:C260"/>
-    <mergeCell ref="D256:D258"/>
-    <mergeCell ref="D259:D260"/>
-    <mergeCell ref="C261:C262"/>
-    <mergeCell ref="C263:C264"/>
-    <mergeCell ref="D261:D262"/>
-    <mergeCell ref="D263:D264"/>
-    <mergeCell ref="C252:C253"/>
-    <mergeCell ref="D252:D253"/>
-    <mergeCell ref="C254:C255"/>
-    <mergeCell ref="D254:D255"/>
-    <mergeCell ref="C256:C258"/>
-    <mergeCell ref="C296:C302"/>
-    <mergeCell ref="D305:D307"/>
-    <mergeCell ref="D296:D302"/>
-    <mergeCell ref="C305:C307"/>
-    <mergeCell ref="B305:B307"/>
-    <mergeCell ref="C284:C287"/>
-    <mergeCell ref="D284:D287"/>
-    <mergeCell ref="C288:C291"/>
-    <mergeCell ref="D288:D291"/>
-    <mergeCell ref="C292:C295"/>
-    <mergeCell ref="D292:D295"/>
-    <mergeCell ref="C227:C228"/>
-    <mergeCell ref="D227:D228"/>
-    <mergeCell ref="C225:C226"/>
-    <mergeCell ref="D225:D226"/>
-    <mergeCell ref="C246:C248"/>
-    <mergeCell ref="C281:C283"/>
-    <mergeCell ref="D281:D283"/>
-    <mergeCell ref="C274:C276"/>
-    <mergeCell ref="D274:D276"/>
-    <mergeCell ref="C277:C280"/>
-    <mergeCell ref="D277:D280"/>
-    <mergeCell ref="C265:C267"/>
-    <mergeCell ref="D265:D267"/>
-    <mergeCell ref="C271:C273"/>
-    <mergeCell ref="D271:D273"/>
-    <mergeCell ref="C268:C270"/>
-    <mergeCell ref="D268:D270"/>
-    <mergeCell ref="B224:B251"/>
-    <mergeCell ref="C206:C207"/>
-    <mergeCell ref="D206:D207"/>
-    <mergeCell ref="C208:C215"/>
-    <mergeCell ref="D208:D215"/>
-    <mergeCell ref="D246:D248"/>
-    <mergeCell ref="C249:C251"/>
-    <mergeCell ref="D249:D251"/>
-    <mergeCell ref="C242:C243"/>
-    <mergeCell ref="D242:D243"/>
-    <mergeCell ref="C244:C245"/>
-    <mergeCell ref="D244:D245"/>
-    <mergeCell ref="C232:C233"/>
-    <mergeCell ref="D232:D233"/>
-    <mergeCell ref="C234:C235"/>
-    <mergeCell ref="D234:D235"/>
-    <mergeCell ref="C236:C237"/>
-    <mergeCell ref="D236:D237"/>
-    <mergeCell ref="C238:C240"/>
-    <mergeCell ref="D238:D240"/>
-    <mergeCell ref="D171:D177"/>
-    <mergeCell ref="C166:C170"/>
-    <mergeCell ref="B164:B170"/>
-    <mergeCell ref="D155:D158"/>
-    <mergeCell ref="C155:C158"/>
-    <mergeCell ref="C216:C223"/>
-    <mergeCell ref="B203:B223"/>
-    <mergeCell ref="D216:D223"/>
-    <mergeCell ref="B194:B195"/>
-    <mergeCell ref="B155:B158"/>
-    <mergeCell ref="B196:B198"/>
-    <mergeCell ref="C150:C151"/>
-    <mergeCell ref="B153:B154"/>
-    <mergeCell ref="C153:C154"/>
-    <mergeCell ref="D153:D154"/>
-    <mergeCell ref="B150:B152"/>
-    <mergeCell ref="D150:D152"/>
-    <mergeCell ref="C203:C204"/>
-    <mergeCell ref="D203:D204"/>
-    <mergeCell ref="C160:C162"/>
-    <mergeCell ref="B160:B163"/>
-    <mergeCell ref="D160:D162"/>
-    <mergeCell ref="C200:C201"/>
-    <mergeCell ref="B200:B201"/>
-    <mergeCell ref="D200:D201"/>
-    <mergeCell ref="D181:D184"/>
-    <mergeCell ref="C188:C191"/>
-    <mergeCell ref="B188:B191"/>
-    <mergeCell ref="D188:D191"/>
-    <mergeCell ref="B179:B180"/>
-    <mergeCell ref="C181:C184"/>
-    <mergeCell ref="B181:B184"/>
-    <mergeCell ref="D166:D170"/>
-    <mergeCell ref="C171:C177"/>
-    <mergeCell ref="B171:B177"/>
-    <mergeCell ref="C147:C148"/>
-    <mergeCell ref="D147:D148"/>
-    <mergeCell ref="D117:D119"/>
-    <mergeCell ref="D63:D65"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="C87:C95"/>
-    <mergeCell ref="B87:B95"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="D104:D106"/>
-    <mergeCell ref="B107:B108"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="B110:B111"/>
-    <mergeCell ref="C130:C131"/>
-    <mergeCell ref="D130:D131"/>
-    <mergeCell ref="B130:B131"/>
-    <mergeCell ref="D132:D134"/>
-    <mergeCell ref="C132:C134"/>
-    <mergeCell ref="B132:B134"/>
-    <mergeCell ref="B147:B149"/>
-    <mergeCell ref="B139:B142"/>
-    <mergeCell ref="C135:C136"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="D27:D31"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="D60:D62"/>
-    <mergeCell ref="C60:C62"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B27:B31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -9788,17 +10204,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43" style="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.33203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.6640625" style="27" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="73.5" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="18"/>
@@ -9809,13 +10225,13 @@
         <v>816</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>829</v>
-      </c>
-      <c r="C1" s="18" t="s">
+        <v>824</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>815</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>7</v>
@@ -9825,364 +10241,651 @@
       <c r="A2" s="18" t="s">
         <v>817</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="34" t="s">
         <v>818</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>824</v>
-      </c>
-      <c r="D2" s="18" t="s">
+      <c r="C2" s="28" t="s">
+        <v>866</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>819</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
         <v>817</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="18" t="s">
-        <v>825</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="23"/>
+    </row>
+    <row r="4" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
         <v>817</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="18" t="s">
-        <v>828</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
-        <v>822</v>
-      </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="18" t="s">
-        <v>826</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>821</v>
-      </c>
+      <c r="B4" s="34"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="23"/>
+    </row>
+    <row r="5" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
+        <v>817</v>
+      </c>
+      <c r="B5" s="34"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="23"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>823</v>
-      </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="18" t="s">
-        <v>827</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
         <v>817</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>831</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>832</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>833</v>
-      </c>
+      <c r="B6" s="34"/>
+      <c r="C6" s="28" t="s">
+        <v>867</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
+        <v>817</v>
+      </c>
+      <c r="B7" s="34"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="23"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>817</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="23"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+      <c r="B8" s="34"/>
+      <c r="C8" s="28" t="s">
+        <v>868</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
         <v>817</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="23"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
+      <c r="B9" s="34"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+    </row>
+    <row r="10" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
         <v>817</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="23"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="23"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="23"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="23"/>
+        <v>822</v>
+      </c>
+      <c r="B11" s="34"/>
+      <c r="C11" s="31" t="s">
+        <v>869</v>
+      </c>
+      <c r="D11" s="30"/>
+    </row>
+    <row r="12" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>822</v>
+      </c>
+      <c r="B12" s="34"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="30"/>
+    </row>
+    <row r="13" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="22" t="s">
+        <v>822</v>
+      </c>
+      <c r="B13" s="34"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="30"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="23"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="23"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>834</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>835</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="23"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="23"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="23"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="23"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="23"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="23"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="23"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="23"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="23"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="23"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="23"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="23"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="23"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="23"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="23"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B32" s="23" t="s">
-        <v>837</v>
-      </c>
-      <c r="C32" s="26" t="s">
-        <v>838</v>
-      </c>
-      <c r="D32" s="24" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="23"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="23"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="23"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="23"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="23"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>840</v>
-      </c>
-      <c r="D38" s="18" t="s">
-        <v>841</v>
-      </c>
+        <v>823</v>
+      </c>
+      <c r="B14" s="34"/>
+      <c r="C14" s="31" t="s">
+        <v>870</v>
+      </c>
+      <c r="D14" s="30"/>
+    </row>
+    <row r="15" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
+        <v>823</v>
+      </c>
+      <c r="B15" s="34"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="30"/>
+    </row>
+    <row r="16" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
+        <v>823</v>
+      </c>
+      <c r="B16" s="34"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="30"/>
+    </row>
+    <row r="17" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>864</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>865</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B18" s="34"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30"/>
+    </row>
+    <row r="19" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B19" s="34"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
+    </row>
+    <row r="20" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B20" s="34"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30"/>
+    </row>
+    <row r="21" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B21" s="34"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
+    </row>
+    <row r="22" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B22" s="34"/>
+      <c r="C22" s="31" t="s">
+        <v>871</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B23" s="34"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="30"/>
+    </row>
+    <row r="24" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B24" s="34"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="30"/>
+    </row>
+    <row r="25" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B25" s="34"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="30"/>
+    </row>
+    <row r="26" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B26" s="34"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="30"/>
+    </row>
+    <row r="27" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B27" s="34"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="30"/>
+    </row>
+    <row r="28" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B28" s="34"/>
+      <c r="C28" s="31" t="s">
+        <v>872</v>
+      </c>
+      <c r="D28" s="35" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B29" s="34"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="30"/>
+    </row>
+    <row r="30" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B30" s="34"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="30"/>
+    </row>
+    <row r="31" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B31" s="34"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="30"/>
+    </row>
+    <row r="32" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B32" s="34"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="30"/>
+    </row>
+    <row r="33" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B33" s="34"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="30"/>
+    </row>
+    <row r="34" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B34" s="34"/>
+      <c r="C34" s="28" t="s">
+        <v>873</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B35" s="34"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="30"/>
+    </row>
+    <row r="36" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B36" s="34"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="30"/>
+    </row>
+    <row r="37" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B37" s="34"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="30"/>
+    </row>
+    <row r="38" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B38" s="34"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="30"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
         <v>817</v>
       </c>
-      <c r="B39" s="18" t="s">
-        <v>842</v>
-      </c>
-      <c r="D39" s="18" t="s">
-        <v>843</v>
+      <c r="B39" s="23" t="s">
+        <v>826</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>827</v>
+      </c>
+      <c r="D39" s="24" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B40" s="23"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="23"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B41" s="23"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="23"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B42" s="23"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="23"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B43" s="23"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="23"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B44" s="23"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="23"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B45" s="23"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="23"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B46" s="23"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="23"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B47" s="23"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="23"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B48" s="23" t="s">
+        <v>829</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>830</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B49" s="23"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="23"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B50" s="23"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="23"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B51" s="23"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="23"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B52" s="23"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="23"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B53" s="23"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="23"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B54" s="23"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="23"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B55" s="23"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="23"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B56" s="23"/>
+      <c r="C56" s="29"/>
+      <c r="D56" s="23"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B57" s="23"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="23"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B58" s="23"/>
+      <c r="C58" s="29"/>
+      <c r="D58" s="23"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B59" s="23"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="23"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B60" s="23"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="23"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B61" s="23"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="23"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B62" s="23"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="23"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B63" s="23"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="23"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B64" s="23" t="s">
+        <v>832</v>
+      </c>
+      <c r="C64" s="28" t="s">
+        <v>833</v>
+      </c>
+      <c r="D64" s="24" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B65" s="23"/>
+      <c r="C65" s="29"/>
+      <c r="D65" s="23"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B66" s="23"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="23"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B67" s="23"/>
+      <c r="C67" s="29"/>
+      <c r="D67" s="23"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B68" s="23"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="23"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B69" s="23"/>
+      <c r="C69" s="29"/>
+      <c r="D69" s="23"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B70" s="18" t="s">
+        <v>835</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B71" s="18" t="s">
+        <v>837</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>838</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="C32:C37"/>
-    <mergeCell ref="D32:D37"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="C7:C15"/>
-    <mergeCell ref="D7:D15"/>
-    <mergeCell ref="B7:B15"/>
-    <mergeCell ref="C16:C31"/>
-    <mergeCell ref="B16:B31"/>
-    <mergeCell ref="D16:D31"/>
+  <mergeCells count="27">
+    <mergeCell ref="B2:B16"/>
+    <mergeCell ref="D17:D21"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="D22:D27"/>
+    <mergeCell ref="C28:C33"/>
+    <mergeCell ref="D28:D33"/>
+    <mergeCell ref="B17:B38"/>
+    <mergeCell ref="C34:C38"/>
+    <mergeCell ref="D34:D38"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D8:D16"/>
+    <mergeCell ref="C64:C69"/>
+    <mergeCell ref="D64:D69"/>
+    <mergeCell ref="B64:B69"/>
+    <mergeCell ref="C39:C47"/>
+    <mergeCell ref="D39:D47"/>
+    <mergeCell ref="B39:B47"/>
+    <mergeCell ref="C48:C63"/>
+    <mergeCell ref="B48:B63"/>
+    <mergeCell ref="D48:D63"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20190127.1437 by YKBKyle
</commit_message>
<xml_diff>
--- a/MultiLanguageNote.xlsx
+++ b/MultiLanguageNote.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1420" yWindow="8020" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="R" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="884">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4703,12 +4703,300 @@
 of the records whose SuppliersID is equal to any number in (9,10,11)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> ProductName
+,UnitPrice
+,SupplierID
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Products
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>WHERE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> ProductName = 'Tofu' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>OR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> 'Konbu';</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">only retrive column ProductName, UnitPrice, SuppliersID
+of the records whose ProductName is 'Tofu' or 'Konbu'.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Note that when the first condition is TRUE, the second conditon will not be checked. That means once 'Tofu' is found, no 'Konbu' records will be retrived.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> ProductID
+,UnitPrice
+,SupplierID
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Products
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>WHERE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> (SupplierID = 9 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>OR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> SupplierID = 11)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>AND</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> UnitPrice &gt; 15;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>only retrive column ProductID, UnitPrice, SuppliersID of the records
+whose SuppliersID is either 9 or 11, and UnitPrice is greater than 15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> *
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Employees
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>WHERE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>NOT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> City='London' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>AND</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>NOT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> City='Seattle';</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>retrive all columns from table Employees
+except the records whose City is either 'London' or 'Seattle'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4780,6 +5068,13 @@
     <font>
       <sz val="14"/>
       <color theme="5"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -10204,10 +10499,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34:D38"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -10569,137 +10864,143 @@
       <c r="C38" s="29"/>
       <c r="D38" s="30"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B39" s="23" t="s">
-        <v>826</v>
-      </c>
+    <row r="39" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B39" s="34"/>
       <c r="C39" s="28" t="s">
-        <v>827</v>
-      </c>
-      <c r="D39" s="24" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B40" s="23"/>
+        <v>878</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B40" s="34"/>
       <c r="C40" s="29"/>
-      <c r="D40" s="23"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B41" s="23"/>
+      <c r="D40" s="30"/>
+    </row>
+    <row r="41" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B41" s="34"/>
       <c r="C41" s="29"/>
-      <c r="D41" s="23"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B42" s="23"/>
+      <c r="D41" s="30"/>
+    </row>
+    <row r="42" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B42" s="34"/>
       <c r="C42" s="29"/>
-      <c r="D42" s="23"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B43" s="23"/>
+      <c r="D42" s="30"/>
+    </row>
+    <row r="43" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B43" s="34"/>
       <c r="C43" s="29"/>
-      <c r="D43" s="23"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B44" s="23"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="23"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B45" s="23"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="23"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B46" s="23"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="23"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B47" s="23"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="23"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B48" s="23" t="s">
-        <v>829</v>
-      </c>
-      <c r="C48" s="28" t="s">
-        <v>830</v>
-      </c>
-      <c r="D48" s="23" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B49" s="23"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="23"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B50" s="23"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="23"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B51" s="23"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="23"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="18" t="s">
-        <v>817</v>
-      </c>
-      <c r="B52" s="23"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="23"/>
+      <c r="D43" s="30"/>
+    </row>
+    <row r="44" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B44" s="34"/>
+      <c r="C44" s="31" t="s">
+        <v>880</v>
+      </c>
+      <c r="D44" s="35" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B45" s="34"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="30"/>
+    </row>
+    <row r="46" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B46" s="34"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="30"/>
+    </row>
+    <row r="47" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B47" s="34"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="30"/>
+    </row>
+    <row r="48" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B48" s="34"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="30"/>
+    </row>
+    <row r="49" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B49" s="34"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="30"/>
+    </row>
+    <row r="50" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B50" s="34"/>
+      <c r="C50" s="31" t="s">
+        <v>882</v>
+      </c>
+      <c r="D50" s="35" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B51" s="34"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="30"/>
+    </row>
+    <row r="52" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B52" s="34"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="30"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="18" t="s">
         <v>817</v>
       </c>
-      <c r="B53" s="23"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="23"/>
+      <c r="B53" s="23" t="s">
+        <v>826</v>
+      </c>
+      <c r="C53" s="28" t="s">
+        <v>827</v>
+      </c>
+      <c r="D53" s="24" t="s">
+        <v>828</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="18" t="s">
@@ -10769,9 +11070,15 @@
       <c r="A62" s="18" t="s">
         <v>817</v>
       </c>
-      <c r="B62" s="23"/>
-      <c r="C62" s="29"/>
-      <c r="D62" s="23"/>
+      <c r="B62" s="23" t="s">
+        <v>829</v>
+      </c>
+      <c r="C62" s="28" t="s">
+        <v>830</v>
+      </c>
+      <c r="D62" s="23" t="s">
+        <v>831</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="18" t="s">
@@ -10785,15 +11092,9 @@
       <c r="A64" s="18" t="s">
         <v>817</v>
       </c>
-      <c r="B64" s="23" t="s">
-        <v>832</v>
-      </c>
-      <c r="C64" s="28" t="s">
-        <v>833</v>
-      </c>
-      <c r="D64" s="24" t="s">
-        <v>834</v>
-      </c>
+      <c r="B64" s="23"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="23"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="18" t="s">
@@ -10839,48 +11140,172 @@
       <c r="A70" s="18" t="s">
         <v>817</v>
       </c>
-      <c r="B70" s="18" t="s">
-        <v>835</v>
-      </c>
-      <c r="D70" s="18" t="s">
-        <v>836</v>
-      </c>
+      <c r="B70" s="23"/>
+      <c r="C70" s="29"/>
+      <c r="D70" s="23"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="18" t="s">
         <v>817</v>
       </c>
-      <c r="B71" s="18" t="s">
+      <c r="B71" s="23"/>
+      <c r="C71" s="29"/>
+      <c r="D71" s="23"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B72" s="23"/>
+      <c r="C72" s="29"/>
+      <c r="D72" s="23"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B73" s="23"/>
+      <c r="C73" s="29"/>
+      <c r="D73" s="23"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B74" s="23"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="23"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B75" s="23"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="23"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B76" s="23"/>
+      <c r="C76" s="29"/>
+      <c r="D76" s="23"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B77" s="23"/>
+      <c r="C77" s="29"/>
+      <c r="D77" s="23"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B78" s="23" t="s">
+        <v>832</v>
+      </c>
+      <c r="C78" s="28" t="s">
+        <v>833</v>
+      </c>
+      <c r="D78" s="24" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B79" s="23"/>
+      <c r="C79" s="29"/>
+      <c r="D79" s="23"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B80" s="23"/>
+      <c r="C80" s="29"/>
+      <c r="D80" s="23"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B81" s="23"/>
+      <c r="C81" s="29"/>
+      <c r="D81" s="23"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B82" s="23"/>
+      <c r="C82" s="29"/>
+      <c r="D82" s="23"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B83" s="23"/>
+      <c r="C83" s="29"/>
+      <c r="D83" s="23"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B84" s="18" t="s">
+        <v>835</v>
+      </c>
+      <c r="D84" s="18" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B85" s="18" t="s">
         <v>837</v>
       </c>
-      <c r="D71" s="18" t="s">
+      <c r="D85" s="18" t="s">
         <v>838</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="33">
+    <mergeCell ref="C39:C43"/>
+    <mergeCell ref="D39:D43"/>
+    <mergeCell ref="C44:C49"/>
+    <mergeCell ref="D44:D49"/>
+    <mergeCell ref="B17:B52"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="D50:D52"/>
     <mergeCell ref="B2:B16"/>
     <mergeCell ref="D17:D21"/>
     <mergeCell ref="C22:C27"/>
     <mergeCell ref="D22:D27"/>
     <mergeCell ref="C28:C33"/>
     <mergeCell ref="D28:D33"/>
-    <mergeCell ref="B17:B38"/>
     <mergeCell ref="C34:C38"/>
     <mergeCell ref="D34:D38"/>
     <mergeCell ref="C8:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="D8:D16"/>
-    <mergeCell ref="C64:C69"/>
-    <mergeCell ref="D64:D69"/>
-    <mergeCell ref="B64:B69"/>
-    <mergeCell ref="C39:C47"/>
-    <mergeCell ref="D39:D47"/>
-    <mergeCell ref="B39:B47"/>
-    <mergeCell ref="C48:C63"/>
-    <mergeCell ref="B48:B63"/>
-    <mergeCell ref="D48:D63"/>
+    <mergeCell ref="C78:C83"/>
+    <mergeCell ref="D78:D83"/>
+    <mergeCell ref="B78:B83"/>
+    <mergeCell ref="C53:C61"/>
+    <mergeCell ref="D53:D61"/>
+    <mergeCell ref="B53:B61"/>
+    <mergeCell ref="C62:C77"/>
+    <mergeCell ref="B62:B77"/>
+    <mergeCell ref="D62:D77"/>
     <mergeCell ref="C17:C21"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="D2:D5"/>

</xml_diff>